<commit_message>
changed pwd in config
changed pwd in config
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="372" windowWidth="22980" windowHeight="9228" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="372" windowWidth="22980" windowHeight="9228" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="91">
   <si>
     <t>City</t>
   </si>
@@ -443,6 +443,19 @@
   <si>
     <t xml:space="preserve">select PAYR_DSPL_NM  from OLE.payer where PAYR_NM='{$payerName}'
 </t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>select * from ole.srch_consol_tbl
+where PROV_TAX_ID_NBR ='{$tin}'
+and CP_PAY_METH_CD &lt;&gt; 'CHK'
+and CP_SETL_DT&gt;='2018-03-30' and CP_SETL_DT&lt;='2018-05-29'
+order by CP_SETL_DT desc</t>
+  </si>
+  <si>
+    <t>Test_1234</t>
   </si>
 </sst>
 </file>
@@ -1251,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1444,8 +1457,16 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1459,7 +1480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1555,7 +1576,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added queries in excel
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="94">
   <si>
     <t>City</t>
   </si>
@@ -459,6 +459,14 @@
   </si>
   <si>
     <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select t.PROV_TIN_NBR  from OLE.PORTAL_USER_TIN t join 
+ OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID 
+ where u.SSO_ID='{$id}' and  u.STS_CD='A'</t>
   </si>
 </sst>
 </file>
@@ -1267,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,7 +1485,19 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
committing changes for CSR
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="9105" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="615" windowWidth="20730" windowHeight="8985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="119">
   <si>
     <t>City</t>
   </si>
@@ -576,52 +576,6 @@
   </si>
   <si>
     <t>select * from ole.EPRA_STATUS where CONSL_PAY_NBR='{$paymentNo}'</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>Select  p.prov_tax_id_nbr
-from PP024.UNCONSOLIDATED_PAYMENT ucp, PP024.CONSOLIDATED_PAYMENT cp, PP024.PROVIDER p
-where cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
-and cp.PROV_KEY_ID = p.PROV_KEY_ID
-and ucp.ORIG_BPR01_CD is not null
-and ucp.ORIG_BPR01_DTTM is not null
-and ucp.UCONSL_PAY_KEY_ID not in (select cup.uconsl_pay_key_id from PP024.CLAIM_UNCONSOLIDATED_PAYMENT cup)
-and cp.setl_dt &lt;= current date
-order by cp.setl_dt desc
-fetch first 1 rows only
-with ur</t>
-  </si>
-  <si>
-    <t>Select cp.consl_pay_nbr, cp.dspl_consl_pay_nbr, cp.setl_dt, cp.pay_meth_cd,(Days(current date) - days(cp.setl_dt)) as date_diff
-from PP024.UNCONSOLIDATED_PAYMENT ucp, PP024.CONSOLIDATED_PAYMENT cp, PP024.PROVIDER p
-where cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
-and cp.PROV_KEY_ID = p.PROV_KEY_ID
-and ucp.ORIG_BPR01_CD is not null
-and ucp.ORIG_BPR01_DTTM is not null
-and ucp.UCONSL_PAY_KEY_ID not in (select cup.uconsl_pay_key_id from PP024.CLAIM_UNCONSOLIDATED_PAYMENT cup)
-and cp.setl_dt &lt;= current date
-and p.prov_tax_id_nbr =  '{$tin}'
-order by cp.setl_dt desc
-fetch first 1 rows only
-with ur</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Select p.prov_tax_id_nbr
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
-where cp.prov_key_id = p.prov_key_id
-and cp.setl_dt &gt; current date - 100 days
-group by p.prov_tax_id_nbr
-having count(*) &lt; 100
-order by count(*) desc
-fetch first row only</t>
   </si>
 </sst>
 </file>
@@ -1430,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,30 +1705,6 @@
       </c>
       <c r="B35" s="7" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="225" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed data file for ach and vcp queries
changed data file for ach and vcp queries
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -570,13 +570,7 @@
 where cp.prov_key_id = p.prov_key_id and p.prov_tax_id_nbr='{$tin}' and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'</t>
   </si>
   <si>
-    <t>SELECT P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
-  </si>
-  <si>
     <t>For Finding Zero Dollar ACH Payment</t>
-  </si>
-  <si>
-    <t>SELECT P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
   </si>
   <si>
     <t>For Finding Zero Dollar VCP Payment</t>
@@ -609,6 +603,12 @@
 having count(*) &lt; 30
 order by count(*) desc
 fetch first row only</t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR , P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1420,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B36" sqref="B36:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1723,7 +1723,7 @@
         <v>113</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -1734,34 +1734,34 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" t="s">
         <v>116</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C37" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing query changes in data file
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -13,12 +13,11 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="137">
   <si>
     <t>City</t>
   </si>
@@ -282,9 +281,6 @@
     <t>AV</t>
   </si>
   <si>
-    <t>select * from OLE.PORTAL_USER p where p.USERNAME='{$id}'</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -325,10 +321,6 @@
   </si>
   <si>
     <t>jsjd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select t.PROV_TIN_NBR from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.USERNAME='{$id}'
-</t>
   </si>
   <si>
     <t>aautomation21</t>
@@ -353,11 +345,6 @@
 where p.EMAIL_ADR_TXT='{$email}' and pv.PAY_PROC_CD_DESC='User Type Code'</t>
   </si>
   <si>
-    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt 
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where p.USERNAME='{$user}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
-  </si>
-  <si>
     <t xml:space="preserve">AUBILL5903 </t>
   </si>
   <si>
@@ -409,26 +396,7 @@
     <t>18</t>
   </si>
   <si>
-    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in( '{$id}' ) and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc
-</t>
-  </si>
-  <si>
-    <t>select * from OLE.PORTAL_USER p join
-OLE.PORTAL_USER_PAYER_TIN py 
-on p.PORTAL_USER_ID=py.PORTAL_USER_ID 
-where  py.PAYR_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
-  </si>
-  <si>
     <t>19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  
-select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
-on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
- on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
-where  bs.IDENTIFIER_NBR='{$tin}'  and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
   </si>
   <si>
     <t>VO</t>
@@ -540,7 +508,58 @@
     <t>For finding Remit payments consolidate number with their settlement date</t>
   </si>
   <si>
-    <t>select  cp.DSPL_CONSL_PAY_NBR,cp.setl_dt,(Days(current date) - days(cp.setl_dt)) as date_diff
+    <t>select DISTINCT  cp.DSPL_CONSL_PAY_NBR, p.PROV_TAX_ID_NBR,cp.setl_dt from PP001.PROVIDER p join PP001.CONSOLIDATED_PAYMENT cp
+on cp.PROV_KEY_ID = p.PROV_KEY_ID
+where cp.DSPL_CONSL_PAY_NBR ='{$paymentNo}'
+order by cp.setl_dt desc
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Select count(*) as RECORD_COUNT
+from {$schema}.CONSOLIDATED_PAYMENT cp, {$schema}.PROVIDER p
+where cp.prov_key_id = p.prov_key_id and p.prov_tax_id_nbr='{$tin}' and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'</t>
+  </si>
+  <si>
+    <t>For Finding Zero Dollar ACH Payment</t>
+  </si>
+  <si>
+    <t>For Finding Zero Dollar VCP Payment</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR , P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>select * from ole.epra_status es join  pp001.consolidated_payment cp
+ on es.CONSL_PAY_NBR=cp.CONSL_PAY_NBR
+where es.PAYR_SCHM_NM='PP001' and cp.DSPL_CONSL_PAY_NBR='{$paymentNo}'</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>select  cp.DSPL_CONSL_PAY_NBR,cp.setl_dt,(Days(current date) - days(cp.setl_dt)) as date_diff,cp.CONSL_PAY_NBR
 from PP001.CONSOLIDATED_PAYMENT cp 
 join OLE.PROC_CTL pc on cp.PROC_CTL_ID=pc.PROC_CTL_ID
 where  cp.CONSL_PAY_NBR not in (select CONSL_PAY_NBR from ole.EPRA_STATUS)
@@ -551,38 +570,18 @@
 with ur</t>
   </si>
   <si>
-    <t>select DISTINCT  cp.DSPL_CONSL_PAY_NBR, p.PROV_TAX_ID_NBR,cp.setl_dt from PP001.PROVIDER p join PP001.CONSOLIDATED_PAYMENT cp
-on cp.PROV_KEY_ID = p.PROV_KEY_ID
-where cp.DSPL_CONSL_PAY_NBR ='{$paymentNo}'
-order by cp.setl_dt desc
-fetch first row only
-with ur</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Select count(*) as RECORD_COUNT
-from {$schema}.CONSOLIDATED_PAYMENT cp, {$schema}.PROVIDER p
-where cp.prov_key_id = p.prov_key_id and p.prov_tax_id_nbr='{$tin}' and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'</t>
-  </si>
-  <si>
-    <t>For Finding Zero Dollar ACH Payment</t>
-  </si>
-  <si>
-    <t>For Finding Zero Dollar VCP Payment</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>37</t>
+    <t>select cs.CLM_DOC_835_LOBJ from PP001.CONSOLIDATED_STORAGE  cs where cs.CONSL_PAY_NBR= '{$consolPayNbr}'</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>delete from PP001.CONSOLIDATED_STORAGE  cs where  cs.CONSL_PAY_NBR= '{$consolPayNbr}'</t>
+  </si>
+  <si>
+    <t>update PP001.CONSOLIDATED_STORAGE  cs
+set cs.CLM_DOC_835_LOBJ='{$clobData}'
+ where  cs.CONSL_PAY_NBR= '{$consolPayNbr}'</t>
   </si>
   <si>
     <t>Select p.prov_tax_id_nbr
@@ -590,25 +589,63 @@
 where cp.prov_key_id = p.prov_key_id
 and cp.setl_dt &gt; current date - 100 days
 group by p.prov_tax_id_nbr
-having count(*) &lt; 30
+having (count(*) between 1 and 30)
 order by count(*) desc
 fetch first row only</t>
   </si>
   <si>
-    <t>Select p.prov_tax_id_nbr
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
-where cp.prov_key_id = p.prov_key_id
-and cp.setl_dt &gt; current date - 180 days
-group by p.prov_tax_id_nbr
-having count(*) &lt; 30
-order by count(*) desc
-fetch first row only</t>
-  </si>
-  <si>
-    <t>SELECT CP.DSPL_CONSL_PAY_NBR , P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
-  </si>
-  <si>
-    <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
+    <t>nonEpra Payments</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>For getting consol pay number from consolidated payment table by passing a particular tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select DISTINCT  cp.DSPL_CONSL_PAY_NBR,cp.CONSL_PAY_NBR,cp.setl_dt,(Days(current date) - days(cp.setl_dt)) as date_diff from PP001.PROVIDER p join PP001.CONSOLIDATED_PAYMENT cp
+on cp.PROV_KEY_ID = p.PROV_KEY_ID
+where p.PROV_TAX_ID_NBR='{$tin}'
+order by cp.setl_dt desc
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p where p.SSO_ID='{$id}'</t>
+  </si>
+  <si>
+    <t>userTest808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select t.PROV_TIN_NBR from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.SSO_ID='{$id}'
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.SSO_ID not in( '{$id}' ) and p.SSO_ID not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc
+</t>
+  </si>
+  <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where p.SSO_ID='{$user}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
+on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
+ on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
+where  bs.IDENTIFIER_NBR='{$tin}'  and p.STS_CD='A' and p.SSO_ID not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p join
+OLE.PORTAL_USER_PAYER_TIN py 
+on p.PORTAL_USER_ID=py.PORTAL_USER_ID 
+where  py.PAYR_TIN_NBR='{$tin}' and p.STS_CD='A' and p.SSO_ID not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
   </si>
 </sst>
 </file>
@@ -647,12 +684,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -668,7 +711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -689,6 +732,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -994,7 +1040,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" activeCellId="1" sqref="I2 H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,7 +1110,7 @@
         <v>29</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1143,7 +1189,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>11</v>
@@ -1417,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:B37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,7 +1549,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1511,7 +1557,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>58</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -1519,15 +1565,15 @@
         <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>80</v>
+      <c r="B11" s="12" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1535,7 +1581,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -1543,7 +1589,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1551,7 +1597,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -1559,209 +1605,255 @@
         <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>111</v>
+        <v>119</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
         <v>99</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
         <v>102</v>
-      </c>
-      <c r="C32" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C37" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="B40" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="7" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1775,7 +1867,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1792,19 +1884,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1812,22 +1904,22 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1835,22 +1927,22 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1858,19 +1950,19 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1878,10 +1970,10 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="D5">
         <v>656565</v>
@@ -1892,13 +1984,13 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1906,22 +1998,22 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1929,22 +2021,22 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing changes for Search Remittance
Committing changes for Search Remittance
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="492" windowWidth="22980" windowHeight="9108" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="9105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,11 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="133">
   <si>
     <t>City</t>
   </si>
@@ -609,6 +608,57 @@
   </si>
   <si>
     <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and cp.setl_dt between (current date - 90 days) and current date
+order by cp.SETL_DT
+fetch first row only
+with ur
+</t>
+  </si>
+  <si>
+    <t>Select cp.DSPL_CONSL_PAY_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and p.prov_tax_id_nbr ='{$tin}'
+order by cp.SETL_DT DESC
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and cp.setl_dt between (current date - 30 days) and current date
+group by p.prov_tax_id_nbr
+having count(*) &lt; 10
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Select ucp.UCONSL_PAY_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp
+where cp.consl_pay_nbr = ucp.consl_pay_nbr
+and cp.prov_key_id = p.prov_key_id
+and p.prov_tax_id_nbr  ='{$tin}'
+order by cp.SETL_DT DESC
+fetch first row only
+with ur</t>
   </si>
 </sst>
 </file>
@@ -997,16 +1047,16 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1417,20 +1467,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:B37"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1441,7 +1491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1452,7 +1502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1471,7 +1521,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1482,7 +1532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1490,7 +1540,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1498,7 +1548,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1506,7 +1556,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -1522,7 +1572,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -1530,7 +1580,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -1546,7 +1596,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1562,7 +1612,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>74</v>
       </c>
@@ -1570,7 +1620,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>75</v>
       </c>
@@ -1578,7 +1628,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1586,7 +1636,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>79</v>
       </c>
@@ -1594,7 +1644,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -1602,7 +1652,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>85</v>
       </c>
@@ -1610,7 +1660,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>87</v>
       </c>
@@ -1618,7 +1668,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>90</v>
       </c>
@@ -1626,7 +1676,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>91</v>
       </c>
@@ -1634,7 +1684,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>93</v>
       </c>
@@ -1642,7 +1692,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>94</v>
       </c>
@@ -1658,7 +1708,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>96</v>
       </c>
@@ -1666,7 +1716,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>98</v>
       </c>
@@ -1685,7 +1735,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="172.9" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>104</v>
       </c>
@@ -1707,7 +1757,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="172.9" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>109</v>
       </c>
@@ -1718,7 +1768,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="115.15" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>113</v>
       </c>
@@ -1734,7 +1784,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>119</v>
       </c>
@@ -1745,7 +1795,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>118</v>
       </c>
@@ -1756,12 +1806,44 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1778,13 +1860,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1962,7 +2044,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding data file mysql connector
adding data file mysql connector
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="151">
   <si>
     <t>City</t>
   </si>
@@ -649,6 +649,66 @@
   </si>
   <si>
     <t>Change it</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Getting user with terms and conditions indicator as N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select * from  OLE.portal_user p  join OLE.portal_user_tin pt
+ on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+ where p.TC_ACCEPT_IND='N' and p.STS_CD='A'  and pt.PROV_TIN_NBR not in ('010553448')
+ and p.SSO_ID not in ('userTest808')
+ order by 
+ p.CREAT_DTTM asc
+ fetch first 1 rows only with ur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> update ole.PORTAL_USER p
+ set p.TC_ACCEPT_IND='N' where p.SSO_ID= '{$id}'</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>select pt.PROV_TIN_NBR, pt.ACCESS_LVL,count(*)  as totalUsers  , pu.EMAIL_ADR_TXT ,pu.FST_NM,pu.LST_NM
+from ole.ENROLLED_PROVIDER ep join  ole.PORTAL_USER_TIN pt   on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
+join ole.PORTAL_USER pu on pu.PORTAL_USER_ID=pt.PORTAL_USER_ID
+group by pt.PROV_TIN_NBR,pt.ACCESS_LVL,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.STS_CD
+having count(*) =2  and pt.ACCESS_LVL='A'   and pu.STS_CD='A'
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select * from OLE.ENROLLED_PROVIDER p where p.ENRL_STS_CD='A' and  p.PROV_TIN_NBR not in ('{$id}')
+ order by p.CREAT_DTTM desc FETCH FIRST 1 ROW ONLY  </t>
+  </si>
+  <si>
+    <t>select pt.PROV_TIN_NBR, pt.ACCESS_LVL,count(*)  as totalUsers  , pu.EMAIL_ADR_TXT ,pu.FST_NM,pu.LST_NM
+from ole.ENROLLED_PROVIDER ep join  ole.PORTAL_USER_TIN pt   on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
+join ole.PORTAL_USER pu on pu.PORTAL_USER_ID=pt.PORTAL_USER_ID
+group by pt.PROV_TIN_NBR,pt.ACCESS_LVL,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.STS_CD
+having count(*) =1 and pt.ACCESS_LVL='A'   and pu.STS_CD='A'
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> update ole.PORTAL_USER p
+ set p.TC_ACCEPT_IND='Y' where p.SSO_ID= '{$id}'</t>
+  </si>
+  <si>
+    <t>48</t>
   </si>
 </sst>
 </file>
@@ -1466,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1860,6 +1920,57 @@
       </c>
       <c r="C43" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing changes for SR
committing changes for SR
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="137">
   <si>
     <t>City</t>
   </si>
@@ -659,6 +659,38 @@
 order by cp.SETL_DT DESC
 fetch first row only
 with ur</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select c.PTNT_ACCT_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and p.PROV_TAX_ID_NBR = '{$tin}'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only
+</t>
+  </si>
+  <si>
+    <t>Select sr.SBSCR_ID, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup, PP001.SUBSCRIBER sr
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and c.SBSCR_KEY_ID = sr.SBSCR_KEY_ID
+and p.PROV_TAX_ID_NBR = '840611484'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>43</t>
   </si>
 </sst>
 </file>
@@ -1467,10 +1499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,6 +1876,22 @@
       </c>
       <c r="B42" s="7" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search Remit Test Cases
Search Remit Test Cases
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="9105" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="555" windowWidth="20730" windowHeight="9045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="146">
   <si>
     <t>City</t>
   </si>
@@ -677,6 +677,9 @@
 </t>
   </si>
   <si>
+    <t>43</t>
+  </si>
+  <si>
     <t>Select sr.SBSCR_ID, cp.SETL_DT
 from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup, PP001.SUBSCRIBER sr
 where cp.prov_key_id = p.prov_key_id
@@ -684,13 +687,67 @@
 and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
 and cup.CLM_KEY_ID = c.CLM_KEY_ID
 and c.SBSCR_KEY_ID = sr.SBSCR_KEY_ID
-and p.PROV_TAX_ID_NBR = '840611484'
+and p.PROV_TAX_ID_NBR ='{$tin}'
 and cp.SETL_DT &lt;= current date 
 order by cp.SETL_DT DESC
 fetch first row only</t>
   </si>
   <si>
-    <t>43</t>
+    <t>Select p.PROV_NPI_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and p.PROV_TAX_ID_NBR ='{$tin}'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Select c.CLM_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and p.PROV_TAX_ID_NBR = '{$tin}'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>Select c.PTNT_FST_NM, c.PTNT_LST_NM, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and p.PROV_TAX_ID_NBR = '{$tin}'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>Select p.PROV_TAX_ID_NBR
+from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where ucp.prov_key_id = p.prov_key_id
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_PAY_AMT = '0.00'
+and date(ucp.PROC_DTTM) between (current date - 30 days) and (current date - 5 days)
+fetch first row only</t>
   </si>
 </sst>
 </file>
@@ -1499,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,10 +1945,47 @@
     </row>
     <row r="44" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>135</v>
+    </row>
+    <row r="45" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test cases for My profile
added test cases for My profile
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="155">
   <si>
     <t>City</t>
   </si>
@@ -620,21 +620,6 @@
     <t>userTest808</t>
   </si>
   <si>
-    <t xml:space="preserve">select t.PROV_TIN_NBR from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.SSO_ID='{$id}'
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.SSO_ID not in( '{$id}' ) and p.SSO_ID not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc
-</t>
-  </si>
-  <si>
-    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt 
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where p.SSO_ID='{$user}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
-  </si>
-  <si>
     <t xml:space="preserve">  
 select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
 on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
@@ -709,6 +694,38 @@
   </si>
   <si>
     <t>48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
+where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.SSO_ID not in( '{$id}' ) order by p.LST_CHG_BY_DTTM desc fetch first 1 rows only_x000D_
+</t>
+  </si>
+  <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
+where p.SSO_ID='{$id}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.SSO_ID='{$id}' order by PROV_TIN_NBR asc
+</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
+  on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
+  on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
+where p.SSO_ID='{$id}'</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_PAYER_TIN pt 
+ on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where p.SSO_ID='{$id}'</t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1620,7 +1637,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -1631,15 +1648,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1647,7 +1664,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -1703,7 +1720,7 @@
         <v>76</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -1711,7 +1728,7 @@
         <v>77</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1924,53 +1941,69 @@
     </row>
     <row r="44" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manage user query fix
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="492" windowWidth="22980" windowHeight="9108" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="19200" windowHeight="8730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="155">
   <si>
     <t>City</t>
   </si>
@@ -696,17 +696,6 @@
     <t>48</t>
   </si>
   <si>
-    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
-where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.SSO_ID not in( '{$id}' ) order by p.LST_CHG_BY_DTTM desc fetch first 1 rows only_x000D_
-</t>
-  </si>
-  <si>
-    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
-where p.SSO_ID='{$id}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
-  </si>
-  <si>
     <t xml:space="preserve">select * from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.SSO_ID='{$id}' order by PROV_TIN_NBR asc
 </t>
   </si>
@@ -726,6 +715,16 @@
     <t>select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_PAYER_TIN pt 
  on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
 where p.SSO_ID='{$id}'</t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
+where pt.PROV_TIN_NBR='{$tin}'and p.STS_CD='A'and (p.SSO_ID is null or p.SSO_ID not in ( '{$id}' ) ) fetch first 1 rows only</t>
+  </si>
+  <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
+where p.USERNAME='{$user}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
   </si>
 </sst>
 </file>
@@ -1123,16 +1122,16 @@
       <selection activeCell="H6" activeCellId="1" sqref="I2 H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1545,18 +1544,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1597,7 +1596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1616,7 +1615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1624,7 +1623,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1632,12 +1631,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -1648,23 +1647,23 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>35</v>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -1675,7 +1674,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>71</v>
       </c>
@@ -1699,7 +1698,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>72</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>75</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>77</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>79</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>84</v>
       </c>
@@ -1755,7 +1754,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>85</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>87</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>90</v>
       </c>
@@ -1798,7 +1797,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>92</v>
       </c>
@@ -1817,7 +1816,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="172.9" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>98</v>
       </c>
@@ -1839,7 +1838,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="172.9" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -1850,7 +1849,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="115.15" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>106</v>
       </c>
@@ -1866,7 +1865,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>112</v>
       </c>
@@ -1877,7 +1876,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>111</v>
       </c>
@@ -1888,7 +1887,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>113</v>
       </c>
@@ -1896,7 +1895,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>116</v>
       </c>
@@ -1904,7 +1903,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -1912,7 +1911,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -1920,7 +1919,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1928,7 +1927,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>127</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>135</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>139</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>143</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>147</v>
       </c>
@@ -1992,18 +1991,18 @@
     </row>
     <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B51" s="7" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2020,13 +2019,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2204,7 +2203,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fisl services code optimization
fisl services code optimization
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="156">
   <si>
     <t>City</t>
   </si>
@@ -633,9 +633,6 @@
 where  py.PAYR_TIN_NBR='{$tin}' and p.STS_CD='A' and p.SSO_ID not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
   </si>
   <si>
-    <t>Change it</t>
-  </si>
-  <si>
     <t>43</t>
   </si>
   <si>
@@ -696,17 +693,6 @@
     <t>48</t>
   </si>
   <si>
-    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
-where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.SSO_ID not in( '{$id}' ) order by p.LST_CHG_BY_DTTM desc fetch first 1 rows only_x000D_
-</t>
-  </si>
-  <si>
-    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
-where p.SSO_ID='{$id}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
-  </si>
-  <si>
     <t xml:space="preserve">select * from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.SSO_ID='{$id}' order by PROV_TIN_NBR asc
 </t>
   </si>
@@ -726,6 +712,354 @@
     <t>select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_PAYER_TIN pt 
  on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
 where p.SSO_ID='{$id}'</t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where pt.PROV_TIN_NBR='{$tin}'and p.STS_CD='A'and (p.SSO_ID is null or p.SSO_ID not in ( '{$id}' ) ) fetch first 1 rows only</t>
+  </si>
+  <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
+where p.USERNAME='{$user}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
+  </si>
+  <si>
+    <t>Select count(*) as RECORD_COUNT
+from {$schema}.CONSOLIDATED_PAYMENT cp join {$schema}.PROVIDER p on 
+cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+on cp.PROC_CTL_ID = pc.PROC_CTL_ID 
+where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+and cp.SETL_DT &gt;='{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'</t>
+  </si>
+  <si>
+    <t>select sum(RECORD_COUNT) as RECORD_COUNT from (Select count(*) as RECORD_COUNT
+   from PP001.CONSOLIDATED_PAYMENT cp join PP001.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP002.CONSOLIDATED_PAYMENT cp join PP002.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP003.CONSOLIDATED_PAYMENT cp join PP003.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP004.CONSOLIDATED_PAYMENT cp join PP004.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP005.CONSOLIDATED_PAYMENT cp join PP005.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP006.CONSOLIDATED_PAYMENT cp join PP006.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP007.CONSOLIDATED_PAYMENT cp join PP007.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP008.CONSOLIDATED_PAYMENT cp join PP008.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP009.CONSOLIDATED_PAYMENT cp join PP009.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP010.CONSOLIDATED_PAYMENT cp join PP010.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP011.CONSOLIDATED_PAYMENT cp join PP011.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP012.CONSOLIDATED_PAYMENT cp join PP012.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP013.CONSOLIDATED_PAYMENT cp join PP013.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP014.CONSOLIDATED_PAYMENT cp join PP014.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP015.CONSOLIDATED_PAYMENT cp join PP015.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP016.CONSOLIDATED_PAYMENT cp join PP016.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP017.CONSOLIDATED_PAYMENT cp join PP017.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP018.CONSOLIDATED_PAYMENT cp join PP018.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP019.CONSOLIDATED_PAYMENT cp join PP019.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP020.CONSOLIDATED_PAYMENT cp join PP020.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP021.CONSOLIDATED_PAYMENT cp join PP021.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP022.CONSOLIDATED_PAYMENT cp join PP022.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP023.CONSOLIDATED_PAYMENT cp join PP023.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP024.CONSOLIDATED_PAYMENT cp join PP024.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP025.CONSOLIDATED_PAYMENT cp join PP025.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP026.CONSOLIDATED_PAYMENT cp join PP026.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP027.CONSOLIDATED_PAYMENT cp join PP027.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP028.CONSOLIDATED_PAYMENT cp join PP028.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP029.CONSOLIDATED_PAYMENT cp join PP029.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP030.CONSOLIDATED_PAYMENT cp join PP030.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP031.CONSOLIDATED_PAYMENT cp join PP031.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP032.CONSOLIDATED_PAYMENT cp join PP032.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP033.CONSOLIDATED_PAYMENT cp join PP033.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP034.CONSOLIDATED_PAYMENT cp join PP034.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP035.CONSOLIDATED_PAYMENT cp join PP035.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP036.CONSOLIDATED_PAYMENT cp join PP036.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP037.CONSOLIDATED_PAYMENT cp join PP037.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP038.CONSOLIDATED_PAYMENT cp join PP038.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP039.CONSOLIDATED_PAYMENT cp join PP039.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP040.CONSOLIDATED_PAYMENT cp join PP040.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP041.CONSOLIDATED_PAYMENT cp join PP041.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP042.CONSOLIDATED_PAYMENT cp join PP042.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP043.CONSOLIDATED_PAYMENT cp join PP043.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP044.CONSOLIDATED_PAYMENT cp join PP044.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP045.CONSOLIDATED_PAYMENT cp join PP045.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP046.CONSOLIDATED_PAYMENT cp join PP046.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP047.CONSOLIDATED_PAYMENT cp join PP047.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}')with ur</t>
   </si>
 </sst>
 </file>
@@ -764,18 +1098,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -791,7 +1119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -812,9 +1140,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1543,20 +1868,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
     <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="50.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1567,7 +1893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +1904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1589,7 +1915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1597,7 +1923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1608,7 +1934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1616,7 +1942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1624,7 +1950,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1632,15 +1958,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -1648,26 +1974,26 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1675,7 +2001,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1683,7 +2009,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -1691,7 +2017,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>71</v>
       </c>
@@ -1839,7 +2165,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -1850,7 +2176,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>106</v>
       </c>
@@ -1858,15 +2184,21 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="E35" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>112</v>
       </c>
@@ -1877,7 +2209,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>111</v>
       </c>
@@ -1888,7 +2220,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>113</v>
       </c>
@@ -1896,7 +2228,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>116</v>
       </c>
@@ -1904,7 +2236,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -1912,7 +2244,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -1920,7 +2252,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1928,7 +2260,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>127</v>
       </c>
@@ -1939,71 +2271,71 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="7" t="s">
+    </row>
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C44" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    </row>
+    <row r="46" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="B46" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="B47" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B47" s="7" t="s">
+    </row>
+    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="B48" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting fisl changes for search remittance
commiting fisl changes for search remittance
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="492" windowWidth="22980" windowHeight="9108" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="564" windowWidth="19416" windowHeight="9048" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="170">
   <si>
     <t>City</t>
   </si>
@@ -281,6 +281,9 @@
     <t>AV</t>
   </si>
   <si>
+    <t>select * from OLE.PORTAL_USER p where p.USERNAME='{$id}'</t>
+  </si>
+  <si>
     <t>Username</t>
   </si>
   <si>
@@ -321,6 +324,10 @@
   </si>
   <si>
     <t>jsjd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select t.PROV_TIN_NBR from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.USERNAME='{$id}'
+</t>
   </si>
   <si>
     <t>aautomation21</t>
@@ -345,6 +352,11 @@
 where p.EMAIL_ADR_TXT='{$email}' and pv.PAY_PROC_CD_DESC='User Type Code'</t>
   </si>
   <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where p.USERNAME='{$user}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
+  </si>
+  <si>
     <t xml:space="preserve">AUBILL5903 </t>
   </si>
   <si>
@@ -396,7 +408,26 @@
     <t>18</t>
   </si>
   <si>
+    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in( '{$id}' ) and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc
+</t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p join
+OLE.PORTAL_USER_PAYER_TIN py 
+on p.PORTAL_USER_ID=py.PORTAL_USER_ID 
+where  py.PAYR_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
+  </si>
+  <si>
     <t>19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
+on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
+ on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
+where  bs.IDENTIFIER_NBR='{$tin}'  and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
   </si>
   <si>
     <t>VO</t>
@@ -508,58 +539,7 @@
     <t>For finding Remit payments consolidate number with their settlement date</t>
   </si>
   <si>
-    <t>select DISTINCT  cp.DSPL_CONSL_PAY_NBR, p.PROV_TAX_ID_NBR,cp.setl_dt from PP001.PROVIDER p join PP001.CONSOLIDATED_PAYMENT cp
-on cp.PROV_KEY_ID = p.PROV_KEY_ID
-where cp.DSPL_CONSL_PAY_NBR ='{$paymentNo}'
-order by cp.setl_dt desc
-fetch first row only
-with ur</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Select count(*) as RECORD_COUNT
-from {$schema}.CONSOLIDATED_PAYMENT cp, {$schema}.PROVIDER p
-where cp.prov_key_id = p.prov_key_id and p.prov_tax_id_nbr='{$tin}' and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'</t>
-  </si>
-  <si>
-    <t>For Finding Zero Dollar ACH Payment</t>
-  </si>
-  <si>
-    <t>For Finding Zero Dollar VCP Payment</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>SELECT CP.DSPL_CONSL_PAY_NBR , P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
-  </si>
-  <si>
-    <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>select * from ole.epra_status es join  pp001.consolidated_payment cp
- on es.CONSL_PAY_NBR=cp.CONSL_PAY_NBR
-where es.PAYR_SCHM_NM='PP001' and cp.DSPL_CONSL_PAY_NBR='{$paymentNo}'</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>select  cp.DSPL_CONSL_PAY_NBR,cp.setl_dt,(Days(current date) - days(cp.setl_dt)) as date_diff,cp.CONSL_PAY_NBR
+    <t>select  cp.DSPL_CONSL_PAY_NBR,cp.setl_dt,(Days(current date) - days(cp.setl_dt)) as date_diff
 from PP001.CONSOLIDATED_PAYMENT cp 
 join OLE.PROC_CTL pc on cp.PROC_CTL_ID=pc.PROC_CTL_ID
 where  cp.CONSL_PAY_NBR not in (select CONSL_PAY_NBR from ole.EPRA_STATUS)
@@ -570,18 +550,38 @@
 with ur</t>
   </si>
   <si>
-    <t>select cs.CLM_DOC_835_LOBJ from PP001.CONSOLIDATED_STORAGE  cs where cs.CONSL_PAY_NBR= '{$consolPayNbr}'</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>delete from PP001.CONSOLIDATED_STORAGE  cs where  cs.CONSL_PAY_NBR= '{$consolPayNbr}'</t>
-  </si>
-  <si>
-    <t>update PP001.CONSOLIDATED_STORAGE  cs
-set cs.CLM_DOC_835_LOBJ='{$clobData}'
- where  cs.CONSL_PAY_NBR= '{$consolPayNbr}'</t>
+    <t>select DISTINCT  cp.DSPL_CONSL_PAY_NBR, p.PROV_TAX_ID_NBR,cp.setl_dt from PP001.PROVIDER p join PP001.CONSOLIDATED_PAYMENT cp
+on cp.PROV_KEY_ID = p.PROV_KEY_ID
+where cp.DSPL_CONSL_PAY_NBR ='{$paymentNo}'
+order by cp.setl_dt desc
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Select count(*) as RECORD_COUNT
+from {$schema}.CONSOLIDATED_PAYMENT cp, {$schema}.PROVIDER p
+where cp.prov_key_id = p.prov_key_id and p.prov_tax_id_nbr='{$tin}' and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'</t>
+  </si>
+  <si>
+    <t>For Finding Zero Dollar ACH Payment</t>
+  </si>
+  <si>
+    <t>For Finding Zero Dollar VCP Payment</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>37</t>
   </si>
   <si>
     <t>Select p.prov_tax_id_nbr
@@ -589,477 +589,302 @@
 where cp.prov_key_id = p.prov_key_id
 and cp.setl_dt &gt; current date - 100 days
 group by p.prov_tax_id_nbr
-having (count(*) between 1 and 30)
+having count(*) &lt; 30
 order by count(*) desc
 fetch first row only</t>
   </si>
   <si>
-    <t>nonEpra Payments</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>For getting consol pay number from consolidated payment table by passing a particular tin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> select DISTINCT  cp.DSPL_CONSL_PAY_NBR,cp.CONSL_PAY_NBR,cp.setl_dt,(Days(current date) - days(cp.setl_dt)) as date_diff from PP001.PROVIDER p join PP001.CONSOLIDATED_PAYMENT cp
-on cp.PROV_KEY_ID = p.PROV_KEY_ID
-where p.PROV_TAX_ID_NBR='{$tin}'
-order by cp.setl_dt desc
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and cp.setl_dt &gt; current date - 180 days
+group by p.prov_tax_id_nbr
+having count(*) &lt; 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR , P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and cp.setl_dt between (current date - 90 days) and current date
+order by cp.SETL_DT
+fetch first row only
+with ur
+</t>
+  </si>
+  <si>
+    <t>Select cp.DSPL_CONSL_PAY_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and p.prov_tax_id_nbr ='{$tin}'
+order by cp.SETL_DT DESC
 fetch first row only
 with ur</t>
   </si>
   <si>
-    <t>select * from OLE.PORTAL_USER p where p.SSO_ID='{$id}'</t>
-  </si>
-  <si>
-    <t>userTest808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  
-select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
-on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
- on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
-where  bs.IDENTIFIER_NBR='{$tin}'  and p.STS_CD='A' and p.SSO_ID not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
-  </si>
-  <si>
-    <t>select * from OLE.PORTAL_USER p join
-OLE.PORTAL_USER_PAYER_TIN py 
-on p.PORTAL_USER_ID=py.PORTAL_USER_ID 
-where  py.PAYR_TIN_NBR='{$tin}' and p.STS_CD='A' and p.SSO_ID not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>Getting user with terms and conditions indicator as N</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> select * from  OLE.portal_user p  join OLE.portal_user_tin pt
- on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
- where p.TC_ACCEPT_IND='N' and p.STS_CD='A'  and pt.PROV_TIN_NBR not in ('010553448')
- and p.SSO_ID not in ('userTest808')
- order by 
- p.CREAT_DTTM asc
- fetch first 1 rows only with ur</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> update ole.PORTAL_USER p
- set p.TC_ACCEPT_IND='N' where p.SSO_ID= '{$id}'</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>select pt.PROV_TIN_NBR, pt.ACCESS_LVL,count(*)  as totalUsers  , pu.EMAIL_ADR_TXT ,pu.FST_NM,pu.LST_NM
-from ole.ENROLLED_PROVIDER ep join  ole.PORTAL_USER_TIN pt   on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
-join ole.PORTAL_USER pu on pu.PORTAL_USER_ID=pt.PORTAL_USER_ID
-group by pt.PROV_TIN_NBR,pt.ACCESS_LVL,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.STS_CD
-having count(*) =2  and pt.ACCESS_LVL='A'   and pu.STS_CD='A'
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Select ucp.UCONSL_PAY_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp
+where cp.consl_pay_nbr = ucp.consl_pay_nbr
+and cp.prov_key_id = p.prov_key_id
+and p.prov_tax_id_nbr  ='{$tin}'
+order by cp.SETL_DT DESC
 fetch first row only
 with ur</t>
   </si>
   <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select c.PTNT_ACCT_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and p.PROV_TAX_ID_NBR = '{$tin}'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only
+</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Select sr.SBSCR_ID, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup, PP001.SUBSCRIBER sr
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and c.SBSCR_KEY_ID = sr.SBSCR_KEY_ID
+and p.PROV_TAX_ID_NBR ='{$tin}'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.PROV_NPI_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and p.PROV_TAX_ID_NBR ='{$tin}'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Select c.CLM_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and p.PROV_TAX_ID_NBR = '{$tin}'
+and cp.SETL_DT &lt;= current date 
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
     <t>47</t>
   </si>
   <si>
-    <t xml:space="preserve"> select * from OLE.ENROLLED_PROVIDER p where p.ENRL_STS_CD='A' and  p.PROV_TIN_NBR not in ('{$id}')
- order by p.CREAT_DTTM desc FETCH FIRST 1 ROW ONLY  </t>
-  </si>
-  <si>
-    <t>select pt.PROV_TIN_NBR, pt.ACCESS_LVL,count(*)  as totalUsers  , pu.EMAIL_ADR_TXT ,pu.FST_NM,pu.LST_NM
-from ole.ENROLLED_PROVIDER ep join  ole.PORTAL_USER_TIN pt   on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
-join ole.PORTAL_USER pu on pu.PORTAL_USER_ID=pt.PORTAL_USER_ID
-group by pt.PROV_TIN_NBR,pt.ACCESS_LVL,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.STS_CD
-having count(*) =1 and pt.ACCESS_LVL='A'   and pu.STS_CD='A'
+    <t>48</t>
+  </si>
+  <si>
+    <t>Select p.PROV_TAX_ID_NBR
+from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where ucp.prov_key_id = p.prov_key_id
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_PAY_AMT = '0.00'
+and date(ucp.PROC_DTTM) between (current date - 30 days) and (current date - 5 days)
+fetch first row only</t>
+  </si>
+  <si>
+    <t>select PROV_TAX_ID_NBR
+from PP001.PROVIDER as p, PP001.CONSOLIDATED_PAYMENT as cp , PP001.NACHA_RESPONSE as nacha
+where p.PROV_KEY_ID =cp.PROV_KEY_ID and nacha.CONSL_PAY_NBR=cp.CONSL_PAY_NBR and RET_TYP_CD='RT'
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>select DSPL_CONSL_PAY_NBR, RET_REASON_CD
+from PP001.PROVIDER as p, PP001.CONSOLIDATED_PAYMENT as cp , PP001.NACHA_RESPONSE as nacha
+where p.PROV_KEY_ID =cp.PROV_KEY_ID and nacha.CONSL_PAY_NBR=cp.CONSL_PAY_NBR and PROV_TAX_ID_NBR='{$tin}'
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>select PROV_TAX_ID_NBR
+from PP001.PROVIDER as p, PP001.UNCONSOLIDATED_PAYMENT as ucp , PP001.NACHA_RESPONSE as nacha
+where p.PROV_KEY_ID =ucp.PROV_KEY_ID and nacha.CONSL_PAY_NBR=ucp.CONSL_PAY_NBR and RET_TYP_CD='RT'
+order by ucp.DEP_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>select UCONSL_PAY_NBR,RET_REASON_CD
+from PP001.PROVIDER as p, PP001.UNCONSOLIDATED_PAYMENT as ucp , PP001.NACHA_RESPONSE as nacha
+where p.PROV_KEY_ID =ucp.PROV_KEY_ID and nacha.CONSL_PAY_NBR=ucp.CONSL_PAY_NBR and RET_TYP_CD='RT'
+order by ucp.DEP_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>Select cp.DSPL_CONSL_PAY_NBR,pay.TYP_DESC,cp.PAY_METH_CD, cp.PAY_STS_TYP_ID
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p,OLE.PAY_STS_TYP pay
+where cp.PROV_KEY_ID = p.PROV_KEY_ID
+and pay.PAY_STS_TYP_ID = cp.PAY_STS_TYP_ID
+and cp.setl_dt &lt;= current date and p.PROV_TAX_ID_NBR='{$tin}' order by cp.setl_dt DESC
 fetch first row only
 with ur</t>
   </si>
   <si>
-    <t xml:space="preserve"> update ole.PORTAL_USER p
- set p.TC_ACCEPT_IND='Y' where p.SSO_ID= '{$id}'</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select * from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.SSO_ID='{$id}' order by PROV_TIN_NBR asc
+    <t xml:space="preserve">By Electronic payment to verify the returned reason </t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP001.CONSOLIDATED_PAYMENT CP, PP001.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>By check number-verify returned reason</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Select cp.DSPL_CONSL_PAY_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p,OLE.PAY_STS_TYP pay
+where cp.PROV_KEY_ID = p.PROV_KEY_ID
+and cp.PAY_METH_CD='NON'
+and cp.PAY_STS_TYP_ID is  null and p.PROV_TAX_ID_NBR='{$tin}'
+and cp.setl_dt &lt;= current date order by cp.setl_dt DESC
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, ole.proc_ctl pc
+where cp.prov_key_id = p.prov_key_id and cp.PROC_CTL_ID=pc.PROC_CTL_ID and pc.EXTRACT_STS_CD='C'
+and cp.setl_dt between (current date - 30 days) and current date
+group by p.prov_tax_id_nbr
+having count(*) &lt; 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>for Payments having meth code as VCP or NON</t>
+  </si>
+  <si>
+    <t>for Payments having DD as Type code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select p.PROV_TAX_ID_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p,OLE.PAY_STS_TYP pay, ole.proc_ctl pc
+where cp.PROV_KEY_ID = p.PROV_KEY_ID and cp.PROC_CTL_ID=pc.PROC_CTL_ID
+and pay.PAY_STS_TYP_ID = cp.PAY_STS_TYP_ID and pc.EXTRACT_STS_CD='C'
+and cp.PAY_METH_CD='{$type}'
+and cp.setl_dt &lt;= current date order by cp.setl_dt DESC
+fetch first row only
+with ur
 </t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
-  on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
-  on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
-where p.SSO_ID='{$id}'</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_PAYER_TIN pt 
- on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where p.SSO_ID='{$id}'</t>
-  </si>
-  <si>
-    <t>select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where pt.PROV_TIN_NBR='{$tin}'and p.STS_CD='A'and (p.SSO_ID is null or p.SSO_ID not in ( '{$id}' ) ) fetch first 1 rows only</t>
-  </si>
-  <si>
-    <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt _x000D_
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID_x000D_
-where p.USERNAME='{$user}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
-  </si>
-  <si>
-    <t>Select count(*) as RECORD_COUNT
-from {$schema}.CONSOLIDATED_PAYMENT cp join {$schema}.PROVIDER p on 
-cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-on cp.PROC_CTL_ID = pc.PROC_CTL_ID 
-where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-and cp.SETL_DT &gt;='{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'</t>
-  </si>
-  <si>
-    <t>select sum(RECORD_COUNT) as RECORD_COUNT from (Select count(*) as RECORD_COUNT
-   from PP001.CONSOLIDATED_PAYMENT cp join PP001.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP002.CONSOLIDATED_PAYMENT cp join PP002.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP003.CONSOLIDATED_PAYMENT cp join PP003.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP004.CONSOLIDATED_PAYMENT cp join PP004.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP005.CONSOLIDATED_PAYMENT cp join PP005.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP006.CONSOLIDATED_PAYMENT cp join PP006.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP007.CONSOLIDATED_PAYMENT cp join PP007.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP008.CONSOLIDATED_PAYMENT cp join PP008.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP009.CONSOLIDATED_PAYMENT cp join PP009.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP010.CONSOLIDATED_PAYMENT cp join PP010.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP011.CONSOLIDATED_PAYMENT cp join PP011.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP012.CONSOLIDATED_PAYMENT cp join PP012.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP013.CONSOLIDATED_PAYMENT cp join PP013.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP014.CONSOLIDATED_PAYMENT cp join PP014.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP015.CONSOLIDATED_PAYMENT cp join PP015.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP016.CONSOLIDATED_PAYMENT cp join PP016.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP017.CONSOLIDATED_PAYMENT cp join PP017.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP018.CONSOLIDATED_PAYMENT cp join PP018.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP019.CONSOLIDATED_PAYMENT cp join PP019.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP020.CONSOLIDATED_PAYMENT cp join PP020.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP021.CONSOLIDATED_PAYMENT cp join PP021.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP022.CONSOLIDATED_PAYMENT cp join PP022.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP023.CONSOLIDATED_PAYMENT cp join PP023.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP024.CONSOLIDATED_PAYMENT cp join PP024.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP025.CONSOLIDATED_PAYMENT cp join PP025.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP026.CONSOLIDATED_PAYMENT cp join PP026.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP027.CONSOLIDATED_PAYMENT cp join PP027.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP028.CONSOLIDATED_PAYMENT cp join PP028.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP029.CONSOLIDATED_PAYMENT cp join PP029.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP030.CONSOLIDATED_PAYMENT cp join PP030.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP031.CONSOLIDATED_PAYMENT cp join PP031.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP032.CONSOLIDATED_PAYMENT cp join PP032.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP033.CONSOLIDATED_PAYMENT cp join PP033.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP034.CONSOLIDATED_PAYMENT cp join PP034.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP035.CONSOLIDATED_PAYMENT cp join PP035.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP036.CONSOLIDATED_PAYMENT cp join PP036.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP037.CONSOLIDATED_PAYMENT cp join PP037.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP038.CONSOLIDATED_PAYMENT cp join PP038.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP039.CONSOLIDATED_PAYMENT cp join PP039.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP040.CONSOLIDATED_PAYMENT cp join PP040.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP041.CONSOLIDATED_PAYMENT cp join PP041.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP042.CONSOLIDATED_PAYMENT cp join PP042.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP043.CONSOLIDATED_PAYMENT cp join PP043.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP044.CONSOLIDATED_PAYMENT cp join PP044.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP045.CONSOLIDATED_PAYMENT cp join PP045.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP046.CONSOLIDATED_PAYMENT cp join PP046.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
-   union
-   Select count(*) as RECORD_COUNT
-   from PP047.CONSOLIDATED_PAYMENT cp join PP047.PROVIDER p on 
-   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
-   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
-   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
-   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}')with ur</t>
+    <t>Select p.PROV_TAX_ID_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p,OLE.PAY_STS_TYP pay, ole.proc_ctl pc
+where cp.PROV_KEY_ID = p.PROV_KEY_ID and cp.PROC_CTL_ID=pc.PROC_CTL_ID
+and cp.PAY_METH_CD='NON' and pc.EXTRACT_STS_CD='C'
+and cp.PAY_STS_TYP_ID is  null
+and cp.setl_dt &lt;= current date order by cp.setl_dt DESC
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>Select cp.DSPL_CONSL_PAY_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, ole.proc_ctl pc, pp001.NACHA_RESPONSE nr
+where cp.PROV_KEY_ID = p.PROV_KEY_ID
+and cp.PROC_CTL_ID = pc.PROC_CTL_ID
+and cp.CONSL_PAY_NBR = nr.CONSL_PAY_NBR
+and pc.EXTRACT_STS_CD = 'C'
+and nr.PAY_METH_CD = 'ACH'
+and nr.RET_STS_CD = 'C'
+and cp.setl_dt &lt;= current date order by cp.setl_dt DESC
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>ACH payments for reoriginated payments</t>
+  </si>
+  <si>
+    <t>Select p.PROV_TAX_ID_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, ole.proc_ctl pc, pp001.NACHA_RESPONSE nr
+where cp.PROV_KEY_ID = p.PROV_KEY_ID
+and cp.PROC_CTL_ID = pc.PROC_CTL_ID
+and cp.CONSL_PAY_NBR = nr.CONSL_PAY_NBR
+and pc.EXTRACT_STS_CD = 'C'
+and nr.PAY_METH_CD = '{$type}'
+and nr.RET_STS_CD = 'C'
+and cp.setl_dt &lt;= current date order by cp.setl_dt DESC
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>Select c.PTNT_FST_NM, c.PTNT_LST_NM, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and p.PROV_TAX_ID_NBR = '{$tin}'
+and cp.SETL_DT &lt;= current date and c.PTNT_FST_NM &lt;&gt; ''
+and c.PTNT_LST_NM &lt;&gt; ''
+order by cp.SETL_DT DESC
+fetch first row only</t>
   </si>
 </sst>
 </file>
@@ -1445,18 +1270,18 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" activeCellId="1" sqref="I2 H6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="14.21875" customWidth="1"/>
     <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
     <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" customWidth="1"/>
     <col min="9" max="9" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1515,7 +1340,7 @@
         <v>29</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1594,7 +1419,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>11</v>
@@ -1868,21 +1693,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="64.21875" customWidth="1"/>
+    <col min="2" max="2" width="82.21875" customWidth="1"/>
     <col min="3" max="3" width="39.44140625" customWidth="1"/>
-    <col min="4" max="4" width="50.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1893,7 +1717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1904,7 +1728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1915,7 +1739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1923,7 +1747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1934,7 +1758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1942,7 +1766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1950,392 +1774,445 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="86.55" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="86.55" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="B26" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="B27" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="172.95" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="172.95" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>97</v>
-      </c>
       <c r="C33" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="86.55" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="8" t="s">
+      <c r="B39" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="188.55" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="101.55" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="159.44999999999999" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" t="s">
         <v>155</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C44" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="144" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="144" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+    </row>
+    <row r="52" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B52" s="7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+    <row r="53" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B53" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>151</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2349,16 +2226,16 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2366,19 +2243,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2386,22 +2263,22 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2409,22 +2286,22 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
         <v>61</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2432,19 +2309,19 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2452,10 +2329,10 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>656565</v>
@@ -2466,13 +2343,13 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2480,22 +2357,22 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
         <v>63</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
         <v>61</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2503,22 +2380,22 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
         <v>61</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing changes for csr search remitance with data file
pushing changes for csr search remitance with data file
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="171">
   <si>
     <t>City</t>
   </si>
@@ -884,6 +884,15 @@
 and cp.SETL_DT &lt;= current date and c.PTNT_FST_NM &lt;&gt; ''
 and c.PTNT_LST_NM &lt;&gt; ''
 order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p 
+where cp.prov_key_id = p.prov_key_id and cp.setl_dt between (current date - 30 days) and current date
+group by p.prov_tax_id_nbr
+having count(*) &lt; 30
+order by count(*) desc
 fetch first row only</t>
   </si>
 </sst>
@@ -1693,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1983,7 +1992,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="172.95" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="172.95" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>109</v>
       </c>
@@ -1994,7 +2003,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>113</v>
       </c>
@@ -2002,7 +2011,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>114</v>
       </c>
@@ -2010,7 +2019,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="86.55" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="86.55" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>119</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>118</v>
       </c>
@@ -2032,7 +2041,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>120</v>
       </c>
@@ -2040,7 +2049,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>124</v>
       </c>
@@ -2048,7 +2057,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>125</v>
       </c>
@@ -2056,7 +2065,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>128</v>
       </c>
@@ -2064,15 +2073,18 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>131</v>
       </c>
@@ -2080,7 +2092,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="188.55" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>133</v>
       </c>
@@ -2088,7 +2100,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="101.55" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>136</v>
       </c>
@@ -2096,7 +2108,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="159.44999999999999" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>138</v>
       </c>
@@ -2104,7 +2116,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>139</v>
       </c>
@@ -2112,7 +2124,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
added missing test cases for view payments payer
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="162">
   <si>
     <t>City</t>
   </si>
@@ -1060,6 +1060,38 @@
    on cp.PROC_CTL_ID = pc.PROC_CTL_ID
    where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
    and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}')with ur</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - {$days} and p.PROV_NPI_NBR is null
+group by p.prov_tax_id_nbr
+having count(*) &lt; 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>For General Payment TIN Only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - {$days} and p.PROV_NPI_NBR is not null
+group by p.prov_tax_id_nbr
+having count(*) &lt; 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>For General Payment NPI Only</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
   </si>
 </sst>
 </file>
@@ -1868,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2244,7 +2276,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -2260,7 +2292,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>127</v>
       </c>
@@ -2271,7 +2303,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>134</v>
       </c>
@@ -2290,7 +2322,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>139</v>
       </c>
@@ -2298,7 +2330,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>140</v>
       </c>
@@ -2314,7 +2346,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>146</v>
       </c>
@@ -2322,7 +2354,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>148</v>
       </c>
@@ -2330,12 +2362,34 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>150</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
csr  saearch remittance cases
csr  saearch remittance cases
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="185">
   <si>
     <t>City</t>
   </si>
@@ -651,59 +651,12 @@
     <t>42</t>
   </si>
   <si>
-    <t xml:space="preserve">Select c.PTNT_ACCT_NBR, cp.SETL_DT
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
-where cp.prov_key_id = p.prov_key_id
-and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
-and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
-and cup.CLM_KEY_ID = c.CLM_KEY_ID
-and p.PROV_TAX_ID_NBR = '{$tin}'
-and cp.SETL_DT &lt;= current date 
-order by cp.SETL_DT DESC
-fetch first row only
-</t>
-  </si>
-  <si>
     <t>43</t>
   </si>
   <si>
-    <t>Select sr.SBSCR_ID, cp.SETL_DT
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup, PP001.SUBSCRIBER sr
-where cp.prov_key_id = p.prov_key_id
-and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
-and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
-and cup.CLM_KEY_ID = c.CLM_KEY_ID
-and c.SBSCR_KEY_ID = sr.SBSCR_KEY_ID
-and p.PROV_TAX_ID_NBR ='{$tin}'
-and cp.SETL_DT &lt;= current date 
-order by cp.SETL_DT DESC
-fetch first row only</t>
-  </si>
-  <si>
-    <t>Select p.PROV_NPI_NBR, cp.SETL_DT
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
-where cp.prov_key_id = p.prov_key_id
-and p.PROV_TAX_ID_NBR ='{$tin}'
-and cp.SETL_DT &lt;= current date 
-order by cp.SETL_DT DESC
-fetch first row only</t>
-  </si>
-  <si>
     <t>44</t>
   </si>
   <si>
-    <t>Select c.CLM_NBR, cp.SETL_DT
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
-where cp.prov_key_id = p.prov_key_id
-and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
-and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
-and cup.CLM_KEY_ID = c.CLM_KEY_ID
-and p.PROV_TAX_ID_NBR = '{$tin}'
-and cp.SETL_DT &lt;= current date 
-order by cp.SETL_DT DESC
-fetch first row only</t>
-  </si>
-  <si>
     <t>45</t>
   </si>
   <si>
@@ -716,50 +669,13 @@
     <t>48</t>
   </si>
   <si>
-    <t>Select p.PROV_TAX_ID_NBR
-from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
-where ucp.prov_key_id = p.prov_key_id
-and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
-and cup.CLM_PAY_AMT = '0.00'
-and date(ucp.PROC_DTTM) between (current date - 30 days) and (current date - 5 days)
-fetch first row only</t>
-  </si>
-  <si>
-    <t>select PROV_TAX_ID_NBR
-from PP001.PROVIDER as p, PP001.CONSOLIDATED_PAYMENT as cp , PP001.NACHA_RESPONSE as nacha
-where p.PROV_KEY_ID =cp.PROV_KEY_ID and nacha.CONSL_PAY_NBR=cp.CONSL_PAY_NBR and RET_TYP_CD='RT'
-order by cp.SETL_DT DESC
-fetch first row only</t>
-  </si>
-  <si>
     <t>49</t>
   </si>
   <si>
-    <t>select DSPL_CONSL_PAY_NBR, RET_REASON_CD
-from PP001.PROVIDER as p, PP001.CONSOLIDATED_PAYMENT as cp , PP001.NACHA_RESPONSE as nacha
-where p.PROV_KEY_ID =cp.PROV_KEY_ID and nacha.CONSL_PAY_NBR=cp.CONSL_PAY_NBR and PROV_TAX_ID_NBR='{$tin}'
-order by cp.SETL_DT DESC
-fetch first row only</t>
-  </si>
-  <si>
     <t>50</t>
   </si>
   <si>
-    <t>select PROV_TAX_ID_NBR
-from PP001.PROVIDER as p, PP001.UNCONSOLIDATED_PAYMENT as ucp , PP001.NACHA_RESPONSE as nacha
-where p.PROV_KEY_ID =ucp.PROV_KEY_ID and nacha.CONSL_PAY_NBR=ucp.CONSL_PAY_NBR and RET_TYP_CD='RT'
-order by ucp.DEP_DT DESC
-fetch first row only</t>
-  </si>
-  <si>
     <t>51</t>
-  </si>
-  <si>
-    <t>select UCONSL_PAY_NBR,RET_REASON_CD
-from PP001.PROVIDER as p, PP001.UNCONSOLIDATED_PAYMENT as ucp , PP001.NACHA_RESPONSE as nacha
-where p.PROV_KEY_ID =ucp.PROV_KEY_ID and nacha.CONSL_PAY_NBR=ucp.CONSL_PAY_NBR and RET_TYP_CD='RT'
-order by ucp.DEP_DT DESC
-fetch first row only</t>
   </si>
   <si>
     <t>52</t>
@@ -777,13 +693,7 @@
 with ur</t>
   </si>
   <si>
-    <t xml:space="preserve">By Electronic payment to verify the returned reason </t>
-  </si>
-  <si>
     <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP001.CONSOLIDATED_PAYMENT CP, PP001.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
-  </si>
-  <si>
-    <t>By check number-verify returned reason</t>
   </si>
   <si>
     <t>54</t>
@@ -874,28 +784,6 @@
 with ur</t>
   </si>
   <si>
-    <t>Select c.PTNT_FST_NM, c.PTNT_LST_NM, cp.SETL_DT
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
-where cp.prov_key_id = p.prov_key_id
-and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
-and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
-and cup.CLM_KEY_ID = c.CLM_KEY_ID
-and p.PROV_TAX_ID_NBR = '{$tin}'
-and cp.SETL_DT &lt;= current date and c.PTNT_FST_NM &lt;&gt; ''
-and c.PTNT_LST_NM &lt;&gt; ''
-order by cp.SETL_DT DESC
-fetch first row only</t>
-  </si>
-  <si>
-    <t>Select p.prov_tax_id_nbr
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p 
-where cp.prov_key_id = p.prov_key_id and cp.setl_dt between (current date - 30 days) and current date
-group by p.prov_tax_id_nbr
-having count(*) &lt; 30
-order by count(*) desc
-fetch first row only</t>
-  </si>
-  <si>
     <t>58</t>
   </si>
   <si>
@@ -939,6 +827,140 @@
   </si>
   <si>
     <t>associate tin with bs user</t>
+  </si>
+  <si>
+    <t>Get the Electronic No For a Tin from above query</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get the tin No for Electronic Payment No Search </t>
+  </si>
+  <si>
+    <t>Get the Check No for a tin from above query</t>
+  </si>
+  <si>
+    <t>select p.PROV_TAX_ID_NBR 
+from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp, OLE.PROC_CTL pc, PP001.CONSOLIDATED_PAYMENT cp
+where cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR and p.PROV_KEY_ID =ucp.PROV_KEY_ID 
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID 
+and pc.EXTRACT_STS_CD='C'
+and cp.setl_dt between current date - 6 MONTHS and current date
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Get the tin No for Check No Search &amp; Electronic No</t>
+  </si>
+  <si>
+    <t>select ucp.UCONSL_PAY_NBR
+from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp,PP001.CONSOLIDATED_PAYMENT cp,OLE.PROC_CTL pc
+where cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and p.PROV_KEY_ID =ucp.PROV_KEY_ID 
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID 
+and p.PROV_TAX_ID_NBR='{$tin}'
+and pc.EXTRACT_STS_CD='C'
+and cp.setl_dt between current date - 6 MONTHS and current date
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>select cp.DSPL_CONSL_PAY_NBR
+from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp,PP001.CONSOLIDATED_PAYMENT cp,OLE.PROC_CTL pc
+where cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and p.PROV_KEY_ID =ucp.PROV_KEY_ID 
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID 
+and p.PROV_TAX_ID_NBR='{$tin}'
+and pc.EXTRACT_STS_CD='C'
+and cp.setl_dt between current date - 6 MONTHS and current date
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Get prov tin number (DOP)</t>
+  </si>
+  <si>
+    <t>select PROV_TAX_ID_NBR
+from PP001.PROVIDER as p,PP001.CONSOLIDATED_PAYMENT cp,OLE.PROC_CTL pc
+where p.PROV_KEY_ID =cp.PROV_KEY_ID
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID
+and cp.setl_dt between (current date - 60 days) and current date
+and pc.EXTRACT_STS_CD='C' 
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select c.PTNT_ACCT_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup,OLE.PROC_CTL pc
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID and cp.PROC_CTL_ID=pc.PROC_CTL_ID
+and p.PROV_TAX_ID_NBR ='{$tin}'
+and pc.EXTRACT_STS_CD='C'
+and cp.SETL_DT between (current date - 60 days) and current date 
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select sr.SBSCR_ID, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup, PP001.SUBSCRIBER sr,OLE.PROC_CTL pc
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and c.SBSCR_KEY_ID = sr.SBSCR_KEY_ID and cp.PROC_CTL_ID=pc.PROC_CTL_ID and pc.EXTRACT_STS_CD='C'
+and p.PROV_TAX_ID_NBR ='{$tin}'
+and cp.SETL_DT between (current date - 60 days) and current date  
+order by cp.SETL_DT DESC
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.PROV_NPI_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p,OLE.PROC_CTL pc
+where cp.prov_key_id = p.prov_key_id and cp.PROC_CTL_ID=pc.PROC_CTL_ID
+and p.PROV_TAX_ID_NBR ='{$tin}'  and pc.EXTRACT_STS_CD='C'
+and cp.SETL_DT between (current date - 60 days) and current date 
+order by cp.SETL_DT DESC
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select c.CLM_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup,OLE.PROC_CTL pc
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID and cp.PROC_CTL_ID=pc.PROC_CTL_ID and pc.EXTRACT_STS_CD='C'
+and p.PROV_TAX_ID_NBR = '{$tin}'
+and cp.SETL_DT between (current date - 60 days) and current date 
+order by cp.SETL_DT DESC
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select c.PTNT_FST_NM, c.PTNT_LST_NM, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup,OLE.PROC_CTL pc
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID and cp.PROC_CTL_ID=pc.PROC_CTL_ID and pc.EXTRACT_STS_CD='C'
+and p.PROV_TAX_ID_NBR = '{$tin}'
+and cp.SETL_DT between (current date - 60 days) and current date  and c.PTNT_FST_NM &lt;&gt; ''
+and c.PTNT_LST_NM &lt;&gt; ''
+order by cp.SETL_DT DESC
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Get Patient first name last name for a tin</t>
+  </si>
+  <si>
+    <t>To get tin by DOP and Zero Payment claims- query taking more than 2 minutes ..need to optimized</t>
+  </si>
+  <si>
+    <t>Select p.PROV_TAX_ID_NBR,cp.SETL_DT
+from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CONSOLIDATED_PAYMENT cp,
+PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup,OLE.PROC_CTL pc
+where ucp.prov_key_id = p.prov_key_id
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID 
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID and pc.EXTRACT_STS_CD='C'
+and cup.CLM_PAY_AMT = '0.00'
+and ucp.PROC_DTTM  between (current date - 180 days) and current date 
+order by ucp.PROC_DTTM DESC
+fetch first row only with ur</t>
   </si>
 </sst>
 </file>
@@ -1749,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2080,7 +2102,7 @@
         <v>118</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
         <v>117</v>
@@ -2102,7 +2124,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="115.95" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>125</v>
       </c>
@@ -2118,201 +2140,213 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>133</v>
-      </c>
       <c r="B44" s="7" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="B48" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="B50" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="B51" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C49" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C51" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>148</v>
-      </c>
       <c r="B52" s="7" t="s">
-        <v>149</v>
+        <v>173</v>
+      </c>
+      <c r="C52" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C57" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="C62" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="72.45" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting latest data file
commiting latest data file
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="207">
   <si>
     <t>City</t>
   </si>
@@ -989,6 +989,263 @@
 order by cp.setl_dt DESC
 fetch first 1 rows only
 with ur</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>select rn.CHECK_NBR
+from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp,PP001.CONSOLIDATED_PAYMENT cp,OLE.PROC_CTL pc,REORIG_NACHA rn
+where rn.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and p.PROV_KEY_ID =ucp.PROV_KEY_ID 
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID 
+and p.PROV_TAX_ID_NBR='{$tin}'
+and pc.EXTRACT_STS_CD='C'
+and cp.setl_dt between current date - 6 MONTHS and current date
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>get check number from Reorigin_nacha table for check payment verifivation</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>select cpd.CHECK_NBR
+from PP001.PROVIDER p, PP001.UNCONSOLIDATED_PAYMENT ucp,PP001.CONSOLIDATED_PAYMENT cp,OLE.PROC_CTL pc,CONSL_PAY_DTL cpd
+where cpd.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and p.PROV_KEY_ID =ucp.PROV_KEY_ID 
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID 
+and p.PROV_TAX_ID_NBR='{$tin}'
+and pc.EXTRACT_STS_CD='C'
+and cp.setl_dt between current date - 6 MONTHS and current date
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>get check number from Consl_pay_dtl table for check payment verifivation</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>select * from ole.SYSTEM_CONFIGURATION sc where sc.PROC_CD in ( 'SRCH_THRSHLD_VAL')</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>select * from ole.SYSTEM_CONFIGURATION sc where sc.PROC_CD in ('SRCH_INTL_FETCH_DAYS') -- 30 Days</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>SELECT PID.PROV_KEY_ID
+from 
+(
+SELECT DISTINCT 'PP001' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP001.PROVIDER UNION
+SELECT DISTINCT 'PP002' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP002.PROVIDER UNION
+SELECT DISTINCT 'PP003' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP003.PROVIDER UNION
+SELECT DISTINCT 'PP004' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP004.PROVIDER UNION
+SELECT DISTINCT 'PP005' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP005.PROVIDER UNION
+SELECT DISTINCT 'PP006' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP006.PROVIDER UNION
+SELECT DISTINCT 'PP007' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP007.PROVIDER UNION
+SELECT DISTINCT 'PP008' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP008.PROVIDER UNION
+SELECT DISTINCT 'PP009' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP009.PROVIDER UNION
+SELECT DISTINCT 'PP010' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP010.PROVIDER UNION
+SELECT DISTINCT 'PP011' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP011.PROVIDER UNION
+SELECT DISTINCT 'PP012' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP012.PROVIDER UNION
+SELECT DISTINCT 'PP013' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP013.PROVIDER UNION
+SELECT DISTINCT 'PP014' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP014.PROVIDER UNION
+SELECT DISTINCT 'PP015' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP015.PROVIDER UNION
+SELECT DISTINCT 'PP016' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP016.PROVIDER UNION
+SELECT DISTINCT 'PP017' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP017.PROVIDER UNION
+SELECT DISTINCT 'PP018' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP018.PROVIDER UNION
+SELECT DISTINCT 'PP019' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP019.PROVIDER UNION
+SELECT DISTINCT 'PP020' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP020.PROVIDER UNION
+SELECT DISTINCT 'PP021' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP021.PROVIDER UNION
+SELECT DISTINCT 'PP022' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP022.PROVIDER UNION
+SELECT DISTINCT 'PP023' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP023.PROVIDER UNION
+SELECT DISTINCT 'PP024' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP024.PROVIDER UNION
+SELECT DISTINCT 'PP025' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP025.PROVIDER UNION
+SELECT DISTINCT 'PP026' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP026.PROVIDER UNION
+SELECT DISTINCT 'PP027' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP027.PROVIDER UNION
+SELECT DISTINCT 'PP028' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP028.PROVIDER UNION
+SELECT DISTINCT 'PP029' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP029.PROVIDER UNION
+SELECT DISTINCT 'PP030' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP030.PROVIDER UNION
+SELECT DISTINCT 'PP031' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP031.PROVIDER UNION
+SELECT DISTINCT 'PP032' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP032.PROVIDER UNION
+SELECT DISTINCT 'PP033' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP033.PROVIDER UNION
+SELECT DISTINCT 'PP034' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP034.PROVIDER UNION
+SELECT DISTINCT 'PP035' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP035.PROVIDER UNION
+SELECT DISTINCT 'PP036' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP036.PROVIDER UNION
+SELECT DISTINCT 'PP037' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP037.PROVIDER UNION
+SELECT DISTINCT 'PP038' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP038.PROVIDER UNION
+SELECT DISTINCT 'PP039' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP039.PROVIDER UNION
+SELECT DISTINCT 'PP040' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP040.PROVIDER UNION
+SELECT DISTINCT 'PP041' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP041.PROVIDER UNION
+SELECT DISTINCT 'PP042' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP042.PROVIDER UNION
+SELECT DISTINCT 'PP043' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP043.PROVIDER UNION
+SELECT DISTINCT 'PP044' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP044.PROVIDER UNION
+SELECT DISTINCT 'PP045' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP045.PROVIDER UNION
+SELECT DISTINCT 'PP046' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP046.PROVIDER UNION
+SELECT DISTINCT 'PP047' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP047.PROVIDER UNION
+SELECT DISTINCT 'PP048' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP048.PROVIDER UNION
+SELECT DISTINCT 'PP049' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP049.PROVIDER UNION
+SELECT DISTINCT 'PP050' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP050.PROVIDER UNION
+SELECT DISTINCT 'PP051' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP051.PROVIDER UNION
+SELECT DISTINCT 'PP052' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP052.PROVIDER UNION
+SELECT DISTINCT 'PP053' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP053.PROVIDER UNION
+SELECT DISTINCT 'PP054' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP054.PROVIDER UNION
+SELECT DISTINCT 'PP055' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP055.PROVIDER UNION
+SELECT DISTINCT 'PP056' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP056.PROVIDER UNION
+SELECT DISTINCT 'PP057' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP057.PROVIDER UNION
+SELECT DISTINCT 'PP058' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP058.PROVIDER UNION
+SELECT DISTINCT 'PP059' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP059.PROVIDER UNION
+SELECT DISTINCT 'PP060' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP060.PROVIDER UNION
+SELECT DISTINCT 'PP061' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP061.PROVIDER UNION
+SELECT DISTINCT 'PP062' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP062.PROVIDER UNION
+SELECT DISTINCT 'PP063' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP063.PROVIDER UNION
+SELECT DISTINCT 'PP064' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP064.PROVIDER UNION
+SELECT DISTINCT 'PP065' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP065.PROVIDER UNION
+SELECT DISTINCT 'PP066' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP066.PROVIDER UNION
+SELECT DISTINCT 'PP067' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP067.PROVIDER UNION
+SELECT DISTINCT 'PP068' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP068.PROVIDER UNION
+SELECT DISTINCT 'PP069' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP069.PROVIDER UNION
+SELECT DISTINCT 'PP070' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP070.PROVIDER UNION
+SELECT DISTINCT 'PP071' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP071.PROVIDER UNION
+SELECT DISTINCT 'PP072' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP072.PROVIDER UNION
+SELECT DISTINCT 'PP073' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP073.PROVIDER UNION
+SELECT DISTINCT 'PP074' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP074.PROVIDER UNION
+SELECT DISTINCT 'PP075' AS PAYER, PROV_KEY_ID, PROV_TAX_ID_NBR FROM PP075.PROVIDER
+)PID
+where 
+PID.PROV_TAX_ID_NBR='{$tin}'</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT count(PID.CONSL_PAY_NBR) as REC_COUNT from 
+(
+SELECT DISTINCT 'PP001' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID,PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP001.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP002' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP002.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP003' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP003.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP004' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP004.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP005' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP005.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP006' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP006.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP007' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP007.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP008' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP008.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP009' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP009.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP010' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP010.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP011' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP011.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP012' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP012.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP013' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP013.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP014' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP014.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP015' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP015.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP016' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP016.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP017' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP017.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP018' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP018.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP019' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP019.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP020' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP020.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP021' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP021.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP022' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP022.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP023' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP023.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP024' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP024.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP025' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP025.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP026' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP026.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP027' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP027.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP028' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP028.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP029' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP029.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP030' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP030.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP031' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP031.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP032' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP032.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP033' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP033.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP034' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP034.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP035' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP035.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP036' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP036.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP037' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP037.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP038' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP038.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP039' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP039.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP040' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP040.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP041' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP041.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP042' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP042.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP043' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP043.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP044' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP044.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP045' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP045.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP046' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP046.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP047' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP047.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP048' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP048.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP049' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP049.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP050' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP050.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP051' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP051.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP052' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP052.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP053' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP053.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP054' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP054.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP055' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP055.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP056' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP056.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP057' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP057.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP058' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP058.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP059' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP059.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP060' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP060.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP061' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP061.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP062' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP062.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP063' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP063.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP064' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP064.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP065' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP065.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP066' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP066.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP067' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP067.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP068' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP068.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP069' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP069.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP070' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP070.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP071' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP071.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP072' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP072.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP073' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP073.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP074' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP074.CONSOLIDATED_PAYMENT UNION
+SELECT DISTINCT 'PP075' AS PAYER, CONSL_PAY_NBR,PAYR_KEY_ID,PROV_KEY_ID,DEP_DT,SETL_DT,CONSL_AMT,PROC_DTTM,AMB_PAY_IND,PAY_METH_CD,INTRL_CTL_ID,PAYMENT_TYPE_INDICATOR,PROC_DT,DSPL_CONSL_PAY_NBR,PULL_FUND_IND,PAYR_BNK_ACCT_ID,PROC_CTL_ID,PAY_STS_TYP_ID, PAY_STS_TYP_DTTM,MCC,PROXY_ID,TRACE_NBR,ARCHV_IND,PAY_ERR_TYP_ID,PAY_ERR_DTTM,VCP_REORIG_DT,EXTRACT_STS_CD,EXTRACT_DTTM FROM PP075.CONSOLIDATED_PAYMENT
+)PID WHERE PID.PROV_KEY_ID in ({$list}) AND PID.PROC_DTTM &gt;= current date - 30 days
+</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select *
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p,
+PP001.CLAIM c, PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = c.CLM_KEY_ID
+and cp.DSPL_CONSL_PAY_NBR='{$dspl_nbr}'
+order by c.PTNT_FST_NM,c.PTNT_MIDL_NM,c.PTNT_LST_NM with ur
+</t>
+  </si>
+  <si>
+    <t>fetch claim level data</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select rp.LST_NM , cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, PP001.RENDERING_PROVIDER rp,PP001.CLAIM_PROVIDER clm_pro,
+PP001.UNCONSOLIDATED_PAYMENT ucp, PP001.CLAIM_UNCONSOLIDATED_PAYMENT cup,OLE.PROC_CTL pc
+where cp.prov_key_id = p.prov_key_id
+and cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and ucp.UCONSL_PAY_KEY_ID = cup.UCONSL_PAY_KEY_ID
+and cup.CLM_KEY_ID = clm_pro.CLM_KEY_ID 
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID
+and rp.RNDR_PROV_KEY_ID=clm_pro.RNDR_PROV_KEY_ID
+and p.PROV_TAX_ID_NBR ='203237708'
+and pc.EXTRACT_STS_CD='C'
+and cp.SETL_DT between (current date - 180 days) and current date 
+order by cp.SETL_DT DESC
+fetch first row only
+</t>
+  </si>
+  <si>
+    <t>Rendering Provider Name</t>
   </si>
 </sst>
 </file>
@@ -1797,10 +2054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2114,7 +2371,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="86.55" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>117</v>
       </c>
@@ -2125,7 +2382,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>116</v>
       </c>
@@ -2136,7 +2393,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>118</v>
       </c>
@@ -2144,7 +2401,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>122</v>
       </c>
@@ -2375,6 +2632,82 @@
       </c>
       <c r="B63" s="7" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C65" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C70" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C71" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrcting duplicate email address query to exclude logged in user email
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="492" windowWidth="22980" windowHeight="9108" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="22980" windowHeight="9105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -272,9 +272,6 @@
     <t>BS</t>
   </si>
   <si>
-    <t>select EMAIL_ADR_TXT from OLE.PORTAL_USER p order by p.Portal_user_id desc FETCH FIRST 1 ROW ONLY</t>
-  </si>
-  <si>
     <t>Loop</t>
   </si>
   <si>
@@ -1092,6 +1089,9 @@
   </si>
   <si>
     <t>52</t>
+  </si>
+  <si>
+    <t>select EMAIL_ADR_TXT from OLE.PORTAL_USER p where p.SSO_ID not in ('{$id}') order by p.Portal_user_id desc FETCH FIRST 1 ROW ONLY</t>
   </si>
 </sst>
 </file>
@@ -1480,16 +1480,16 @@
       <selection activeCell="H6" activeCellId="1" sqref="I2 H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1518,7 +1518,7 @@
         <v>28</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1597,7 +1597,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>14</v>
@@ -1626,7 +1626,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>11</v>
@@ -1902,19 +1902,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="64.21875" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
-    <col min="4" max="4" width="50.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1974,28 +1974,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -2003,26 +2003,26 @@
         <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -2030,15 +2030,15 @@
         <v>36</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -2046,350 +2046,350 @@
         <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="7" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="7" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="B25" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="100.9" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="B28" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="172.9" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" s="7" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="7" t="s">
+    </row>
+    <row r="33" spans="1:5" ht="172.9" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="C33" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:5" ht="115.15" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="86.45" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="B35" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="86.45" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+    </row>
+    <row r="37" spans="1:5" ht="86.45" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="86.45" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="7" t="s">
+    </row>
+    <row r="39" spans="1:5" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="B39" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="7" t="s">
+    </row>
+    <row r="40" spans="1:5" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="B40" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="B41" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="7" t="s">
+    </row>
+    <row r="42" spans="1:5" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:5" ht="115.15" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" t="s">
         <v>134</v>
       </c>
-      <c r="B44" s="7" t="s">
+    </row>
+    <row r="45" spans="1:5" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C44" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    </row>
+    <row r="46" spans="1:5" ht="158.44999999999999" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="B46" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="158.44999999999999" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B47" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="7" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+      <c r="B51" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" t="s">
         <v>156</v>
-      </c>
-      <c r="C52" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" t="s">
         <v>158</v>
-      </c>
-      <c r="C53" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2406,13 +2406,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2420,19 +2420,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2440,22 +2440,22 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2463,22 +2463,22 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="D3" t="s">
-        <v>61</v>
-      </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2486,19 +2486,19 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2506,10 +2506,10 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5">
         <v>656565</v>
@@ -2520,13 +2520,13 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2534,22 +2534,22 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2557,22 +2557,22 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
         <v>66</v>
       </c>
-      <c r="D8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
-      </c>
       <c r="F8" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2590,7 +2590,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final Data file added
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="19420" windowHeight="9050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="564" windowWidth="19416" windowHeight="9048" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="474">
   <si>
     <t>City</t>
   </si>
@@ -1994,6 +1994,126 @@
   </si>
   <si>
     <t>Select CONT_ID,TEXT_VAL from ole.content where CONT_NM='BeginEnrollmentPage' order by CONT_ID ASC</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Select sa.ANSWER_TXT from ole.SURVEY_ANSWER sa order by sa.ANSWER_SEQ ASC with ur</t>
+  </si>
+  <si>
+    <t>select sq.QUESTION_TXT from ole.SURVEY_QUESTION sq order by sq.QUESTION_SEQ ASC with ur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select count(*) as RECORD_COUNT
+from ole.SURVEY_RESPONSE sr, ole.SURVEY_ANSWER sa
+where sr.SURVEY_ANS_ID = sa.SURVEY_ANS_ID
+and sa.ANSWER_TXT = 'Other'
+and sr.CREAT_DTTM &gt; '{$timestamp}'
+with ur
+</t>
+  </si>
+  <si>
+    <t>select * from OLE.ENROLLED_PROVIDER e where e.ENRL_STS_CD='A' FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>TIN is enrolled and Active</t>
+  </si>
+  <si>
+    <t>select * from OLE.ENROLLED_PROVIDER e where e.ENRL_STS_CD='PE' FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>TIN is enrolled and in Pre-enrollment Status</t>
+  </si>
+  <si>
+    <t>select * from OLE.ENROLLED_PROVIDER e where e.ENRL_STS_CD='PE' AND e.AUTO_ENRL_STS_CD IS NOT NULL FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>TIN was auto-enrolled but in Pre-enrollment Status</t>
+  </si>
+  <si>
+    <t>select * from OLE.ENROLLED_PROVIDER e where e.ENRL_STS_CD='I' AND e.BLOCK_TIN_IND='Y' FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>TIN is enrolled but Inactive and blocked status</t>
+  </si>
+  <si>
+    <t>select * from OLE.ENROLLED_PROVIDER e where e.ENRL_STS_CD='I' AND e.BLOCK_TIN_IND='N' FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>TIN is enrolled, Inactive and unblocked status</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%TIN is eligible%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>Content Managed Validation</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%Please be advised%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%Organization name, mailing information%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%Administrators are able%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%The primary contact should%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%The secondary contact should%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%Banking information%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%W-9 must be signed%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -2612,16 +2732,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3032,20 +3152,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="82.21875" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3056,7 +3176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -3067,7 +3187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -3078,7 +3198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -3086,7 +3206,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3097,7 +3217,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -3105,7 +3225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -3113,7 +3233,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -3121,7 +3241,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -3137,7 +3257,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="86.55" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -3145,7 +3265,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -3153,7 +3273,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -3161,7 +3281,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -3169,7 +3289,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -3177,7 +3297,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>74</v>
       </c>
@@ -3185,7 +3305,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>75</v>
       </c>
@@ -3193,7 +3313,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>78</v>
       </c>
@@ -3201,7 +3321,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="101" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>79</v>
       </c>
@@ -3209,7 +3329,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="86.55" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -3217,7 +3337,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>85</v>
       </c>
@@ -3233,7 +3353,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>90</v>
       </c>
@@ -3241,7 +3361,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>91</v>
       </c>
@@ -3249,7 +3369,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="101" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>93</v>
       </c>
@@ -3257,7 +3377,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>94</v>
       </c>
@@ -3265,7 +3385,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>95</v>
       </c>
@@ -3273,7 +3393,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="101" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>96</v>
       </c>
@@ -3281,7 +3401,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>98</v>
       </c>
@@ -3289,7 +3409,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>99</v>
       </c>
@@ -3300,7 +3420,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="187.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>102</v>
       </c>
@@ -3333,7 +3453,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>111</v>
       </c>
@@ -3341,7 +3461,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="58.05" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>112</v>
       </c>
@@ -3371,7 +3491,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>118</v>
       </c>
@@ -3379,7 +3499,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="101.55" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>122</v>
       </c>
@@ -3387,7 +3507,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>123</v>
       </c>
@@ -3403,7 +3523,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="101.55" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>127</v>
       </c>
@@ -3417,7 +3537,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="188.55" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>129</v>
       </c>
@@ -3425,7 +3545,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="203" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="202.95" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>130</v>
       </c>
@@ -3433,7 +3553,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="101.55" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>131</v>
       </c>
@@ -3441,7 +3561,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="188.55" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>132</v>
       </c>
@@ -3449,7 +3569,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="203" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="202.95" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>133</v>
       </c>
@@ -3471,7 +3591,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>135</v>
       </c>
@@ -3482,7 +3602,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>136</v>
       </c>
@@ -3493,7 +3613,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>137</v>
       </c>
@@ -3504,7 +3624,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>138</v>
       </c>
@@ -3515,7 +3635,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>139</v>
       </c>
@@ -3526,7 +3646,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="101.55" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>140</v>
       </c>
@@ -3545,7 +3665,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>144</v>
       </c>
@@ -3572,7 +3692,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="159.44999999999999" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>156</v>
       </c>
@@ -3583,7 +3703,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="159.44999999999999" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>159</v>
       </c>
@@ -3594,12 +3714,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>161</v>
       </c>
@@ -3610,7 +3730,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="72.45" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>162</v>
       </c>
@@ -3618,7 +3738,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>186</v>
       </c>
@@ -3629,7 +3749,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>187</v>
       </c>
@@ -3640,7 +3760,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>192</v>
       </c>
@@ -3648,7 +3768,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="28.95" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>193</v>
       </c>
@@ -3683,7 +3803,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="246.45" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>207</v>
       </c>
@@ -3694,7 +3814,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>209</v>
       </c>
@@ -3702,7 +3822,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>290</v>
       </c>
@@ -3710,7 +3830,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>291</v>
       </c>
@@ -3718,7 +3838,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>294</v>
       </c>
@@ -3726,7 +3846,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>296</v>
       </c>
@@ -3734,7 +3854,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>368</v>
       </c>
@@ -3742,7 +3862,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>369</v>
       </c>
@@ -3750,7 +3870,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>370</v>
       </c>
@@ -3758,7 +3878,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>372</v>
       </c>
@@ -3766,7 +3886,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>373</v>
       </c>
@@ -3774,7 +3894,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>375</v>
       </c>
@@ -3782,7 +3902,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>377</v>
       </c>
@@ -3790,7 +3910,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>378</v>
       </c>
@@ -3798,7 +3918,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>379</v>
       </c>
@@ -3806,7 +3926,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>380</v>
       </c>
@@ -3814,7 +3934,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>382</v>
       </c>
@@ -3822,7 +3942,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>383</v>
       </c>
@@ -3830,7 +3950,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>385</v>
       </c>
@@ -3838,7 +3958,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>396</v>
       </c>
@@ -3846,7 +3966,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>397</v>
       </c>
@@ -3854,7 +3974,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>399</v>
       </c>
@@ -3862,7 +3982,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>402</v>
       </c>
@@ -3870,7 +3990,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>404</v>
       </c>
@@ -3878,7 +3998,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>406</v>
       </c>
@@ -3886,7 +4006,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>408</v>
       </c>
@@ -3894,7 +4014,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>409</v>
       </c>
@@ -3902,7 +4022,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>412</v>
       </c>
@@ -3910,7 +4030,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>417</v>
       </c>
@@ -3918,7 +4038,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>418</v>
       </c>
@@ -3926,7 +4046,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>419</v>
       </c>
@@ -3934,7 +4054,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>420</v>
       </c>
@@ -3942,7 +4062,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" ht="246.45" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>421</v>
       </c>
@@ -3964,7 +4084,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="290" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" ht="288" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>424</v>
       </c>
@@ -3975,7 +4095,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>427</v>
       </c>
@@ -3983,7 +4103,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>429</v>
       </c>
@@ -3991,12 +4111,179 @@
         <v>428</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>434</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>435</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="B112" t="s">
+        <v>442</v>
+      </c>
+      <c r="C112" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B113" t="s">
+        <v>444</v>
+      </c>
+      <c r="C113" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B114" t="s">
+        <v>446</v>
+      </c>
+      <c r="C114" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B115" t="s">
+        <v>448</v>
+      </c>
+      <c r="C115" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="B116" t="s">
+        <v>450</v>
+      </c>
+      <c r="C116" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="B117" t="s">
+        <v>452</v>
+      </c>
+      <c r="C117" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B118" t="s">
+        <v>454</v>
+      </c>
+      <c r="C118" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B119" t="s">
+        <v>455</v>
+      </c>
+      <c r="C119" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B120" t="s">
+        <v>456</v>
+      </c>
+      <c r="C120" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="B121" t="s">
+        <v>457</v>
+      </c>
+      <c r="C121" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="B122" t="s">
+        <v>458</v>
+      </c>
+      <c r="C122" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B123" t="s">
+        <v>459</v>
+      </c>
+      <c r="C123" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="B124" t="s">
+        <v>460</v>
+      </c>
+      <c r="C124" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -4013,13 +4300,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -4199,13 +4486,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>210</v>
       </c>
@@ -4213,7 +4500,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>212</v>
       </c>
@@ -4221,7 +4508,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>214</v>
       </c>
@@ -4229,55 +4516,55 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>217</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>218</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>219</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>220</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>221</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>222</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>223</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>224</v>
       </c>
@@ -4285,7 +4572,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>226</v>
       </c>
@@ -4293,7 +4580,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>228</v>
       </c>
@@ -4301,7 +4588,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
@@ -4309,7 +4596,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>231</v>
       </c>
@@ -4317,7 +4604,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>233</v>
       </c>
@@ -4325,7 +4612,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>235</v>
       </c>
@@ -4333,7 +4620,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>237</v>
       </c>
@@ -4341,7 +4628,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>239</v>
       </c>
@@ -4349,7 +4636,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>241</v>
       </c>
@@ -4357,7 +4644,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>243</v>
       </c>
@@ -4365,31 +4652,31 @@
         <v>244</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>248</v>
       </c>
@@ -4397,7 +4684,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>250</v>
       </c>
@@ -4405,7 +4692,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>252</v>
       </c>
@@ -4413,7 +4700,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>254</v>
       </c>
@@ -4421,7 +4708,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>255</v>
       </c>
@@ -4429,7 +4716,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>257</v>
       </c>
@@ -4437,7 +4724,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>259</v>
       </c>
@@ -4445,7 +4732,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>261</v>
       </c>
@@ -4453,7 +4740,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>262</v>
       </c>
@@ -4461,7 +4748,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>263</v>
       </c>
@@ -4469,7 +4756,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>265</v>
       </c>
@@ -4477,7 +4764,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>267</v>
       </c>
@@ -4485,7 +4772,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>269</v>
       </c>
@@ -4493,7 +4780,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>271</v>
       </c>
@@ -4501,7 +4788,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>273</v>
       </c>
@@ -4509,7 +4796,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>275</v>
       </c>
@@ -4517,7 +4804,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>277</v>
       </c>
@@ -4525,7 +4812,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
         <v>278</v>
       </c>
@@ -4533,7 +4820,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>279</v>
       </c>
@@ -4541,7 +4828,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>281</v>
       </c>
@@ -4549,7 +4836,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>282</v>
       </c>
@@ -4557,7 +4844,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>283</v>
       </c>
@@ -4565,7 +4852,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>285</v>
       </c>
@@ -4573,7 +4860,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>286</v>
       </c>
@@ -4581,7 +4868,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>288</v>
       </c>
@@ -4615,10 +4902,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="85.36328125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="85.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4837,7 +5124,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
         <v>352</v>
       </c>
@@ -4845,7 +5132,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
         <v>354</v>
       </c>
@@ -4853,7 +5140,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>356</v>
       </c>
@@ -4861,7 +5148,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>358</v>
       </c>
@@ -4869,7 +5156,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>360</v>
       </c>
@@ -4877,7 +5164,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>362</v>
       </c>
@@ -4885,7 +5172,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>364</v>
       </c>
@@ -4893,7 +5180,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
         <v>366</v>
       </c>

</xml_diff>

<commit_message>
added queries in data file
added queries in data file
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="478">
   <si>
     <t>City</t>
   </si>
@@ -2114,6 +2114,18 @@
   </si>
   <si>
     <t>123</t>
+  </si>
+  <si>
+    <t>select p.EMAIL_ADR_TXT from OLE.PORTAL_USER p  where p.EMAIL_ADR_TXT not in ('$email}') order by p.Portal_user_id desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>Select c.TEXT_VAL from ole.content c where c.CONT_NM ='EnrollOrgInfo' and c.SUB_CAT='{$subject}'</t>
   </si>
 </sst>
 </file>
@@ -3152,10 +3164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4284,6 +4296,22 @@
       </c>
       <c r="C124" t="s">
         <v>453</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B125" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B126" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for provider view payments after QA testing
Fixes for provider view payments after QA testing
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="528">
   <si>
     <t>City</t>
   </si>
@@ -587,9 +587,6 @@
 fetch first row only</t>
   </si>
   <si>
-    <t>SELECT CP.DSPL_CONSL_PAY_NBR , P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
-  </si>
-  <si>
     <t>38</t>
   </si>
   <si>
@@ -674,9 +671,6 @@
 and cp.setl_dt &lt;= current date and p.PROV_TAX_ID_NBR='{$tin}' order by cp.setl_dt DESC
 fetch first row only
 with ur</t>
-  </si>
-  <si>
-    <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, (Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP001.CONSOLIDATED_PAYMENT CP, PP001.PROVIDER P WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY</t>
   </si>
   <si>
     <t>54</t>
@@ -2116,9 +2110,6 @@
     <t>123</t>
   </si>
   <si>
-    <t>select p.EMAIL_ADR_TXT from OLE.PORTAL_USER p  where p.EMAIL_ADR_TXT not in ('$email}') order by p.Portal_user_id desc FETCH FIRST 1 ROW ONLY</t>
-  </si>
-  <si>
     <t>125</t>
   </si>
   <si>
@@ -2126,6 +2117,615 @@
   </si>
   <si>
     <t>Select c.TEXT_VAL from ole.content c where c.CONT_NM ='EnrollOrgInfo' and c.SUB_CAT='{$subject}'</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and cp.setl_dt &gt; current date - 60 days
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>select sum(RECORD_COUNT) as RECORD_COUNT from (Select count(*) as RECORD_COUNT
+   from PP001.CONSOLIDATED_PAYMENT cp join PP001.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP002.CONSOLIDATED_PAYMENT cp join PP002.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP003.CONSOLIDATED_PAYMENT cp join PP003.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP004.CONSOLIDATED_PAYMENT cp join PP004.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP005.CONSOLIDATED_PAYMENT cp join PP005.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP006.CONSOLIDATED_PAYMENT cp join PP006.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP007.CONSOLIDATED_PAYMENT cp join PP007.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP008.CONSOLIDATED_PAYMENT cp join PP008.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP009.CONSOLIDATED_PAYMENT cp join PP009.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP010.CONSOLIDATED_PAYMENT cp join PP010.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP011.CONSOLIDATED_PAYMENT cp join PP011.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP012.CONSOLIDATED_PAYMENT cp join PP012.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP013.CONSOLIDATED_PAYMENT cp join PP013.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP014.CONSOLIDATED_PAYMENT cp join PP014.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP015.CONSOLIDATED_PAYMENT cp join PP015.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP016.CONSOLIDATED_PAYMENT cp join PP016.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP017.CONSOLIDATED_PAYMENT cp join PP017.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP018.CONSOLIDATED_PAYMENT cp join PP018.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP019.CONSOLIDATED_PAYMENT cp join PP019.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP020.CONSOLIDATED_PAYMENT cp join PP020.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP021.CONSOLIDATED_PAYMENT cp join PP021.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP022.CONSOLIDATED_PAYMENT cp join PP022.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP023.CONSOLIDATED_PAYMENT cp join PP023.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP024.CONSOLIDATED_PAYMENT cp join PP024.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP025.CONSOLIDATED_PAYMENT cp join PP025.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP026.CONSOLIDATED_PAYMENT cp join PP026.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP027.CONSOLIDATED_PAYMENT cp join PP027.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP028.CONSOLIDATED_PAYMENT cp join PP028.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP029.CONSOLIDATED_PAYMENT cp join PP029.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP030.CONSOLIDATED_PAYMENT cp join PP030.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP031.CONSOLIDATED_PAYMENT cp join PP031.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP032.CONSOLIDATED_PAYMENT cp join PP032.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP033.CONSOLIDATED_PAYMENT cp join PP033.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP034.CONSOLIDATED_PAYMENT cp join PP034.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP035.CONSOLIDATED_PAYMENT cp join PP035.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP036.CONSOLIDATED_PAYMENT cp join PP036.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP037.CONSOLIDATED_PAYMENT cp join PP037.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP038.CONSOLIDATED_PAYMENT cp join PP038.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP039.CONSOLIDATED_PAYMENT cp join PP039.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP040.CONSOLIDATED_PAYMENT cp join PP040.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP041.CONSOLIDATED_PAYMENT cp join PP041.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP042.CONSOLIDATED_PAYMENT cp join PP042.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP043.CONSOLIDATED_PAYMENT cp join PP043.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP044.CONSOLIDATED_PAYMENT cp join PP044.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP045.CONSOLIDATED_PAYMENT cp join PP045.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP046.CONSOLIDATED_PAYMENT cp join PP046.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}'
+   union
+   Select count(*) as RECORD_COUNT
+   from PP047.CONSOLIDATED_PAYMENT cp join PP047.PROVIDER p on 
+   cp.prov_key_id = p.prov_key_id join  OLE.PROC_CTL pc
+   on cp.PROC_CTL_ID = pc.PROC_CTL_ID
+   where p.prov_tax_id_nbr='{$tin}' and pc.EXTRACT_STS_CD ='C'
+   and cp.SETL_DT &gt;= '{$fromDate}' and cp.SETL_DT &lt;='{$toDate}')with ur</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and cp.setl_dt &gt; current date - 31 days
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>For getting tin with payments in last 60/90 days</t>
+  </si>
+  <si>
+    <t>select p.EMAIL_ADR_TXT from OLE.PORTAL_USER p  where p.EMAIL_ADR_TXT not in ('{$email}') order by p.Portal_user_id desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
+where cp.prov_key_id = p.prov_key_id
+and cp.setl_dt between '{$fromDate}' and '{$toDate}' 
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>For getting tin with payments in last 30 days</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>For General Payment NPI Only-last 30 days</t>
+  </si>
+  <si>
+    <t>For General Payment NPI Only - last 60/90 days</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 30 days and p.PROV_NPI_NBR is not null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 60 days and p.PROV_NPI_NBR is not null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>For getting tin with payments in last 4-6,9,13 months</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt between '{$fromDate}' and '{$toDate}' and p.PROV_NPI_NBR is not null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>For General Payment NPI Only-last 4-6,9,13 months</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>For General Payment TIN Only for last 30 days</t>
+  </si>
+  <si>
+    <t>For General Payment TIN Only for last 60/90 days</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt between '{$fromDate}' and '{$toDate}' and p.PROV_NPI_NBR is null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>For General Payment TIN Only for last 4-6,,13 months</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 30 days and p.PROV_NPI_NBR is null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 60 days and p.PROV_NPI_NBR is null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>Archive payments for last 30 days</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>Archive payments for last 60/90 days</t>
+  </si>
+  <si>
+    <t>Archive payments for last4-6,9,13 months</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 60 days and cp.ARCHV_IND='Y'
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt between '{$fromDate}' and '{$toDate}' and cp.ARCHV_IND='Y'
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 30 days and cp.ARCHV_IND='Y'
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 30 days and cp.ARCHV_IND not in ('Y')
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Active only payments for last 30 days</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>Active only payments for last 60/90 days</t>
+  </si>
+  <si>
+    <t>Active only payments for last4-6,9,13 months</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt between '{$fromDate}' and '{$toDate}' and cp.ARCHV_IND not in ('Y')
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 60 days and cp.ARCHV_IND not in ('Y')
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR , P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, 
+(Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP024.CONSOLIDATED_PAYMENT CP, PP024.PROVIDER P,OLE.ENROLLED_PROVIDER ep,OLE.PROC_CTL PC
+WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID  AND p.PROV_TAX_ID_NBR=ep.PROV_TIN_NBR
+and PC.PROC_CTL_ID = CP.PROC_CTL_ID 
+and ep.ENRL_STS_CD='A' and PC.EXTRACT_STS_CD = 'C' AND CP.SETL_DT &lt;= current date 
+AND CP.PAY_METH_CD = 'NON' and CP.CONSL_AMT = '0.00' 
+AND CP.PAY_STS_TYP_ID IS NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY with ur</t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR, P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT, 
+(Days(current date) - days(CP.SETL_DT)) as DATE_DIFF FROM PP001.CONSOLIDATED_PAYMENT CP,
+ PP001.PROVIDER P,OLE.ENROLLED_PROVIDER ep,OLE.PROC_CTL PC WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID 
+ AND p.PROV_TAX_ID_NBR=ep.PROV_TIN_NBR and PC.PROC_CTL_ID = CP.PROC_CTL_ID 
+ and ep.ENRL_STS_CD='A' and PC.EXTRACT_STS_CD = 'C'
+ AND CP.SETL_DT &lt;= current date AND CP.PAY_METH_CD = 'NON' 
+ and CP.CONSL_AMT = '0.00' AND CP.PAY_STS_TYP_ID IS NOT NULL ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY with ur</t>
+  </si>
+  <si>
+    <t>SELECT CP.DSPL_CONSL_PAY_NBR , P.PROV_TAX_ID_NBR, CP.PAY_STS_TYP_ID, CP.CONSL_AMT, CP.SETL_DT,(Days(current date) - days(CP.SETL_DT)) as DATE_DIFF 
+FROM PP001.CONSOLIDATED_PAYMENT CP, PP001.PROVIDER P,OLE.ENROLLED_PROVIDER ep,OLE.PROC_CTL PC
+WHERE CP.PROV_KEY_ID = P.PROV_KEY_ID AND p.PROV_TAX_ID_NBR=ep.PROV_TIN_NBR
+and PC.PROC_CTL_ID = CP.PROC_CTL_ID 
+and ep.ENRL_STS_CD='A' and PC.EXTRACT_STS_CD = 'C' AND CP.SETL_DT &lt;= current date 
+AND CP.PAYMENT_TYPE_INDICATOR='M'
+ORDER BY CP.SETL_DT DESC FETCH FIRST 1 ROWS ONLY with ur</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>Getting tin from Market type filter as Medical</t>
   </si>
 </sst>
 </file>
@@ -3164,10 +3764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3426,7 +4026,7 @@
         <v>99</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
         <v>103</v>
@@ -3437,7 +4037,7 @@
         <v>102</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>104</v>
@@ -3448,7 +4048,7 @@
         <v>105</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C32" t="s">
         <v>106</v>
@@ -3459,7 +4059,7 @@
         <v>107</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>108</v>
@@ -3481,29 +4081,29 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>121</v>
+        <v>523</v>
       </c>
       <c r="C36" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>116</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>142</v>
+        <v>524</v>
       </c>
       <c r="C37" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="115.95" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>118</v>
       </c>
@@ -3511,807 +4111,991 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="101.55" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B40" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="115.95" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="B41" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B42" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="101.55" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="188.55" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="B43" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="202.95" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="101.55" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
-        <v>131</v>
-      </c>
       <c r="B45" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="188.55" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="202.95" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="174" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C48" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C49" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C50" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C52" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C53" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="101.55" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="174" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="174" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="159.44999999999999" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" t="s">
         <v>156</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C59" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="159.44999999999999" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C60" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="C62" t="s">
         <v>163</v>
-      </c>
-      <c r="C62" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="72.45" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C64" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="28.95" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B70" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C70" t="s">
         <v>203</v>
-      </c>
-      <c r="C70" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="246.45" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C71" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B79" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="246.45" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="C103" t="s">
         <v>421</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="C103" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="348" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C104" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="288" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C105" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B110" s="7" t="s">
         <v>437</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>438</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B112" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C112" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B113" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C113" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B114" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C114" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B115" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C115" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B116" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C116" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B117" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C117" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B118" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C118" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B119" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C119" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B120" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C120" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B121" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C121" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B122" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C122" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B123" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C123" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B124" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C124" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B125" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B126" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A127" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="B126" t="s">
-        <v>474</v>
+      <c r="B127" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C127" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A128" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="C128" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A130" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="C130" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="C131" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C132" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="C133" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="C134" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A135" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="C135" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A136" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="C136" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A137" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="C137" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A138" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="C138" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A139" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="C139" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A140" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="C140" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C141" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="C142" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A143" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="C143" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -4522,98 +5306,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B4" s="16"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B7" s="16"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B9" s="16"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B10" s="16"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B11" s="16"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -4621,156 +5405,156 @@
         <v>45</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B18" s="21" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B19" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B20" s="21" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B21" s="21" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B22" s="21" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B28" s="14" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>55</v>
@@ -4778,130 +5562,130 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -4938,282 +5722,282 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B17" s="26" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="25" t="s">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="25" t="s">
         <v>330</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B18" s="26" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="25" t="s">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B19" s="26" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="25" t="s">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B20" s="26" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="25" t="s">
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="s">
         <v>336</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B21" s="26" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="25" t="s">
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="25" t="s">
         <v>338</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B22" s="26" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="25" t="s">
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="25" t="s">
         <v>340</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B23" s="26" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="25" t="s">
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="25" t="s">
         <v>342</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B24" s="26" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="25" t="s">
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="25" t="s">
         <v>344</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B25" s="26" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="25" t="s">
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="25" t="s">
         <v>346</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B26" s="26" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="25" t="s">
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B27" s="26" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="25" t="s">
-        <v>350</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for View PAyments
Fixes for View PAyments
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="541">
   <si>
     <t>City</t>
   </si>
@@ -2726,6 +2726,73 @@
   </si>
   <si>
     <t>Getting tin from Market type filter as Medical</t>
+  </si>
+  <si>
+    <t>Last 90 days</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>Npi last 90 days</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>archive only 90 days</t>
+  </si>
+  <si>
+    <t>active only 90 days</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 90 days and cp.ARCHV_IND='Y'
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 90 days and cp.ARCHV_IND not in ('Y')
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 90 days and p.PROV_NPI_NBR is null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 90 days and p.PROV_NPI_NBR is not null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>147</t>
   </si>
 </sst>
 </file>
@@ -3764,10 +3831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D143"/>
+  <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5096,6 +5163,61 @@
       </c>
       <c r="C143" t="s">
         <v>527</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A144" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C144" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A145" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="C145" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A146" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="C146" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A147" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="C147" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A148" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C148" t="s">
+        <v>531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes for view payments Payer
changes for view payments Payer
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -3833,8 +3833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
data file query change for last 30/60 days
data file query change for last 30/60 days
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="542">
   <si>
     <t>City</t>
   </si>
@@ -2120,16 +2120,6 @@
   </si>
   <si>
     <t>126</t>
-  </si>
-  <si>
-    <t>Select p.prov_tax_id_nbr
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
-where cp.prov_key_id = p.prov_key_id
-and cp.setl_dt &gt; current date - 60 days
-group by p.prov_tax_id_nbr
-having count(*) between 1 and 30
-order by count(*) desc
-fetch first row only</t>
   </si>
   <si>
     <t>127</t>
@@ -2468,16 +2458,6 @@
     <t>128</t>
   </si>
   <si>
-    <t>Select p.prov_tax_id_nbr
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p
-where cp.prov_key_id = p.prov_key_id
-and cp.setl_dt &gt; current date - 31 days
-group by p.prov_tax_id_nbr
-having count(*) between 1 and 30
-order by count(*) desc
-fetch first row only</t>
-  </si>
-  <si>
     <t>129</t>
   </si>
   <si>
@@ -2522,16 +2502,6 @@
 fetch first row only</t>
   </si>
   <si>
-    <t>Select p.prov_tax_id_nbr
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
-and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
-and cp.setl_dt &gt; current date - 60 days and p.PROV_NPI_NBR is not null
-group by p.prov_tax_id_nbr
-having count(*) between 1 and 30
-order by count(*) desc
-fetch first row only</t>
-  </si>
-  <si>
     <t>For getting tin with payments in last 4-6,9,13 months</t>
   </si>
   <si>
@@ -2793,6 +2763,46 @@
   </si>
   <si>
     <t>147</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL pc
+where  pc.PROC_CTL_ID = cp.PROC_CTL_ID  and cp.prov_key_id = p.prov_key_id and pc.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 60 days
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 90 days 
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 31 days 
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 60 days 
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
   </si>
 </sst>
 </file>
@@ -3833,8 +3843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4153,7 +4163,7 @@
         <v>117</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C36" t="s">
         <v>114</v>
@@ -4164,7 +4174,7 @@
         <v>116</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C37" t="s">
         <v>115</v>
@@ -4978,246 +4988,246 @@
         <v>472</v>
       </c>
       <c r="B126" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>475</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>476</v>
+        <v>538</v>
       </c>
       <c r="C127" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C128" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="B129" s="8" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A130" s="5" t="s">
-        <v>481</v>
-      </c>
       <c r="B130" s="7" t="s">
-        <v>480</v>
+        <v>540</v>
       </c>
       <c r="C130" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>491</v>
+        <v>541</v>
       </c>
       <c r="C131" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C132" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C133" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C134" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C135" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C136" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C137" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C138" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C139" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C140" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C141" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="B142" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="B142" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="C142" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C143" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B144" s="7" t="s">
         <v>539</v>
       </c>
       <c r="C144" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C145" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C146" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C147" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C148" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding queries in data file for Avneet;s user story of BS create enrollment
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="562">
   <si>
     <t>City</t>
   </si>
@@ -2815,6 +2815,54 @@
 and c.PTNT_LST_NM &lt;&gt; ''
 order by cp.SETL_DT DESC
 fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>select * from OLE.BILLING_SERVICE b where b.ENRL_STS_CD='A' FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>BS TIN is enrolled and Active</t>
+  </si>
+  <si>
+    <t>select * from OLE.BILLING_SERVICE b where b.IDENTIFIER_NBR='{$tin}' FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>BS TIN Details</t>
+  </si>
+  <si>
+    <t>select * from OLE.BILLING_SERVICE b where b.ENRL_STS_CD='PE' FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>BS TIN is in pending enrollment</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%Your TIN/SSN is already enrolled%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>BS Content Managed Validation</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%The TIN/SSN you entered is enrolled and active for Electronic Payments and Statements%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.content where TEXT_VAL like '%Your TIN is currently in a pending enrollment status%' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
   </si>
 </sst>
 </file>
@@ -3862,10 +3910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4324,7 +4372,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>135</v>
       </c>
@@ -4335,7 +4383,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>136</v>
       </c>
@@ -4346,7 +4394,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>137</v>
       </c>
@@ -4357,7 +4405,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>138</v>
       </c>
@@ -4368,7 +4416,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="101.55" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>139</v>
       </c>
@@ -4376,7 +4424,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>141</v>
       </c>
@@ -4387,7 +4435,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>142</v>
       </c>
@@ -4395,7 +4443,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>149</v>
       </c>
@@ -4406,7 +4454,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>150</v>
       </c>
@@ -4414,7 +4462,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="159.44999999999999" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>154</v>
       </c>
@@ -4425,7 +4473,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="159.44999999999999" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>157</v>
       </c>
@@ -4436,12 +4484,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>159</v>
       </c>
@@ -4452,7 +4500,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="72.45" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>160</v>
       </c>
@@ -4460,7 +4508,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>181</v>
       </c>
@@ -4471,7 +4519,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="145.05000000000001" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>182</v>
       </c>
@@ -4482,7 +4530,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>187</v>
       </c>
@@ -4490,7 +4538,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="28.95" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>188</v>
       </c>
@@ -4498,7 +4546,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>189</v>
       </c>
@@ -4506,7 +4554,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>190</v>
       </c>
@@ -4525,7 +4573,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="246.45" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>202</v>
       </c>
@@ -4752,7 +4800,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>412</v>
       </c>
@@ -4760,7 +4808,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>413</v>
       </c>
@@ -4768,7 +4816,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>414</v>
       </c>
@@ -4776,7 +4824,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>415</v>
       </c>
@@ -4784,7 +4832,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="246.45" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>416</v>
       </c>
@@ -4795,7 +4843,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="348" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>417</v>
       </c>
@@ -5261,6 +5309,72 @@
       </c>
       <c r="C148" t="s">
         <v>524</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="B149" t="s">
+        <v>546</v>
+      </c>
+      <c r="C149" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A150" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="C150" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="B151" t="s">
+        <v>550</v>
+      </c>
+      <c r="C151" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A152" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="C152" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A153" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="C153" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A154" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="C154" t="s">
+        <v>553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
my profile test cases added, they somehow got overwritten in master
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="586">
   <si>
     <t>City</t>
   </si>
@@ -2936,6 +2936,46 @@
 and p.PROV_TAX_ID_NBR ='{$tin}'
 order by cp.SETL_DT DESC
 fetch first row only</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>INSERT INTO `eps_automation`.`statistics` (`className`, `passedTests`, `failedTests`, `createDt`, `endDt`, `runningCount`, `host`) VALUES ('{$testClass}', '{$passedTests}', '{$failedTests}', '{$createDt}', '{$endDt}', '1', '{$host}');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.PORTAL_USER_TIN t join OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.SSO_ID='{$id}' order by PROV_TIN_NBR asc
+</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>My Profile Provider details</t>
+  </si>
+  <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
+  on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
+  on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
+where p.SSO_ID='{$id}'</t>
+  </si>
+  <si>
+    <t>select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_PAYER_TIN pt 
+ on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where p.SSO_ID='{$id}'</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER_TIN t , OLE.PORTAL_USER u ,OLE.ENROLLED_PROVIDER ep
+where t.PORTAL_USER_ID=u.PORTAL_USER_ID
+and t.PROV_TIN_NBR=ep.PROV_TIN_NBR 
+and  u.SSO_ID='{$id}' and ep.ENRL_STS_CD='A'
+order by t.PROV_TIN_NBR asc</t>
   </si>
 </sst>
 </file>
@@ -3983,10 +4023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4933,7 +4973,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="288" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>417</v>
       </c>
@@ -4984,7 +5024,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>431</v>
       </c>
@@ -5401,7 +5441,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>555</v>
       </c>
@@ -5498,6 +5538,46 @@
       </c>
       <c r="C158" t="s">
         <v>572</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="B159" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A160" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="C160" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A162" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="B162" s="7" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B164" s="7" t="s">
+        <v>578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missed manage user cases
Added missed manage user cases
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="592">
   <si>
     <t>City</t>
   </si>
@@ -2981,6 +2981,30 @@
   </si>
   <si>
     <t>Page Content for BS Enrollment Submitted page.</t>
+  </si>
+  <si>
+    <t>select pt.PROV_TIN_NBR, pt.ACCESS_LVL,count(*)  as totalUsers  , pu.EMAIL_ADR_TXT ,pu.FST_NM,pu.LST_NM
+from ole.ENROLLED_PROVIDER ep join  ole.PORTAL_USER_TIN pt   on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
+join ole.PORTAL_USER pu on pu.PORTAL_USER_ID=pt.PORTAL_USER_ID
+group by pt.PROV_TIN_NBR,pt.ACCESS_LVL,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.STS_CD
+having count(*) =1 and pt.ACCESS_LVL='A'   and pu.STS_CD='A'
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>select pt.PROV_TIN_NBR, pt.ACCESS_LVL,count(*)  as totalUsers  , pu.EMAIL_ADR_TXT ,pu.FST_NM,pu.LST_NM
+from ole.ENROLLED_PROVIDER ep join  ole.PORTAL_USER_TIN pt   on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
+join ole.PORTAL_USER pu on pu.PORTAL_USER_ID=pt.PORTAL_USER_ID
+group by pt.PROV_TIN_NBR,pt.ACCESS_LVL,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.STS_CD
+having count(*) =2  and pt.ACCESS_LVL='A'   and pu.STS_CD='A'
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>164</t>
   </si>
 </sst>
 </file>
@@ -4028,10 +4052,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5591,8 +5615,21 @@
         <v>587</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B164" s="7"/>
+    <row r="164" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A164" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A165" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>589</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added testcases in Create Enrollment
added testcases in Create Enrollment
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="564" windowWidth="19416" windowHeight="9048" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="19420" windowHeight="9050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="594">
   <si>
     <t>City</t>
   </si>
@@ -2977,10 +2977,28 @@
     <t>162</t>
   </si>
   <si>
-    <t>Select  cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL  from ole.CONTENT where CONT_NM = 'CreateEnrollmentSubmittedBS'</t>
-  </si>
-  <si>
     <t>Page Content for BS Enrollment Submitted page.</t>
+  </si>
+  <si>
+    <t>Select cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL from ole.CONTENT where CONT_NM = 'CreateEnrollmentSubmittedBS'</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>Page Content for Identify Administrators</t>
+  </si>
+  <si>
+    <t>Select  cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL  from ole.CONTENT where CONT_DESC = 'Identify Admins Page'</t>
+  </si>
+  <si>
+    <t>select FST_NM,MIDDLE_INIT,LST_NM,EMAIL_ADR_TXT,TEL_NBR from  OLE.PORTAL_USER p where EMAIL_ADR_TXT ='{$email}'</t>
   </si>
 </sst>
 </file>
@@ -3608,16 +3626,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
-    <col min="8" max="8" width="26.77734375" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4028,20 +4046,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="82.88671875" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="82.90625" customWidth="1"/>
+    <col min="3" max="3" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4052,7 +4070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4063,7 +4081,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4074,7 +4092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4082,7 +4100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4093,7 +4111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4101,7 +4119,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4109,7 +4127,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4117,7 +4135,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4133,7 +4151,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="86.55" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4141,7 +4159,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4149,7 +4167,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4157,7 +4175,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.55" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4165,7 +4183,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4173,7 +4191,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>74</v>
       </c>
@@ -4181,7 +4199,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>75</v>
       </c>
@@ -4189,7 +4207,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>78</v>
       </c>
@@ -4197,7 +4215,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="101" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>79</v>
       </c>
@@ -4205,7 +4223,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="86.55" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -4213,7 +4231,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>85</v>
       </c>
@@ -4229,7 +4247,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>90</v>
       </c>
@@ -4237,7 +4255,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>91</v>
       </c>
@@ -4245,7 +4263,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="101" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>93</v>
       </c>
@@ -4253,7 +4271,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.95" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>94</v>
       </c>
@@ -4261,7 +4279,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>95</v>
       </c>
@@ -4269,7 +4287,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="100.95" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="101" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>96</v>
       </c>
@@ -4277,7 +4295,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>98</v>
       </c>
@@ -4285,7 +4303,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>99</v>
       </c>
@@ -4296,7 +4314,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>102</v>
       </c>
@@ -4329,7 +4347,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="115.95" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>111</v>
       </c>
@@ -4337,7 +4355,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="58.05" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>112</v>
       </c>
@@ -4367,7 +4385,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>118</v>
       </c>
@@ -4375,7 +4393,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>121</v>
       </c>
@@ -4383,7 +4401,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>122</v>
       </c>
@@ -4391,7 +4409,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>125</v>
       </c>
@@ -4399,7 +4417,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>126</v>
       </c>
@@ -4413,7 +4431,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>128</v>
       </c>
@@ -4424,7 +4442,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="201.65" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>129</v>
       </c>
@@ -4435,7 +4453,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>130</v>
       </c>
@@ -4446,7 +4464,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>131</v>
       </c>
@@ -4457,7 +4475,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="201.65" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>132</v>
       </c>
@@ -4479,7 +4497,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="115.95" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>134</v>
       </c>
@@ -4501,7 +4519,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>136</v>
       </c>
@@ -4534,7 +4552,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>139</v>
       </c>
@@ -4542,7 +4560,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>141</v>
       </c>
@@ -4553,7 +4571,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>142</v>
       </c>
@@ -4561,7 +4579,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>148</v>
       </c>
@@ -4572,7 +4590,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>149</v>
       </c>
@@ -4654,7 +4672,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>185</v>
       </c>
@@ -4662,7 +4680,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>186</v>
       </c>
@@ -4697,7 +4715,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="244.75" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>200</v>
       </c>
@@ -4708,7 +4726,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>202</v>
       </c>
@@ -4716,7 +4734,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>283</v>
       </c>
@@ -4724,7 +4742,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>284</v>
       </c>
@@ -4732,7 +4750,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>287</v>
       </c>
@@ -4740,7 +4758,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>289</v>
       </c>
@@ -4748,7 +4766,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>361</v>
       </c>
@@ -4756,7 +4774,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>362</v>
       </c>
@@ -4764,7 +4782,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>363</v>
       </c>
@@ -4772,7 +4790,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>365</v>
       </c>
@@ -4780,7 +4798,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>366</v>
       </c>
@@ -4788,7 +4806,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>368</v>
       </c>
@@ -4796,7 +4814,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>370</v>
       </c>
@@ -4804,7 +4822,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>371</v>
       </c>
@@ -4812,7 +4830,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>372</v>
       </c>
@@ -4820,7 +4838,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>373</v>
       </c>
@@ -4828,7 +4846,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>375</v>
       </c>
@@ -4836,7 +4854,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>376</v>
       </c>
@@ -4844,7 +4862,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>378</v>
       </c>
@@ -4852,7 +4870,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>389</v>
       </c>
@@ -4860,7 +4878,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>390</v>
       </c>
@@ -4868,7 +4886,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>392</v>
       </c>
@@ -4876,7 +4894,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>395</v>
       </c>
@@ -4884,7 +4902,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>397</v>
       </c>
@@ -4892,7 +4910,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>399</v>
       </c>
@@ -4900,7 +4918,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>401</v>
       </c>
@@ -4908,7 +4926,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>402</v>
       </c>
@@ -4916,7 +4934,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>405</v>
       </c>
@@ -4924,7 +4942,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>410</v>
       </c>
@@ -4932,7 +4950,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>411</v>
       </c>
@@ -4940,7 +4958,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>412</v>
       </c>
@@ -4948,7 +4966,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>413</v>
       </c>
@@ -4956,7 +4974,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="244.75" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>414</v>
       </c>
@@ -4967,7 +4985,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="345.65" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>415</v>
       </c>
@@ -4978,7 +4996,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="273.64999999999998" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>417</v>
       </c>
@@ -4989,7 +5007,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>420</v>
       </c>
@@ -4997,7 +5015,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>422</v>
       </c>
@@ -5005,7 +5023,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>427</v>
       </c>
@@ -5013,7 +5031,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>429</v>
       </c>
@@ -5021,7 +5039,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>430</v>
       </c>
@@ -5029,7 +5047,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>431</v>
       </c>
@@ -5037,7 +5055,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>454</v>
       </c>
@@ -5048,7 +5066,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>455</v>
       </c>
@@ -5059,7 +5077,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>456</v>
       </c>
@@ -5070,7 +5088,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>457</v>
       </c>
@@ -5081,7 +5099,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>458</v>
       </c>
@@ -5092,7 +5110,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>459</v>
       </c>
@@ -5103,7 +5121,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>460</v>
       </c>
@@ -5114,7 +5132,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>461</v>
       </c>
@@ -5125,7 +5143,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>462</v>
       </c>
@@ -5136,7 +5154,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>463</v>
       </c>
@@ -5147,7 +5165,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>464</v>
       </c>
@@ -5158,7 +5176,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>465</v>
       </c>
@@ -5169,7 +5187,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>466</v>
       </c>
@@ -5180,7 +5198,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>468</v>
       </c>
@@ -5188,7 +5206,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>467</v>
       </c>
@@ -5196,7 +5214,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>470</v>
       </c>
@@ -5207,7 +5225,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>471</v>
       </c>
@@ -5218,7 +5236,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>473</v>
       </c>
@@ -5226,7 +5244,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>474</v>
       </c>
@@ -5237,7 +5255,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>479</v>
       </c>
@@ -5248,7 +5266,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>480</v>
       </c>
@@ -5259,7 +5277,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>485</v>
       </c>
@@ -5270,7 +5288,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>487</v>
       </c>
@@ -5281,7 +5299,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>488</v>
       </c>
@@ -5292,7 +5310,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>492</v>
       </c>
@@ -5303,7 +5321,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>496</v>
       </c>
@@ -5314,7 +5332,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>498</v>
       </c>
@@ -5325,7 +5343,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>499</v>
       </c>
@@ -5336,7 +5354,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>505</v>
       </c>
@@ -5347,7 +5365,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>508</v>
       </c>
@@ -5358,7 +5376,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>509</v>
       </c>
@@ -5369,7 +5387,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>517</v>
       </c>
@@ -5380,7 +5398,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>520</v>
       </c>
@@ -5391,7 +5409,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>521</v>
       </c>
@@ -5402,7 +5420,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>523</v>
       </c>
@@ -5413,7 +5431,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>526</v>
       </c>
@@ -5424,7 +5442,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>531</v>
       </c>
@@ -5435,7 +5453,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>554</v>
       </c>
@@ -5446,7 +5464,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>555</v>
       </c>
@@ -5457,7 +5475,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>556</v>
       </c>
@@ -5468,7 +5486,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>557</v>
       </c>
@@ -5479,7 +5497,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>558</v>
       </c>
@@ -5490,7 +5508,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>559</v>
       </c>
@@ -5501,7 +5519,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>561</v>
       </c>
@@ -5512,7 +5530,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>563</v>
       </c>
@@ -5523,7 +5541,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>567</v>
       </c>
@@ -5534,7 +5552,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>568</v>
       </c>
@@ -5545,11 +5563,11 @@
         <v>572</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="7" t="s">
         <v>583</v>
       </c>
     </row>
@@ -5564,7 +5582,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>581</v>
       </c>
@@ -5572,7 +5590,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>582</v>
       </c>
@@ -5580,19 +5598,40 @@
         <v>580</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
         <v>585</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="C163" t="s">
         <v>586</v>
       </c>
-      <c r="C163" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B164" s="7"/>
+    </row>
+    <row r="164" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A164" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="C164" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A165" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" s="5" t="s">
+        <v>590</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5608,13 +5647,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -5794,13 +5833,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="68.21875" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>203</v>
       </c>
@@ -5808,7 +5847,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>205</v>
       </c>
@@ -5816,7 +5855,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>207</v>
       </c>
@@ -5824,55 +5863,55 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>211</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>212</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>213</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>214</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>215</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>217</v>
       </c>
@@ -5880,7 +5919,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>219</v>
       </c>
@@ -5888,7 +5927,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>221</v>
       </c>
@@ -5896,7 +5935,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
@@ -5904,7 +5943,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>224</v>
       </c>
@@ -5912,7 +5951,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>226</v>
       </c>
@@ -5920,7 +5959,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>228</v>
       </c>
@@ -5928,7 +5967,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>230</v>
       </c>
@@ -5936,7 +5975,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>232</v>
       </c>
@@ -5944,7 +5983,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>234</v>
       </c>
@@ -5952,7 +5991,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>236</v>
       </c>
@@ -5960,31 +5999,31 @@
         <v>237</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>241</v>
       </c>
@@ -5992,7 +6031,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>243</v>
       </c>
@@ -6000,7 +6039,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>245</v>
       </c>
@@ -6008,7 +6047,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>247</v>
       </c>
@@ -6016,7 +6055,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>248</v>
       </c>
@@ -6024,7 +6063,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>250</v>
       </c>
@@ -6032,7 +6071,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>252</v>
       </c>
@@ -6040,7 +6079,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>254</v>
       </c>
@@ -6048,7 +6087,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>255</v>
       </c>
@@ -6056,7 +6095,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>256</v>
       </c>
@@ -6064,7 +6103,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
         <v>258</v>
       </c>
@@ -6072,7 +6111,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>260</v>
       </c>
@@ -6080,7 +6119,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>262</v>
       </c>
@@ -6088,7 +6127,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
         <v>264</v>
       </c>
@@ -6096,7 +6135,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
         <v>266</v>
       </c>
@@ -6104,7 +6143,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
         <v>268</v>
       </c>
@@ -6112,7 +6151,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
         <v>270</v>
       </c>
@@ -6120,7 +6159,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
       <c r="A44" s="13" t="s">
         <v>271</v>
       </c>
@@ -6128,7 +6167,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
         <v>272</v>
       </c>
@@ -6136,7 +6175,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>274</v>
       </c>
@@ -6144,7 +6183,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
         <v>275</v>
       </c>
@@ -6152,7 +6191,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
         <v>276</v>
       </c>
@@ -6160,7 +6199,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
         <v>278</v>
       </c>
@@ -6168,7 +6207,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
         <v>279</v>
       </c>
@@ -6176,7 +6215,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
         <v>281</v>
       </c>
@@ -6210,10 +6249,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="85.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="85.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6432,7 +6471,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="25" t="s">
         <v>345</v>
       </c>
@@ -6440,7 +6479,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="25" t="s">
         <v>347</v>
       </c>
@@ -6448,7 +6487,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="25" t="s">
         <v>349</v>
       </c>
@@ -6456,7 +6495,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="25" t="s">
         <v>351</v>
       </c>
@@ -6464,7 +6503,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="25" t="s">
         <v>353</v>
       </c>
@@ -6472,7 +6511,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="25" t="s">
         <v>355</v>
       </c>
@@ -6480,7 +6519,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="25" t="s">
         <v>357</v>
       </c>
@@ -6488,7 +6527,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="25" t="s">
         <v>359</v>
       </c>

</xml_diff>

<commit_message>
Changes done in Data file and US1247779, US1064240
Changes done in Data file and US1247779, US1064240
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="19420" windowHeight="9050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="13920" windowHeight="3590" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <definedName name="Platform">[1]Sheet2!$A$1:$A$11</definedName>
     <definedName name="URL">[1]Sheet2!$E:$E</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="624">
   <si>
     <t>City</t>
   </si>
@@ -351,13 +351,6 @@
   </si>
   <si>
     <t>Test@123</t>
-  </si>
-  <si>
-    <t>select * from OLE.PORTAL_USER p
- join ole.pay_proc_val pv on p.USER_TYP=pv.PAY_PROC_ACPT_CD_VAL
- join OLE.portal_user_tin pt 
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where p.EMAIL_ADR_TXT='{$email}' and pv.PAY_PROC_CD_DESC='User Type Code'</t>
   </si>
   <si>
     <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt 
@@ -2977,10 +2970,28 @@
     <t>162</t>
   </si>
   <si>
+    <t>Select  cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL  from ole.CONTENT where CONT_NM = 'CreateEnrollmentSubmittedBS'</t>
+  </si>
+  <si>
     <t>Page Content for BS Enrollment Submitted page.</t>
   </si>
   <si>
-    <t>Select cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL from ole.CONTENT where CONT_NM = 'CreateEnrollmentSubmittedBS'</t>
+    <t>select pt.PROV_TIN_NBR, pt.ACCESS_LVL,count(*)  as totalUsers  , pu.EMAIL_ADR_TXT ,pu.FST_NM,pu.LST_NM
+from ole.ENROLLED_PROVIDER ep join  ole.PORTAL_USER_TIN pt   on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
+join ole.PORTAL_USER pu on pu.PORTAL_USER_ID=pt.PORTAL_USER_ID
+group by pt.PROV_TIN_NBR,pt.ACCESS_LVL,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.STS_CD
+having count(*) =1 and pt.ACCESS_LVL='A'   and pu.STS_CD='A'
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>select pt.PROV_TIN_NBR, pt.ACCESS_LVL,count(*)  as totalUsers  , pu.EMAIL_ADR_TXT ,pu.FST_NM,pu.LST_NM
+from ole.ENROLLED_PROVIDER ep join  ole.PORTAL_USER_TIN pt   on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
+join ole.PORTAL_USER pu on pu.PORTAL_USER_ID=pt.PORTAL_USER_ID
+group by pt.PROV_TIN_NBR,pt.ACCESS_LVL,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.STS_CD
+having count(*) =2  and pt.ACCESS_LVL='A'   and pu.STS_CD='A'
+fetch first row only
+with ur</t>
   </si>
   <si>
     <t>163</t>
@@ -2989,16 +3000,108 @@
     <t>164</t>
   </si>
   <si>
+    <t>BS Page Content verification</t>
+  </si>
+  <si>
+    <t>Select TEXT_VAL from ole.CONTENT where CONT_NM ='BillingServiceInformationPage'</t>
+  </si>
+  <si>
     <t>165</t>
   </si>
   <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>186</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>Select  cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL  from ole.CONTENT where CONT_DESC = 'Identify Admins Page'</t>
+  </si>
+  <si>
+    <t>select FST_NM,MIDDLE_INIT,LST_NM,EMAIL_ADR_TXT,TEL_NBR from  OLE.PORTAL_USER p where EMAIL_ADR_TXT ='{$email}'</t>
+  </si>
+  <si>
+    <t>select TEXT_VAL from ole.content where CONT_NM = 'NewChooseEnrollmentPage' and SUB_CAT='txt.cancelenrollment'</t>
+  </si>
+  <si>
+    <t>select TEXT_VAL from ole.CONTENT where CONT_NM like 'ConfirmUserBS'</t>
+  </si>
+  <si>
     <t>Page Content for Identify Administrators</t>
   </si>
   <si>
-    <t>Select  cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL  from ole.CONTENT where CONT_DESC = 'Identify Admins Page'</t>
-  </si>
-  <si>
-    <t>select FST_NM,MIDDLE_INIT,LST_NM,EMAIL_ADR_TXT,TEL_NBR from  OLE.PORTAL_USER p where EMAIL_ADR_TXT ='{$email}'</t>
+    <t>DB value for Cancel Enrollment button</t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p
+ join ole.pay_proc_val pv on p.USER_TYP=pv.PAY_PROC_ACPT_CD_VAL
+ join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID join OLE.enrolled_provider ep
+on ep.PROV_TIN_NBR=pt.PROV_TIN_NBR
+where p.EMAIL_ADR_TXT='{$email}' and pv.PAY_PROC_CD_DESC='User Type Code'</t>
   </si>
 </sst>
 </file>
@@ -3772,7 +3875,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>11</v>
@@ -3882,7 +3985,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -3908,7 +4011,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -3934,7 +4037,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -3960,7 +4063,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -3986,7 +4089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4012,7 +4115,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4046,10 +4149,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D166"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4135,7 +4238,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4143,12 +4246,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>64</v>
+        <v>623</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
@@ -4156,7 +4259,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
@@ -4164,7 +4267,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
@@ -4172,7 +4275,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -4180,7 +4283,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
@@ -4188,1449 +4291,1585 @@
         <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="101" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="101" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="101" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="174" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" t="s">
         <v>105</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C32" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C43" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="201.65" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B44" s="27" t="s">
+        <v>537</v>
+      </c>
+      <c r="C44" t="s">
         <v>538</v>
-      </c>
-      <c r="C44" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="C46" t="s">
         <v>541</v>
-      </c>
-      <c r="C46" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="201.65" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="174" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" t="s">
         <v>165</v>
-      </c>
-      <c r="C51" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="C59" t="s">
         <v>153</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="C59" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" t="s">
         <v>193</v>
-      </c>
-      <c r="C60" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C61" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" t="s">
         <v>182</v>
-      </c>
-      <c r="C64" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B65" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>181</v>
-      </c>
       <c r="C65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C70" t="s">
         <v>197</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="C70" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="244.75" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B71" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>201</v>
-      </c>
       <c r="C71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>284</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>287</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>289</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B79" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B81" s="7" t="s">
         <v>366</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>368</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>376</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>378</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>390</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B92" s="7" t="s">
         <v>392</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B97" s="7" t="s">
         <v>402</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="244.75" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C103" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="345.65" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C104" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="273.64999999999998" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="C105" t="s">
         <v>417</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="C105" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B108" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="B108" s="7" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B112" t="s">
+        <v>434</v>
+      </c>
+      <c r="C112" t="s">
         <v>435</v>
-      </c>
-      <c r="C112" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B113" t="s">
+        <v>436</v>
+      </c>
+      <c r="C113" t="s">
         <v>437</v>
-      </c>
-      <c r="C113" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B114" t="s">
+        <v>438</v>
+      </c>
+      <c r="C114" t="s">
         <v>439</v>
-      </c>
-      <c r="C114" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B115" t="s">
+        <v>440</v>
+      </c>
+      <c r="C115" t="s">
         <v>441</v>
-      </c>
-      <c r="C115" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B116" t="s">
+        <v>442</v>
+      </c>
+      <c r="C116" t="s">
         <v>443</v>
-      </c>
-      <c r="C116" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B117" t="s">
+        <v>444</v>
+      </c>
+      <c r="C117" t="s">
         <v>445</v>
-      </c>
-      <c r="C117" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B118" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C118" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B119" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C119" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B120" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C120" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B121" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C121" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B122" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C122" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B123" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C123" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B124" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C124" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B125" t="s">
         <v>468</v>
-      </c>
-      <c r="B125" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B126" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C127" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C128" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C130" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B131" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="C131" t="s">
         <v>535</v>
-      </c>
-      <c r="C131" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="C132" t="s">
         <v>480</v>
-      </c>
-      <c r="B132" s="7" t="s">
-        <v>482</v>
-      </c>
-      <c r="C132" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="C133" t="s">
         <v>485</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="C133" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C134" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C135" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C136" t="s">
         <v>492</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="C136" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="C137" t="s">
         <v>496</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="C137" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C138" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C139" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B140" s="7" t="s">
         <v>505</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="C140" t="s">
         <v>506</v>
-      </c>
-      <c r="C140" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C141" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C142" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="C143" t="s">
         <v>517</v>
-      </c>
-      <c r="B143" s="7" t="s">
-        <v>516</v>
-      </c>
-      <c r="C143" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C144" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="C145" t="s">
         <v>521</v>
-      </c>
-      <c r="B145" s="7" t="s">
-        <v>529</v>
-      </c>
-      <c r="C145" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="C146" t="s">
         <v>523</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>527</v>
-      </c>
-      <c r="C146" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C147" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C148" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B149" t="s">
+        <v>543</v>
+      </c>
+      <c r="C149" t="s">
         <v>544</v>
-      </c>
-      <c r="C149" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B150" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="C150" t="s">
         <v>546</v>
-      </c>
-      <c r="C150" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B151" t="s">
+        <v>547</v>
+      </c>
+      <c r="C151" t="s">
         <v>548</v>
-      </c>
-      <c r="C151" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B152" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="C152" t="s">
         <v>550</v>
-      </c>
-      <c r="C152" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C153" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C154" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="115.25" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C155" t="s">
         <v>561</v>
-      </c>
-      <c r="B155" s="7" t="s">
-        <v>560</v>
-      </c>
-      <c r="C155" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="C156" t="s">
         <v>563</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>565</v>
-      </c>
-      <c r="C156" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C157" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="187.25" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B158" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="C158" t="s">
         <v>571</v>
       </c>
-      <c r="C158" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="159" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
-        <v>576</v>
-      </c>
-      <c r="B159" s="7" t="s">
-        <v>583</v>
+        <v>575</v>
+      </c>
+      <c r="B159" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="C160" t="s">
         <v>577</v>
-      </c>
-      <c r="B160" s="7" t="s">
-        <v>584</v>
-      </c>
-      <c r="C160" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="B163" s="7" t="s">
         <v>585</v>
-      </c>
-      <c r="B163" s="7" t="s">
-        <v>587</v>
       </c>
       <c r="C163" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+      <c r="A165" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="B165" s="7" t="s">
         <v>588</v>
-      </c>
-      <c r="B164" s="7" t="s">
-        <v>592</v>
-      </c>
-      <c r="C164" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A165" s="5" t="s">
-        <v>589</v>
-      </c>
-      <c r="B165" s="7" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
-        <v>590</v>
+        <v>593</v>
+      </c>
+      <c r="B166" t="s">
+        <v>592</v>
+      </c>
+      <c r="C166" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A167" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C167" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A168" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A169" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C169" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" s="5" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" s="5" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" s="5" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" s="5" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" s="5" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" s="5" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" s="5" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" s="5" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" s="5" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" s="5" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" s="5" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" s="5" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" s="5" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" s="5" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" s="5" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" s="5" t="s">
+        <v>616</v>
       </c>
     </row>
   </sheetData>
@@ -5739,7 +5978,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -5778,13 +6017,13 @@
         <v>47</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
         <v>63</v>
@@ -5801,13 +6040,13 @@
         <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>63</v>
@@ -5841,255 +6080,255 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>203</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>205</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>207</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" s="16"/>
     </row>
     <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" s="16"/>
     </row>
     <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="16"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="B9" s="16"/>
-    </row>
-    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="B11" s="16"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="B11" s="16"/>
-    </row>
-    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="B12" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="B12" s="18" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="B13" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="B13" s="19" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="B14" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="B16" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="19" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="B17" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B17" s="19" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="B18" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="21" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="B19" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="B19" s="21" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="B20" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="B20" s="21" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+      <c r="B21" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="B21" s="21" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="13" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="B22" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="B22" s="21" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="13" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B27" s="16" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="13" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="B28" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="14" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="13" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
+      <c r="B29" s="14" t="s">
         <v>245</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31" s="21" t="s">
         <v>248</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B32" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B33" s="16" t="s">
         <v>252</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>55</v>
@@ -6097,130 +6336,130 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B36" s="21" t="s">
         <v>256</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B37" s="21" t="s">
         <v>258</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B38" s="21" t="s">
         <v>260</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>262</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B40" s="21" t="s">
         <v>264</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>266</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>268</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
       <c r="A44" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B45" s="21" t="s">
         <v>272</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" s="21" t="s">
         <v>276</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B50" s="21" t="s">
         <v>279</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="B51" s="21" t="s">
         <v>281</v>
-      </c>
-      <c r="B51" s="21" t="s">
-        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -6257,282 +6496,282 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>291</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>293</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>295</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>297</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>299</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>301</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>303</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>305</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="B9" s="26" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="25" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+      <c r="B10" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="B10" s="26" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="25" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25" t="s">
+      <c r="B11" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="B11" s="26" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="25" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25" t="s">
+      <c r="B12" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="B12" s="26" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="25" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25" t="s">
+      <c r="B13" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="B13" s="26" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="25" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25" t="s">
+      <c r="B14" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="B14" s="26" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="25" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="25" t="s">
+      <c r="B15" s="26" t="s">
         <v>319</v>
       </c>
-      <c r="B15" s="26" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="25" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25" t="s">
+      <c r="B16" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="B16" s="26" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="25" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="B17" s="26" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="25" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25" t="s">
+      <c r="B18" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="B18" s="26" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="25" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="25" t="s">
+      <c r="B19" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="B19" s="26" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="25" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25" t="s">
+      <c r="B20" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="B20" s="26" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="25" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
+      <c r="B21" s="26" t="s">
         <v>331</v>
       </c>
-      <c r="B21" s="26" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="25" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25" t="s">
+      <c r="B22" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="B22" s="26" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="25" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="25" t="s">
+      <c r="B23" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="B23" s="26" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="25" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="25" t="s">
+      <c r="B24" s="26" t="s">
         <v>337</v>
       </c>
-      <c r="B24" s="26" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="25" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="25" t="s">
+      <c r="B25" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="B25" s="26" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="25" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="25" t="s">
+      <c r="B26" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="B26" s="26" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="25" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="25" t="s">
+      <c r="B27" s="26" t="s">
         <v>343</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="B28" s="26" t="s">
         <v>345</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="B29" s="26" t="s">
         <v>347</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="B30" s="26" t="s">
         <v>349</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="B31" s="26" t="s">
         <v>351</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="B32" s="26" t="s">
         <v>353</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="25" t="s">
+        <v>354</v>
+      </c>
+      <c r="B33" s="26" t="s">
         <v>355</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="25" t="s">
+        <v>356</v>
+      </c>
+      <c r="B34" s="26" t="s">
         <v>357</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="B35" s="26" t="s">
         <v>359</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amit and Madhavi test cases reviewed
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="647">
   <si>
     <t>City</t>
   </si>
@@ -3129,6 +3129,48 @@
   </si>
   <si>
     <t>Select TEXT_VAL from OLE.CONTENT where CONT_NM='FinancialInfoTIN' and SUB_CAT IN ('txt.howdoimfintin','txt.ifyourofintin','txt.ifyourofintin2')  with ur</t>
+  </si>
+  <si>
+    <t>Select  cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL  from ole.CONTENT where CONT_NM like '%EnrollOrgInfo%' order by CREAT_DTTM desc</t>
+  </si>
+  <si>
+    <t>select MKT_TYP_DESC from ole.MARKET_TYPE where MKT_TYP_CATGY='{$mktTyp}' order by MKT_TYP_DESC asc</t>
+  </si>
+  <si>
+    <t>Select  cast(CLOB_VAL as varchar(32000)) as clobval,TEXT_VAL  from ole.CONTENT where CONT_NM like '%EnrollSelectPayMeths%' order by CREAT_DTTM desc</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.payer where PAYR_ACTV_IND='Y' and PAY_METH_OFR_CD='{$ofrCod1}' or PAY_METH_OFR_CD='{$ofrCod2}'order by PAYR_DSPL_NM asc</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.payer where PAYR_ACTV_IND='Y' order by SORT_ORDER,PAYR_DSPL_NM asc</t>
+  </si>
+  <si>
+    <t>Enroll Org info Page Content Verification</t>
+  </si>
+  <si>
+    <t>Select Pay Methods Page Content Validation</t>
+  </si>
+  <si>
+    <t>Select Pay Methoda Page Payer List Verification</t>
+  </si>
+  <si>
+    <t>Select Pay Methods Page Payer Method Code Verification</t>
+  </si>
+  <si>
+    <t>Market Type Description</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>70165</t>
+  </si>
+  <si>
+    <t>2508796866</t>
+  </si>
+  <si>
+    <t>New Orleans</t>
   </si>
 </sst>
 </file>
@@ -3750,10 +3792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4168,6 +4210,32 @@
         <v>29</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>646</v>
+      </c>
+      <c r="C16" t="s">
+        <v>643</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4178,8 +4246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174:C174"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5815,31 +5883,37 @@
         <v>445</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
         <v>599</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="7" t="s">
         <v>625</v>
       </c>
       <c r="C172" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
         <v>600</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="7" t="s">
         <v>627</v>
       </c>
       <c r="C173" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="5" t="s">
         <v>601</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="C174" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
@@ -5872,24 +5946,48 @@
         <v>631</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B178" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="C178" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B179" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="C179" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B180" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="C180" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
         <v>608</v>
+      </c>
+      <c r="B181" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="C181" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Code merge of Prashant C,Athyusha and Sahil
Code merged on behalf of Prashant C,Athyusha and Sahil
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2430" windowWidth="13920" windowHeight="3590" activeTab="1"/>
+    <workbookView xWindow="-1095" yWindow="2445" windowWidth="22320" windowHeight="5805" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,12 @@
     <definedName name="URL">[1]Sheet2!$E:$E</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A216:C221"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="793">
   <si>
     <t>City</t>
   </si>
@@ -3178,6 +3179,684 @@
   <si>
     <t>select * from OLE.PORTAL_USER p where p.SSO_ID='{$id}'</t>
   </si>
+  <si>
+    <t>Select DISTINCT PROV_TAX_ID_NBR,CP_SETL_DT from OLE.SRCH_CONSOL_TBL where ucp_consl_pay_nbr in
+(select consl_pay_nbr from pp001.unconsolidated_payment
+where proc_ctl_id in
+(select proc_ctl_id from ole.proc_ctl
+where EXTRACT_STS_CD = 'C'
+and PAYR_ALS_NM in ('UHCPE5')
+order by proc_ctl_id desc fetch first 1 row only))
+and cp_pay_meth_cd = 'ACH' ORDER BY CP_SETL_DT DESC fetch first 1 row only</t>
+  </si>
+  <si>
+    <t>Gets TIN Number</t>
+  </si>
+  <si>
+    <t>Select ORG_NM from OLE.ENROLLED_PROVIDER WHERE ENRL_STS_CD = 'A' AND PROV_TIN_NBR = '{$ui_Org1}'</t>
+  </si>
+  <si>
+    <t>Get Organization Name</t>
+  </si>
+  <si>
+    <t>Select DISTINCT PAYR_SCHM_NM from OLE.PAYER where PAYR_DSPL_NM = '{$ui_Payer}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Payer Schema </t>
+  </si>
+  <si>
+    <t>Select DISTINCT UCP_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where CP_DSPL_CONSL_PAY_NBR = '{$paymentNum}'</t>
+  </si>
+  <si>
+    <t>Get UCP_CONSL_PAY_NBR</t>
+  </si>
+  <si>
+    <t>Select DISTINCT CP_SETL_DT from OLE.SRCH_CONSOL_TBL where CP_DSPL_CONSL_PAY_NBR = '{$paymentNum}'</t>
+  </si>
+  <si>
+    <t>Get CP_SETL_DT</t>
+  </si>
+  <si>
+    <t>Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 4
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Get CP_DSPL_CONSL_PAY_NBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Select DISTINCT PROV_TAX_ID_NBR from OLE.SRCH_CONSOL_TBL where CP_DSPL_CONSL_PAY_NBR IN
+(Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1))</t>
+  </si>
+  <si>
+    <t>Select  PROV_ADJ_RSN_CD,PROV_ADJ_ID,PROV_PAYR_ADJ_AMT from PP001.PROVIDER_PAYOR_ADJUSTMENT where CONSL_PAY_NBR IN
+(SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 4
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Get PLB Data from DB for Multiple PLB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Select COUNT(DISTINCT RMRK_TYP_RSN_CD) AS COUNT from EPS.REMARK_TYPE_REASON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Remark Codes </t>
+  </si>
+  <si>
+    <t>Select COUNT(DISTINCT CLM_ADJ_RSN_CD) AS COUNT from EPS.CLAIM_ADJUSTMENT_REASON</t>
+  </si>
+  <si>
+    <t>Get Adjustment Resn Codes</t>
+  </si>
+  <si>
+    <t>Select DISTINCT PAYR_SCHM_NM from OLE.PAYER where  PAYR_DSPL_NM = 'TRICARE WEST'</t>
+  </si>
+  <si>
+    <t>Get PAYR_SCHM_NM</t>
+  </si>
+  <si>
+    <t>Select PROV_KEY_ID from PP009.CONSOLIDATED_PAYMENT order by SETL_DT DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>Get PROV_KEY_ID for TRICARE</t>
+  </si>
+  <si>
+    <t>Select DISTINCT PROV_TAX_ID_NBR from PP009.PROVIDER  where PROV_KEY_ID IN
+(Select PROV_KEY_ID from PP009.CONSOLIDATED_PAYMENT order by SETL_DT DESC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Get PROV_TIN_NBR for Tricare</t>
+  </si>
+  <si>
+    <t>Select DISTINCT DSPL_CONSL_PAY_NBR from PP009.CONSOLIDATED_PAYMENT where PROV_KEY_ID IN
+(Select PROV_KEY_ID from PP009.CONSOLIDATED_PAYMENT order by SETL_DT DESC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Get Electronic Payment Number for Tricare</t>
+  </si>
+  <si>
+    <t>Select DISTINCT DESC_TXT from EPS.REMARK_TYPE_REASON</t>
+  </si>
+  <si>
+    <t>Get Remark Codes Descriptions</t>
+  </si>
+  <si>
+    <t>Select DISTINCT PAYR_SCHM_NM from OLE.PAYER where PAYR_835_ID IN
+(Select DISTINCT PAYR_835_ID from OLE.SUB_PAYER where SUB_PAYR_DSPL_NM ='{$UIPayer}')</t>
+  </si>
+  <si>
+    <t>Get PAYR_SCHM_NM from Sub Payer and Payer Table</t>
+  </si>
+  <si>
+    <t>Select DISTINCT PROV_TAX_ID_NBR from OLE.SRCH_CONSOL_TBL where CP_DSPL_CONSL_PAY_NBR IN
+(Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 4
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)) FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>Get TIN for Multiple PLB Adj</t>
+  </si>
+  <si>
+    <t>Get Electronic Payment Number for PLB Only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Data for PLB Only </t>
+  </si>
+  <si>
+    <t>(Select DISTINCT PAYR_SCHM_NM from OLE.PAYER where PAYR_835_ID IN 
+(Select DISTINCT PAYR_835_ID from OLE.SUB_PAYER where SUB_PAYR_DSPL_NM = '{$ui_Payer}'))</t>
+  </si>
+  <si>
+    <t>SELECT * FROM OLE.EPRA_STATUS WHERE CONSL_PAY_NBR='{$paymentNumDB}' fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Epra Status Code</t>
+  </si>
+  <si>
+    <t>User Event Log</t>
+  </si>
+  <si>
+    <t>Select p.PROV_NPI_NBR, cp.SETL_DT
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p,OLE.PROC_CTL pc
+where cp.prov_key_id = p.prov_key_id and cp.PROC_CTL_ID=pc.PROC_CTL_ID
+and p.PROV_TAX_ID_NBR ='020619423'  and pc.EXTRACT_STS_CD='C'
+and cp.SETL_DT between (current date - 180 days) and current date 
+order by cp.SETL_DT DESC
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Instead of query 44 using this for UPA Provider Admin as we have Hardcoded Tin for UPA (time being)</t>
+  </si>
+  <si>
+    <t>Get TIN for PAYER User Type</t>
+  </si>
+  <si>
+    <t>Get TIN for PROVIDER ADMIN</t>
+  </si>
+  <si>
+    <t>Delete from OLE.EPRA_STATUS where CONSL_PAY_NBR ='{$CONSL_PAY_NBR}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To Check EPRA STATUS </t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>192</t>
+  </si>
+  <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>194</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>206</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>218</t>
+  </si>
+  <si>
+    <t>219</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>229</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>232</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>235</t>
+  </si>
+  <si>
+    <t>236</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>238</t>
+  </si>
+  <si>
+    <t>239</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.PAYER where PAYR_ACTV_IND = 'Y' and SORT_ORDER not in ('999') order by  SORT_ORDER asc with ur</t>
+  </si>
+  <si>
+    <t>We will get the list of all the Active Patient Payers</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.PAYER where PAYR_ACTV_IND = 'Y' and SORT_ORDER in ('999') order by  PAYR_DSPL_NM asc with ur</t>
+  </si>
+  <si>
+    <t>We will get the list of all the Active Payers</t>
+  </si>
+  <si>
+    <t>Select p.PROV_TAX_ID_NBR, cp.SETL_DT from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL pc, ole.ENROLLED_PROVIDER ep
+where  pc.PROC_CTL_ID = cp.PROC_CTL_ID  and cp.prov_key_id = p.prov_key_id and ep.PROV_TIN_NBR = p.PROV_TAX_ID_NBR
+and pc.EXTRACT_STS_CD = 'C'
+and ep.ENRL_STS_CD = 'A'
+order by SETL_DT desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>select DATA_BUNDLE_ID, INCL_835_IND, INCL_PAYR_PRA_IND, INCL_EPRA_IND, CREAT_DTTM from ole.DATA_BUNDLE db where db.PROV_TIN_NBR = '{$Prov_tin_nbr}' order by CREAT_DTTM desc fetch first row only</t>
+  </si>
+  <si>
+    <t>We will get the File Type Indicators of Data Bundle Request.</t>
+  </si>
+  <si>
+    <t>select PROV_TIN_NBR, FILE_NM from ole.DATA_BUNDLE 
+where STS_CD = 'C' 
+and FILE_NM is not null 
+and LST_CHG_BY_DTTM &gt; Current Date - 7 days
+order by CREAT_DTTM desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Find the completed Data Bundle for all the TINs</t>
+  </si>
+  <si>
+    <t>select ORG_NM from ole.ENROLLED_PROVIDER where prov_tin_nbr =  '{$Prov_tin_nbr}'</t>
+  </si>
+  <si>
+    <t>Find the Organisation Name of the TIN</t>
+  </si>
+  <si>
+    <t>select PAYR_SCHM_NM, PAYR_DSPL_NM from ole.payer where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where SSO_ID= '{$id}'))</t>
+  </si>
+  <si>
+    <t>Get the Payer and Schema for the SSO ID for Payer</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr, cp.SETL_DT
+from {$Schema}.CONSOLIDATED_PAYMENT cp, {$Schema}.PROVIDER p, OLE.PROC_CTL PC, ole.ENROLLED_PROVIDER ep
+WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and p.PROV_TAX_ID_NBR = ep.PROV_TIN_NBR
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 385 days 
+and ep.ENRL_STS_CD ='A'
+order by cp.SETL_DT desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Get the TIN and Setl_dt for the Schema retrieved from above query</t>
+  </si>
+  <si>
+    <t>select PROV_TIN_NBR, FILE_NM from ole.DATA_BUNDLE where PROV_TIN_NBR = '{$Prov_tin_nbr}'
+and STS_CD = 'C' and FILE_NM is not null and LST_CHG_BY_DTTM &gt; Current Date - 7 days order by LST_CHG_BY_DTTM desc fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Find the completed Data Bundle for BS</t>
+  </si>
+  <si>
+    <t>Delete from OLE.ppra_status p where p.CONSL_PAY_NBR ='{$CONSL_PAY_NBR}'</t>
+  </si>
+  <si>
+    <t>delete from ole.ppra_status_dtl d where d.ppra_status_id in(select p.ppra_status_id from ole.ppra_status p where p.CONSL_PAY_NBR ='{$CONSL_PAY_NBR}')</t>
+  </si>
+  <si>
+    <t>SELECT * FROM OLE.ppra_status WHERE CONSL_PAY_NBR='{$CONSL_PAY_NBR}'</t>
+  </si>
+  <si>
+    <t>select * from ole.PORTAL_USER where SSO_ID = '{$UserID}'</t>
+  </si>
+  <si>
+    <t>Get PROV_TIN_NBR for PLB Adjustments</t>
+  </si>
+  <si>
+    <t>select PAYR_SCHM_NM from ole.payer where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where SSO_ID= '{$id}'))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Schema Name for Payer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Provider Tin for Payer User for Remit/Claim Detail </t>
+  </si>
+  <si>
+    <t>select prov_tax_id_nbr from {$schema}.provider where prov_key_id in (select PROV_KEY_ID from {$schema}.consolidated_payment
+where pay_meth_cd = 'ACH' and proc_ctl_id in (select proc_ctl_id from ole.proc_ctl where EXTRACT_STS_CD in ('C') and OVALL_PROC_STS_CD in ('C','X') and SRCH_TBL_STS_CD = 'C' order by proc_ctl_id desc))
+ORDER BY PROC_DTTM DESC
+FETCH FIRST ROW ONLY WITH UR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get PLB Adj TIN for Payer </t>
+  </si>
+  <si>
+    <t>Select DISTINCT PROV_TAX_ID_NBR from OLE.SRCH_CONSOL_TBL where CP_DSPL_CONSL_PAY_NBR IN
+(Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM {$schema}.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)) FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Select  PROV_ADJ_RSN_CD,PROV_ADJ_ID,PROV_PAYR_ADJ_AMT from PP001.PROVIDER_PAYOR_ADJUSTMENT where CONSL_PAY_NBR IN
+(SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM PP018.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Get Electronic Payment Number for PLB Only for Payer</t>
+  </si>
+  <si>
+    <t>Select  PROV_ADJ_RSN_CD,PROV_ADJ_ID,PROV_PAYR_ADJ_AMT from PP018.PROVIDER_PAYOR_ADJUSTMENT where CONSL_PAY_NBR IN
+(SELECT CONSL_PAY_NBR
+FROM PP018.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Get Data for PLB Only for Payer</t>
+  </si>
+  <si>
+    <t>select prov_tin_nbr AS PROV_TAX_ID_NBR from ole.portal_user_tin
+where portal_user_id in (select portal_user_id from ole.portal_user where sso_id = '{$id}')
+and prov_tin_nbr in (select prov_tax_id_nbr from pp018.provider where prov_key_id in (select PROV_KEY_ID from pp018.consolidated_payment
+where proc_ctl_id in (select proc_ctl_id from ole.proc_ctl where EXTRACT_STS_CD in ('X','C') and OVALL_PROC_STS_CD in ('C','X') and SRCH_TBL_STS_CD = 'C' order by proc_ctl_id desc)))
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT * FROM
+(
+-- For ranking the records
+SELECT PROV_TIN_NBR as PROV_TAX_ID_NBR, USER_TYP, STS_CD,PROV_NPI_NBR,LST_NM,SBSCR_ID,PTNT_FST_NM,PTNT_LST_NM,PTNT_ACCT_NBR,CLM_NBR, DSPL_CONSL_PAY_NBR, CONSL_PAY_NBR, SETL_DT, PAYR_SCHM_NM, PAYR_835_ID, CLAIMCOUNT, PORTAL_USER_ID, USERNAME, 'Performance_2252017' AS EPSPWD, OPTUMID, 'Payables@125' AS OPTUMPWD,
+ROW_NUMBER() OVER (PARTITION BY PROV_TIN_NBR, USER_TYP, STS_CD,PROV_NPI_NBR,LST_NM,SBSCR_ID,PTNT_FST_NM,PTNT_LST_NM,PTNT_ACCT_NBR,CLM_NBR,DSPL_CONSL_PAY_NBR, CONSL_PAY_NBR, SETL_DT, PAYR_SCHM_NM, PAYR_835_ID, CLAIMCOUNT ORDER BY PORTAL_USER_ID, USERNAME, OPTUMID) AS USER_RANK
+FROM (
+-- Main SQL that extracts the data
+SELECT PU.PORTAL_USER_ID, PU.USERNAME, TRIM(PU.SSO_ID) AS OPTUMID, PUT.PROV_TIN_NBR, PU.USER_TYP, PU.STS_CD,
+SC.CP_DSPL_CONSL_PAY_NBR AS DSPL_CONSL_PAY_NBR, SC.UCP_CONSL_PAY_NBR AS CONSL_PAY_NBR, TO_CHAR(SC.CP_SETL_DT,'MM/DD/YYYY') as SETL_DT, SC.PAYR_SCHM_NM, SC.PYR_SEC_PAYR_ID AS PAYR_835_ID,
+SC.PROV_NPI_NBR,SCL.RP_UPPER_LST_NM as LST_NM,SCL.SUB_SBSCR_ID as SBSCR_ID, SCL.CLM_PTNT_FST_NM as PTNT_FST_NM, SCL.CLM_PTNT_LST_NM as PTNT_LST_NM,
+SCL.CLM_PTNT_ACCT_NBR as PTNT_ACCT_NBR, SCL.CLM_NBR as CLM_NBR,
+COUNT(DISTINCT SCL.CLM_KEY_ID) as CLAIMCOUNT
+FROM OLE.PORTAL_USER PU, OLE.PORTAL_USER_TIN PUT, OLE.EPRA_STATUS EP, OLE.SRCH_CONSOL_TBL SC, OLE.SRCH_CLAIM_TBL SCL
+WHERE PU.PORTAL_USER_ID = PUT.PORTAL_USER_ID -- Join PU with PUT
+AND PUT.PROV_TIN_NBR=SC.PROV_TAX_ID_NBR-- Join SC with PUT
+AND SC.UCP_UCONSL_PAY_KEY_ID = SCL.CUP_UCONSL_PAY_KEY_ID-- Join SC with SCL
+AND SC.PAYR_SCHM_NM=SCL.PAYR_SCHM_NM-- Join SC with SCL- Payer
+AND SC.PAYR_SCHM_NM = 'PP008'-- &lt;&lt;Change Payer Schema Name here&gt;&gt;
+AND SC.CP_SETL_DT BETWEEN '2019-03-01' AND '2019-05-15' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
+AND PU.STS_CD='A'
+AND PU.USER_TYP='P'
+AND EP.PRIORITY = '{$priority}'
+AND SCL.RP_UPPER_LST_NM != '' 
+AND SC.UCP_CONSL_PAY_NBR NOT IN 
+(SELECT DISTINCT EP.CONSL_PAY_NBR FROM OLE.EPRA_STATUS EP WHERE EP.CONSL_PAY_NBR=SC.UCP_CONSL_PAY_NBR)-- Payment ID shouldn't exist in EPRA_STATUS
+AND PU.SSO_ID = '{$id}'
+GROUP BY PU.PORTAL_USER_ID, PU.USERNAME, PU.SSO_ID, PUT.PROV_TIN_NBR, PU.USER_TYP, PU.STS_CD,
+SC.CP_DSPL_CONSL_PAY_NBR, SC.UCP_CONSL_PAY_NBR, TO_CHAR(SC.CP_SETL_DT,'MM/DD/YYYY'), SC.PAYR_SCHM_NM, SC.PYR_SEC_PAYR_ID,
+SC.PROV_NPI_NBR,SCL.RP_UPPER_LST_NM,SCL.SUB_SBSCR_ID , SCL.CLM_PTNT_FST_NM , SCL.CLM_PTNT_LST_NM ,
+SCL.CLM_PTNT_ACCT_NBR , SCL.CLM_NBR 
+HAVING COUNT(DISTINCT SCL.CLM_KEY_ID) BETWEEN 1 AND 10  -- &lt;&lt; Change the claim count range here &gt;&gt;
+----FETCH FIRST  ROW ONLY
+)
+)DUPLUSR
+WHERE DUPLUSR.USER_RANK=1 AND LST_NM != '' AND PROV_NPI_NBR IS NOT NULL
+ORDER BY SETL_DT DESC
+fetch first row only
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  select sc.Payr_schm_nm, sc.CP_DSPL_CONSL_PAY_NBR as DSPL_CONSL_PAY_NBR, sc.CP_SETL_DT as SETL_DT, sc.UCP_CONSL_PAY_NBR as CONSL_PAY_NBR,
+sc.PROV_NPI_NBR, sc.PROV_TAX_ID_NBR, es.claim_cnt, ct.clm_nbr, ct.CLM_PTNT_ACCT_NBR as PTNT_ACCT_NBR,ct.SUB_SBSCR_ID as SBSCR_ID, ct.CLM_PTNT_FST_NM as PTNT_FST_NM, ct.CLM_PTNT_LST_NM as PTNT_LST_NM,
+ct.RP_UPPER_LST_NM as LST_NM
+from ole.srch_consol_tbl sc, ole.epra_status es, ole.srch_claim_tbl ct
+where es.REQ_STS = 'C' and es.PRIORITY =  '{$priority}'
+and sc.ucp_consl_pay_nbr = es.consl_pay_nbr
+and sc.UCP_UCONSL_PAY_KEY_ID = ct.CUP_UCONSL_PAY_KEY_ID
+and sc.PAYR_SCHM_NM='PP008'
+and sc.prov_tax_id_nbr in (select PROV_TIN_NBR from ole.PORTAL_USER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sso_id = '{$id}'))
+and ct.RP_UPPER_LST_NM != '' AND es.claim_cnt IS NOT NULL AND sc.PROV_NPI_NBR IS NOT NULL
+order by sc.CP_SETL_DT desc
+fetch first 1 row only
+</t>
+  </si>
+  <si>
+    <t>For EPRA Generated for Provider</t>
+  </si>
+  <si>
+    <t>select sc.Payr_schm_nm, sc.CP_DSPL_CONSL_PAY_NBR as DSPL_CONSL_PAY_NBR, sc.CP_SETL_DT as SETL_DT, sc.UCP_CONSL_PAY_NBR as CONSL_PAY_NBR,
+sc.PROV_NPI_NBR, sc.PROV_TAX_ID_NBR, es.claim_cnt, ct.clm_nbr, ct.CLM_PTNT_ACCT_NBR as PTNT_ACCT_NBR, ct.CLM_SBSCR_KEY_ID as SBSCR_ID, ct.CLM_PTNT_FST_NM as PTNT_FST_NM, ct.CLM_PTNT_LST_NM as PTNT_LST_NM,
+ct.RP_UPPER_LST_NM as LST_NM
+from ole.srch_consol_tbl sc, ole.epra_status es, ole.srch_claim_tbl ct
+where es.REQ_STS = 'C' and es.PRIORITY =  '{$priority}'
+and sc.ucp_consl_pay_nbr = es.consl_pay_nbr
+and sc.UCP_UCONSL_PAY_KEY_ID = ct.CUP_UCONSL_PAY_KEY_ID
+AND ct.RP_UPPER_LST_NM != '' 
+and es.PAYR_SCHM_NM in
+(select PAYR_SCHM_NM from ole.Payer where payr_tin_nbr in
+(select Payr_tin_nbr from ole.portal_user_payer_tin where portal_user_id in
+(select portal_user_id from ole.portal_user where sso_id = '{$id}')))
+order by es.epra_status_id desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPRA Generated Payer </t>
+  </si>
+  <si>
+    <t>Get PROV_TIN for EPRA Module</t>
+  </si>
+  <si>
+    <t>SELECT PROV_TIN_NBR as PROV_TAX_ID_NBR,PROV_NPI_NBR,LST_NM,SBSCR_ID,PTNT_FST_NM,PTNT_LST_NM,PTNT_ACCT_NBR,CLM_NBR, DSPL_CONSL_PAY_NBR, CONSL_PAY_NBR, SETL_DT, PAYR_SCHM_NM, PAYR_835_ID, CLAIMCOUNT,
+ROW_NUMBER() OVER (PARTITION BY PROV_TIN_NBR,PROV_NPI_NBR,LST_NM,SBSCR_ID,PTNT_FST_NM,PTNT_LST_NM,PTNT_ACCT_NBR,CLM_NBR,DSPL_CONSL_PAY_NBR, CONSL_PAY_NBR, SETL_DT, PAYR_SCHM_NM, PAYR_835_ID, CLAIMCOUNT) AS USER_RANK
+FROM (
+        SELECT 
+                SC.PROV_TAX_ID_NBR AS PROV_TIN_NBR, 
+                SC.CP_DSPL_CONSL_PAY_NBR AS DSPL_CONSL_PAY_NBR, 
+                SC.UCP_CONSL_PAY_NBR AS CONSL_PAY_NBR, 
+                TO_CHAR(SC.CP_SETL_DT,'MM/DD/YYYY') as SETL_DT, 
+                SC.PAYR_SCHM_NM, 
+                SC.PYR_SEC_PAYR_ID AS PAYR_835_ID,
+                SC.PROV_NPI_NBR,
+                SCL.RP_UPPER_LST_NM as LST_NM,
+                SCL.SUB_SBSCR_ID as SBSCR_ID, 
+                SCL.CLM_PTNT_FST_NM as PTNT_FST_NM, 
+                SCL.CLM_PTNT_LST_NM as PTNT_LST_NM,
+                SCL.CLM_PTNT_ACCT_NBR as PTNT_ACCT_NBR, 
+                SCL.CLM_NBR as CLM_NBR,
+                COUNT(DISTINCT SCL.CLM_KEY_ID) as CLAIMCOUNT
+        FROM (SELECT * FROM OLE.SRCH_CONSOL_TBL WHERE PAYR_SCHM_NM = 'PP008' AND CP_PAY_METH_CD = 'ACH'
+                AND CP_SETL_DT BETWEEN '2019-03-01' AND '2019-05-15') SC
+        LEFT JOIN OLE.SRCH_CLAIM_TBL SCL 
+                ON SCL.CUP_UCONSL_PAY_KEY_ID = SC.UCP_UCONSL_PAY_KEY_ID 
+        WHERE
+                SC.UCP_CONSL_PAY_NBR NOT IN 
+                        (SELECT DISTINCT EP.CONSL_PAY_NBR FROM OLE.EPRA_STATUS EP where EP.PRIORITY = '{$priority}')
+        And SC.PROV_TAX_ID_NBR in (SELECT PROV_TIN_NBR FROM OLE.BILLING_SERVICE_PROVIDER WHERE BILLING_SERVICE_ID IN 
+                                        (SELECT BILLING_SERVICE_ID FROM OLE.PORTAL_USER_BS_TIN WHERE PORTAL_USER_ID IN 
+                                        (SELECT PORTAL_USER_ID FROM OLE.PORTAL_USER WHERE SSO_ID = '{$id}' AND STS_CD = 'A')) and STS_CD = 'A')
+        GROUP BY 
+                SC.PROV_TAX_ID_NBR, 
+                SC.CP_DSPL_CONSL_PAY_NBR, 
+                SC.UCP_CONSL_PAY_NBR, 
+                TO_CHAR(SC.CP_SETL_DT,'MM/DD/YYYY'), 
+                SC.PAYR_SCHM_NM, 
+                SC.PYR_SEC_PAYR_ID,
+                SC.PROV_NPI_NBR,
+                SCL.RP_UPPER_LST_NM,
+                SCL.SUB_SBSCR_ID, 
+                SCL.CLM_PTNT_FST_NM, 
+                SCL.CLM_PTNT_LST_NM, 
+                SCL.CLM_PTNT_ACCT_NBR, 
+                SCL.CLM_NBR                        
+        HAVING COUNT(DISTINCT SCL.CLM_KEY_ID) BETWEEN 1 AND 150
+        FETCH FIRST  ROW ONLY
+)</t>
+  </si>
+  <si>
+    <t>EPRA for BS</t>
+  </si>
+  <si>
+    <t>select sc.Payr_schm_nm, sc.CP_DSPL_CONSL_PAY_NBR as DSPL_CONSL_PAY_NBR, sc.CP_SETL_DT as SETL_DT, sc.UCP_CONSL_PAY_NBR as CONSL_PAY_NBR,
+sc.PROV_NPI_NBR, sc.PROV_TAX_ID_NBR, es.claim_cnt, ct.clm_nbr, ct.CLM_PTNT_ACCT_NBR as PTNT_ACCT_NBR, ct.CLM_SBSCR_KEY_ID as SBSCR_ID, ct.CLM_PTNT_FST_NM as PTNT_FST_NM, ct.CLM_PTNT_LST_NM as PTNT_LST_NM,
+ct.RP_UPPER_LST_NM as LST_NM
+from ole.srch_consol_tbl sc, ole.epra_status es, ole.srch_claim_tbl ct
+where es.REQ_STS = 'C' and es.PRIORITY =  '{$priority}'
+and sc.ucp_consl_pay_nbr = es.consl_pay_nbr
+and sc.UCP_UCONSL_PAY_KEY_ID = ct.CUP_UCONSL_PAY_KEY_ID
+and sc.prov_tax_id_nbr in
+(SELECT PROV_TIN_NBR FROM OLE.BILLING_SERVICE_PROVIDER WHERE BILLING_SERVICE_ID IN (SELECT BILLING_SERVICE_ID FROM OLE.PORTAL_USER_BS_TIN 
+WHERE PORTAL_USER_ID IN (SELECT PORTAL_USER_ID FROM OLE.PORTAL_USER WHERE SSO_ID = '{$id}')))
+AND ct.RP_UPPER_LST_NM != ''
+order by sc.CP_SETL_DT desc
+fetch first 1 row only</t>
+  </si>
+  <si>
+    <t>Get PROV_TIN_NBR for EPRAGENERATED BS</t>
+  </si>
+  <si>
+    <t>SELECT * FROM
+(
+-- For ranking the records
+SELECT PROV_TIN_NBR as PROV_TAX_ID_NBR, USER_TYP, STS_CD,PROV_NPI_NBR,LST_NM,SBSCR_ID,PTNT_FST_NM,PTNT_LST_NM,PTNT_ACCT_NBR,CLM_NBR, DSPL_CONSL_PAY_NBR, CONSL_PAY_NBR, SETL_DT, PAYR_SCHM_NM, PAYR_835_ID, CLAIMCOUNT, PORTAL_USER_ID, USERNAME, 'Performance_2252017' AS EPSPWD, OPTUMID, 'Payables@125' AS OPTUMPWD,
+ROW_NUMBER() OVER (PARTITION BY PROV_TIN_NBR, USER_TYP, STS_CD,PROV_NPI_NBR,LST_NM,SBSCR_ID,PTNT_FST_NM,PTNT_LST_NM,PTNT_ACCT_NBR,CLM_NBR,DSPL_CONSL_PAY_NBR, CONSL_PAY_NBR, SETL_DT, PAYR_SCHM_NM, PAYR_835_ID, CLAIMCOUNT ORDER BY PORTAL_USER_ID, USERNAME, OPTUMID) AS USER_RANK
+FROM (
+-- Main SQL that extracts the data
+SELECT PU.PORTAL_USER_ID, PU.USERNAME, TRIM(PU.SSO_ID) AS OPTUMID, PUT.PROV_TIN_NBR, PU.USER_TYP, PU.STS_CD,
+SC.CP_DSPL_CONSL_PAY_NBR AS DSPL_CONSL_PAY_NBR, SC.UCP_CONSL_PAY_NBR AS CONSL_PAY_NBR, TO_CHAR(SC.CP_SETL_DT,'MM/DD/YYYY') as SETL_DT, SC.PAYR_SCHM_NM, SC.PYR_SEC_PAYR_ID AS PAYR_835_ID,
+SC.PROV_NPI_NBR,SCL.RP_UPPER_LST_NM as LST_NM,SCL.SUB_SBSCR_ID as SBSCR_ID, SCL.CLM_PTNT_FST_NM as PTNT_FST_NM, SCL.CLM_PTNT_LST_NM as PTNT_LST_NM, SCL.CLM_UPER_PTNT_LST_NM AS REND_PROV_NM,
+SCL.CLM_PTNT_ACCT_NBR as PTNT_ACCT_NBR, SCL.CLM_NBR as CLM_NBR,
+COUNT(DISTINCT SCL.CLM_KEY_ID) as CLAIMCOUNT
+FROM OLE.PORTAL_USER PU, OLE.PORTAL_USER_TIN PUT, OLE.EPRA_STATUS EP, OLE.SRCH_CONSOL_TBL SC, OLE.SRCH_CLAIM_TBL SCL
+WHERE PU.PORTAL_USER_ID = PUT.PORTAL_USER_ID -- Join PU with PUT
+AND PUT.PROV_TIN_NBR=SC.PROV_TAX_ID_NBR-- Join SC with PUT
+AND SC.UCP_UCONSL_PAY_KEY_ID = SCL.CUP_UCONSL_PAY_KEY_ID-- Join SC with SCL
+AND SC.PAYR_SCHM_NM=SCL.PAYR_SCHM_NM-- Join SC with SCL- Payer
+AND SC.PAYR_SCHM_NM = 'PP018'-- &lt;&lt;Change Payer Schema Name here&gt;&gt;
+AND SC.CP_SETL_DT BETWEEN '2019-03-01' AND '2019-05-15' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
+AND PU.STS_CD='A'
+AND PU.USER_TYP='P'
+AND EP.PRIORITY = '{$priority}'
+and SCL.CLM_PTNT_ACCT_NBR != '0'
+AND SC.UCP_CONSL_PAY_NBR NOT IN 
+(SELECT DISTINCT EP.CONSL_PAY_NBR FROM OLE.EPRA_STATUS EP WHERE EP.CONSL_PAY_NBR=SC.UCP_CONSL_PAY_NBR)-- Payment ID shouldn't exist in EPRA_STATUS
+GROUP BY PU.PORTAL_USER_ID, PU.USERNAME, PU.SSO_ID, PUT.PROV_TIN_NBR, PU.USER_TYP, PU.STS_CD,
+SC.CP_DSPL_CONSL_PAY_NBR, SC.UCP_CONSL_PAY_NBR, TO_CHAR(SC.CP_SETL_DT,'MM/DD/YYYY'), SC.PAYR_SCHM_NM, SC.PYR_SEC_PAYR_ID,
+SC.PROV_NPI_NBR,SCL.RP_UPPER_LST_NM,SCL.SUB_SBSCR_ID , SCL.CLM_PTNT_FST_NM , SCL.CLM_PTNT_LST_NM ,
+SCL.CLM_PTNT_ACCT_NBR , SCL.CLM_NBR , SCL.CLM_UPER_PTNT_LST_NM
+HAVING COUNT(DISTINCT SCL.CLM_KEY_ID) BETWEEN 1 AND 10  -- &lt;&lt; Change the claim count range here &gt;&gt;
+FETCH FIRST  ROW ONLY
+)
+)DUPLUSR
+WHERE DUPLUSR.USER_RANK=1
+fetch first row only</t>
+  </si>
+  <si>
+    <t>select * from ole.user_evnt_log
+where (EVNT_MSG like '%DataAccess:SUCCESS%' and
+EVNT_MSG like '%EPRA%')order by CREAT_DTTM desc fetch first row only</t>
+  </si>
 </sst>
 </file>
 
@@ -3336,7 +4015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3383,6 +4062,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3394,6 +4076,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3402,110 +4087,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="TestExecution"/>
       <sheetName val="Sheet2"/>
-      <sheetName val="MasterCredentials"/>
-      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Android</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>http://apsrd4468:8080/Fulfillment-UI/resources/index.html</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Chrome</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v xml:space="preserve">http://stglive.myuhc.com/msuperuser </v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>IExplorer</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v xml:space="preserve">http://offline.myuhc.com/msuperuser </v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>FireFox</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>https://systest1.myuhc.com/msuperuser</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Safari</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>https://systest2.myuhc.com/msuperuser</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Sauce</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>https://sys2.myuhc.com/msuperuser</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Sauce-chrome</v>
-          </cell>
-          <cell r="E7" t="str">
-            <v>http://apsrt0451.uhc.com:8080/walgreens/guest/login</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Sauce-firefox</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>https://systest6.uhconline.com/b2c/</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Sauce-ie</v>
-          </cell>
-          <cell r="E9" t="str">
-            <v>https://systest4.uhconline.com/</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Sauce-andriod</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v xml:space="preserve">http://apsrt0340:18080/prweb/PRServlet/ </v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Sauce-iphone</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>https://ohpe-test2.optum.com/trans/loginUser.uol</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12" t="str">
-            <v>http://apsrt1684.uhc.com:9080/ormsui/index.html#/</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3804,16 +4389,16 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4060,7 +4645,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4086,7 +4671,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4112,7 +4697,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4138,7 +4723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4164,7 +4749,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4190,7 +4775,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4216,7 +4801,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -4250,20 +4835,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D189"/>
+  <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A207" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C209" sqref="C209"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="82.90625" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="136.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4274,7 +4859,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4285,7 +4870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4296,7 +4881,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4304,7 +4889,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4315,7 +4900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4323,7 +4908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4331,7 +4916,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4339,7 +4924,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4347,7 +4932,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4355,7 +4940,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4363,7 +4948,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4371,7 +4956,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4379,7 +4964,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4387,7 +4972,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4395,7 +4980,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -4403,7 +4988,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -4411,7 +4996,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -4419,7 +5004,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -4427,7 +5012,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
@@ -4435,7 +5020,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -4443,7 +5028,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
@@ -4451,7 +5036,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
@@ -4459,7 +5044,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -4467,7 +5052,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>91</v>
       </c>
@@ -4475,7 +5060,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>92</v>
       </c>
@@ -4483,7 +5068,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
@@ -4491,7 +5076,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>94</v>
       </c>
@@ -4499,7 +5084,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>96</v>
       </c>
@@ -4507,7 +5092,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>97</v>
       </c>
@@ -4518,7 +5103,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -4529,7 +5114,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
@@ -4540,7 +5125,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="187.35" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -4551,7 +5136,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>109</v>
       </c>
@@ -4559,7 +5144,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>110</v>
       </c>
@@ -4567,7 +5152,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
@@ -4578,7 +5163,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>114</v>
       </c>
@@ -4589,7 +5174,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
@@ -4597,7 +5182,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>119</v>
       </c>
@@ -4605,7 +5190,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>120</v>
       </c>
@@ -4613,7 +5198,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>123</v>
       </c>
@@ -4621,7 +5206,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>124</v>
       </c>
@@ -4635,7 +5220,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>126</v>
       </c>
@@ -4646,7 +5231,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="203" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>127</v>
       </c>
@@ -4657,7 +5242,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -4668,7 +5253,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -4679,7 +5264,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="203" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>130</v>
       </c>
@@ -4690,7 +5275,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>131</v>
       </c>
@@ -4701,7 +5286,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>132</v>
       </c>
@@ -4712,7 +5297,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>133</v>
       </c>
@@ -4723,7 +5308,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>134</v>
       </c>
@@ -4734,7 +5319,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>135</v>
       </c>
@@ -4745,7 +5330,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>136</v>
       </c>
@@ -4756,7 +5341,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>137</v>
       </c>
@@ -4764,7 +5349,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>139</v>
       </c>
@@ -4775,7 +5360,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>140</v>
       </c>
@@ -4783,7 +5368,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>146</v>
       </c>
@@ -4794,7 +5379,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>147</v>
       </c>
@@ -4802,7 +5387,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>151</v>
       </c>
@@ -4813,7 +5398,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>153</v>
       </c>
@@ -4824,7 +5409,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>154</v>
       </c>
@@ -4835,7 +5420,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>155</v>
       </c>
@@ -4846,7 +5431,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>156</v>
       </c>
@@ -4854,7 +5439,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>177</v>
       </c>
@@ -4865,7 +5450,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>178</v>
       </c>
@@ -4876,7 +5461,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>183</v>
       </c>
@@ -4884,7 +5469,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>184</v>
       </c>
@@ -4892,7 +5477,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>185</v>
       </c>
@@ -4900,7 +5485,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>186</v>
       </c>
@@ -4908,7 +5493,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>195</v>
       </c>
@@ -4919,7 +5504,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>198</v>
       </c>
@@ -4930,7 +5515,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>200</v>
       </c>
@@ -4938,7 +5523,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>281</v>
       </c>
@@ -4946,7 +5531,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>282</v>
       </c>
@@ -4954,7 +5539,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>285</v>
       </c>
@@ -4962,7 +5547,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>287</v>
       </c>
@@ -4970,7 +5555,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>359</v>
       </c>
@@ -4978,7 +5563,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>360</v>
       </c>
@@ -4986,7 +5571,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>361</v>
       </c>
@@ -4994,7 +5579,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>363</v>
       </c>
@@ -5002,7 +5587,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>364</v>
       </c>
@@ -5010,7 +5595,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>366</v>
       </c>
@@ -5018,7 +5603,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>368</v>
       </c>
@@ -5026,7 +5611,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>369</v>
       </c>
@@ -5034,7 +5619,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>370</v>
       </c>
@@ -5042,7 +5627,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>371</v>
       </c>
@@ -5050,7 +5635,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>373</v>
       </c>
@@ -5058,7 +5643,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>374</v>
       </c>
@@ -5066,7 +5651,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>376</v>
       </c>
@@ -5074,7 +5659,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>387</v>
       </c>
@@ -5082,7 +5667,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>388</v>
       </c>
@@ -5090,7 +5675,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>390</v>
       </c>
@@ -5098,7 +5683,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>393</v>
       </c>
@@ -5106,7 +5691,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>395</v>
       </c>
@@ -5114,7 +5699,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>397</v>
       </c>
@@ -5122,7 +5707,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>399</v>
       </c>
@@ -5130,7 +5715,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>400</v>
       </c>
@@ -5138,7 +5723,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>403</v>
       </c>
@@ -5146,7 +5731,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>408</v>
       </c>
@@ -5154,7 +5739,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>409</v>
       </c>
@@ -5162,7 +5747,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>410</v>
       </c>
@@ -5170,7 +5755,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>411</v>
       </c>
@@ -5178,7 +5763,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" ht="187.35" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>412</v>
       </c>
@@ -5189,7 +5774,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="348" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>413</v>
       </c>
@@ -5200,7 +5785,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" ht="230.45" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>415</v>
       </c>
@@ -5211,7 +5796,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>418</v>
       </c>
@@ -5219,7 +5804,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>420</v>
       </c>
@@ -5227,7 +5812,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>425</v>
       </c>
@@ -5235,7 +5820,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>427</v>
       </c>
@@ -5243,7 +5828,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>428</v>
       </c>
@@ -5251,7 +5836,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>429</v>
       </c>
@@ -5259,7 +5844,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>452</v>
       </c>
@@ -5270,7 +5855,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>453</v>
       </c>
@@ -5281,7 +5866,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>454</v>
       </c>
@@ -5292,7 +5877,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>455</v>
       </c>
@@ -5303,7 +5888,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>456</v>
       </c>
@@ -5314,7 +5899,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>457</v>
       </c>
@@ -5325,7 +5910,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>458</v>
       </c>
@@ -5336,7 +5921,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>459</v>
       </c>
@@ -5347,7 +5932,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>460</v>
       </c>
@@ -5358,7 +5943,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>461</v>
       </c>
@@ -5369,7 +5954,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>462</v>
       </c>
@@ -5380,7 +5965,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>463</v>
       </c>
@@ -5391,7 +5976,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>464</v>
       </c>
@@ -5402,7 +5987,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>466</v>
       </c>
@@ -5410,7 +5995,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>465</v>
       </c>
@@ -5418,7 +6003,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>468</v>
       </c>
@@ -5429,7 +6014,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>469</v>
       </c>
@@ -5440,7 +6025,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>471</v>
       </c>
@@ -5448,7 +6033,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>472</v>
       </c>
@@ -5459,7 +6044,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>477</v>
       </c>
@@ -5470,7 +6055,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>478</v>
       </c>
@@ -5481,7 +6066,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>483</v>
       </c>
@@ -5492,7 +6077,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>485</v>
       </c>
@@ -5503,7 +6088,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>486</v>
       </c>
@@ -5514,7 +6099,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>490</v>
       </c>
@@ -5525,7 +6110,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>494</v>
       </c>
@@ -5536,7 +6121,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>496</v>
       </c>
@@ -5547,7 +6132,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>497</v>
       </c>
@@ -5558,7 +6143,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>503</v>
       </c>
@@ -5569,7 +6154,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>506</v>
       </c>
@@ -5580,7 +6165,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>507</v>
       </c>
@@ -5591,7 +6176,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>515</v>
       </c>
@@ -5602,7 +6187,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>518</v>
       </c>
@@ -5613,7 +6198,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>519</v>
       </c>
@@ -5624,7 +6209,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>521</v>
       </c>
@@ -5635,7 +6220,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>524</v>
       </c>
@@ -5646,7 +6231,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>529</v>
       </c>
@@ -5657,7 +6242,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>552</v>
       </c>
@@ -5668,7 +6253,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>553</v>
       </c>
@@ -5679,7 +6264,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>554</v>
       </c>
@@ -5690,7 +6275,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>555</v>
       </c>
@@ -5701,7 +6286,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>556</v>
       </c>
@@ -5712,7 +6297,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>557</v>
       </c>
@@ -5723,7 +6308,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>559</v>
       </c>
@@ -5734,7 +6319,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>561</v>
       </c>
@@ -5745,7 +6330,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>565</v>
       </c>
@@ -5756,7 +6341,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>566</v>
       </c>
@@ -5767,7 +6352,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>574</v>
       </c>
@@ -5775,7 +6360,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>575</v>
       </c>
@@ -5786,7 +6371,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>579</v>
       </c>
@@ -5794,7 +6379,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>580</v>
       </c>
@@ -5802,7 +6387,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>583</v>
       </c>
@@ -5813,7 +6398,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>588</v>
       </c>
@@ -5821,7 +6406,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>589</v>
       </c>
@@ -5829,7 +6414,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>592</v>
       </c>
@@ -5840,7 +6425,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>593</v>
       </c>
@@ -5851,7 +6436,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>594</v>
       </c>
@@ -5859,7 +6444,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>595</v>
       </c>
@@ -5870,7 +6455,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>596</v>
       </c>
@@ -5878,7 +6463,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>597</v>
       </c>
@@ -5889,7 +6474,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>598</v>
       </c>
@@ -5900,7 +6485,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>599</v>
       </c>
@@ -5911,7 +6496,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>600</v>
       </c>
@@ -5922,7 +6507,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>601</v>
       </c>
@@ -5930,7 +6515,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>602</v>
       </c>
@@ -5941,7 +6526,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>603</v>
       </c>
@@ -5952,7 +6537,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>604</v>
       </c>
@@ -5963,7 +6548,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>605</v>
       </c>
@@ -5974,7 +6559,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>606</v>
       </c>
@@ -5985,7 +6570,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>607</v>
       </c>
@@ -5996,7 +6581,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>608</v>
       </c>
@@ -6007,39 +6592,587 @@
         <v>647</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B183" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="C183" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B184" t="s">
+        <v>651</v>
+      </c>
+      <c r="C184" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B185" t="s">
+        <v>653</v>
+      </c>
+      <c r="C185" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B186" t="s">
+        <v>655</v>
+      </c>
+      <c r="C186" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B187" t="s">
+        <v>657</v>
+      </c>
+      <c r="C187" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B188" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="C188" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>615</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="C189" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A190" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="C190" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
+      <c r="A191" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="C191" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A192" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="C192" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="B193" t="s">
+        <v>665</v>
+      </c>
+      <c r="C193" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B194" t="s">
+        <v>667</v>
+      </c>
+      <c r="C194" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="B195" t="s">
+        <v>669</v>
+      </c>
+      <c r="C195" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="B196" t="s">
+        <v>671</v>
+      </c>
+      <c r="C196" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="C197" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="C198" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="B199" t="s">
+        <v>677</v>
+      </c>
+      <c r="C199" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="B200" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="C200" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="C201" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A202" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="B202" s="7" t="s">
+        <v>774</v>
+      </c>
+      <c r="C202" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A203" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="C203" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="B204" s="7" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A205" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="C205" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A206" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="B206" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="C206" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="B207" t="s">
+        <v>686</v>
+      </c>
+      <c r="C207" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A208" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="C208" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A209" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="C209" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="B210" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="C210" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="B211" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="C211" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="C212" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A213" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="B213" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="C213" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A214" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="B214" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="C214" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A215" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="C215" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A216" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="B216" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="C216" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A217" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="B217" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="C217" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A218" s="5">
+        <v>217</v>
+      </c>
+      <c r="B218" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="C218" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A219" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="C219" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="B220" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="C220" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="5" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="5" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="5" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="5" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="B228" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B229" s="28" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="B230" s="7" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="B231" s="7" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="B232" t="s">
+        <v>746</v>
+      </c>
+      <c r="C232" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="B233" t="s">
+        <v>748</v>
+      </c>
+      <c r="C233" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A234" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="B235" t="s">
+        <v>751</v>
+      </c>
+      <c r="C235" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A236" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="B236" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="C236" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="B237" t="s">
+        <v>755</v>
+      </c>
+      <c r="C237" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="B238" t="s">
+        <v>757</v>
+      </c>
+      <c r="C238" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A239" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="B239" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="C239" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A240" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="B240" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="C240" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="5" t="s">
+        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -6056,13 +7189,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -6242,13 +7375,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>201</v>
       </c>
@@ -6256,7 +7389,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>203</v>
       </c>
@@ -6264,7 +7397,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>205</v>
       </c>
@@ -6272,55 +7405,55 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>208</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>211</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>212</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>215</v>
       </c>
@@ -6328,7 +7461,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>217</v>
       </c>
@@ -6336,7 +7469,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>219</v>
       </c>
@@ -6344,7 +7477,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>44</v>
       </c>
@@ -6352,7 +7485,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>222</v>
       </c>
@@ -6360,7 +7493,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>224</v>
       </c>
@@ -6368,7 +7501,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>226</v>
       </c>
@@ -6376,7 +7509,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>228</v>
       </c>
@@ -6384,7 +7517,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>230</v>
       </c>
@@ -6392,7 +7525,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>232</v>
       </c>
@@ -6400,7 +7533,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>234</v>
       </c>
@@ -6408,31 +7541,31 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>239</v>
       </c>
@@ -6440,7 +7573,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>241</v>
       </c>
@@ -6448,7 +7581,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>243</v>
       </c>
@@ -6456,7 +7589,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>245</v>
       </c>
@@ -6464,7 +7597,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>246</v>
       </c>
@@ -6472,7 +7605,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>248</v>
       </c>
@@ -6480,7 +7613,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>250</v>
       </c>
@@ -6488,7 +7621,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>252</v>
       </c>
@@ -6496,7 +7629,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>253</v>
       </c>
@@ -6504,7 +7637,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>254</v>
       </c>
@@ -6512,7 +7645,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>256</v>
       </c>
@@ -6520,7 +7653,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>258</v>
       </c>
@@ -6528,7 +7661,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>260</v>
       </c>
@@ -6536,7 +7669,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>262</v>
       </c>
@@ -6544,7 +7677,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>264</v>
       </c>
@@ -6552,7 +7685,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>266</v>
       </c>
@@ -6560,7 +7693,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>268</v>
       </c>
@@ -6568,7 +7701,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
         <v>269</v>
       </c>
@@ -6576,7 +7709,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>270</v>
       </c>
@@ -6584,7 +7717,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>272</v>
       </c>
@@ -6592,7 +7725,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>273</v>
       </c>
@@ -6600,7 +7733,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>274</v>
       </c>
@@ -6608,7 +7741,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>276</v>
       </c>
@@ -6616,7 +7749,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>277</v>
       </c>
@@ -6624,7 +7757,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>279</v>
       </c>
@@ -6658,13 +7791,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="85.36328125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>289</v>
       </c>
@@ -6672,7 +7805,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>291</v>
       </c>
@@ -6680,7 +7813,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>293</v>
       </c>
@@ -6688,7 +7821,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>295</v>
       </c>
@@ -6696,7 +7829,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>297</v>
       </c>
@@ -6704,7 +7837,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>299</v>
       </c>
@@ -6712,7 +7845,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>301</v>
       </c>
@@ -6720,7 +7853,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>303</v>
       </c>
@@ -6728,7 +7861,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>305</v>
       </c>
@@ -6736,7 +7869,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>307</v>
       </c>
@@ -6744,7 +7877,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>309</v>
       </c>
@@ -6752,7 +7885,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>311</v>
       </c>
@@ -6760,7 +7893,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>313</v>
       </c>
@@ -6768,7 +7901,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>315</v>
       </c>
@@ -6776,7 +7909,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>317</v>
       </c>
@@ -6784,7 +7917,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>319</v>
       </c>
@@ -6792,7 +7925,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
         <v>321</v>
       </c>
@@ -6800,7 +7933,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>323</v>
       </c>
@@ -6808,7 +7941,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>325</v>
       </c>
@@ -6816,7 +7949,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
         <v>327</v>
       </c>
@@ -6824,7 +7957,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>329</v>
       </c>
@@ -6832,7 +7965,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>331</v>
       </c>
@@ -6840,7 +7973,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
         <v>333</v>
       </c>
@@ -6848,7 +7981,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>335</v>
       </c>
@@ -6856,7 +7989,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
         <v>337</v>
       </c>
@@ -6864,7 +7997,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
         <v>339</v>
       </c>
@@ -6872,7 +8005,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
         <v>341</v>
       </c>
@@ -6880,7 +8013,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
         <v>343</v>
       </c>
@@ -6888,7 +8021,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
         <v>345</v>
       </c>
@@ -6896,7 +8029,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>347</v>
       </c>
@@ -6904,7 +8037,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>349</v>
       </c>
@@ -6912,7 +8045,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>351</v>
       </c>
@@ -6920,7 +8053,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>353</v>
       </c>
@@ -6928,7 +8061,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>355</v>
       </c>
@@ -6936,7 +8069,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
         <v>357</v>
       </c>

</xml_diff>

<commit_message>
Athyusha Changes pushed by Rahul
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1100" yWindow="2450" windowWidth="19420" windowHeight="5810" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="24180" windowHeight="5760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <definedName name="URL">[1]Sheet2!$E:$E</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -3815,6 +3816,17 @@
     <t>Get PROV_TIN_NBR for EPRAGENERATED BS</t>
   </si>
   <si>
+    <t>Select TEXT_VAL from OLE.CONTENT  WHERE  CONT_NM='FinancialInfoTIN' order by CREAT_DTTM desc</t>
+  </si>
+  <si>
+    <t>Finantial Institution Info Page</t>
+  </si>
+  <si>
+    <t>select * from ole.user_evnt_log
+where (EVNT_MSG like '%DataAccess:SUCCESS%' and
+EVNT_MSG like '%EPRA%') and CREAT_BY_ID='{$id}' order by CREAT_DTTM desc fetch first row only</t>
+  </si>
+  <si>
     <t>SELECT * FROM
 (
 -- For ranking the records
@@ -3833,13 +3845,14 @@
 AND SC.UCP_UCONSL_PAY_KEY_ID = SCL.CUP_UCONSL_PAY_KEY_ID-- Join SC with SCL
 AND SC.PAYR_SCHM_NM=SCL.PAYR_SCHM_NM-- Join SC with SCL- Payer
 AND SC.PAYR_SCHM_NM = 'PP018'-- &lt;&lt;Change Payer Schema Name here&gt;&gt;
-AND SC.CP_SETL_DT BETWEEN '2019-03-01' AND '2019-05-15' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
+AND SC.CP_SETL_DT BETWEEN '2020-03-01' AND '2020-04-09' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
 AND PU.STS_CD='A'
 AND PU.USER_TYP='P'
 AND EP.PRIORITY = '{$priority}'
 and SCL.CLM_PTNT_ACCT_NBR != '0'
+AND SC.PROV_NPI_NBR != ''
 AND SC.UCP_CONSL_PAY_NBR NOT IN 
-(SELECT DISTINCT EP.CONSL_PAY_NBR FROM OLE.EPRA_STATUS EP WHERE EP.CONSL_PAY_NBR=SC.UCP_CONSL_PAY_NBR)-- Payment ID shouldn't exist in EPRA_STATUS
+(SELECT DISTINCT EP.CONSL_PAY_NBR FROM OLE.EPRA_STATUS EP)-- Payment ID shouldn't exist in EPRA_STATUS
 GROUP BY PU.PORTAL_USER_ID, PU.USERNAME, PU.SSO_ID, PUT.PROV_TIN_NBR, PU.USER_TYP, PU.STS_CD,
 SC.CP_DSPL_CONSL_PAY_NBR, SC.UCP_CONSL_PAY_NBR, TO_CHAR(SC.CP_SETL_DT,'MM/DD/YYYY'), SC.PAYR_SCHM_NM, SC.PYR_SEC_PAYR_ID,
 SC.PROV_NPI_NBR,SCL.RP_UPPER_LST_NM,SCL.SUB_SBSCR_ID , SCL.CLM_PTNT_FST_NM , SCL.CLM_PTNT_LST_NM ,
@@ -3850,17 +3863,6 @@
 )DUPLUSR
 WHERE DUPLUSR.USER_RANK=1
 fetch first row only</t>
-  </si>
-  <si>
-    <t>select * from ole.user_evnt_log
-where (EVNT_MSG like '%DataAccess:SUCCESS%' and
-EVNT_MSG like '%EPRA%')order by CREAT_DTTM desc fetch first row only</t>
-  </si>
-  <si>
-    <t>Select TEXT_VAL from OLE.CONTENT  WHERE  CONT_NM='FinancialInfoTIN' order by CREAT_DTTM desc</t>
-  </si>
-  <si>
-    <t>Finantial Institution Info Page</t>
   </si>
 </sst>
 </file>
@@ -4394,19 +4396,19 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4435,7 +4437,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4464,7 +4466,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4488,7 +4490,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4517,7 +4519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4546,7 +4548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4572,7 +4574,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4598,7 +4600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4624,7 +4626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4650,7 +4652,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4676,7 +4678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4702,7 +4704,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4728,7 +4730,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4754,7 +4756,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4780,7 +4782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4806,7 +4808,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -4842,18 +4844,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C237" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="136.54296875" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="136.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4864,7 +4866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4875,7 +4877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4886,7 +4888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4894,7 +4896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4905,7 +4907,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4913,7 +4915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4921,7 +4923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4929,7 +4931,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4937,7 +4939,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4953,7 +4955,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4961,7 +4963,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4969,7 +4971,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4977,7 +4979,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4985,7 +4987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -4993,7 +4995,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -5001,7 +5003,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -5009,7 +5011,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -5025,7 +5027,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -5041,7 +5043,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
@@ -5049,7 +5051,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -5065,7 +5067,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>92</v>
       </c>
@@ -5073,7 +5075,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
@@ -5081,7 +5083,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>94</v>
       </c>
@@ -5089,7 +5091,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>96</v>
       </c>
@@ -5108,7 +5110,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -5119,7 +5121,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
@@ -5130,7 +5132,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="187.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="187.35" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -5141,7 +5143,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>109</v>
       </c>
@@ -5149,7 +5151,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>110</v>
       </c>
@@ -5157,7 +5159,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
@@ -5168,7 +5170,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>114</v>
       </c>
@@ -5179,7 +5181,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
@@ -5187,7 +5189,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>119</v>
       </c>
@@ -5195,7 +5197,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>120</v>
       </c>
@@ -5203,7 +5205,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>123</v>
       </c>
@@ -5211,7 +5213,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>124</v>
       </c>
@@ -5225,7 +5227,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>126</v>
       </c>
@@ -5236,7 +5238,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>127</v>
       </c>
@@ -5247,7 +5249,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -5258,7 +5260,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -5269,7 +5271,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>130</v>
       </c>
@@ -5280,7 +5282,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>131</v>
       </c>
@@ -5291,7 +5293,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>132</v>
       </c>
@@ -5302,7 +5304,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>133</v>
       </c>
@@ -5313,7 +5315,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>134</v>
       </c>
@@ -5324,7 +5326,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>135</v>
       </c>
@@ -5335,7 +5337,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>136</v>
       </c>
@@ -5346,7 +5348,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>137</v>
       </c>
@@ -5354,7 +5356,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>139</v>
       </c>
@@ -5365,7 +5367,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>140</v>
       </c>
@@ -5373,7 +5375,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>146</v>
       </c>
@@ -5384,7 +5386,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>147</v>
       </c>
@@ -5403,7 +5405,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>153</v>
       </c>
@@ -5425,7 +5427,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>155</v>
       </c>
@@ -5436,7 +5438,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>156</v>
       </c>
@@ -5444,7 +5446,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>177</v>
       </c>
@@ -5455,7 +5457,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>178</v>
       </c>
@@ -5466,7 +5468,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>183</v>
       </c>
@@ -5474,7 +5476,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>184</v>
       </c>
@@ -5520,7 +5522,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>200</v>
       </c>
@@ -5528,7 +5530,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>281</v>
       </c>
@@ -5536,7 +5538,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>282</v>
       </c>
@@ -5544,7 +5546,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>285</v>
       </c>
@@ -5552,7 +5554,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>287</v>
       </c>
@@ -5560,7 +5562,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>359</v>
       </c>
@@ -5568,7 +5570,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>360</v>
       </c>
@@ -5576,7 +5578,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>361</v>
       </c>
@@ -5584,7 +5586,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>363</v>
       </c>
@@ -5592,7 +5594,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>364</v>
       </c>
@@ -5600,7 +5602,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>366</v>
       </c>
@@ -5608,7 +5610,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>368</v>
       </c>
@@ -5616,7 +5618,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>369</v>
       </c>
@@ -5624,7 +5626,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>370</v>
       </c>
@@ -5632,7 +5634,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>371</v>
       </c>
@@ -5640,7 +5642,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>373</v>
       </c>
@@ -5648,7 +5650,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>374</v>
       </c>
@@ -5656,7 +5658,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>376</v>
       </c>
@@ -5664,7 +5666,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>387</v>
       </c>
@@ -5672,7 +5674,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>388</v>
       </c>
@@ -5680,7 +5682,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>390</v>
       </c>
@@ -5688,7 +5690,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>393</v>
       </c>
@@ -5696,7 +5698,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>395</v>
       </c>
@@ -5704,7 +5706,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>397</v>
       </c>
@@ -5712,7 +5714,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>399</v>
       </c>
@@ -5720,7 +5722,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>400</v>
       </c>
@@ -5728,7 +5730,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>403</v>
       </c>
@@ -5736,7 +5738,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>408</v>
       </c>
@@ -5744,7 +5746,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>409</v>
       </c>
@@ -5752,7 +5754,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>410</v>
       </c>
@@ -5760,7 +5762,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>411</v>
       </c>
@@ -5768,7 +5770,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="187.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="187.35" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>412</v>
       </c>
@@ -5779,7 +5781,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="273.64999999999998" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>413</v>
       </c>
@@ -5790,7 +5792,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="230.5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="230.45" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>415</v>
       </c>
@@ -5801,7 +5803,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>418</v>
       </c>
@@ -5809,7 +5811,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>420</v>
       </c>
@@ -5817,7 +5819,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>425</v>
       </c>
@@ -5825,7 +5827,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>427</v>
       </c>
@@ -5833,7 +5835,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>428</v>
       </c>
@@ -5841,7 +5843,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>429</v>
       </c>
@@ -5849,7 +5851,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>452</v>
       </c>
@@ -5860,7 +5862,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>453</v>
       </c>
@@ -5871,7 +5873,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>454</v>
       </c>
@@ -5882,7 +5884,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>455</v>
       </c>
@@ -5893,7 +5895,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>456</v>
       </c>
@@ -5904,7 +5906,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>457</v>
       </c>
@@ -5915,7 +5917,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>458</v>
       </c>
@@ -5926,7 +5928,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>459</v>
       </c>
@@ -5937,7 +5939,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>460</v>
       </c>
@@ -5948,7 +5950,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>461</v>
       </c>
@@ -5959,7 +5961,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>462</v>
       </c>
@@ -5970,7 +5972,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>463</v>
       </c>
@@ -5981,7 +5983,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>464</v>
       </c>
@@ -5992,7 +5994,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>466</v>
       </c>
@@ -6000,7 +6002,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>465</v>
       </c>
@@ -6008,7 +6010,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>468</v>
       </c>
@@ -6019,7 +6021,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>469</v>
       </c>
@@ -6030,7 +6032,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>471</v>
       </c>
@@ -6038,7 +6040,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>472</v>
       </c>
@@ -6049,7 +6051,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>477</v>
       </c>
@@ -6060,7 +6062,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>478</v>
       </c>
@@ -6071,7 +6073,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>483</v>
       </c>
@@ -6082,7 +6084,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>485</v>
       </c>
@@ -6093,7 +6095,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>486</v>
       </c>
@@ -6104,7 +6106,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>490</v>
       </c>
@@ -6115,7 +6117,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>494</v>
       </c>
@@ -6126,7 +6128,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>496</v>
       </c>
@@ -6137,7 +6139,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>497</v>
       </c>
@@ -6148,7 +6150,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>503</v>
       </c>
@@ -6159,7 +6161,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>506</v>
       </c>
@@ -6170,7 +6172,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>507</v>
       </c>
@@ -6181,7 +6183,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>515</v>
       </c>
@@ -6192,7 +6194,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>518</v>
       </c>
@@ -6203,7 +6205,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>519</v>
       </c>
@@ -6214,7 +6216,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>521</v>
       </c>
@@ -6225,7 +6227,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>524</v>
       </c>
@@ -6236,7 +6238,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>529</v>
       </c>
@@ -6247,7 +6249,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>552</v>
       </c>
@@ -6258,7 +6260,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>553</v>
       </c>
@@ -6269,7 +6271,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>554</v>
       </c>
@@ -6280,7 +6282,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>555</v>
       </c>
@@ -6291,7 +6293,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>556</v>
       </c>
@@ -6302,7 +6304,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>557</v>
       </c>
@@ -6313,7 +6315,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>559</v>
       </c>
@@ -6324,7 +6326,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>561</v>
       </c>
@@ -6335,7 +6337,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>565</v>
       </c>
@@ -6346,7 +6348,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>566</v>
       </c>
@@ -6357,7 +6359,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>574</v>
       </c>
@@ -6376,7 +6378,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>579</v>
       </c>
@@ -6384,7 +6386,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>580</v>
       </c>
@@ -6392,7 +6394,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>583</v>
       </c>
@@ -6403,7 +6405,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>588</v>
       </c>
@@ -6411,7 +6413,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>589</v>
       </c>
@@ -6419,7 +6421,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>592</v>
       </c>
@@ -6430,7 +6432,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>593</v>
       </c>
@@ -6441,7 +6443,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>594</v>
       </c>
@@ -6449,7 +6451,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>595</v>
       </c>
@@ -6460,7 +6462,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>596</v>
       </c>
@@ -6468,7 +6470,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>597</v>
       </c>
@@ -6479,7 +6481,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>598</v>
       </c>
@@ -6490,7 +6492,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>599</v>
       </c>
@@ -6501,7 +6503,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>600</v>
       </c>
@@ -6512,7 +6514,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>601</v>
       </c>
@@ -6520,7 +6522,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>602</v>
       </c>
@@ -6531,7 +6533,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>603</v>
       </c>
@@ -6542,7 +6544,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>604</v>
       </c>
@@ -6553,7 +6555,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>605</v>
       </c>
@@ -6564,7 +6566,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>606</v>
       </c>
@@ -6575,7 +6577,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>607</v>
       </c>
@@ -6586,7 +6588,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>608</v>
       </c>
@@ -6597,7 +6599,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>609</v>
       </c>
@@ -6608,7 +6610,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>610</v>
       </c>
@@ -6619,7 +6621,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>611</v>
       </c>
@@ -6630,7 +6632,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>612</v>
       </c>
@@ -6641,7 +6643,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>613</v>
       </c>
@@ -6663,7 +6665,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>615</v>
       </c>
@@ -6685,7 +6687,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>696</v>
       </c>
@@ -6707,7 +6709,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>698</v>
       </c>
@@ -6718,7 +6720,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>699</v>
       </c>
@@ -6729,7 +6731,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>700</v>
       </c>
@@ -6740,7 +6742,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>701</v>
       </c>
@@ -6773,7 +6775,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>704</v>
       </c>
@@ -6858,7 +6860,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>712</v>
       </c>
@@ -6874,7 +6876,7 @@
         <v>713</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C208" t="s">
         <v>688</v>
@@ -6891,7 +6893,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>715</v>
       </c>
@@ -6907,13 +6909,13 @@
         <v>716</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="C211" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
         <v>717</v>
       </c>
@@ -6924,7 +6926,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>718</v>
       </c>
@@ -6935,7 +6937,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>719</v>
       </c>
@@ -6946,7 +6948,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>720</v>
       </c>
@@ -6957,7 +6959,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>721</v>
       </c>
@@ -6968,7 +6970,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>722</v>
       </c>
@@ -6979,7 +6981,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -6990,7 +6992,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>723</v>
       </c>
@@ -7001,7 +7003,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="203" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>724</v>
       </c>
@@ -7012,42 +7014,42 @@
         <v>790</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>732</v>
       </c>
@@ -7055,7 +7057,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
         <v>733</v>
       </c>
@@ -7063,7 +7065,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>734</v>
       </c>
@@ -7071,7 +7073,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>735</v>
       </c>
@@ -7079,7 +7081,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>736</v>
       </c>
@@ -7090,7 +7092,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>737</v>
       </c>
@@ -7101,7 +7103,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>738</v>
       </c>
@@ -7109,7 +7111,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>739</v>
       </c>
@@ -7120,7 +7122,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
         <v>740</v>
       </c>
@@ -7131,7 +7133,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>741</v>
       </c>
@@ -7142,7 +7144,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>742</v>
       </c>
@@ -7153,7 +7155,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>743</v>
       </c>
@@ -7164,7 +7166,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>744</v>
       </c>
@@ -7175,15 +7177,15 @@
         <v>762</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
         <v>745</v>
       </c>
       <c r="B241" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C241" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -7200,13 +7202,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -7386,13 +7388,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>201</v>
       </c>
@@ -7400,7 +7402,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>203</v>
       </c>
@@ -7408,7 +7410,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>205</v>
       </c>
@@ -7416,55 +7418,55 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>208</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>211</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>212</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>215</v>
       </c>
@@ -7472,7 +7474,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>217</v>
       </c>
@@ -7480,7 +7482,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>219</v>
       </c>
@@ -7488,7 +7490,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>44</v>
       </c>
@@ -7496,7 +7498,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>222</v>
       </c>
@@ -7504,7 +7506,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>224</v>
       </c>
@@ -7512,7 +7514,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>226</v>
       </c>
@@ -7520,7 +7522,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>228</v>
       </c>
@@ -7528,7 +7530,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>230</v>
       </c>
@@ -7536,7 +7538,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>232</v>
       </c>
@@ -7544,7 +7546,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>234</v>
       </c>
@@ -7552,31 +7554,31 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>239</v>
       </c>
@@ -7584,7 +7586,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>241</v>
       </c>
@@ -7592,7 +7594,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>243</v>
       </c>
@@ -7600,7 +7602,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>245</v>
       </c>
@@ -7608,7 +7610,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>246</v>
       </c>
@@ -7616,7 +7618,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>248</v>
       </c>
@@ -7624,7 +7626,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>250</v>
       </c>
@@ -7632,7 +7634,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>252</v>
       </c>
@@ -7640,7 +7642,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>253</v>
       </c>
@@ -7648,7 +7650,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>254</v>
       </c>
@@ -7656,7 +7658,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>256</v>
       </c>
@@ -7664,7 +7666,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>258</v>
       </c>
@@ -7672,7 +7674,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>260</v>
       </c>
@@ -7680,7 +7682,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>262</v>
       </c>
@@ -7688,7 +7690,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>264</v>
       </c>
@@ -7696,7 +7698,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>266</v>
       </c>
@@ -7704,7 +7706,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>268</v>
       </c>
@@ -7712,7 +7714,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>269</v>
       </c>
@@ -7720,7 +7722,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>270</v>
       </c>
@@ -7728,7 +7730,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>272</v>
       </c>
@@ -7736,7 +7738,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>273</v>
       </c>
@@ -7744,7 +7746,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>274</v>
       </c>
@@ -7752,7 +7754,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>276</v>
       </c>
@@ -7760,7 +7762,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>277</v>
       </c>
@@ -7768,7 +7770,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>279</v>
       </c>
@@ -7802,13 +7804,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="85.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>289</v>
       </c>
@@ -7816,7 +7818,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>291</v>
       </c>
@@ -7824,7 +7826,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>293</v>
       </c>
@@ -7832,7 +7834,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>295</v>
       </c>
@@ -7840,7 +7842,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>297</v>
       </c>
@@ -7848,7 +7850,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>299</v>
       </c>
@@ -7856,7 +7858,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>301</v>
       </c>
@@ -7864,7 +7866,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>303</v>
       </c>
@@ -7872,7 +7874,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>305</v>
       </c>
@@ -7880,7 +7882,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>307</v>
       </c>
@@ -7888,7 +7890,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>309</v>
       </c>
@@ -7896,7 +7898,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>311</v>
       </c>
@@ -7904,7 +7906,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>313</v>
       </c>
@@ -7912,7 +7914,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>315</v>
       </c>
@@ -7920,7 +7922,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>317</v>
       </c>
@@ -7928,7 +7930,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>319</v>
       </c>
@@ -7936,7 +7938,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>321</v>
       </c>
@@ -7944,7 +7946,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>323</v>
       </c>
@@ -7952,7 +7954,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>325</v>
       </c>
@@ -7960,7 +7962,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>327</v>
       </c>
@@ -7968,7 +7970,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>329</v>
       </c>
@@ -7976,7 +7978,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
         <v>331</v>
       </c>
@@ -7984,7 +7986,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>333</v>
       </c>
@@ -7992,7 +7994,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>335</v>
       </c>
@@ -8000,7 +8002,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>337</v>
       </c>
@@ -8008,7 +8010,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>339</v>
       </c>
@@ -8016,7 +8018,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>341</v>
       </c>
@@ -8024,7 +8026,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>343</v>
       </c>
@@ -8032,7 +8034,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
         <v>345</v>
       </c>
@@ -8040,7 +8042,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25" t="s">
         <v>347</v>
       </c>
@@ -8048,7 +8050,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
         <v>349</v>
       </c>
@@ -8056,7 +8058,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>351</v>
       </c>
@@ -8064,7 +8066,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>353</v>
       </c>
@@ -8072,7 +8074,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
         <v>355</v>
       </c>
@@ -8080,7 +8082,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
         <v>357</v>
       </c>

</xml_diff>

<commit_message>
Claim Detail Adding few loops
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2450" windowWidth="19420" windowHeight="5760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22260" windowHeight="5745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="805">
   <si>
     <t>City</t>
   </si>
@@ -3876,6 +3876,53 @@
   </si>
   <si>
     <t>delete from ole.BILLING_SERVICE_PROVIDER where PROV_TIN_NBR='{$tin}' and CREAT_BY_ID='Automation'</t>
+  </si>
+  <si>
+    <t>select prov_tin_nbr AS PROV_TAX_ID_NBR from ole.portal_user_tin
+where portal_user_id in (select portal_user_id from ole.portal_user where sso_id = '{$id}')
+and prov_tin_nbr in (select prov_tax_id_nbr from pp001.provider where prov_key_id in (select PROV_KEY_ID from pp001.consolidated_payment
+where proc_ctl_id in (select proc_ctl_id from ole.proc_ctl where EXTRACT_STS_CD in ('X','C') and OVALL_PROC_STS_CD in ('C','X') and SRCH_TBL_STS_CD = 'C' order by proc_ctl_id desc)))
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>Get TIN for Remit and Claim Detail</t>
+  </si>
+  <si>
+    <t>SELECT SC.CP_DSPL_CONSL_PAY_NBR, PA.CONSL_PAY_NBR
+FROM OLE.SRCH_CONSOL_TBL SC
+LEFT JOIN PP001.PROVIDER_PAYOR_ADJUSTMENT PA ON SC.UCP_CONSL_PAY_NBR = PA.CONSL_PAY_NBR
+WHERE PROV_TAX_ID_NBR = '{$tin}'
+GROUP BY PA.CONSL_PAY_NBR, SC.CP_DSPL_CONSL_PAY_NBR
+HAVING COUNT(*) = 4
+ORDER BY PA.CONSL_PAY_NBR ASC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT SC.CP_DSPL_CONSL_PAY_NBR, PA.CONSL_PAY_NBR
+FROM OLE.SRCH_CONSOL_TBL SC
+LEFT JOIN PP001.PROVIDER_PAYOR_ADJUSTMENT PA ON SC.UCP_CONSL_PAY_NBR = PA.CONSL_PAY_NBR
+WHERE PROV_TAX_ID_NBR = '{$tin}'
+GROUP BY PA.CONSL_PAY_NBR, SC.CP_DSPL_CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY PA.CONSL_PAY_NBR ASC LIMIT 1</t>
+  </si>
+  <si>
+    <t>GET DSPL_CONSL_PAY_NBR for Remit and Claim Detail for Multiple PLB</t>
+  </si>
+  <si>
+    <t>GET DSPL_CONSL_PAY_NBR for Remit and Claim Detail for PLB</t>
+  </si>
+  <si>
+    <t>Select  PROV_ADJ_RSN_CD,PROV_ADJ_ID,PROV_PAYR_ADJ_AMT from PP001.PROVIDER_PAYOR_ADJUSTMENT where CONSL_PAY_NBR IN
+(SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+WHERE CONSL_PAY_NBR = '{$consl_pay_nbr}'
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 4
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Get Data for Multiple PLB for Remit Detail</t>
   </si>
 </sst>
 </file>
@@ -4409,19 +4456,19 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4450,7 +4497,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4479,7 +4526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4503,7 +4550,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4532,7 +4579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4561,7 +4608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4587,7 +4634,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4613,7 +4660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4639,7 +4686,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4665,7 +4712,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4691,7 +4738,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4717,7 +4764,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4743,7 +4790,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4769,7 +4816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4795,7 +4842,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4821,7 +4868,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -4855,20 +4902,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D241"/>
+  <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B222" sqref="B222"/>
+    <sheetView tabSelected="1" topLeftCell="A233" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D239" sqref="D239"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="136.54296875" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="136.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4879,7 +4926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4890,7 +4937,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4901,7 +4948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4909,7 +4956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4920,7 +4967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4928,7 +4975,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4936,7 +4983,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4944,7 +4991,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4952,7 +4999,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4968,7 +5015,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4976,7 +5023,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4984,7 +5031,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4992,7 +5039,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5000,7 +5047,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5008,7 +5055,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -5016,7 +5063,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -5024,7 +5071,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -5040,7 +5087,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -5056,7 +5103,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
@@ -5064,7 +5111,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -5080,7 +5127,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>92</v>
       </c>
@@ -5088,7 +5135,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
@@ -5096,7 +5143,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>94</v>
       </c>
@@ -5104,7 +5151,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>96</v>
       </c>
@@ -5123,7 +5170,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -5134,7 +5181,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
@@ -5145,7 +5192,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="187.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="187.35" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -5156,7 +5203,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>109</v>
       </c>
@@ -5164,7 +5211,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>110</v>
       </c>
@@ -5172,7 +5219,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
@@ -5183,7 +5230,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>114</v>
       </c>
@@ -5194,7 +5241,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
@@ -5202,7 +5249,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>119</v>
       </c>
@@ -5210,7 +5257,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>120</v>
       </c>
@@ -5218,7 +5265,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>123</v>
       </c>
@@ -5226,7 +5273,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>124</v>
       </c>
@@ -5240,7 +5287,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>126</v>
       </c>
@@ -5251,7 +5298,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>127</v>
       </c>
@@ -5262,7 +5309,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -5273,7 +5320,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -5284,7 +5331,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>130</v>
       </c>
@@ -5295,7 +5342,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>131</v>
       </c>
@@ -5306,7 +5353,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>132</v>
       </c>
@@ -5317,7 +5364,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>133</v>
       </c>
@@ -5328,7 +5375,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>134</v>
       </c>
@@ -5339,7 +5386,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>135</v>
       </c>
@@ -5350,7 +5397,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>136</v>
       </c>
@@ -5361,7 +5408,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>137</v>
       </c>
@@ -5369,7 +5416,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>139</v>
       </c>
@@ -5380,7 +5427,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>140</v>
       </c>
@@ -5388,7 +5435,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>146</v>
       </c>
@@ -5399,7 +5446,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>147</v>
       </c>
@@ -5418,7 +5465,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>153</v>
       </c>
@@ -5440,7 +5487,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>155</v>
       </c>
@@ -5451,7 +5498,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>156</v>
       </c>
@@ -5459,7 +5506,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>177</v>
       </c>
@@ -5470,7 +5517,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>178</v>
       </c>
@@ -5481,7 +5528,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>183</v>
       </c>
@@ -5489,7 +5536,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>184</v>
       </c>
@@ -5535,7 +5582,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>200</v>
       </c>
@@ -5543,7 +5590,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>281</v>
       </c>
@@ -5551,7 +5598,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>282</v>
       </c>
@@ -5559,7 +5606,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>285</v>
       </c>
@@ -5567,7 +5614,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>287</v>
       </c>
@@ -5575,7 +5622,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>359</v>
       </c>
@@ -5583,7 +5630,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>360</v>
       </c>
@@ -5591,7 +5638,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>361</v>
       </c>
@@ -5599,7 +5646,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>363</v>
       </c>
@@ -5607,7 +5654,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>364</v>
       </c>
@@ -5615,7 +5662,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>366</v>
       </c>
@@ -5623,7 +5670,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>368</v>
       </c>
@@ -5631,7 +5678,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>369</v>
       </c>
@@ -5639,7 +5686,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>370</v>
       </c>
@@ -5647,7 +5694,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>371</v>
       </c>
@@ -5655,7 +5702,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>373</v>
       </c>
@@ -5663,7 +5710,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>374</v>
       </c>
@@ -5671,7 +5718,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>376</v>
       </c>
@@ -5679,7 +5726,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>387</v>
       </c>
@@ -5687,7 +5734,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>388</v>
       </c>
@@ -5695,7 +5742,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>390</v>
       </c>
@@ -5703,7 +5750,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>393</v>
       </c>
@@ -5711,7 +5758,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>395</v>
       </c>
@@ -5719,7 +5766,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>397</v>
       </c>
@@ -5727,7 +5774,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>399</v>
       </c>
@@ -5735,7 +5782,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>400</v>
       </c>
@@ -5743,7 +5790,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>403</v>
       </c>
@@ -5751,7 +5798,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>408</v>
       </c>
@@ -5759,7 +5806,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>409</v>
       </c>
@@ -5767,7 +5814,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>410</v>
       </c>
@@ -5775,7 +5822,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>411</v>
       </c>
@@ -5783,7 +5830,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="187.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="187.35" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>412</v>
       </c>
@@ -5794,7 +5841,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="273.64999999999998" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>413</v>
       </c>
@@ -5805,7 +5852,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="230.5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="230.45" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>415</v>
       </c>
@@ -5816,7 +5863,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>418</v>
       </c>
@@ -5824,7 +5871,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>420</v>
       </c>
@@ -5832,7 +5879,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>425</v>
       </c>
@@ -5840,7 +5887,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>427</v>
       </c>
@@ -5848,7 +5895,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>428</v>
       </c>
@@ -5856,7 +5903,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>429</v>
       </c>
@@ -5864,7 +5911,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>452</v>
       </c>
@@ -5875,7 +5922,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>453</v>
       </c>
@@ -5886,7 +5933,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>454</v>
       </c>
@@ -5897,7 +5944,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>455</v>
       </c>
@@ -5908,7 +5955,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>456</v>
       </c>
@@ -5919,7 +5966,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>457</v>
       </c>
@@ -5930,7 +5977,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>458</v>
       </c>
@@ -5941,7 +5988,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>459</v>
       </c>
@@ -5952,7 +5999,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>460</v>
       </c>
@@ -5963,7 +6010,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>461</v>
       </c>
@@ -5974,7 +6021,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>462</v>
       </c>
@@ -5985,7 +6032,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>463</v>
       </c>
@@ -5996,7 +6043,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>464</v>
       </c>
@@ -6007,7 +6054,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>466</v>
       </c>
@@ -6015,7 +6062,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>465</v>
       </c>
@@ -6023,7 +6070,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>468</v>
       </c>
@@ -6034,7 +6081,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>469</v>
       </c>
@@ -6045,7 +6092,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>471</v>
       </c>
@@ -6053,7 +6100,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>472</v>
       </c>
@@ -6064,7 +6111,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>477</v>
       </c>
@@ -6075,7 +6122,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>478</v>
       </c>
@@ -6086,7 +6133,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>483</v>
       </c>
@@ -6097,7 +6144,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>485</v>
       </c>
@@ -6108,7 +6155,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>486</v>
       </c>
@@ -6119,7 +6166,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>490</v>
       </c>
@@ -6130,7 +6177,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>494</v>
       </c>
@@ -6141,7 +6188,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>496</v>
       </c>
@@ -6152,7 +6199,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>497</v>
       </c>
@@ -6163,7 +6210,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>503</v>
       </c>
@@ -6174,7 +6221,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>506</v>
       </c>
@@ -6185,7 +6232,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>507</v>
       </c>
@@ -6196,7 +6243,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>515</v>
       </c>
@@ -6207,7 +6254,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>518</v>
       </c>
@@ -6218,7 +6265,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>519</v>
       </c>
@@ -6229,7 +6276,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>521</v>
       </c>
@@ -6240,7 +6287,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>524</v>
       </c>
@@ -6251,7 +6298,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>529</v>
       </c>
@@ -6262,7 +6309,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>552</v>
       </c>
@@ -6273,7 +6320,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>553</v>
       </c>
@@ -6284,7 +6331,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>554</v>
       </c>
@@ -6295,7 +6342,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>555</v>
       </c>
@@ -6306,7 +6353,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>556</v>
       </c>
@@ -6317,7 +6364,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>557</v>
       </c>
@@ -6328,7 +6375,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>559</v>
       </c>
@@ -6339,7 +6386,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>561</v>
       </c>
@@ -6350,7 +6397,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>565</v>
       </c>
@@ -6361,7 +6408,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>566</v>
       </c>
@@ -6372,7 +6419,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>574</v>
       </c>
@@ -6391,7 +6438,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>579</v>
       </c>
@@ -6399,7 +6446,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>580</v>
       </c>
@@ -6407,7 +6454,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>583</v>
       </c>
@@ -6418,7 +6465,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>588</v>
       </c>
@@ -6426,7 +6473,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>589</v>
       </c>
@@ -6434,7 +6481,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>592</v>
       </c>
@@ -6445,7 +6492,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>593</v>
       </c>
@@ -6456,7 +6503,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>594</v>
       </c>
@@ -6464,7 +6511,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>595</v>
       </c>
@@ -6475,7 +6522,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>596</v>
       </c>
@@ -6483,7 +6530,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>597</v>
       </c>
@@ -6494,7 +6541,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>598</v>
       </c>
@@ -6505,7 +6552,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>599</v>
       </c>
@@ -6516,7 +6563,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>600</v>
       </c>
@@ -6527,7 +6574,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>601</v>
       </c>
@@ -6535,7 +6582,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>602</v>
       </c>
@@ -6546,7 +6593,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>603</v>
       </c>
@@ -6557,7 +6604,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>604</v>
       </c>
@@ -6568,7 +6615,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>605</v>
       </c>
@@ -6579,7 +6626,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>606</v>
       </c>
@@ -6590,7 +6637,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>607</v>
       </c>
@@ -6601,7 +6648,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>608</v>
       </c>
@@ -6612,7 +6659,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>609</v>
       </c>
@@ -6623,7 +6670,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>610</v>
       </c>
@@ -6634,7 +6681,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>611</v>
       </c>
@@ -6645,7 +6692,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>612</v>
       </c>
@@ -6656,7 +6703,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>613</v>
       </c>
@@ -6678,7 +6725,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>615</v>
       </c>
@@ -6700,7 +6747,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>696</v>
       </c>
@@ -6722,7 +6769,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>698</v>
       </c>
@@ -6733,7 +6780,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>699</v>
       </c>
@@ -6744,7 +6791,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>700</v>
       </c>
@@ -6755,7 +6802,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>701</v>
       </c>
@@ -6788,7 +6835,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>704</v>
       </c>
@@ -6821,7 +6868,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" ht="72.599999999999994" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>707</v>
       </c>
@@ -6843,7 +6890,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
         <v>709</v>
       </c>
@@ -6873,7 +6920,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A207" s="5" t="s">
         <v>712</v>
       </c>
@@ -6895,7 +6942,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" ht="101.45" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
         <v>714</v>
       </c>
@@ -6906,7 +6953,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A210" s="5" t="s">
         <v>715</v>
       </c>
@@ -6939,7 +6986,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A213" s="5" t="s">
         <v>718</v>
       </c>
@@ -6950,7 +6997,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" ht="72.599999999999994" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
         <v>719</v>
       </c>
@@ -6972,7 +7019,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" ht="72.599999999999994" x14ac:dyDescent="0.35">
       <c r="A216" s="5" t="s">
         <v>721</v>
       </c>
@@ -7016,7 +7063,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="203" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" ht="203.1" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>724</v>
       </c>
@@ -7035,7 +7082,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>726</v>
       </c>
@@ -7043,32 +7090,50 @@
         <v>796</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B223" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="C223" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B224" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="C224" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B225" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="C225" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>732</v>
       </c>
@@ -7076,7 +7141,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
         <v>733</v>
       </c>
@@ -7084,7 +7149,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>734</v>
       </c>
@@ -7092,7 +7157,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>735</v>
       </c>
@@ -7100,7 +7165,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>736</v>
       </c>
@@ -7111,7 +7176,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>737</v>
       </c>
@@ -7122,7 +7187,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>738</v>
       </c>
@@ -7130,7 +7195,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>739</v>
       </c>
@@ -7141,7 +7206,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
         <v>740</v>
       </c>
@@ -7152,7 +7217,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>741</v>
       </c>
@@ -7163,7 +7228,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>742</v>
       </c>
@@ -7174,7 +7239,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>743</v>
       </c>
@@ -7185,7 +7250,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>744</v>
       </c>
@@ -7196,7 +7261,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
         <v>745</v>
       </c>
@@ -7205,6 +7270,17 @@
       </c>
       <c r="C241" t="s">
         <v>792</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="C242" t="s">
+        <v>804</v>
       </c>
     </row>
   </sheetData>
@@ -7221,13 +7297,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -7407,13 +7483,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>201</v>
       </c>
@@ -7421,7 +7497,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>203</v>
       </c>
@@ -7429,7 +7505,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>205</v>
       </c>
@@ -7437,55 +7513,55 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>208</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>211</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>212</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>215</v>
       </c>
@@ -7493,7 +7569,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>217</v>
       </c>
@@ -7501,7 +7577,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>219</v>
       </c>
@@ -7509,7 +7585,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>44</v>
       </c>
@@ -7517,7 +7593,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>222</v>
       </c>
@@ -7525,7 +7601,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>224</v>
       </c>
@@ -7533,7 +7609,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>226</v>
       </c>
@@ -7541,7 +7617,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>228</v>
       </c>
@@ -7549,7 +7625,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>230</v>
       </c>
@@ -7557,7 +7633,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>232</v>
       </c>
@@ -7565,7 +7641,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>234</v>
       </c>
@@ -7573,31 +7649,31 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>239</v>
       </c>
@@ -7605,7 +7681,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>241</v>
       </c>
@@ -7613,7 +7689,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>243</v>
       </c>
@@ -7621,7 +7697,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>245</v>
       </c>
@@ -7629,7 +7705,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>246</v>
       </c>
@@ -7637,7 +7713,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>248</v>
       </c>
@@ -7645,7 +7721,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>250</v>
       </c>
@@ -7653,7 +7729,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>252</v>
       </c>
@@ -7661,7 +7737,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>253</v>
       </c>
@@ -7669,7 +7745,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>254</v>
       </c>
@@ -7677,7 +7753,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
         <v>256</v>
       </c>
@@ -7685,7 +7761,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>258</v>
       </c>
@@ -7693,7 +7769,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>260</v>
       </c>
@@ -7701,7 +7777,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
         <v>262</v>
       </c>
@@ -7709,7 +7785,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
         <v>264</v>
       </c>
@@ -7717,7 +7793,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>266</v>
       </c>
@@ -7725,7 +7801,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>268</v>
       </c>
@@ -7733,7 +7809,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>269</v>
       </c>
@@ -7741,7 +7817,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>270</v>
       </c>
@@ -7749,7 +7825,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>272</v>
       </c>
@@ -7757,7 +7833,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>273</v>
       </c>
@@ -7765,7 +7841,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>274</v>
       </c>
@@ -7773,7 +7849,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>276</v>
       </c>
@@ -7781,7 +7857,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>277</v>
       </c>
@@ -7789,7 +7865,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>279</v>
       </c>
@@ -7823,13 +7899,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="85.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>289</v>
       </c>
@@ -7837,7 +7913,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>291</v>
       </c>
@@ -7845,7 +7921,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>293</v>
       </c>
@@ -7853,7 +7929,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>295</v>
       </c>
@@ -7861,7 +7937,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>297</v>
       </c>
@@ -7869,7 +7945,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>299</v>
       </c>
@@ -7877,7 +7953,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>301</v>
       </c>
@@ -7885,7 +7961,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>303</v>
       </c>
@@ -7893,7 +7969,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>305</v>
       </c>
@@ -7901,7 +7977,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>307</v>
       </c>
@@ -7909,7 +7985,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>309</v>
       </c>
@@ -7917,7 +7993,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>311</v>
       </c>
@@ -7925,7 +8001,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>313</v>
       </c>
@@ -7933,7 +8009,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
         <v>315</v>
       </c>
@@ -7941,7 +8017,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="25" t="s">
         <v>317</v>
       </c>
@@ -7949,7 +8025,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="25" t="s">
         <v>319</v>
       </c>
@@ -7957,7 +8033,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="25" t="s">
         <v>321</v>
       </c>
@@ -7965,7 +8041,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="25" t="s">
         <v>323</v>
       </c>
@@ -7973,7 +8049,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="25" t="s">
         <v>325</v>
       </c>
@@ -7981,7 +8057,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="25" t="s">
         <v>327</v>
       </c>
@@ -7989,7 +8065,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="25" t="s">
         <v>329</v>
       </c>
@@ -7997,7 +8073,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="25" t="s">
         <v>331</v>
       </c>
@@ -8005,7 +8081,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="25" t="s">
         <v>333</v>
       </c>
@@ -8013,7 +8089,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="25" t="s">
         <v>335</v>
       </c>
@@ -8021,7 +8097,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="25" t="s">
         <v>337</v>
       </c>
@@ -8029,7 +8105,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="25" t="s">
         <v>339</v>
       </c>
@@ -8037,7 +8113,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="25" t="s">
         <v>341</v>
       </c>
@@ -8045,7 +8121,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="25" t="s">
         <v>343</v>
       </c>
@@ -8053,7 +8129,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="25" t="s">
         <v>345</v>
       </c>
@@ -8061,7 +8137,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="25" t="s">
         <v>347</v>
       </c>
@@ -8069,7 +8145,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="25" t="s">
         <v>349</v>
       </c>
@@ -8077,7 +8153,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="25" t="s">
         <v>351</v>
       </c>
@@ -8085,7 +8161,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="25" t="s">
         <v>353</v>
       </c>
@@ -8093,7 +8169,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="25" t="s">
         <v>355</v>
       </c>
@@ -8101,7 +8177,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="25" t="s">
         <v>357</v>
       </c>

</xml_diff>

<commit_message>
EPRA ViewPayments module updated
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22260" windowHeight="5745" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2450" windowWidth="19420" windowHeight="5750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -3864,17 +3864,6 @@
 fetch first row only</t>
   </si>
   <si>
-    <t>Select p.prov_tax_id_nbr, cp.DSPL_CONSL_PAY_NBR, cp.SETL_DT, cp.CONSL_PAY_NBR
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
-and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
-AND cp.setl_dt BETWEEN '{$fromDate}' AND '{$toDate}' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
- and cp.CONSL_PAY_NBR not in (select CONSL_PAY_NBR from ole.EPRA_STATUS)
-group by p.prov_tax_id_nbr, cp.DSPL_CONSL_PAY_NBR, cp.SETL_DT, cp.CONSL_PAY_NBR
-having count(*) between 1 and 30
-order by count(*) desc
-fetch first row only</t>
-  </si>
-  <si>
     <t>delete from ole.BILLING_SERVICE_PROVIDER where PROV_TIN_NBR='{$tin}' and CREAT_BY_ID='Automation'</t>
   </si>
   <si>
@@ -3923,6 +3912,19 @@
   </si>
   <si>
     <t>Get Data for Multiple PLB for Remit Detail</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr, cp.DSPL_CONSL_PAY_NBR, cp.SETL_DT, cp.CONSL_PAY_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC, ole.ENROLLED_PROVIDER ep WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and ep.PROV_TIN_NBR = p.PROV_TAX_ID_NBR
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+AND cp.setl_dt BETWEEN '2020-04-01' AND '2020-04-20' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
+and cp.CONSL_PAY_NBR not in (select CONSL_PAY_NBR from ole.EPRA_STATUS)
+and ep.ENRL_STS_CD = 'A'
+group by p.prov_tax_id_nbr, cp.DSPL_CONSL_PAY_NBR, cp.SETL_DT, cp.CONSL_PAY_NBR
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
   </si>
 </sst>
 </file>
@@ -4456,19 +4458,19 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4497,7 +4499,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4526,7 +4528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4550,7 +4552,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4579,7 +4581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4608,7 +4610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4634,7 +4636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4660,7 +4662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4686,7 +4688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4712,7 +4714,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4738,7 +4740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4764,7 +4766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4790,7 +4792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4816,7 +4818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4842,7 +4844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4868,7 +4870,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -4904,18 +4906,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D239" sqref="D239"/>
+    <sheetView tabSelected="1" topLeftCell="A221" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B221" sqref="B221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="136.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="136.54296875" customWidth="1"/>
+    <col min="3" max="3" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4926,7 +4928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4937,7 +4939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4948,7 +4950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4956,7 +4958,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4967,7 +4969,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4975,7 +4977,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4983,7 +4985,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4991,7 +4993,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4999,7 +5001,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5015,7 +5017,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -5023,7 +5025,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5031,7 +5033,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5039,7 +5041,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5047,7 +5049,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5055,7 +5057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -5063,7 +5065,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -5071,7 +5073,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -5087,7 +5089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -5103,7 +5105,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
@@ -5111,7 +5113,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -5127,7 +5129,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>92</v>
       </c>
@@ -5135,7 +5137,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
@@ -5143,7 +5145,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>94</v>
       </c>
@@ -5151,7 +5153,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>96</v>
       </c>
@@ -5170,7 +5172,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -5181,7 +5183,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
@@ -5192,7 +5194,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="187.35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="187.4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -5203,7 +5205,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>109</v>
       </c>
@@ -5211,7 +5213,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="43.4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>110</v>
       </c>
@@ -5219,7 +5221,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
@@ -5230,7 +5232,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>114</v>
       </c>
@@ -5241,7 +5243,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
@@ -5249,7 +5251,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>119</v>
       </c>
@@ -5257,7 +5259,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>120</v>
       </c>
@@ -5265,7 +5267,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>123</v>
       </c>
@@ -5273,7 +5275,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>124</v>
       </c>
@@ -5287,7 +5289,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>126</v>
       </c>
@@ -5298,7 +5300,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>127</v>
       </c>
@@ -5309,7 +5311,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -5320,7 +5322,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -5331,7 +5333,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="172.7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>130</v>
       </c>
@@ -5342,7 +5344,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>131</v>
       </c>
@@ -5353,7 +5355,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>132</v>
       </c>
@@ -5364,7 +5366,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>133</v>
       </c>
@@ -5375,7 +5377,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>134</v>
       </c>
@@ -5386,7 +5388,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>135</v>
       </c>
@@ -5397,7 +5399,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>136</v>
       </c>
@@ -5408,7 +5410,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>137</v>
       </c>
@@ -5416,7 +5418,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>139</v>
       </c>
@@ -5427,7 +5429,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>140</v>
       </c>
@@ -5435,7 +5437,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>146</v>
       </c>
@@ -5446,7 +5448,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>147</v>
       </c>
@@ -5465,7 +5467,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>153</v>
       </c>
@@ -5487,7 +5489,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>155</v>
       </c>
@@ -5498,7 +5500,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>156</v>
       </c>
@@ -5506,7 +5508,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>177</v>
       </c>
@@ -5517,7 +5519,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>178</v>
       </c>
@@ -5528,7 +5530,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>183</v>
       </c>
@@ -5536,7 +5538,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>184</v>
       </c>
@@ -5582,7 +5584,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>200</v>
       </c>
@@ -5590,7 +5592,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>281</v>
       </c>
@@ -5598,7 +5600,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>282</v>
       </c>
@@ -5606,7 +5608,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>285</v>
       </c>
@@ -5614,7 +5616,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>287</v>
       </c>
@@ -5622,7 +5624,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>359</v>
       </c>
@@ -5630,7 +5632,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>360</v>
       </c>
@@ -5638,7 +5640,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>361</v>
       </c>
@@ -5646,7 +5648,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>363</v>
       </c>
@@ -5654,7 +5656,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>364</v>
       </c>
@@ -5662,7 +5664,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>366</v>
       </c>
@@ -5670,7 +5672,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>368</v>
       </c>
@@ -5678,7 +5680,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>369</v>
       </c>
@@ -5686,7 +5688,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>370</v>
       </c>
@@ -5694,7 +5696,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>371</v>
       </c>
@@ -5702,7 +5704,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>373</v>
       </c>
@@ -5710,7 +5712,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>374</v>
       </c>
@@ -5718,7 +5720,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>376</v>
       </c>
@@ -5726,7 +5728,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>387</v>
       </c>
@@ -5734,7 +5736,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>388</v>
       </c>
@@ -5742,7 +5744,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>390</v>
       </c>
@@ -5750,7 +5752,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>393</v>
       </c>
@@ -5758,7 +5760,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>395</v>
       </c>
@@ -5766,7 +5768,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>397</v>
       </c>
@@ -5774,7 +5776,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>399</v>
       </c>
@@ -5782,7 +5784,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>400</v>
       </c>
@@ -5790,7 +5792,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>403</v>
       </c>
@@ -5798,7 +5800,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>408</v>
       </c>
@@ -5806,7 +5808,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>409</v>
       </c>
@@ -5814,7 +5816,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>410</v>
       </c>
@@ -5822,7 +5824,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>411</v>
       </c>
@@ -5830,7 +5832,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="187.35" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="187.4" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>412</v>
       </c>
@@ -5841,7 +5843,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="273.64999999999998" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>413</v>
       </c>
@@ -5852,7 +5854,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="230.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="230.5" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>415</v>
       </c>
@@ -5863,7 +5865,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>418</v>
       </c>
@@ -5871,7 +5873,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>420</v>
       </c>
@@ -5879,7 +5881,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>425</v>
       </c>
@@ -5887,7 +5889,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>427</v>
       </c>
@@ -5895,7 +5897,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>428</v>
       </c>
@@ -5903,7 +5905,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>429</v>
       </c>
@@ -5911,7 +5913,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>452</v>
       </c>
@@ -5922,7 +5924,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>453</v>
       </c>
@@ -5933,7 +5935,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>454</v>
       </c>
@@ -5944,7 +5946,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>455</v>
       </c>
@@ -5955,7 +5957,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>456</v>
       </c>
@@ -5966,7 +5968,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>457</v>
       </c>
@@ -5977,7 +5979,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>458</v>
       </c>
@@ -5988,7 +5990,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>459</v>
       </c>
@@ -5999,7 +6001,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>460</v>
       </c>
@@ -6010,7 +6012,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>461</v>
       </c>
@@ -6021,7 +6023,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>462</v>
       </c>
@@ -6032,7 +6034,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>463</v>
       </c>
@@ -6043,7 +6045,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>464</v>
       </c>
@@ -6054,7 +6056,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>466</v>
       </c>
@@ -6062,7 +6064,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>465</v>
       </c>
@@ -6070,7 +6072,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>468</v>
       </c>
@@ -6081,7 +6083,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>469</v>
       </c>
@@ -6092,7 +6094,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>471</v>
       </c>
@@ -6100,7 +6102,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>472</v>
       </c>
@@ -6111,7 +6113,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>477</v>
       </c>
@@ -6122,7 +6124,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>478</v>
       </c>
@@ -6133,7 +6135,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>483</v>
       </c>
@@ -6144,7 +6146,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>485</v>
       </c>
@@ -6155,7 +6157,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>486</v>
       </c>
@@ -6166,7 +6168,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>490</v>
       </c>
@@ -6177,7 +6179,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>494</v>
       </c>
@@ -6188,7 +6190,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>496</v>
       </c>
@@ -6199,7 +6201,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>497</v>
       </c>
@@ -6210,7 +6212,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>503</v>
       </c>
@@ -6221,7 +6223,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>506</v>
       </c>
@@ -6232,7 +6234,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>507</v>
       </c>
@@ -6243,7 +6245,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>515</v>
       </c>
@@ -6254,7 +6256,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>518</v>
       </c>
@@ -6265,7 +6267,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>519</v>
       </c>
@@ -6276,7 +6278,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>521</v>
       </c>
@@ -6287,7 +6289,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>524</v>
       </c>
@@ -6298,7 +6300,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>529</v>
       </c>
@@ -6309,7 +6311,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>552</v>
       </c>
@@ -6320,7 +6322,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>553</v>
       </c>
@@ -6331,7 +6333,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>554</v>
       </c>
@@ -6342,7 +6344,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>555</v>
       </c>
@@ -6353,7 +6355,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>556</v>
       </c>
@@ -6364,7 +6366,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>557</v>
       </c>
@@ -6375,7 +6377,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="86.45" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>559</v>
       </c>
@@ -6386,7 +6388,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>561</v>
       </c>
@@ -6397,7 +6399,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>565</v>
       </c>
@@ -6408,7 +6410,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="158.44999999999999" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>566</v>
       </c>
@@ -6419,7 +6421,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>574</v>
       </c>
@@ -6438,7 +6440,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>579</v>
       </c>
@@ -6446,7 +6448,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.35" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>580</v>
       </c>
@@ -6454,7 +6456,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
         <v>583</v>
       </c>
@@ -6465,7 +6467,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>588</v>
       </c>
@@ -6473,7 +6475,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>589</v>
       </c>
@@ -6481,7 +6483,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>592</v>
       </c>
@@ -6492,7 +6494,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>593</v>
       </c>
@@ -6503,7 +6505,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>594</v>
       </c>
@@ -6511,7 +6513,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>595</v>
       </c>
@@ -6522,7 +6524,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>596</v>
       </c>
@@ -6530,7 +6532,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>597</v>
       </c>
@@ -6541,7 +6543,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>598</v>
       </c>
@@ -6552,7 +6554,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>599</v>
       </c>
@@ -6563,7 +6565,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>600</v>
       </c>
@@ -6574,7 +6576,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>601</v>
       </c>
@@ -6582,7 +6584,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>602</v>
       </c>
@@ -6593,7 +6595,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>603</v>
       </c>
@@ -6604,7 +6606,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>604</v>
       </c>
@@ -6615,7 +6617,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>605</v>
       </c>
@@ -6626,7 +6628,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="28.7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>606</v>
       </c>
@@ -6637,7 +6639,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>607</v>
       </c>
@@ -6648,7 +6650,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>608</v>
       </c>
@@ -6659,7 +6661,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="115.35" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>609</v>
       </c>
@@ -6670,7 +6672,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>610</v>
       </c>
@@ -6681,7 +6683,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>611</v>
       </c>
@@ -6692,7 +6694,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>612</v>
       </c>
@@ -6703,7 +6705,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>613</v>
       </c>
@@ -6725,7 +6727,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="100.7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>615</v>
       </c>
@@ -6769,7 +6771,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>698</v>
       </c>
@@ -6780,7 +6782,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>699</v>
       </c>
@@ -6791,7 +6793,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>700</v>
       </c>
@@ -6802,7 +6804,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>701</v>
       </c>
@@ -6835,7 +6837,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>704</v>
       </c>
@@ -6868,7 +6870,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72.599999999999994" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" ht="72.650000000000006" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>707</v>
       </c>
@@ -6890,7 +6892,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" ht="29.15" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
         <v>709</v>
       </c>
@@ -6920,7 +6922,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" s="5" t="s">
         <v>712</v>
       </c>
@@ -6942,7 +6944,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="101.45" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
         <v>714</v>
       </c>
@@ -6953,7 +6955,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" s="5" t="s">
         <v>715</v>
       </c>
@@ -6986,7 +6988,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" ht="29.15" x14ac:dyDescent="0.35">
       <c r="A213" s="5" t="s">
         <v>718</v>
       </c>
@@ -6997,7 +6999,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72.599999999999994" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" ht="72.650000000000006" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
         <v>719</v>
       </c>
@@ -7019,7 +7021,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72.599999999999994" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" ht="72.650000000000006" x14ac:dyDescent="0.35">
       <c r="A216" s="5" t="s">
         <v>721</v>
       </c>
@@ -7063,7 +7065,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="203.1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" ht="203.15" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>724</v>
       </c>
@@ -7074,20 +7076,20 @@
         <v>790</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A221" s="5" t="s">
         <v>725</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>726</v>
       </c>
       <c r="B222" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -7095,10 +7097,10 @@
         <v>727</v>
       </c>
       <c r="B223" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="C223" t="s">
         <v>797</v>
-      </c>
-      <c r="C223" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -7106,10 +7108,10 @@
         <v>728</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C224" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -7117,23 +7119,23 @@
         <v>729</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C225" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>732</v>
       </c>
@@ -7141,7 +7143,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
         <v>733</v>
       </c>
@@ -7149,7 +7151,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>734</v>
       </c>
@@ -7157,7 +7159,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>735</v>
       </c>
@@ -7165,7 +7167,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>736</v>
       </c>
@@ -7176,7 +7178,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>737</v>
       </c>
@@ -7195,7 +7197,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>739</v>
       </c>
@@ -7217,7 +7219,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>741</v>
       </c>
@@ -7228,7 +7230,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>742</v>
       </c>
@@ -7250,7 +7252,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A240" s="5" t="s">
         <v>744</v>
       </c>
@@ -7261,7 +7263,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" s="5" t="s">
         <v>745</v>
       </c>
@@ -7272,15 +7274,15 @@
         <v>792</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>241</v>
       </c>
       <c r="B242" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="C242" t="s">
         <v>803</v>
-      </c>
-      <c r="C242" t="s">
-        <v>804</v>
       </c>
     </row>
   </sheetData>
@@ -7297,13 +7299,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -7483,13 +7485,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>201</v>
       </c>
@@ -7497,7 +7499,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>203</v>
       </c>
@@ -7505,7 +7507,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>205</v>
       </c>
@@ -7513,55 +7515,55 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>208</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>211</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>212</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>215</v>
       </c>
@@ -7569,7 +7571,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>217</v>
       </c>
@@ -7577,7 +7579,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>219</v>
       </c>
@@ -7585,7 +7587,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>44</v>
       </c>
@@ -7593,7 +7595,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>222</v>
       </c>
@@ -7601,7 +7603,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>224</v>
       </c>
@@ -7609,7 +7611,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>226</v>
       </c>
@@ -7617,7 +7619,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>228</v>
       </c>
@@ -7625,7 +7627,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>230</v>
       </c>
@@ -7633,7 +7635,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>232</v>
       </c>
@@ -7641,7 +7643,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>234</v>
       </c>
@@ -7649,31 +7651,31 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>239</v>
       </c>
@@ -7681,7 +7683,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>241</v>
       </c>
@@ -7689,7 +7691,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>243</v>
       </c>
@@ -7697,7 +7699,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>245</v>
       </c>
@@ -7705,7 +7707,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>246</v>
       </c>
@@ -7713,7 +7715,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>248</v>
       </c>
@@ -7721,7 +7723,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>250</v>
       </c>
@@ -7729,7 +7731,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>252</v>
       </c>
@@ -7737,7 +7739,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>253</v>
       </c>
@@ -7745,7 +7747,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>254</v>
       </c>
@@ -7753,7 +7755,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
         <v>256</v>
       </c>
@@ -7761,7 +7763,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>258</v>
       </c>
@@ -7769,7 +7771,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>260</v>
       </c>
@@ -7777,7 +7779,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
         <v>262</v>
       </c>
@@ -7785,7 +7787,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
         <v>264</v>
       </c>
@@ -7793,7 +7795,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
         <v>266</v>
       </c>
@@ -7801,7 +7803,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
         <v>268</v>
       </c>
@@ -7809,7 +7811,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
       <c r="A44" s="13" t="s">
         <v>269</v>
       </c>
@@ -7817,7 +7819,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
         <v>270</v>
       </c>
@@ -7825,7 +7827,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>272</v>
       </c>
@@ -7833,7 +7835,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
         <v>273</v>
       </c>
@@ -7841,7 +7843,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
         <v>274</v>
       </c>
@@ -7849,7 +7851,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
         <v>276</v>
       </c>
@@ -7857,7 +7859,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
         <v>277</v>
       </c>
@@ -7865,7 +7867,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
         <v>279</v>
       </c>
@@ -7899,13 +7901,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="85.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>289</v>
       </c>
@@ -7913,7 +7915,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>291</v>
       </c>
@@ -7921,7 +7923,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>293</v>
       </c>
@@ -7929,7 +7931,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>295</v>
       </c>
@@ -7937,7 +7939,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>297</v>
       </c>
@@ -7945,7 +7947,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>299</v>
       </c>
@@ -7953,7 +7955,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>301</v>
       </c>
@@ -7961,7 +7963,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>303</v>
       </c>
@@ -7969,7 +7971,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>305</v>
       </c>
@@ -7977,7 +7979,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>307</v>
       </c>
@@ -7985,7 +7987,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>309</v>
       </c>
@@ -7993,7 +7995,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>311</v>
       </c>
@@ -8001,7 +8003,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>313</v>
       </c>
@@ -8009,7 +8011,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
         <v>315</v>
       </c>
@@ -8017,7 +8019,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="25" t="s">
         <v>317</v>
       </c>
@@ -8025,7 +8027,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="25" t="s">
         <v>319</v>
       </c>
@@ -8033,7 +8035,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="25" t="s">
         <v>321</v>
       </c>
@@ -8041,7 +8043,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="25" t="s">
         <v>323</v>
       </c>
@@ -8049,7 +8051,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="25" t="s">
         <v>325</v>
       </c>
@@ -8057,7 +8059,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="25" t="s">
         <v>327</v>
       </c>
@@ -8065,7 +8067,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="21" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="25" t="s">
         <v>329</v>
       </c>
@@ -8073,7 +8075,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="25" t="s">
         <v>331</v>
       </c>
@@ -8081,7 +8083,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="23" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="25" t="s">
         <v>333</v>
       </c>
@@ -8089,7 +8091,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="25" t="s">
         <v>335</v>
       </c>
@@ -8097,7 +8099,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="25" t="s">
         <v>337</v>
       </c>
@@ -8105,7 +8107,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="26" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="25" t="s">
         <v>339</v>
       </c>
@@ -8113,7 +8115,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="27" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="25" t="s">
         <v>341</v>
       </c>
@@ -8121,7 +8123,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="28" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="25" t="s">
         <v>343</v>
       </c>
@@ -8129,7 +8131,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="25" t="s">
         <v>345</v>
       </c>
@@ -8137,7 +8139,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="25" t="s">
         <v>347</v>
       </c>
@@ -8145,7 +8147,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="31" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="25" t="s">
         <v>349</v>
       </c>
@@ -8153,7 +8155,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="25" t="s">
         <v>351</v>
       </c>
@@ -8161,7 +8163,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="25" t="s">
         <v>353</v>
       </c>
@@ -8169,7 +8171,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="34" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="25" t="s">
         <v>355</v>
       </c>
@@ -8177,7 +8179,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="25" t="s">
         <v>357</v>
       </c>

</xml_diff>

<commit_message>
EPRA Payer query changed and feature file
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tathyush\Desktop\Final_Branch_Master\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E247E70C-25E5-49A3-87DC-558608F55C27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2450" windowWidth="19420" windowHeight="5750" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="807">
   <si>
     <t>City</t>
   </si>
@@ -3826,6 +3832,76 @@
 EVNT_MSG like '%EPRA%') and CREAT_BY_ID='{$id}' order by CREAT_DTTM desc fetch first row only</t>
   </si>
   <si>
+    <t>delete from ole.BILLING_SERVICE_PROVIDER where PROV_TIN_NBR='{$tin}' and CREAT_BY_ID='Automation'</t>
+  </si>
+  <si>
+    <t>select prov_tin_nbr AS PROV_TAX_ID_NBR from ole.portal_user_tin
+where portal_user_id in (select portal_user_id from ole.portal_user where sso_id = '{$id}')
+and prov_tin_nbr in (select prov_tax_id_nbr from pp001.provider where prov_key_id in (select PROV_KEY_ID from pp001.consolidated_payment
+where proc_ctl_id in (select proc_ctl_id from ole.proc_ctl where EXTRACT_STS_CD in ('X','C') and OVALL_PROC_STS_CD in ('C','X') and SRCH_TBL_STS_CD = 'C' order by proc_ctl_id desc)))
+fetch first row only
+with ur</t>
+  </si>
+  <si>
+    <t>Get TIN for Remit and Claim Detail</t>
+  </si>
+  <si>
+    <t>SELECT SC.CP_DSPL_CONSL_PAY_NBR, PA.CONSL_PAY_NBR
+FROM OLE.SRCH_CONSOL_TBL SC
+LEFT JOIN PP001.PROVIDER_PAYOR_ADJUSTMENT PA ON SC.UCP_CONSL_PAY_NBR = PA.CONSL_PAY_NBR
+WHERE PROV_TAX_ID_NBR = '{$tin}'
+GROUP BY PA.CONSL_PAY_NBR, SC.CP_DSPL_CONSL_PAY_NBR
+HAVING COUNT(*) = 4
+ORDER BY PA.CONSL_PAY_NBR ASC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT SC.CP_DSPL_CONSL_PAY_NBR, PA.CONSL_PAY_NBR
+FROM OLE.SRCH_CONSOL_TBL SC
+LEFT JOIN PP001.PROVIDER_PAYOR_ADJUSTMENT PA ON SC.UCP_CONSL_PAY_NBR = PA.CONSL_PAY_NBR
+WHERE PROV_TAX_ID_NBR = '{$tin}'
+GROUP BY PA.CONSL_PAY_NBR, SC.CP_DSPL_CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY PA.CONSL_PAY_NBR ASC LIMIT 1</t>
+  </si>
+  <si>
+    <t>GET DSPL_CONSL_PAY_NBR for Remit and Claim Detail for Multiple PLB</t>
+  </si>
+  <si>
+    <t>GET DSPL_CONSL_PAY_NBR for Remit and Claim Detail for PLB</t>
+  </si>
+  <si>
+    <t>Select  PROV_ADJ_RSN_CD,PROV_ADJ_ID,PROV_PAYR_ADJ_AMT from PP001.PROVIDER_PAYOR_ADJUSTMENT where CONSL_PAY_NBR IN
+(SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+WHERE CONSL_PAY_NBR = '{$consl_pay_nbr}'
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 4
+ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>Get Data for Multiple PLB for Remit Detail</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr, cp.DSPL_CONSL_PAY_NBR, cp.SETL_DT, cp.CONSL_PAY_NBR
+from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC, ole.ENROLLED_PROVIDER ep WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and ep.PROV_TIN_NBR = p.PROV_TAX_ID_NBR
+and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
+AND cp.setl_dt BETWEEN '{$fromDate}' AND '{$toDate}' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
+and cp.CONSL_PAY_NBR not in (select CONSL_PAY_NBR from ole.EPRA_STATUS)
+and ep.ENRL_STS_CD = 'A'
+group by p.prov_tax_id_nbr, cp.DSPL_CONSL_PAY_NBR, cp.SETL_DT, cp.CONSL_PAY_NBR
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) AS TIN_COUNT FROM OLE.PORTAL_USER PU, OLE.PORTAL_USER_PAYER_TIN PUP, OLE.PAYER_ENROLLED_PROVIDER PEP 
+WHERE PU.PORTAL_USER_ID = PUP.PORTAL_USER_ID AND PUP.PAYR_TIN_NBR = PEP.PAYR_TIN_NBR AND PU.SSO_ID = '{$id}' AND PEP.PROV_TIN_NBR = '{$tin}' with ur</t>
+  </si>
+  <si>
+    <t>Check the TIN is associated or not for Payer</t>
+  </si>
+  <si>
     <t>SELECT * FROM
 (
 -- For ranking the records
@@ -3838,18 +3914,22 @@
 SC.PROV_NPI_NBR,SCL.RP_UPPER_LST_NM as LST_NM,SCL.SUB_SBSCR_ID as SBSCR_ID, SCL.CLM_PTNT_FST_NM as PTNT_FST_NM, SCL.CLM_PTNT_LST_NM as PTNT_LST_NM, SCL.CLM_UPER_PTNT_LST_NM AS REND_PROV_NM,
 SCL.CLM_PTNT_ACCT_NBR as PTNT_ACCT_NBR, SCL.CLM_NBR as CLM_NBR,
 COUNT(DISTINCT SCL.CLM_KEY_ID) as CLAIMCOUNT
-FROM OLE.PORTAL_USER PU, OLE.PORTAL_USER_TIN PUT, OLE.EPRA_STATUS EP, OLE.SRCH_CONSOL_TBL SC, OLE.SRCH_CLAIM_TBL SCL
+FROM OLE.PORTAL_USER PU, OLE.PORTAL_USER_TIN PUT, OLE.EPRA_STATUS EP, OLE.SRCH_CONSOL_TBL SC, OLE.SRCH_CLAIM_TBL SCL, pp018.consolidated_payment CP, ole.PROC_CTL PC
 WHERE PU.PORTAL_USER_ID = PUT.PORTAL_USER_ID -- Join PU with PUT
 AND PUT.PROV_TIN_NBR=SC.PROV_TAX_ID_NBR-- Join SC with PUT
 AND SC.UCP_UCONSL_PAY_KEY_ID = SCL.CUP_UCONSL_PAY_KEY_ID-- Join SC with SCL
 AND SC.PAYR_SCHM_NM=SCL.PAYR_SCHM_NM-- Join SC with SCL- Payer
 AND SC.PAYR_SCHM_NM = 'PP018'-- &lt;&lt;Change Payer Schema Name here&gt;&gt;
-AND SC.CP_SETL_DT BETWEEN '2020-03-01' AND '2020-04-09' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
+AND CP.CONSL_PAY_NBR = SC.UCP_CONSL_PAY_NBR
+AND PC.PROC_CTL_ID = CP.PROC_CTL_ID
+---AND SC.CP_SETL_DT BETWEEN '2020-03-01' AND '2020-04-09' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
+AND SC.CP_SETL_DT LIKE '2020%'
 AND PU.STS_CD='A'
 AND PU.USER_TYP='P'
 AND EP.PRIORITY = '{$priority}'
-and SCL.CLM_PTNT_ACCT_NBR != '0'
-AND SC.PROV_NPI_NBR != ''
+---and SCL.CLM_PTNT_ACCT_NBR != '0'
+--AND SC.PROV_NPI_NBR != ''
+AND PC.EXTRACT_STS_CD = 'C'
 AND SC.UCP_CONSL_PAY_NBR NOT IN 
 (SELECT DISTINCT EP.CONSL_PAY_NBR FROM OLE.EPRA_STATUS EP)-- Payment ID shouldn't exist in EPRA_STATUS
 GROUP BY PU.PORTAL_USER_ID, PU.USERNAME, PU.SSO_ID, PUT.PROV_TIN_NBR, PU.USER_TYP, PU.STS_CD,
@@ -3863,74 +3943,11 @@
 WHERE DUPLUSR.USER_RANK=1
 fetch first row only</t>
   </si>
-  <si>
-    <t>delete from ole.BILLING_SERVICE_PROVIDER where PROV_TIN_NBR='{$tin}' and CREAT_BY_ID='Automation'</t>
-  </si>
-  <si>
-    <t>select prov_tin_nbr AS PROV_TAX_ID_NBR from ole.portal_user_tin
-where portal_user_id in (select portal_user_id from ole.portal_user where sso_id = '{$id}')
-and prov_tin_nbr in (select prov_tax_id_nbr from pp001.provider where prov_key_id in (select PROV_KEY_ID from pp001.consolidated_payment
-where proc_ctl_id in (select proc_ctl_id from ole.proc_ctl where EXTRACT_STS_CD in ('X','C') and OVALL_PROC_STS_CD in ('C','X') and SRCH_TBL_STS_CD = 'C' order by proc_ctl_id desc)))
-fetch first row only
-with ur</t>
-  </si>
-  <si>
-    <t>Get TIN for Remit and Claim Detail</t>
-  </si>
-  <si>
-    <t>SELECT SC.CP_DSPL_CONSL_PAY_NBR, PA.CONSL_PAY_NBR
-FROM OLE.SRCH_CONSOL_TBL SC
-LEFT JOIN PP001.PROVIDER_PAYOR_ADJUSTMENT PA ON SC.UCP_CONSL_PAY_NBR = PA.CONSL_PAY_NBR
-WHERE PROV_TAX_ID_NBR = '{$tin}'
-GROUP BY PA.CONSL_PAY_NBR, SC.CP_DSPL_CONSL_PAY_NBR
-HAVING COUNT(*) = 4
-ORDER BY PA.CONSL_PAY_NBR ASC LIMIT 1</t>
-  </si>
-  <si>
-    <t>SELECT SC.CP_DSPL_CONSL_PAY_NBR, PA.CONSL_PAY_NBR
-FROM OLE.SRCH_CONSOL_TBL SC
-LEFT JOIN PP001.PROVIDER_PAYOR_ADJUSTMENT PA ON SC.UCP_CONSL_PAY_NBR = PA.CONSL_PAY_NBR
-WHERE PROV_TAX_ID_NBR = '{$tin}'
-GROUP BY PA.CONSL_PAY_NBR, SC.CP_DSPL_CONSL_PAY_NBR
-HAVING COUNT(*) = 2
-ORDER BY PA.CONSL_PAY_NBR ASC LIMIT 1</t>
-  </si>
-  <si>
-    <t>GET DSPL_CONSL_PAY_NBR for Remit and Claim Detail for Multiple PLB</t>
-  </si>
-  <si>
-    <t>GET DSPL_CONSL_PAY_NBR for Remit and Claim Detail for PLB</t>
-  </si>
-  <si>
-    <t>Select  PROV_ADJ_RSN_CD,PROV_ADJ_ID,PROV_PAYR_ADJ_AMT from PP001.PROVIDER_PAYOR_ADJUSTMENT where CONSL_PAY_NBR IN
-(SELECT CONSL_PAY_NBR
-FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
-WHERE CONSL_PAY_NBR = '{$consl_pay_nbr}'
-GROUP BY CONSL_PAY_NBR
-HAVING COUNT(*) = 4
-ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
-  </si>
-  <si>
-    <t>Get Data for Multiple PLB for Remit Detail</t>
-  </si>
-  <si>
-    <t>Select p.prov_tax_id_nbr, cp.DSPL_CONSL_PAY_NBR, cp.SETL_DT, cp.CONSL_PAY_NBR
-from PP001.CONSOLIDATED_PAYMENT cp, PP001.PROVIDER p, OLE.PROC_CTL PC, ole.ENROLLED_PROVIDER ep WHERE PC.PROC_CTL_ID = CP.PROC_CTL_ID
-and ep.PROV_TIN_NBR = p.PROV_TAX_ID_NBR
-and cp.prov_key_id = p.prov_key_id AND PC.EXTRACT_STS_CD = 'C'
-AND cp.setl_dt BETWEEN '{$fromDate}' AND '{$toDate}' -- &lt;&lt;Change Claim Settlement Date range here &gt;&gt;
-and cp.CONSL_PAY_NBR not in (select CONSL_PAY_NBR from ole.EPRA_STATUS)
-and ep.ENRL_STS_CD = 'A'
-group by p.prov_tax_id_nbr, cp.DSPL_CONSL_PAY_NBR, cp.SETL_DT, cp.CONSL_PAY_NBR
-having count(*) between 1 and 30
-order by count(*) desc
-fetch first row only</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4208,7 +4225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4241,9 +4258,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4276,6 +4310,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4451,26 +4502,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4499,7 +4550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4528,7 +4579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4552,7 +4603,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4581,7 +4632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4610,7 +4661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4636,7 +4687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4662,7 +4713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4688,7 +4739,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -4714,7 +4765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4740,7 +4791,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4766,7 +4817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4792,7 +4843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4818,7 +4869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4844,7 +4895,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4870,7 +4921,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -4903,21 +4954,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D242"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B221" sqref="B221"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C211" sqref="C211"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="136.54296875" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="136.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4928,7 +4979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4939,7 +4990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4950,7 +5001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4958,7 +5009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4969,7 +5020,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4977,7 +5028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4985,7 +5036,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4993,7 +5044,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -5001,7 +5052,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5009,7 +5060,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -5017,7 +5068,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -5025,7 +5076,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5033,7 +5084,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5041,7 +5092,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5049,7 +5100,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5057,7 +5108,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -5065,7 +5116,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -5073,7 +5124,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -5081,7 +5132,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
@@ -5089,7 +5140,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -5097,7 +5148,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
@@ -5105,7 +5156,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
@@ -5113,7 +5164,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -5121,7 +5172,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>91</v>
       </c>
@@ -5129,7 +5180,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>92</v>
       </c>
@@ -5137,7 +5188,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
@@ -5145,7 +5196,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>94</v>
       </c>
@@ -5153,7 +5204,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>96</v>
       </c>
@@ -5161,7 +5212,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>97</v>
       </c>
@@ -5172,7 +5223,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -5183,7 +5234,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
@@ -5194,7 +5245,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="187.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -5205,7 +5256,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>109</v>
       </c>
@@ -5213,7 +5264,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>110</v>
       </c>
@@ -5221,7 +5272,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
@@ -5232,7 +5283,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>114</v>
       </c>
@@ -5243,7 +5294,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
@@ -5251,7 +5302,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>119</v>
       </c>
@@ -5259,7 +5310,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>120</v>
       </c>
@@ -5267,7 +5318,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>123</v>
       </c>
@@ -5275,7 +5326,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>124</v>
       </c>
@@ -5289,7 +5340,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>126</v>
       </c>
@@ -5300,7 +5351,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>127</v>
       </c>
@@ -5311,7 +5362,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -5322,7 +5373,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -5333,7 +5384,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="172.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>130</v>
       </c>
@@ -5344,7 +5395,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>131</v>
       </c>
@@ -5355,7 +5406,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>132</v>
       </c>
@@ -5366,7 +5417,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>133</v>
       </c>
@@ -5377,7 +5428,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>134</v>
       </c>
@@ -5388,7 +5439,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>135</v>
       </c>
@@ -5399,7 +5450,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>136</v>
       </c>
@@ -5410,7 +5461,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>137</v>
       </c>
@@ -5418,7 +5469,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>139</v>
       </c>
@@ -5429,7 +5480,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>140</v>
       </c>
@@ -5437,7 +5488,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>146</v>
       </c>
@@ -5448,7 +5499,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>147</v>
       </c>
@@ -5456,7 +5507,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>151</v>
       </c>
@@ -5467,7 +5518,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>153</v>
       </c>
@@ -5478,7 +5529,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>154</v>
       </c>
@@ -5489,7 +5540,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>155</v>
       </c>
@@ -5500,7 +5551,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>156</v>
       </c>
@@ -5508,7 +5559,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>177</v>
       </c>
@@ -5519,7 +5570,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="129.65" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>178</v>
       </c>
@@ -5530,7 +5581,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>183</v>
       </c>
@@ -5538,7 +5589,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>184</v>
       </c>
@@ -5546,7 +5597,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>185</v>
       </c>
@@ -5554,7 +5605,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>186</v>
       </c>
@@ -5562,7 +5613,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>195</v>
       </c>
@@ -5573,7 +5624,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>198</v>
       </c>
@@ -5584,7 +5635,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>200</v>
       </c>
@@ -5592,7 +5643,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>281</v>
       </c>
@@ -5600,7 +5651,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>282</v>
       </c>
@@ -5608,7 +5659,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>285</v>
       </c>
@@ -5616,7 +5667,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>287</v>
       </c>
@@ -5624,7 +5675,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>359</v>
       </c>
@@ -5632,7 +5683,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>360</v>
       </c>
@@ -5640,7 +5691,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>361</v>
       </c>
@@ -5648,7 +5699,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>363</v>
       </c>
@@ -5656,7 +5707,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>364</v>
       </c>
@@ -5664,7 +5715,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>366</v>
       </c>
@@ -5672,7 +5723,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>368</v>
       </c>
@@ -5680,7 +5731,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>369</v>
       </c>
@@ -5688,7 +5739,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>370</v>
       </c>
@@ -5696,7 +5747,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>371</v>
       </c>
@@ -5704,7 +5755,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>373</v>
       </c>
@@ -5712,7 +5763,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>374</v>
       </c>
@@ -5720,7 +5771,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>376</v>
       </c>
@@ -5728,7 +5779,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>387</v>
       </c>
@@ -5736,7 +5787,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>388</v>
       </c>
@@ -5744,7 +5795,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>390</v>
       </c>
@@ -5752,7 +5803,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>393</v>
       </c>
@@ -5760,7 +5811,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>395</v>
       </c>
@@ -5768,7 +5819,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>397</v>
       </c>
@@ -5776,7 +5827,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>399</v>
       </c>
@@ -5784,7 +5835,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>400</v>
       </c>
@@ -5792,7 +5843,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>403</v>
       </c>
@@ -5800,7 +5851,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>408</v>
       </c>
@@ -5808,7 +5859,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>409</v>
       </c>
@@ -5816,7 +5867,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>410</v>
       </c>
@@ -5824,7 +5875,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>411</v>
       </c>
@@ -5832,7 +5883,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="187.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>412</v>
       </c>
@@ -5843,7 +5894,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="273.64999999999998" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="285" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>413</v>
       </c>
@@ -5854,7 +5905,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="230.5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>415</v>
       </c>
@@ -5865,7 +5916,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>418</v>
       </c>
@@ -5873,7 +5924,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>420</v>
       </c>
@@ -5881,7 +5932,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>425</v>
       </c>
@@ -5889,7 +5940,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>427</v>
       </c>
@@ -5897,7 +5948,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>428</v>
       </c>
@@ -5905,7 +5956,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>429</v>
       </c>
@@ -5913,7 +5964,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>452</v>
       </c>
@@ -5924,7 +5975,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>453</v>
       </c>
@@ -5935,7 +5986,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>454</v>
       </c>
@@ -5946,7 +5997,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>455</v>
       </c>
@@ -5957,7 +6008,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>456</v>
       </c>
@@ -5968,7 +6019,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>457</v>
       </c>
@@ -5979,7 +6030,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>458</v>
       </c>
@@ -5990,7 +6041,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>459</v>
       </c>
@@ -6001,7 +6052,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>460</v>
       </c>
@@ -6012,7 +6063,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>461</v>
       </c>
@@ -6023,7 +6074,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>462</v>
       </c>
@@ -6034,7 +6085,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>463</v>
       </c>
@@ -6045,7 +6096,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>464</v>
       </c>
@@ -6056,7 +6107,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>466</v>
       </c>
@@ -6064,7 +6115,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>465</v>
       </c>
@@ -6072,7 +6123,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>468</v>
       </c>
@@ -6083,7 +6134,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>469</v>
       </c>
@@ -6094,7 +6145,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>471</v>
       </c>
@@ -6102,7 +6153,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>472</v>
       </c>
@@ -6113,7 +6164,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>477</v>
       </c>
@@ -6124,7 +6175,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>478</v>
       </c>
@@ -6135,7 +6186,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>483</v>
       </c>
@@ -6146,7 +6197,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>485</v>
       </c>
@@ -6157,7 +6208,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>486</v>
       </c>
@@ -6168,7 +6219,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>490</v>
       </c>
@@ -6179,7 +6230,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>494</v>
       </c>
@@ -6190,7 +6241,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>496</v>
       </c>
@@ -6201,7 +6252,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>497</v>
       </c>
@@ -6212,7 +6263,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>503</v>
       </c>
@@ -6223,7 +6274,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>506</v>
       </c>
@@ -6234,7 +6285,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>507</v>
       </c>
@@ -6245,7 +6296,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>515</v>
       </c>
@@ -6256,7 +6307,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>518</v>
       </c>
@@ -6267,7 +6318,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>519</v>
       </c>
@@ -6278,7 +6329,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>521</v>
       </c>
@@ -6289,7 +6340,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>524</v>
       </c>
@@ -6300,7 +6351,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>529</v>
       </c>
@@ -6311,7 +6362,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>552</v>
       </c>
@@ -6322,7 +6373,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>553</v>
       </c>
@@ -6333,7 +6384,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>554</v>
       </c>
@@ -6344,7 +6395,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>555</v>
       </c>
@@ -6355,7 +6406,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>556</v>
       </c>
@@ -6366,7 +6417,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>557</v>
       </c>
@@ -6377,7 +6428,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="86.5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>559</v>
       </c>
@@ -6388,7 +6439,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>561</v>
       </c>
@@ -6399,7 +6450,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>565</v>
       </c>
@@ -6410,7 +6461,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="158.5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>566</v>
       </c>
@@ -6421,7 +6472,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>574</v>
       </c>
@@ -6429,7 +6480,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>575</v>
       </c>
@@ -6440,7 +6491,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="57.65" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>579</v>
       </c>
@@ -6448,7 +6499,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>580</v>
       </c>
@@ -6456,7 +6507,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>583</v>
       </c>
@@ -6467,7 +6518,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>588</v>
       </c>
@@ -6475,7 +6526,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>589</v>
       </c>
@@ -6483,7 +6534,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>592</v>
       </c>
@@ -6494,7 +6545,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>593</v>
       </c>
@@ -6505,7 +6556,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>594</v>
       </c>
@@ -6513,7 +6564,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>595</v>
       </c>
@@ -6524,7 +6575,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>596</v>
       </c>
@@ -6532,7 +6583,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>597</v>
       </c>
@@ -6543,7 +6594,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>598</v>
       </c>
@@ -6554,7 +6605,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>599</v>
       </c>
@@ -6565,7 +6616,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>600</v>
       </c>
@@ -6576,7 +6627,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>601</v>
       </c>
@@ -6584,7 +6635,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>602</v>
       </c>
@@ -6595,7 +6646,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>603</v>
       </c>
@@ -6606,7 +6657,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>604</v>
       </c>
@@ -6617,7 +6668,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>605</v>
       </c>
@@ -6628,7 +6679,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="28.75" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>606</v>
       </c>
@@ -6639,7 +6690,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>607</v>
       </c>
@@ -6650,7 +6701,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>608</v>
       </c>
@@ -6661,7 +6712,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="115.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>609</v>
       </c>
@@ -6672,7 +6723,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>610</v>
       </c>
@@ -6683,7 +6734,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>611</v>
       </c>
@@ -6694,7 +6745,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>612</v>
       </c>
@@ -6705,7 +6756,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>613</v>
       </c>
@@ -6716,7 +6767,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>614</v>
       </c>
@@ -6727,7 +6778,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="100.75" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>615</v>
       </c>
@@ -6738,7 +6789,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>695</v>
       </c>
@@ -6771,7 +6822,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>698</v>
       </c>
@@ -6782,7 +6833,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>699</v>
       </c>
@@ -6793,7 +6844,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>700</v>
       </c>
@@ -6804,7 +6855,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>701</v>
       </c>
@@ -6837,7 +6888,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>704</v>
       </c>
@@ -6870,7 +6921,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72.650000000000006" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>707</v>
       </c>
@@ -6881,7 +6932,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>708</v>
       </c>
@@ -6892,7 +6943,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29.15" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>709</v>
       </c>
@@ -6900,7 +6951,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>710</v>
       </c>
@@ -6911,7 +6962,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>711</v>
       </c>
@@ -6922,7 +6973,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>712</v>
       </c>
@@ -6933,7 +6984,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>713</v>
       </c>
@@ -6944,7 +6995,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>714</v>
       </c>
@@ -6955,7 +7006,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>715</v>
       </c>
@@ -6966,18 +7017,18 @@
         <v>694</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>716</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>794</v>
+        <v>806</v>
       </c>
       <c r="C211" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
         <v>717</v>
       </c>
@@ -6988,7 +7039,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="29.15" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>718</v>
       </c>
@@ -6999,7 +7050,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72.650000000000006" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>719</v>
       </c>
@@ -7010,7 +7061,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>720</v>
       </c>
@@ -7021,7 +7072,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72.650000000000006" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>721</v>
       </c>
@@ -7032,7 +7083,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>722</v>
       </c>
@@ -7043,7 +7094,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -7054,7 +7105,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>723</v>
       </c>
@@ -7065,7 +7116,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="203.15" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>724</v>
       </c>
@@ -7076,20 +7127,20 @@
         <v>790</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>725</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>726</v>
       </c>
       <c r="B222" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -7097,10 +7148,10 @@
         <v>727</v>
       </c>
       <c r="B223" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="C223" t="s">
         <v>796</v>
-      </c>
-      <c r="C223" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -7108,34 +7159,34 @@
         <v>728</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C224" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>729</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C225" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>732</v>
       </c>
@@ -7143,7 +7194,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
         <v>733</v>
       </c>
@@ -7151,7 +7202,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>734</v>
       </c>
@@ -7159,7 +7210,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>735</v>
       </c>
@@ -7167,7 +7218,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>736</v>
       </c>
@@ -7178,7 +7229,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>737</v>
       </c>
@@ -7189,7 +7240,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>738</v>
       </c>
@@ -7197,7 +7248,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>739</v>
       </c>
@@ -7208,7 +7259,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
         <v>740</v>
       </c>
@@ -7219,7 +7270,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>741</v>
       </c>
@@ -7230,7 +7281,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>742</v>
       </c>
@@ -7241,7 +7292,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>743</v>
       </c>
@@ -7252,7 +7303,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>744</v>
       </c>
@@ -7263,7 +7314,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
         <v>745</v>
       </c>
@@ -7274,15 +7325,26 @@
         <v>792</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
       <c r="B242" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="C242" t="s">
         <v>802</v>
       </c>
-      <c r="C242" t="s">
-        <v>803</v>
+    </row>
+    <row r="243" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="C243" t="s">
+        <v>805</v>
       </c>
     </row>
   </sheetData>
@@ -7292,23 +7354,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7328,7 +7390,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -7351,7 +7413,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -7374,7 +7436,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -7394,7 +7456,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -7408,7 +7470,7 @@
         <v>656565</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -7422,7 +7484,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -7445,7 +7507,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -7470,7 +7532,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7478,20 +7540,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>201</v>
       </c>
@@ -7499,7 +7561,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>203</v>
       </c>
@@ -7507,7 +7569,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>205</v>
       </c>
@@ -7515,55 +7577,55 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>208</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>211</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>212</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>215</v>
       </c>
@@ -7571,7 +7633,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>217</v>
       </c>
@@ -7579,7 +7641,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>219</v>
       </c>
@@ -7587,7 +7649,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>44</v>
       </c>
@@ -7595,7 +7657,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>222</v>
       </c>
@@ -7603,7 +7665,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>224</v>
       </c>
@@ -7611,7 +7673,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>226</v>
       </c>
@@ -7619,7 +7681,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>228</v>
       </c>
@@ -7627,7 +7689,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>230</v>
       </c>
@@ -7635,7 +7697,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>232</v>
       </c>
@@ -7643,7 +7705,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>234</v>
       </c>
@@ -7651,31 +7713,31 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>239</v>
       </c>
@@ -7683,7 +7745,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>241</v>
       </c>
@@ -7691,7 +7753,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>243</v>
       </c>
@@ -7699,7 +7761,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>245</v>
       </c>
@@ -7707,7 +7769,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>246</v>
       </c>
@@ -7715,7 +7777,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>248</v>
       </c>
@@ -7723,7 +7785,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>250</v>
       </c>
@@ -7731,7 +7793,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>252</v>
       </c>
@@ -7739,7 +7801,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>253</v>
       </c>
@@ -7747,7 +7809,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>254</v>
       </c>
@@ -7755,7 +7817,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>256</v>
       </c>
@@ -7763,7 +7825,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>258</v>
       </c>
@@ -7771,7 +7833,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>260</v>
       </c>
@@ -7779,7 +7841,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>262</v>
       </c>
@@ -7787,7 +7849,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>264</v>
       </c>
@@ -7795,7 +7857,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>266</v>
       </c>
@@ -7803,7 +7865,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>268</v>
       </c>
@@ -7811,7 +7873,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>269</v>
       </c>
@@ -7819,7 +7881,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>270</v>
       </c>
@@ -7827,7 +7889,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>272</v>
       </c>
@@ -7835,7 +7897,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>273</v>
       </c>
@@ -7843,7 +7905,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>274</v>
       </c>
@@ -7851,7 +7913,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>276</v>
       </c>
@@ -7859,7 +7921,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>277</v>
       </c>
@@ -7867,7 +7929,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>279</v>
       </c>
@@ -7877,37 +7939,37 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>Platform</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B9 B12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B9 B12" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>URL</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B26" r:id="rId1" location="tip.1486618499489"/>
-    <hyperlink ref="B3" r:id="rId2" location="tip.1492608750540"/>
-    <hyperlink ref="B27" r:id="rId3"/>
-    <hyperlink ref="B30" r:id="rId4" location="tip.1486618499489"/>
-    <hyperlink ref="B33" r:id="rId5"/>
+    <hyperlink ref="B26" r:id="rId1" location="tip.1486618499489" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" location="tip.1492608750540" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B27" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B30" r:id="rId4" location="tip.1486618499489" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="B33" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="85.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>289</v>
       </c>
@@ -7915,7 +7977,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>291</v>
       </c>
@@ -7923,7 +7985,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>293</v>
       </c>
@@ -7931,7 +7993,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>295</v>
       </c>
@@ -7939,7 +8001,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>297</v>
       </c>
@@ -7947,7 +8009,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>299</v>
       </c>
@@ -7955,7 +8017,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>301</v>
       </c>
@@ -7963,7 +8025,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>303</v>
       </c>
@@ -7971,7 +8033,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>305</v>
       </c>
@@ -7979,7 +8041,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>307</v>
       </c>
@@ -7987,7 +8049,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>309</v>
       </c>
@@ -7995,7 +8057,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>311</v>
       </c>
@@ -8003,7 +8065,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>313</v>
       </c>
@@ -8011,7 +8073,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>315</v>
       </c>
@@ -8019,7 +8081,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>317</v>
       </c>
@@ -8027,7 +8089,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>319</v>
       </c>
@@ -8035,7 +8097,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>321</v>
       </c>
@@ -8043,7 +8105,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>323</v>
       </c>
@@ -8051,7 +8113,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>325</v>
       </c>
@@ -8059,7 +8121,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>327</v>
       </c>
@@ -8067,7 +8129,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>329</v>
       </c>
@@ -8075,7 +8137,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
         <v>331</v>
       </c>
@@ -8083,7 +8145,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>333</v>
       </c>
@@ -8091,7 +8153,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>335</v>
       </c>
@@ -8099,7 +8161,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>337</v>
       </c>
@@ -8107,7 +8169,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>339</v>
       </c>
@@ -8115,7 +8177,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>341</v>
       </c>
@@ -8123,7 +8185,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>343</v>
       </c>
@@ -8131,7 +8193,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
         <v>345</v>
       </c>
@@ -8139,7 +8201,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25" t="s">
         <v>347</v>
       </c>
@@ -8147,7 +8209,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
         <v>349</v>
       </c>
@@ -8155,7 +8217,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>351</v>
       </c>
@@ -8163,7 +8225,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>353</v>
       </c>
@@ -8171,7 +8233,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
         <v>355</v>
       </c>
@@ -8179,7 +8241,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
         <v>357</v>
       </c>

</xml_diff>

<commit_message>
Adding RTN cases in feature file
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CucumberEditEnrollment\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16842CB5-B79E-41B4-BB4D-86C14366E97E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD4DC67-5BCD-4D52-81F6-370387CB676D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="826">
   <si>
     <t>City</t>
   </si>
@@ -4024,6 +4024,12 @@
     <t xml:space="preserve">SELECT * FROM ole.PROVIDER_BANKING_ACCOUNT bc JOIN ole.PAYMENT_DESIGNATION pd
 ON bc.PROV_BNK_ACCT_ID=pd.PROV_BNK_ACCT_ID
 WHERE bc.PROV_TIN_NBR='{$tin}' AND pd.BNK_ACCT_LVL_TYP_ID=4 ORDER BY bc.LST_CHG_BY_DTTM </t>
+  </si>
+  <si>
+    <t>select PAYR_NM from ole.PAYER where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sts_cd = 'PU' and USER_TYP = 'PA')) Limit 1</t>
+  </si>
+  <si>
+    <t>250</t>
   </si>
 </sst>
 </file>
@@ -5137,10 +5143,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D250"/>
+  <dimension ref="A1:D251"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B250" sqref="B250"/>
+      <selection activeCell="A251" sqref="A251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7586,6 +7592,14 @@
       </c>
       <c r="B250" s="7" t="s">
         <v>821</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A251" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="B251" s="7" t="s">
+        <v>824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Purged user data file with queries
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CucumberEditEnrollment\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD4DC67-5BCD-4D52-81F6-370387CB676D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D895DF-2A3F-4CA6-B8D8-4720D07F5F19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="836">
   <si>
     <t>City</t>
   </si>
@@ -4026,10 +4026,65 @@
 WHERE bc.PROV_TIN_NBR='{$tin}' AND pd.BNK_ACCT_LVL_TYP_ID=4 ORDER BY bc.LST_CHG_BY_DTTM </t>
   </si>
   <si>
-    <t>select PAYR_NM from ole.PAYER where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sts_cd = 'PU' and USER_TYP = 'PA')) Limit 1</t>
-  </si>
-  <si>
     <t>250</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.PAYER where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sts_cd = 'PU' and USER_TYP = 'PA')) Limit 1</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.PAYER where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sts_cd not in( 'PU') and USER_TYP = 'PA')) Limit 1</t>
+  </si>
+  <si>
+    <t>251</t>
+  </si>
+  <si>
+    <t>252</t>
+  </si>
+  <si>
+    <t>select * from 
+(SELECT DISTINCT pu.PORTAL_USER_ID ,pu.STS_CD, pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT , 
+CASE WHEN length(lower(pu.MIDDLE_INIT)) &gt; 0
+THEN
+trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) || ' ' || lower(pu.MIDDLE_INIT)) 
+ELSE trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) ) 
+END as FullName 
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID
+WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
+ORDER BY FullName asc)</t>
+  </si>
+  <si>
+    <t>Getting All users associated with the payer including Purged</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>Excluding Purged users</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>select * from 
+(SELECT DISTINCT pu.PORTAL_USER_ID , pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT , 
+CASE WHEN length(lower(pu.MIDDLE_INIT)) &gt; 0
+THEN
+trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) || ' ' || lower(pu.MIDDLE_INIT)) 
+ELSE trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) ) 
+END as FullName 
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID
+WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
+and pu.STS_CD not in('PU')
+ORDER BY FullName asc)</t>
+  </si>
+  <si>
+    <t>SELECT pu.PORTAL_USER_ID , pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT, pu.USERNAME,pu.LST_CHG_BY_ID,pu.LST_CHG_BY_DTTM
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID 
+WHERE pt.PAYR_TIN_NBR in(select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
+and pu.STS_CD = 'PU'</t>
   </si>
 </sst>
 </file>
@@ -5143,17 +5198,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D251"/>
+  <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A251" sqref="A251"/>
+    <sheetView tabSelected="1" topLeftCell="A254" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B258" sqref="B258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.81640625" customWidth="1"/>
     <col min="2" max="2" width="136.54296875" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="3" max="3" width="47.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -7596,10 +7651,48 @@
     </row>
     <row r="251" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A251" s="5" t="s">
+        <v>824</v>
+      </c>
+      <c r="B251" s="7" t="s">
         <v>825</v>
       </c>
-      <c r="B251" s="7" t="s">
-        <v>824</v>
+    </row>
+    <row r="252" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A252" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="B252" s="7" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A253" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="B253" s="7" t="s">
+        <v>829</v>
+      </c>
+      <c r="C253" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A254" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="B254" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="C254" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A255" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="B255" s="7" t="s">
+        <v>835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated manage user fix for disabled tin query
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1058\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CucumberFinal1\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CE1BAC-6C63-4EB9-AAFA-657D10F66EE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CC6AA5-1910-4B1E-84A8-45F19AB740DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="849">
   <si>
     <t>City</t>
   </si>
@@ -4136,6 +4136,58 @@
 order by cp.SETL_DT DESC
 fetch first row only with ur</t>
   </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p where p.{$srchBy}='{$value}'</t>
+  </si>
+  <si>
+    <t>select * from ole.PORTAL_USER where USER_TYP='{$userType}' and STS_CD='A' and uuid is not null  and TC_ACCEPT_IND='Y'
+order by PORTAL_USER_ID desc fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>select PT.PROV_TIN_NBR from OLE.PORTAL_USER P
+inner join OLE.PORTAL_USER_TIN PT on PT.PORTAL_USER_ID=P.PORTAL_USER_ID 
+where PT.ACCESS_LVL='A' and P.STS_CD = 'A' and PT.PROV_TIN_NBR not in ('')
+group by PT.PROV_TIN_NBR, PT.ACCESS_LVL
+having count(*)=1 limit 1</t>
+  </si>
+  <si>
+    <t>select * from ole.portal_user p inner join OLE.PORTAL_USER_TIN PT on PT.PORTAL_USER_ID=P.PORTAL_USER_ID
+where PT.PROV_TIN_NBR='{$tin}' and PT.ACCESS_LVL='A' and P.STS_CD = 'A'</t>
+  </si>
+  <si>
+    <t>select PT.PROV_TIN_NBR from OLE.PORTAL_USER P
+inner join OLE.PORTAL_USER_TIN PT on PT.PORTAL_USER_ID=P.PORTAL_USER_ID 
+where PT.ACCESS_LVL='A' and P.STS_CD = 'A' and PT.PROV_TIN_NBR not in ('')
+group by PT.PROV_TIN_NBR, PT.ACCESS_LVL
+having count(*)&gt;1 limit 1</t>
+  </si>
+  <si>
+    <t>252</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>256</t>
+  </si>
+  <si>
+    <t>Manage Users disabled tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User emulation </t>
+  </si>
+  <si>
+    <t>Tin with 1 active admin</t>
+  </si>
+  <si>
+    <t>Tin with more than 1 active admin</t>
+  </si>
 </sst>
 </file>
 
@@ -4294,7 +4346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4348,6 +4400,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4370,13 +4425,14 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="TestExecution"/>
       <sheetName val="Sheet2"/>
-      <sheetName val="TestExecution"/>
       <sheetName val="MasterCredentials"/>
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
         <row r="1">
           <cell r="A1" t="str">
             <v>Android</v>
@@ -4471,7 +4527,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
     </sheetDataSet>
@@ -5252,10 +5307,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D252"/>
+  <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="C253" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C257" sqref="C257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7741,6 +7796,61 @@
       </c>
       <c r="C252" t="s">
         <v>832</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A253" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="B253" s="31" t="s">
+        <v>835</v>
+      </c>
+      <c r="C253" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A254" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="B254" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="C254" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A255" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B255" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="C255" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A256" s="5" t="s">
+        <v>843</v>
+      </c>
+      <c r="B256" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="C256" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A257" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="B257" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="C257" t="s">
+        <v>848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manage users missed cases added
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CucumberFinal1\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HighAvalibility\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CC6AA5-1910-4B1E-84A8-45F19AB740DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B279E0-B6D5-4D5B-B644-872CFDE3EA82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="852">
   <si>
     <t>City</t>
   </si>
@@ -4187,6 +4187,24 @@
   </si>
   <si>
     <t>Tin with more than 1 active admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select t.PROV_TIN_NBR,t.PORTAL_USER_ID from OLE.PORTAL_USER_TIN t 
+join OLE.PORTAL_USER u 
+on t.PORTAL_USER_ID=u.PORTAL_USER_ID 
+join OLE.ENROLLED_PROVIDER e 
+on e.PROV_TIN_NBR=t.PROV_TIN_NBR                                                                                                                                               
+where u.SSO_ID='{$id}'
+and e.ENRL_STS_CD='A'
+and t.PROV_TIN_NBR not in (select t.PROV_TIN_NBR from OLE.PORTAL_USER_TIN t join 
+OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID where u.SSO_ID='{$activeUserID}') 
+</t>
+  </si>
+  <si>
+    <t>Adding tin for active user in manage users</t>
+  </si>
+  <si>
+    <t>257</t>
   </si>
 </sst>
 </file>
@@ -5307,10 +5325,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D257"/>
+  <dimension ref="A1:D258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C253" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C257" sqref="C257"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A258" sqref="A258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7851,6 +7869,17 @@
       </c>
       <c r="C257" t="s">
         <v>848</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+      <c r="A258" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="B258" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="C258" t="s">
+        <v>850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added cases for UPA Payer Purged user story _ US2711909
Added cases for UPA Payer Purged user story _ US2711909
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CucumberEditEnrollment\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnnCucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D895DF-2A3F-4CA6-B8D8-4720D07F5F19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AC5798-0A62-45CB-95BA-B970F9B10410}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="838">
   <si>
     <t>City</t>
   </si>
@@ -4041,19 +4041,6 @@
     <t>252</t>
   </si>
   <si>
-    <t>select * from 
-(SELECT DISTINCT pu.PORTAL_USER_ID ,pu.STS_CD, pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT , 
-CASE WHEN length(lower(pu.MIDDLE_INIT)) &gt; 0
-THEN
-trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) || ' ' || lower(pu.MIDDLE_INIT)) 
-ELSE trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) ) 
-END as FullName 
-FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
-ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID
-WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
-ORDER BY FullName asc)</t>
-  </si>
-  <si>
     <t>Getting All users associated with the payer including Purged</t>
   </si>
   <si>
@@ -4085,6 +4072,28 @@
 ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID 
 WHERE pt.PAYR_TIN_NBR in(select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
 and pu.STS_CD = 'PU'</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>select * from ole.PAYER p join OLE.PORTAL_USER_PAYER_TIN pt
+on p.PAYR_TIN_NBR=pt.PAYR_TIN_NBR join ole.PORTAL_USER pu
+on  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID 
+where pu.SSO_ID='{$id}'</t>
+  </si>
+  <si>
+    <t>select * from 
+(SELECT DISTINCT pu.PORTAL_USER_ID ,pu.STS_CD, pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT , 
+CASE WHEN length(lower(pu.MIDDLE_INIT)) &gt; 0
+THEN
+trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) || ' ' || lower(pu.MIDDLE_INIT)) 
+ELSE trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) ) 
+END as FullName 
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID
+WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}') and pu.USER_TYP='PA'
+ORDER BY FullName asc)</t>
   </si>
 </sst>
 </file>
@@ -5086,7 +5095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5112,7 +5121,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5198,10 +5207,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D255"/>
+  <dimension ref="A1:D256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B258" sqref="B258"/>
+    <sheetView tabSelected="1" topLeftCell="B253" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B253" sqref="B253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7670,29 +7679,37 @@
         <v>828</v>
       </c>
       <c r="B253" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="C253" t="s">
         <v>829</v>
-      </c>
-      <c r="C253" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="174" x14ac:dyDescent="0.35">
       <c r="A254" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="B254" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="C254" t="s">
         <v>831</v>
-      </c>
-      <c r="B254" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="C254" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A255" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B255" s="7" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A256" s="5" t="s">
         <v>835</v>
+      </c>
+      <c r="B256" s="7" t="s">
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -7981,7 +7998,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>216</v>
       </c>
@@ -8405,7 +8422,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="25" t="s">
         <v>310</v>
       </c>
@@ -8413,7 +8430,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="25" t="s">
         <v>312</v>
       </c>

</xml_diff>

<commit_message>
Purged US changes for Aug Release
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnnCucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrish38\Documents\GitCucumber\AugRelease\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AC5798-0A62-45CB-95BA-B970F9B10410}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28BA5FE-1ADC-478E-93CF-EA138A782255}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="843">
   <si>
     <t>City</t>
   </si>
@@ -4095,6 +4095,29 @@
 WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}') and pu.USER_TYP='PA'
 ORDER BY FullName asc)</t>
   </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER_HISTORY where USER_TYP='P' and STS_CD='PU' and MOD_TYP_CD='PUP'
+  order by LST_CHG_BY_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>SELECT pu.PORTAL_USER_ID,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.USER_TYP,pu.STS_CD,pu.LST_CHG_BY_DTTM,pu.LST_CHG_BY_ID,put.PROV_TIN_NBR
+FROM OLE.PORTAL_USER pu
+INNER JOIN OLE.PORTAL_USER_TIN put ON pu.PORTAL_USER_ID = put.PORTAL_USER_ID
+INNER JOIN OLE.PORTAL_USER_HISTORY puh ON pu.PORTAL_USER_ID = puh.PORTAL_USER_ID
+WHERE pu.STS_CD ='PU' AND pu.USER_TYP ='P' AND puh.MOD_TYP_CD='PUP'
+order by LST_CHG_BY_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>Purged User Tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select t.PROV_TIN_NBR  from OLE.PORTAL_USER_TIN t join 
+ OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID 
+ where u.SSO_ID='{$id}' and  u.STS_CD='PU'</t>
+  </si>
+  <si>
+    <t>Purge User Tin in dropdown</t>
+  </si>
 </sst>
 </file>
 
@@ -4253,7 +4276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4302,6 +4325,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5207,10 +5233,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D256"/>
+  <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B253" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B253" sqref="B253"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7710,6 +7736,36 @@
       </c>
       <c r="B256" s="7" t="s">
         <v>836</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A257">
+        <v>256</v>
+      </c>
+      <c r="B257" s="7" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A258">
+        <v>257</v>
+      </c>
+      <c r="B258" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="C258" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A259">
+        <v>258</v>
+      </c>
+      <c r="B259" s="29" t="s">
+        <v>841</v>
+      </c>
+      <c r="C259" t="s">
+        <v>842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushing Manage Users US2499639
Pushing Manage Users US2499639
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CucumberEditEnrollment\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manand10\Documents\megha back up\Documents\BackUp\Documents\EPS\InSprintAutomation\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D895DF-2A3F-4CA6-B8D8-4720D07F5F19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60C6AAB-3260-4A81-A85B-CD1782AE44C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="837">
   <si>
     <t>City</t>
   </si>
@@ -4085,6 +4085,13 @@
 ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID 
 WHERE pt.PAYR_TIN_NBR in(select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
 and pu.STS_CD = 'PU'</t>
+  </si>
+  <si>
+    <t>SELECT pu.PORTAL_USER_ID , pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT, pu.USERNAME,pu.LST_CHG_BY_ID,pu.LST_CHG_BY_DTTM 
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_BS_TIN bt 
+ON pu.PORTAL_USER_ID=bt.PORTAL_USER_ID JOIN OLE.BILLING_SERVICE bs
+ON bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
+WHERE  bs.IDENTIFIER_NBR='{$tin}' AND pu.STS_CD='PU'</t>
   </si>
 </sst>
 </file>
@@ -4749,22 +4756,22 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4793,7 +4800,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4822,7 +4829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4846,7 +4853,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -4875,7 +4882,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -4904,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -4930,7 +4937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -4956,7 +4963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -4982,7 +4989,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -5008,7 +5015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5034,7 +5041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -5060,7 +5067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -5086,7 +5093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5112,7 +5119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5138,7 +5145,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5164,7 +5171,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5198,20 +5205,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D255"/>
+  <dimension ref="A1:D257"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A254" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B258" sqref="B258"/>
+      <selection activeCell="B255" sqref="B255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="136.54296875" customWidth="1"/>
-    <col min="3" max="3" width="47.1796875" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="136.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5222,7 +5229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -5233,7 +5240,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -5244,7 +5251,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -5252,7 +5259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5263,7 +5270,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -5271,7 +5278,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -5279,7 +5286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -5287,7 +5294,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -5295,7 +5302,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5303,7 +5310,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -5311,7 +5318,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -5319,7 +5326,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5327,7 +5334,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5335,7 +5342,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5343,7 +5350,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5351,7 +5358,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -5359,7 +5366,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -5367,7 +5374,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -5375,7 +5382,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
@@ -5383,7 +5390,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -5391,7 +5398,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
@@ -5399,7 +5406,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
@@ -5407,7 +5414,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -5415,7 +5422,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>90</v>
       </c>
@@ -5423,7 +5430,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>91</v>
       </c>
@@ -5431,7 +5438,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>92</v>
       </c>
@@ -5439,7 +5446,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>93</v>
       </c>
@@ -5447,7 +5454,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>95</v>
       </c>
@@ -5455,7 +5462,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>96</v>
       </c>
@@ -5466,7 +5473,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>99</v>
       </c>
@@ -5477,7 +5484,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>102</v>
       </c>
@@ -5488,7 +5495,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>104</v>
       </c>
@@ -5499,7 +5506,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>108</v>
       </c>
@@ -5507,7 +5514,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>109</v>
       </c>
@@ -5515,7 +5522,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>114</v>
       </c>
@@ -5526,7 +5533,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>113</v>
       </c>
@@ -5537,7 +5544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>115</v>
       </c>
@@ -5545,7 +5552,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>118</v>
       </c>
@@ -5553,7 +5560,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>119</v>
       </c>
@@ -5561,7 +5568,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>122</v>
       </c>
@@ -5569,7 +5576,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>123</v>
       </c>
@@ -5583,7 +5590,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>125</v>
       </c>
@@ -5594,7 +5601,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>126</v>
       </c>
@@ -5605,7 +5612,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>127</v>
       </c>
@@ -5616,7 +5623,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>128</v>
       </c>
@@ -5627,7 +5634,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>129</v>
       </c>
@@ -5638,7 +5645,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>130</v>
       </c>
@@ -5649,7 +5656,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>131</v>
       </c>
@@ -5660,7 +5667,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>132</v>
       </c>
@@ -5671,7 +5678,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>133</v>
       </c>
@@ -5682,7 +5689,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>134</v>
       </c>
@@ -5693,7 +5700,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>135</v>
       </c>
@@ -5704,7 +5711,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>136</v>
       </c>
@@ -5712,7 +5719,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>138</v>
       </c>
@@ -5723,7 +5730,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>139</v>
       </c>
@@ -5731,7 +5738,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>145</v>
       </c>
@@ -5742,7 +5749,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>146</v>
       </c>
@@ -5750,7 +5757,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>150</v>
       </c>
@@ -5761,7 +5768,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>152</v>
       </c>
@@ -5772,7 +5779,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>153</v>
       </c>
@@ -5783,7 +5790,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>154</v>
       </c>
@@ -5794,7 +5801,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>155</v>
       </c>
@@ -5802,7 +5809,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>176</v>
       </c>
@@ -5813,7 +5820,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>177</v>
       </c>
@@ -5824,7 +5831,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>182</v>
       </c>
@@ -5832,7 +5839,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>183</v>
       </c>
@@ -5840,7 +5847,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>184</v>
       </c>
@@ -5848,7 +5855,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>185</v>
       </c>
@@ -5856,7 +5863,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>194</v>
       </c>
@@ -5867,7 +5874,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>197</v>
       </c>
@@ -5878,7 +5885,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>199</v>
       </c>
@@ -5886,7 +5893,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>280</v>
       </c>
@@ -5894,7 +5901,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>281</v>
       </c>
@@ -5902,7 +5909,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>284</v>
       </c>
@@ -5910,7 +5917,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>286</v>
       </c>
@@ -5918,7 +5925,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>358</v>
       </c>
@@ -5926,7 +5933,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>359</v>
       </c>
@@ -5934,7 +5941,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>360</v>
       </c>
@@ -5942,7 +5949,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>362</v>
       </c>
@@ -5950,7 +5957,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>363</v>
       </c>
@@ -5958,7 +5965,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>365</v>
       </c>
@@ -5966,7 +5973,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>367</v>
       </c>
@@ -5974,7 +5981,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>368</v>
       </c>
@@ -5982,7 +5989,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>369</v>
       </c>
@@ -5990,7 +5997,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>370</v>
       </c>
@@ -5998,7 +6005,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>372</v>
       </c>
@@ -6006,7 +6013,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>373</v>
       </c>
@@ -6014,7 +6021,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>375</v>
       </c>
@@ -6022,7 +6029,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>386</v>
       </c>
@@ -6030,7 +6037,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>387</v>
       </c>
@@ -6038,7 +6045,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>389</v>
       </c>
@@ -6046,7 +6053,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>392</v>
       </c>
@@ -6054,7 +6061,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>394</v>
       </c>
@@ -6062,7 +6069,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>396</v>
       </c>
@@ -6070,7 +6077,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>398</v>
       </c>
@@ -6078,7 +6085,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>399</v>
       </c>
@@ -6086,7 +6093,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>402</v>
       </c>
@@ -6094,7 +6101,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>407</v>
       </c>
@@ -6102,7 +6109,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>408</v>
       </c>
@@ -6110,7 +6117,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>409</v>
       </c>
@@ -6118,7 +6125,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>410</v>
       </c>
@@ -6126,7 +6133,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>411</v>
       </c>
@@ -6137,7 +6144,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>412</v>
       </c>
@@ -6148,7 +6155,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="232" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>414</v>
       </c>
@@ -6159,7 +6166,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>417</v>
       </c>
@@ -6167,7 +6174,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>419</v>
       </c>
@@ -6175,7 +6182,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>424</v>
       </c>
@@ -6183,7 +6190,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>426</v>
       </c>
@@ -6191,7 +6198,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>427</v>
       </c>
@@ -6199,7 +6206,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>428</v>
       </c>
@@ -6207,7 +6214,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>451</v>
       </c>
@@ -6218,7 +6225,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>452</v>
       </c>
@@ -6229,7 +6236,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>453</v>
       </c>
@@ -6240,7 +6247,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>454</v>
       </c>
@@ -6251,7 +6258,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>455</v>
       </c>
@@ -6262,7 +6269,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>456</v>
       </c>
@@ -6273,7 +6280,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>457</v>
       </c>
@@ -6284,7 +6291,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>458</v>
       </c>
@@ -6295,7 +6302,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>459</v>
       </c>
@@ -6306,7 +6313,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>460</v>
       </c>
@@ -6317,7 +6324,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>461</v>
       </c>
@@ -6328,7 +6335,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>462</v>
       </c>
@@ -6339,7 +6346,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>463</v>
       </c>
@@ -6350,7 +6357,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>465</v>
       </c>
@@ -6358,7 +6365,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>464</v>
       </c>
@@ -6366,7 +6373,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>467</v>
       </c>
@@ -6377,7 +6384,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>468</v>
       </c>
@@ -6388,7 +6395,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>470</v>
       </c>
@@ -6396,7 +6403,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>471</v>
       </c>
@@ -6407,7 +6414,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>476</v>
       </c>
@@ -6418,7 +6425,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>477</v>
       </c>
@@ -6429,7 +6436,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>482</v>
       </c>
@@ -6440,7 +6447,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>484</v>
       </c>
@@ -6451,7 +6458,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>485</v>
       </c>
@@ -6462,7 +6469,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>489</v>
       </c>
@@ -6473,7 +6480,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>493</v>
       </c>
@@ -6484,7 +6491,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>495</v>
       </c>
@@ -6495,7 +6502,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>496</v>
       </c>
@@ -6506,7 +6513,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>502</v>
       </c>
@@ -6517,7 +6524,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>505</v>
       </c>
@@ -6528,7 +6535,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>506</v>
       </c>
@@ -6539,7 +6546,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>514</v>
       </c>
@@ -6550,7 +6557,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>517</v>
       </c>
@@ -6561,7 +6568,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>518</v>
       </c>
@@ -6572,7 +6579,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>520</v>
       </c>
@@ -6583,7 +6590,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>523</v>
       </c>
@@ -6594,7 +6601,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>528</v>
       </c>
@@ -6605,7 +6612,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>551</v>
       </c>
@@ -6616,7 +6623,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>552</v>
       </c>
@@ -6627,7 +6634,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>553</v>
       </c>
@@ -6638,7 +6645,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>554</v>
       </c>
@@ -6649,7 +6656,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>555</v>
       </c>
@@ -6660,7 +6667,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>556</v>
       </c>
@@ -6671,7 +6678,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>558</v>
       </c>
@@ -6682,7 +6689,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>560</v>
       </c>
@@ -6693,7 +6700,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>564</v>
       </c>
@@ -6704,7 +6711,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>565</v>
       </c>
@@ -6715,7 +6722,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>573</v>
       </c>
@@ -6723,7 +6730,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>574</v>
       </c>
@@ -6734,7 +6741,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>578</v>
       </c>
@@ -6742,7 +6749,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>579</v>
       </c>
@@ -6750,7 +6757,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>582</v>
       </c>
@@ -6761,7 +6768,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>587</v>
       </c>
@@ -6769,7 +6776,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>588</v>
       </c>
@@ -6777,7 +6784,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>591</v>
       </c>
@@ -6788,7 +6795,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>592</v>
       </c>
@@ -6799,7 +6806,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>593</v>
       </c>
@@ -6807,7 +6814,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>594</v>
       </c>
@@ -6818,7 +6825,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>595</v>
       </c>
@@ -6826,7 +6833,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>596</v>
       </c>
@@ -6837,7 +6844,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>597</v>
       </c>
@@ -6848,7 +6855,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>598</v>
       </c>
@@ -6859,7 +6866,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>599</v>
       </c>
@@ -6870,7 +6877,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>600</v>
       </c>
@@ -6878,7 +6885,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>601</v>
       </c>
@@ -6889,7 +6896,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>602</v>
       </c>
@@ -6900,7 +6907,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>603</v>
       </c>
@@ -6911,7 +6918,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>604</v>
       </c>
@@ -6922,7 +6929,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>605</v>
       </c>
@@ -6933,7 +6940,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>606</v>
       </c>
@@ -6944,7 +6951,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>607</v>
       </c>
@@ -6955,7 +6962,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>608</v>
       </c>
@@ -6966,7 +6973,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>609</v>
       </c>
@@ -6977,7 +6984,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>610</v>
       </c>
@@ -6988,7 +6995,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>611</v>
       </c>
@@ -6999,7 +7006,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>612</v>
       </c>
@@ -7010,7 +7017,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>613</v>
       </c>
@@ -7021,7 +7028,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>614</v>
       </c>
@@ -7032,7 +7039,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>694</v>
       </c>
@@ -7043,7 +7050,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>695</v>
       </c>
@@ -7054,7 +7061,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>696</v>
       </c>
@@ -7065,7 +7072,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>697</v>
       </c>
@@ -7076,7 +7083,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
         <v>698</v>
       </c>
@@ -7087,7 +7094,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>699</v>
       </c>
@@ -7098,7 +7105,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>700</v>
       </c>
@@ -7109,7 +7116,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>701</v>
       </c>
@@ -7120,7 +7127,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>702</v>
       </c>
@@ -7131,7 +7138,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>703</v>
       </c>
@@ -7142,7 +7149,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
         <v>704</v>
       </c>
@@ -7153,7 +7160,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>705</v>
       </c>
@@ -7164,7 +7171,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>706</v>
       </c>
@@ -7175,7 +7182,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>707</v>
       </c>
@@ -7186,7 +7193,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>708</v>
       </c>
@@ -7194,7 +7201,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
         <v>709</v>
       </c>
@@ -7205,7 +7212,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>710</v>
       </c>
@@ -7216,7 +7223,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>711</v>
       </c>
@@ -7227,7 +7234,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>712</v>
       </c>
@@ -7238,7 +7245,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>713</v>
       </c>
@@ -7249,7 +7256,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
         <v>714</v>
       </c>
@@ -7260,7 +7267,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>715</v>
       </c>
@@ -7271,7 +7278,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
         <v>716</v>
       </c>
@@ -7282,7 +7289,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
         <v>717</v>
       </c>
@@ -7293,7 +7300,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>718</v>
       </c>
@@ -7304,7 +7311,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
         <v>719</v>
       </c>
@@ -7315,7 +7322,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>720</v>
       </c>
@@ -7326,7 +7333,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
         <v>721</v>
       </c>
@@ -7337,7 +7344,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -7348,7 +7355,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
         <v>722</v>
       </c>
@@ -7359,7 +7366,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="203" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
         <v>723</v>
       </c>
@@ -7370,7 +7377,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
         <v>724</v>
       </c>
@@ -7378,7 +7385,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
         <v>725</v>
       </c>
@@ -7386,7 +7393,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
         <v>726</v>
       </c>
@@ -7397,7 +7404,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
         <v>727</v>
       </c>
@@ -7408,7 +7415,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A225" s="5" t="s">
         <v>728</v>
       </c>
@@ -7419,17 +7426,17 @@
         <v>799</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>731</v>
       </c>
@@ -7437,7 +7444,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>732</v>
       </c>
@@ -7445,7 +7452,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>733</v>
       </c>
@@ -7453,7 +7460,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
         <v>734</v>
       </c>
@@ -7461,7 +7468,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>735</v>
       </c>
@@ -7472,7 +7479,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>736</v>
       </c>
@@ -7483,7 +7490,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>737</v>
       </c>
@@ -7491,7 +7498,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="5" t="s">
         <v>738</v>
       </c>
@@ -7502,7 +7509,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
         <v>739</v>
       </c>
@@ -7513,7 +7520,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
         <v>740</v>
       </c>
@@ -7524,7 +7531,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
         <v>741</v>
       </c>
@@ -7535,7 +7542,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>742</v>
       </c>
@@ -7546,7 +7553,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
         <v>743</v>
       </c>
@@ -7557,7 +7564,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
         <v>744</v>
       </c>
@@ -7568,7 +7575,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>810</v>
       </c>
@@ -7579,7 +7586,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>811</v>
       </c>
@@ -7590,7 +7597,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>812</v>
       </c>
@@ -7601,7 +7608,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>813</v>
       </c>
@@ -7609,7 +7616,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
         <v>815</v>
       </c>
@@ -7617,7 +7624,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
         <v>816</v>
       </c>
@@ -7625,7 +7632,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>818</v>
       </c>
@@ -7633,7 +7640,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
         <v>820</v>
       </c>
@@ -7641,7 +7648,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
         <v>822</v>
       </c>
@@ -7649,7 +7656,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
         <v>824</v>
       </c>
@@ -7657,7 +7664,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A252" s="5" t="s">
         <v>827</v>
       </c>
@@ -7665,7 +7672,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A253" s="5" t="s">
         <v>828</v>
       </c>
@@ -7676,7 +7683,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A254" s="5" t="s">
         <v>831</v>
       </c>
@@ -7687,12 +7694,25 @@
         <v>832</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
         <v>833</v>
       </c>
       <c r="B255" s="7" t="s">
         <v>835</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>256</v>
+      </c>
+      <c r="B257" s="7" t="s">
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -7709,16 +7729,16 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7738,7 +7758,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -7761,7 +7781,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -7784,7 +7804,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -7804,7 +7824,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -7818,7 +7838,7 @@
         <v>656565</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -7832,7 +7852,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -7855,7 +7875,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -7895,13 +7915,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>200</v>
       </c>
@@ -7909,7 +7929,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>202</v>
       </c>
@@ -7917,7 +7937,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>204</v>
       </c>
@@ -7925,55 +7945,55 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>206</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>208</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>211</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>212</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>213</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>214</v>
       </c>
@@ -7981,7 +8001,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>216</v>
       </c>
@@ -7989,7 +8009,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>218</v>
       </c>
@@ -7997,7 +8017,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>44</v>
       </c>
@@ -8005,7 +8025,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>221</v>
       </c>
@@ -8013,7 +8033,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>223</v>
       </c>
@@ -8021,7 +8041,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>225</v>
       </c>
@@ -8029,7 +8049,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>227</v>
       </c>
@@ -8037,7 +8057,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>229</v>
       </c>
@@ -8045,7 +8065,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>231</v>
       </c>
@@ -8053,7 +8073,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>233</v>
       </c>
@@ -8061,31 +8081,31 @@
         <v>234</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>238</v>
       </c>
@@ -8093,7 +8113,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>240</v>
       </c>
@@ -8101,7 +8121,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>242</v>
       </c>
@@ -8109,7 +8129,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>244</v>
       </c>
@@ -8117,7 +8137,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>245</v>
       </c>
@@ -8125,7 +8145,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>247</v>
       </c>
@@ -8133,7 +8153,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>249</v>
       </c>
@@ -8141,7 +8161,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>251</v>
       </c>
@@ -8149,7 +8169,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>252</v>
       </c>
@@ -8157,7 +8177,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>253</v>
       </c>
@@ -8165,7 +8185,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>255</v>
       </c>
@@ -8173,7 +8193,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>257</v>
       </c>
@@ -8181,7 +8201,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>259</v>
       </c>
@@ -8189,7 +8209,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>261</v>
       </c>
@@ -8197,7 +8217,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>263</v>
       </c>
@@ -8205,7 +8225,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>265</v>
       </c>
@@ -8213,7 +8233,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>267</v>
       </c>
@@ -8221,7 +8241,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
         <v>268</v>
       </c>
@@ -8229,7 +8249,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>269</v>
       </c>
@@ -8237,7 +8257,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>271</v>
       </c>
@@ -8245,7 +8265,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>272</v>
       </c>
@@ -8253,7 +8273,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>273</v>
       </c>
@@ -8261,7 +8281,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>275</v>
       </c>
@@ -8269,7 +8289,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>276</v>
       </c>
@@ -8277,7 +8297,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>278</v>
       </c>
@@ -8309,15 +8329,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="85.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="85.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>288</v>
       </c>
@@ -8325,7 +8347,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>290</v>
       </c>
@@ -8333,7 +8355,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>292</v>
       </c>
@@ -8341,7 +8363,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>294</v>
       </c>
@@ -8349,7 +8371,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>296</v>
       </c>
@@ -8357,7 +8379,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>298</v>
       </c>
@@ -8365,7 +8387,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>300</v>
       </c>
@@ -8373,7 +8395,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>302</v>
       </c>
@@ -8381,7 +8403,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>304</v>
       </c>
@@ -8389,7 +8411,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>306</v>
       </c>
@@ -8397,7 +8419,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>308</v>
       </c>
@@ -8405,7 +8427,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>310</v>
       </c>
@@ -8413,7 +8435,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>312</v>
       </c>
@@ -8421,7 +8443,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>314</v>
       </c>
@@ -8429,7 +8451,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>316</v>
       </c>
@@ -8437,7 +8459,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>318</v>
       </c>
@@ -8445,7 +8467,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
         <v>320</v>
       </c>
@@ -8453,7 +8475,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>322</v>
       </c>
@@ -8461,7 +8483,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>324</v>
       </c>
@@ -8469,7 +8491,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
         <v>326</v>
       </c>
@@ -8477,7 +8499,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>328</v>
       </c>
@@ -8485,7 +8507,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>330</v>
       </c>
@@ -8493,7 +8515,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
         <v>332</v>
       </c>
@@ -8501,7 +8523,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>334</v>
       </c>
@@ -8509,7 +8531,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
         <v>336</v>
       </c>
@@ -8517,7 +8539,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
         <v>338</v>
       </c>
@@ -8525,7 +8547,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
         <v>340</v>
       </c>
@@ -8533,7 +8555,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
         <v>342</v>
       </c>
@@ -8541,7 +8563,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
         <v>344</v>
       </c>
@@ -8549,7 +8571,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>346</v>
       </c>
@@ -8557,7 +8579,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>348</v>
       </c>
@@ -8565,7 +8587,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>350</v>
       </c>
@@ -8573,7 +8595,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>352</v>
       </c>
@@ -8581,7 +8603,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>354</v>
       </c>
@@ -8589,7 +8611,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
         <v>356</v>
       </c>

</xml_diff>

<commit_message>
appending rahuls changes for august release
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnnCucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3723F72D-C321-4794-A676-999C9416E6E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3C41F0-1D21-4FDB-9F7B-86A22B027FD2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="889">
   <si>
     <t>City</t>
   </si>
@@ -4315,6 +4315,38 @@
   <si>
     <t>select * from ole.portal_user_history where portal_user_id ='{$portalUserID}' and sts_cd='PU' fetch first row only</t>
   </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER_HISTORY where USER_TYP='P' and STS_CD='PU' and MOD_TYP_CD='PUP'
+  order by LST_CHG_BY_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>SELECT pu.PORTAL_USER_ID,pu.EMAIL_ADR_TXT,pu.FST_NM,pu.LST_NM,pu.USER_TYP,pu.STS_CD,pu.LST_CHG_BY_DTTM,pu.LST_CHG_BY_ID,put.PROV_TIN_NBR
+FROM OLE.PORTAL_USER pu
+INNER JOIN OLE.PORTAL_USER_TIN put ON pu.PORTAL_USER_ID = put.PORTAL_USER_ID
+INNER JOIN OLE.PORTAL_USER_HISTORY puh ON pu.PORTAL_USER_ID = puh.PORTAL_USER_ID
+WHERE pu.STS_CD ='PU' AND pu.USER_TYP ='P' AND puh.MOD_TYP_CD='PUP'
+order by LST_CHG_BY_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>Purged User Tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select t.PROV_TIN_NBR  from OLE.PORTAL_USER_TIN t join 
+ OLE.PORTAL_USER u on t.PORTAL_USER_ID=u.PORTAL_USER_ID 
+ where u.SSO_ID='{$id}' and  u.STS_CD='PU'</t>
+  </si>
+  <si>
+    <t>Purge User Tin in dropdown</t>
+  </si>
+  <si>
+    <t>269</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>271</t>
+  </si>
 </sst>
 </file>
 
@@ -4473,7 +4505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4528,6 +4560,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5434,10 +5469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D269"/>
+  <dimension ref="A1:D272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B270" sqref="B270"/>
+    <sheetView tabSelected="1" topLeftCell="A267" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B271" sqref="B271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8098,6 +8133,36 @@
       </c>
       <c r="B269" s="7" t="s">
         <v>880</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A270" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="B270" s="7" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A271" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="B271" s="7" t="s">
+        <v>882</v>
+      </c>
+      <c r="C271" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A272" s="5" t="s">
+        <v>888</v>
+      </c>
+      <c r="B272" s="32" t="s">
+        <v>884</v>
+      </c>
+      <c r="C272" t="s">
+        <v>885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data file from athyusha
updated data file from athyusha
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HighAvalibility\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkasula\git\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B279E0-B6D5-4D5B-B644-872CFDE3EA82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791689E9-D663-4005-8396-84FDB307B880}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Login" sheetId="6" r:id="rId3"/>
     <sheet name="TestExecution" sheetId="7" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
+    <sheet name="Automation Tag List" sheetId="9" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Platform">[1]Sheet2!$A$1:$A$11</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="861">
   <si>
     <t>City</t>
   </si>
@@ -4205,6 +4206,36 @@
   </si>
   <si>
     <t>257</t>
+  </si>
+  <si>
+    <t>Tag Names</t>
+  </si>
+  <si>
+    <t>User Story No</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>@UPARegression @UPAActivateAccount @FeatureLevel</t>
+  </si>
+  <si>
+    <t>US2707371</t>
+  </si>
+  <si>
+    <t>Verify the changes done in Activate Account page</t>
+  </si>
+  <si>
+    <t>gets details from portal user history table based on the email</t>
+  </si>
+  <si>
+    <t>Select PORTAL_USER_HISTORY_ID,FST_NM,SSO_ID,UUID,TEL_NBR,TXT_ALERT_IND,LST_SPLASH_IND,LST_SPLASH_ID from OLE.PORTAL_USER_HISTORY p where p.EMAIL_ADR_TXT='{$email}' order by lst_chg_by_dttm desc</t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p join
+OLE.PORTAL_USER_PAYER_TIN py 
+on p.PORTAL_USER_ID=py.PORTAL_USER_ID 
+where  py.PAYR_TIN_NBR=(select PAYR_TIN_NBR FROM OLE.PAYER WHERE PAYR_NM ='{$tin}') and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
   </si>
 </sst>
 </file>
@@ -4879,19 +4910,19 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4920,7 +4951,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4949,7 +4980,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -4973,7 +5004,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -5002,7 +5033,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5031,7 +5062,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -5057,7 +5088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -5083,7 +5114,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -5109,7 +5140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -5135,7 +5166,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5161,7 +5192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -5187,7 +5218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -5213,7 +5244,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5239,7 +5270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5265,7 +5296,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5291,7 +5322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5325,20 +5356,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D258"/>
+  <dimension ref="A1:D260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A258" sqref="A258"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B260" sqref="B260"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="136.54296875" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="136.5546875" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5349,7 +5380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -5360,7 +5391,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -5371,7 +5402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -5379,7 +5410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5390,7 +5421,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -5398,7 +5429,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -5406,7 +5437,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -5414,7 +5445,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -5422,7 +5453,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5430,7 +5461,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -5438,7 +5469,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -5446,7 +5477,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5454,7 +5485,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5462,7 +5493,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5470,7 +5501,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5478,7 +5509,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -5486,7 +5517,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -5494,7 +5525,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -5502,7 +5533,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
@@ -5510,7 +5541,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -5518,7 +5549,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
@@ -5526,7 +5557,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
@@ -5534,7 +5565,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -5542,7 +5573,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>91</v>
       </c>
@@ -5550,7 +5581,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>92</v>
       </c>
@@ -5558,7 +5589,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
@@ -5566,7 +5597,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>94</v>
       </c>
@@ -5574,7 +5605,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>96</v>
       </c>
@@ -5582,7 +5613,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>97</v>
       </c>
@@ -5593,7 +5624,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -5604,7 +5635,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
@@ -5615,7 +5646,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -5626,7 +5657,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>109</v>
       </c>
@@ -5634,7 +5665,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>110</v>
       </c>
@@ -5642,7 +5673,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
@@ -5653,7 +5684,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>114</v>
       </c>
@@ -5664,7 +5695,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
@@ -5672,7 +5703,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>119</v>
       </c>
@@ -5680,7 +5711,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>120</v>
       </c>
@@ -5688,7 +5719,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>123</v>
       </c>
@@ -5696,7 +5727,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>124</v>
       </c>
@@ -5710,7 +5741,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>126</v>
       </c>
@@ -5721,7 +5752,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>127</v>
       </c>
@@ -5732,7 +5763,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -5743,7 +5774,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -5754,7 +5785,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>130</v>
       </c>
@@ -5765,7 +5796,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>131</v>
       </c>
@@ -5776,7 +5807,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>132</v>
       </c>
@@ -5787,7 +5818,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>133</v>
       </c>
@@ -5798,7 +5829,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>134</v>
       </c>
@@ -5809,7 +5840,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>135</v>
       </c>
@@ -5820,7 +5851,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>136</v>
       </c>
@@ -5831,7 +5862,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>137</v>
       </c>
@@ -5839,7 +5870,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>139</v>
       </c>
@@ -5850,7 +5881,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>140</v>
       </c>
@@ -5858,7 +5889,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>146</v>
       </c>
@@ -5869,7 +5900,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>147</v>
       </c>
@@ -5877,7 +5908,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>151</v>
       </c>
@@ -5888,7 +5919,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>153</v>
       </c>
@@ -5899,7 +5930,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>154</v>
       </c>
@@ -5910,7 +5941,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>155</v>
       </c>
@@ -5921,7 +5952,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>156</v>
       </c>
@@ -5929,7 +5960,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>175</v>
       </c>
@@ -5940,7 +5971,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>176</v>
       </c>
@@ -5951,7 +5982,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>181</v>
       </c>
@@ -5959,7 +5990,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>182</v>
       </c>
@@ -5967,7 +5998,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>183</v>
       </c>
@@ -5975,7 +6006,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>184</v>
       </c>
@@ -5983,7 +6014,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>192</v>
       </c>
@@ -5994,7 +6025,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="232" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>195</v>
       </c>
@@ -6005,7 +6036,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>196</v>
       </c>
@@ -6013,7 +6044,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>277</v>
       </c>
@@ -6021,7 +6052,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>278</v>
       </c>
@@ -6029,7 +6060,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>281</v>
       </c>
@@ -6037,7 +6068,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>283</v>
       </c>
@@ -6045,7 +6076,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>355</v>
       </c>
@@ -6053,7 +6084,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>356</v>
       </c>
@@ -6061,7 +6092,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>357</v>
       </c>
@@ -6069,7 +6100,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>359</v>
       </c>
@@ -6077,7 +6108,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>360</v>
       </c>
@@ -6085,7 +6116,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>362</v>
       </c>
@@ -6093,7 +6124,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>364</v>
       </c>
@@ -6101,7 +6132,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>365</v>
       </c>
@@ -6109,7 +6140,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>366</v>
       </c>
@@ -6117,7 +6148,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>367</v>
       </c>
@@ -6125,7 +6156,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>369</v>
       </c>
@@ -6133,7 +6164,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>370</v>
       </c>
@@ -6141,7 +6172,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>372</v>
       </c>
@@ -6149,7 +6180,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>383</v>
       </c>
@@ -6157,7 +6188,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>384</v>
       </c>
@@ -6165,7 +6196,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>386</v>
       </c>
@@ -6173,7 +6204,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>389</v>
       </c>
@@ -6181,7 +6212,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>391</v>
       </c>
@@ -6189,7 +6220,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>393</v>
       </c>
@@ -6197,7 +6228,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>395</v>
       </c>
@@ -6205,7 +6236,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>396</v>
       </c>
@@ -6213,7 +6244,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>399</v>
       </c>
@@ -6221,7 +6252,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>404</v>
       </c>
@@ -6229,7 +6260,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>405</v>
       </c>
@@ -6237,7 +6268,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>406</v>
       </c>
@@ -6245,7 +6276,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>407</v>
       </c>
@@ -6253,7 +6284,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>408</v>
       </c>
@@ -6264,7 +6295,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>409</v>
       </c>
@@ -6275,7 +6306,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="232" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>411</v>
       </c>
@@ -6286,7 +6317,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>414</v>
       </c>
@@ -6294,7 +6325,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>416</v>
       </c>
@@ -6302,7 +6333,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>421</v>
       </c>
@@ -6310,7 +6341,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>423</v>
       </c>
@@ -6318,7 +6349,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>424</v>
       </c>
@@ -6326,7 +6357,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>425</v>
       </c>
@@ -6334,7 +6365,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>448</v>
       </c>
@@ -6345,7 +6376,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>449</v>
       </c>
@@ -6356,7 +6387,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>450</v>
       </c>
@@ -6367,7 +6398,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>451</v>
       </c>
@@ -6378,7 +6409,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>452</v>
       </c>
@@ -6389,7 +6420,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>453</v>
       </c>
@@ -6400,7 +6431,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>454</v>
       </c>
@@ -6411,7 +6442,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>455</v>
       </c>
@@ -6422,7 +6453,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>456</v>
       </c>
@@ -6433,7 +6464,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>457</v>
       </c>
@@ -6444,7 +6475,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>458</v>
       </c>
@@ -6455,7 +6486,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>459</v>
       </c>
@@ -6466,7 +6497,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>460</v>
       </c>
@@ -6477,7 +6508,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>462</v>
       </c>
@@ -6485,7 +6516,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>461</v>
       </c>
@@ -6493,7 +6524,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>464</v>
       </c>
@@ -6504,7 +6535,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>465</v>
       </c>
@@ -6515,7 +6546,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>467</v>
       </c>
@@ -6523,7 +6554,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>468</v>
       </c>
@@ -6534,7 +6565,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>472</v>
       </c>
@@ -6545,7 +6576,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>473</v>
       </c>
@@ -6556,7 +6587,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>476</v>
       </c>
@@ -6567,7 +6598,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>478</v>
       </c>
@@ -6578,7 +6609,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>479</v>
       </c>
@@ -6589,7 +6620,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>482</v>
       </c>
@@ -6600,7 +6631,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>484</v>
       </c>
@@ -6611,7 +6642,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>486</v>
       </c>
@@ -6622,7 +6653,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>487</v>
       </c>
@@ -6633,7 +6664,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>490</v>
       </c>
@@ -6644,7 +6675,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>492</v>
       </c>
@@ -6655,7 +6686,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>493</v>
       </c>
@@ -6666,7 +6697,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>499</v>
       </c>
@@ -6677,7 +6708,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>502</v>
       </c>
@@ -6688,7 +6719,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>503</v>
       </c>
@@ -6699,7 +6730,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>505</v>
       </c>
@@ -6710,7 +6741,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>508</v>
       </c>
@@ -6721,7 +6752,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>509</v>
       </c>
@@ -6732,7 +6763,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>529</v>
       </c>
@@ -6743,7 +6774,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>530</v>
       </c>
@@ -6754,7 +6785,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>531</v>
       </c>
@@ -6765,7 +6796,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>532</v>
       </c>
@@ -6776,7 +6807,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>533</v>
       </c>
@@ -6787,7 +6818,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>534</v>
       </c>
@@ -6798,7 +6829,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>536</v>
       </c>
@@ -6809,7 +6840,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>538</v>
       </c>
@@ -6820,7 +6851,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>542</v>
       </c>
@@ -6831,7 +6862,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>543</v>
       </c>
@@ -6842,7 +6873,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>548</v>
       </c>
@@ -6850,7 +6881,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>549</v>
       </c>
@@ -6861,7 +6892,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>553</v>
       </c>
@@ -6869,7 +6900,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>554</v>
       </c>
@@ -6877,7 +6908,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>557</v>
       </c>
@@ -6888,7 +6919,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>562</v>
       </c>
@@ -6896,7 +6927,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>563</v>
       </c>
@@ -6904,7 +6935,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>566</v>
       </c>
@@ -6915,7 +6946,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>567</v>
       </c>
@@ -6926,7 +6957,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>568</v>
       </c>
@@ -6934,7 +6965,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>569</v>
       </c>
@@ -6945,7 +6976,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>570</v>
       </c>
@@ -6953,7 +6984,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>571</v>
       </c>
@@ -6964,7 +6995,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>572</v>
       </c>
@@ -6975,7 +7006,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>573</v>
       </c>
@@ -6986,7 +7017,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>574</v>
       </c>
@@ -6997,7 +7028,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>575</v>
       </c>
@@ -7005,7 +7036,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>576</v>
       </c>
@@ -7016,7 +7047,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>577</v>
       </c>
@@ -7027,7 +7058,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>578</v>
       </c>
@@ -7038,7 +7069,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>579</v>
       </c>
@@ -7049,7 +7080,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>580</v>
       </c>
@@ -7060,7 +7091,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>581</v>
       </c>
@@ -7071,7 +7102,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>582</v>
       </c>
@@ -7082,7 +7113,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>583</v>
       </c>
@@ -7093,7 +7124,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>584</v>
       </c>
@@ -7104,7 +7135,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>585</v>
       </c>
@@ -7115,7 +7146,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>586</v>
       </c>
@@ -7126,7 +7157,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>587</v>
       </c>
@@ -7137,7 +7168,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>588</v>
       </c>
@@ -7148,7 +7179,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>589</v>
       </c>
@@ -7159,7 +7190,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>669</v>
       </c>
@@ -7170,7 +7201,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>670</v>
       </c>
@@ -7181,7 +7212,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>671</v>
       </c>
@@ -7192,7 +7223,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>672</v>
       </c>
@@ -7203,7 +7234,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
         <v>673</v>
       </c>
@@ -7214,7 +7245,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>674</v>
       </c>
@@ -7225,7 +7256,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>675</v>
       </c>
@@ -7236,7 +7267,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>676</v>
       </c>
@@ -7247,7 +7278,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>677</v>
       </c>
@@ -7258,7 +7289,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>678</v>
       </c>
@@ -7269,7 +7300,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
         <v>679</v>
       </c>
@@ -7280,7 +7311,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>680</v>
       </c>
@@ -7291,7 +7322,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>681</v>
       </c>
@@ -7302,7 +7333,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>682</v>
       </c>
@@ -7313,7 +7344,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>683</v>
       </c>
@@ -7321,7 +7352,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
         <v>684</v>
       </c>
@@ -7332,7 +7363,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>685</v>
       </c>
@@ -7343,7 +7374,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>686</v>
       </c>
@@ -7354,7 +7385,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>687</v>
       </c>
@@ -7365,7 +7396,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>688</v>
       </c>
@@ -7376,7 +7407,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
         <v>689</v>
       </c>
@@ -7387,7 +7418,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>690</v>
       </c>
@@ -7398,7 +7429,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
         <v>691</v>
       </c>
@@ -7409,7 +7440,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
         <v>692</v>
       </c>
@@ -7420,7 +7451,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>693</v>
       </c>
@@ -7431,7 +7462,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
         <v>694</v>
       </c>
@@ -7442,7 +7473,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>695</v>
       </c>
@@ -7453,7 +7484,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
         <v>696</v>
       </c>
@@ -7464,7 +7495,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -7475,7 +7506,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
         <v>697</v>
       </c>
@@ -7486,7 +7517,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="203" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
         <v>698</v>
       </c>
@@ -7497,7 +7528,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
         <v>699</v>
       </c>
@@ -7505,7 +7536,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
         <v>700</v>
       </c>
@@ -7513,7 +7544,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
         <v>701</v>
       </c>
@@ -7524,7 +7555,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
         <v>702</v>
       </c>
@@ -7535,7 +7566,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A225" s="5" t="s">
         <v>703</v>
       </c>
@@ -7546,17 +7577,17 @@
         <v>774</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>706</v>
       </c>
@@ -7564,7 +7595,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>707</v>
       </c>
@@ -7572,7 +7603,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>708</v>
       </c>
@@ -7580,7 +7611,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
         <v>709</v>
       </c>
@@ -7588,7 +7619,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>710</v>
       </c>
@@ -7599,7 +7630,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>711</v>
       </c>
@@ -7610,7 +7641,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>712</v>
       </c>
@@ -7618,7 +7649,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="5" t="s">
         <v>713</v>
       </c>
@@ -7629,7 +7660,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
         <v>714</v>
       </c>
@@ -7640,7 +7671,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
         <v>715</v>
       </c>
@@ -7651,7 +7682,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
         <v>716</v>
       </c>
@@ -7662,7 +7693,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>717</v>
       </c>
@@ -7673,7 +7704,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
         <v>718</v>
       </c>
@@ -7684,7 +7715,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
         <v>719</v>
       </c>
@@ -7695,7 +7726,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>787</v>
       </c>
@@ -7706,7 +7737,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>788</v>
       </c>
@@ -7717,7 +7748,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>789</v>
       </c>
@@ -7728,7 +7759,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>791</v>
       </c>
@@ -7739,7 +7770,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
         <v>796</v>
       </c>
@@ -7750,7 +7781,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
         <v>801</v>
       </c>
@@ -7761,7 +7792,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>804</v>
       </c>
@@ -7772,7 +7803,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
         <v>807</v>
       </c>
@@ -7783,7 +7814,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
         <v>827</v>
       </c>
@@ -7794,7 +7825,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
         <v>830</v>
       </c>
@@ -7805,7 +7836,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A252" s="5" t="s">
         <v>833</v>
       </c>
@@ -7816,7 +7847,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="5" t="s">
         <v>840</v>
       </c>
@@ -7827,7 +7858,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A254" s="5" t="s">
         <v>841</v>
       </c>
@@ -7838,7 +7869,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
         <v>842</v>
       </c>
@@ -7849,7 +7880,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A256" s="5" t="s">
         <v>843</v>
       </c>
@@ -7860,7 +7891,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A257" s="5" t="s">
         <v>844</v>
       </c>
@@ -7871,7 +7902,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="145" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A258" s="5" t="s">
         <v>851</v>
       </c>
@@ -7880,6 +7911,25 @@
       </c>
       <c r="C258" t="s">
         <v>850</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A259" s="5">
+        <v>258</v>
+      </c>
+      <c r="B259" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="C259" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A260" s="5">
+        <v>259</v>
+      </c>
+      <c r="B260" s="7" t="s">
+        <v>860</v>
       </c>
     </row>
   </sheetData>
@@ -7896,16 +7946,16 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7925,7 +7975,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -7948,7 +7998,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -7971,7 +8021,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -7991,7 +8041,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -8005,7 +8055,7 @@
         <v>656565</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -8019,7 +8069,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -8042,7 +8092,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -8082,13 +8132,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>197</v>
       </c>
@@ -8096,7 +8146,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>199</v>
       </c>
@@ -8104,7 +8154,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>201</v>
       </c>
@@ -8112,55 +8162,55 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>203</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>205</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>206</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>208</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>211</v>
       </c>
@@ -8168,7 +8218,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>213</v>
       </c>
@@ -8176,7 +8226,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>215</v>
       </c>
@@ -8184,7 +8234,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>44</v>
       </c>
@@ -8192,7 +8242,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>218</v>
       </c>
@@ -8200,7 +8250,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>220</v>
       </c>
@@ -8208,7 +8258,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>222</v>
       </c>
@@ -8216,7 +8266,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>224</v>
       </c>
@@ -8224,7 +8274,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>226</v>
       </c>
@@ -8232,7 +8282,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>228</v>
       </c>
@@ -8240,7 +8290,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>230</v>
       </c>
@@ -8248,31 +8298,31 @@
         <v>231</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>235</v>
       </c>
@@ -8280,7 +8330,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>237</v>
       </c>
@@ -8288,7 +8338,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>239</v>
       </c>
@@ -8296,7 +8346,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>241</v>
       </c>
@@ -8304,7 +8354,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>242</v>
       </c>
@@ -8312,7 +8362,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>244</v>
       </c>
@@ -8320,7 +8370,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>246</v>
       </c>
@@ -8328,7 +8378,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>248</v>
       </c>
@@ -8336,7 +8386,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>249</v>
       </c>
@@ -8344,7 +8394,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>250</v>
       </c>
@@ -8352,7 +8402,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>252</v>
       </c>
@@ -8360,7 +8410,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>254</v>
       </c>
@@ -8368,7 +8418,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>256</v>
       </c>
@@ -8376,7 +8426,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>258</v>
       </c>
@@ -8384,7 +8434,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>260</v>
       </c>
@@ -8392,7 +8442,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>262</v>
       </c>
@@ -8400,7 +8450,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>264</v>
       </c>
@@ -8408,7 +8458,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
         <v>265</v>
       </c>
@@ -8416,7 +8466,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>266</v>
       </c>
@@ -8424,7 +8474,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>268</v>
       </c>
@@ -8432,7 +8482,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>269</v>
       </c>
@@ -8440,7 +8490,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>270</v>
       </c>
@@ -8448,7 +8498,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>272</v>
       </c>
@@ -8456,7 +8506,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>273</v>
       </c>
@@ -8464,7 +8514,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>275</v>
       </c>
@@ -8498,13 +8548,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="85.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="85.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>285</v>
       </c>
@@ -8512,7 +8562,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>287</v>
       </c>
@@ -8520,7 +8570,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>289</v>
       </c>
@@ -8528,7 +8578,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>291</v>
       </c>
@@ -8536,7 +8586,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>293</v>
       </c>
@@ -8544,7 +8594,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>295</v>
       </c>
@@ -8552,7 +8602,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>297</v>
       </c>
@@ -8560,7 +8610,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>299</v>
       </c>
@@ -8568,7 +8618,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>301</v>
       </c>
@@ -8576,7 +8626,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>303</v>
       </c>
@@ -8584,7 +8634,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>305</v>
       </c>
@@ -8592,7 +8642,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>307</v>
       </c>
@@ -8600,7 +8650,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>309</v>
       </c>
@@ -8608,7 +8658,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>311</v>
       </c>
@@ -8616,7 +8666,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>313</v>
       </c>
@@ -8624,7 +8674,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>315</v>
       </c>
@@ -8632,7 +8682,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
         <v>317</v>
       </c>
@@ -8640,7 +8690,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>319</v>
       </c>
@@ -8648,7 +8698,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>321</v>
       </c>
@@ -8656,7 +8706,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
         <v>323</v>
       </c>
@@ -8664,7 +8714,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>325</v>
       </c>
@@ -8672,7 +8722,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>327</v>
       </c>
@@ -8680,7 +8730,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
         <v>329</v>
       </c>
@@ -8688,7 +8738,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>331</v>
       </c>
@@ -8696,7 +8746,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
         <v>333</v>
       </c>
@@ -8704,7 +8754,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
         <v>335</v>
       </c>
@@ -8712,7 +8762,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
         <v>337</v>
       </c>
@@ -8720,7 +8770,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
         <v>339</v>
       </c>
@@ -8728,7 +8778,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
         <v>341</v>
       </c>
@@ -8736,7 +8786,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>343</v>
       </c>
@@ -8744,7 +8794,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>345</v>
       </c>
@@ -8752,7 +8802,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>347</v>
       </c>
@@ -8760,7 +8810,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>349</v>
       </c>
@@ -8768,7 +8818,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>351</v>
       </c>
@@ -8776,7 +8826,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
         <v>353</v>
       </c>
@@ -8788,4 +8838,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16592FEF-48E9-415D-9DDC-007B8657F147}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B2" t="s">
+        <v>856</v>
+      </c>
+      <c r="C2" t="s">
+        <v>857</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rahul's data file changes for abn validator
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkasula\git\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrish38\Documents\GitCucumber\ABNMasterMerge\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791689E9-D663-4005-8396-84FDB307B880}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73FAD2B-2CE6-43F6-99CE-0C0C548BB411}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,9 @@
     <sheet name="Login" sheetId="6" r:id="rId3"/>
     <sheet name="TestExecution" sheetId="7" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
-    <sheet name="Automation Tag List" sheetId="9" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="Platform">[1]Sheet2!$A$1:$A$11</definedName>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="876">
   <si>
     <t>City</t>
   </si>
@@ -4208,41 +4207,86 @@
     <t>257</t>
   </si>
   <si>
-    <t>Tag Names</t>
-  </si>
-  <si>
-    <t>User Story No</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>@UPARegression @UPAActivateAccount @FeatureLevel</t>
-  </si>
-  <si>
-    <t>US2707371</t>
-  </si>
-  <si>
-    <t>Verify the changes done in Activate Account page</t>
+    <t>select * from OLE.SYSTEM_CONFIGURATION WHERE proc_cd='ABA_API' and proc_tag_desc='CALL_ABA_API'</t>
+  </si>
+  <si>
+    <t>107004776</t>
+  </si>
+  <si>
+    <t>ValidRoutingNos</t>
+  </si>
+  <si>
+    <t>ValidAddr</t>
+  </si>
+  <si>
+    <t>ValidAddr2</t>
+  </si>
+  <si>
+    <t>COMPASS BANK</t>
+  </si>
+  <si>
+    <t>GUARANTY BANK AND TRUST CO</t>
+  </si>
+  <si>
+    <t>PO BOX 10566</t>
+  </si>
+  <si>
+    <t>P O BOX 5847</t>
+  </si>
+  <si>
+    <t>102000021</t>
+  </si>
+  <si>
+    <t>BIRMINGHAM, AL 35296-0000</t>
+  </si>
+  <si>
+    <t>DENVER, CO 80217-5847</t>
+  </si>
+  <si>
+    <t>111000614</t>
+  </si>
+  <si>
+    <t>061000104</t>
+  </si>
+  <si>
+    <t>205-297-6866</t>
+  </si>
+  <si>
+    <t>303-293-5499</t>
+  </si>
+  <si>
+    <t>121000248</t>
+  </si>
+  <si>
+    <t>071921891</t>
+  </si>
+  <si>
+    <t>074908594</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>Select PORTAL_USER_HISTORY_ID,FST_NM,SSO_ID,UUID,TEL_NBR,TXT_ALERT_IND,LST_SPLASH_IND,LST_SPLASH_ID from OLE.PORTAL_USER_HISTORY p where p.EMAIL_ADR_TXT='{$email}' order by lst_chg_by_dttm desc</t>
   </si>
   <si>
     <t>gets details from portal user history table based on the email</t>
-  </si>
-  <si>
-    <t>Select PORTAL_USER_HISTORY_ID,FST_NM,SSO_ID,UUID,TEL_NBR,TXT_ALERT_IND,LST_SPLASH_IND,LST_SPLASH_ID from OLE.PORTAL_USER_HISTORY p where p.EMAIL_ADR_TXT='{$email}' order by lst_chg_by_dttm desc</t>
   </si>
   <si>
     <t>select * from OLE.PORTAL_USER p join
 OLE.PORTAL_USER_PAYER_TIN py 
 on p.PORTAL_USER_ID=py.PORTAL_USER_ID 
 where  py.PAYR_TIN_NBR=(select PAYR_TIN_NBR FROM OLE.PAYER WHERE PAYR_NM ='{$tin}') and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>ABA Validator Switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4315,6 +4359,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Frutiger"/>
     </font>
   </fonts>
   <fills count="5">
@@ -4395,7 +4445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4451,6 +4501,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4904,25 +4960,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
-    <col min="8" max="8" width="26.77734375" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="10" max="10" width="15.08984375" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4950,8 +5009,17 @@
       <c r="I1" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4979,8 +5047,17 @@
       <c r="I2" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>857</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -5003,8 +5080,17 @@
         <v>39</v>
       </c>
       <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="4" t="s">
+        <v>853</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>859</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -5032,8 +5118,17 @@
       <c r="I4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="4" t="s">
+        <v>861</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>862</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5061,8 +5156,13 @@
       <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="4" t="s">
+        <v>864</v>
+      </c>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -5087,8 +5187,17 @@
       <c r="H6" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="K6" s="32" t="s">
+        <v>866</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -5113,8 +5222,11 @@
       <c r="H7" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="4" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -5139,8 +5251,11 @@
       <c r="H8" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="4" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -5165,8 +5280,11 @@
       <c r="H9" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="4" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5192,7 +5310,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -5218,7 +5336,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -5244,7 +5362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5270,7 +5388,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5296,7 +5414,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5322,7 +5440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5345,6 +5463,32 @@
         <v>26</v>
       </c>
       <c r="H16" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>853</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -5356,20 +5500,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D260"/>
+  <dimension ref="A1:D261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A257" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B260" sqref="B260"/>
+    <sheetView tabSelected="1" topLeftCell="A258" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D260" sqref="D260"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="136.5546875" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="136.54296875" customWidth="1"/>
+    <col min="3" max="3" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5380,7 +5524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -5391,7 +5535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -5402,7 +5546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="58">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -5410,7 +5554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="29">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -5421,7 +5565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -5429,7 +5573,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -5437,7 +5581,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -5445,7 +5589,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="29">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -5453,7 +5597,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="87">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5461,7 +5605,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="72.5">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -5469,7 +5613,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.5">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -5477,7 +5621,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="58">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -5485,7 +5629,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -5493,7 +5637,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="58">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -5501,7 +5645,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="29">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -5509,7 +5653,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -5517,7 +5661,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -5525,7 +5669,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="87">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -5533,7 +5677,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="72.5">
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
@@ -5541,7 +5685,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="29">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -5549,7 +5693,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
@@ -5557,7 +5701,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="29">
       <c r="A23" s="5" t="s">
         <v>88</v>
       </c>
@@ -5565,7 +5709,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.5">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -5573,7 +5717,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="72.5">
       <c r="A25" s="5" t="s">
         <v>91</v>
       </c>
@@ -5581,7 +5725,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
         <v>92</v>
       </c>
@@ -5589,7 +5733,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="130.5">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
@@ -5597,7 +5741,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="87">
       <c r="A28" s="5" t="s">
         <v>94</v>
       </c>
@@ -5605,7 +5749,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="29">
       <c r="A29" s="5" t="s">
         <v>96</v>
       </c>
@@ -5613,7 +5757,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="145">
       <c r="A30" s="5" t="s">
         <v>97</v>
       </c>
@@ -5624,7 +5768,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="159.5">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -5635,7 +5779,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="159.5">
       <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
@@ -5646,7 +5790,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="188.5">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -5657,7 +5801,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="116">
       <c r="A34" s="5" t="s">
         <v>109</v>
       </c>
@@ -5665,7 +5809,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="43.5">
       <c r="A35" s="5" t="s">
         <v>110</v>
       </c>
@@ -5673,7 +5817,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="116">
       <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
@@ -5684,7 +5828,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="101.5">
       <c r="A37" s="5" t="s">
         <v>114</v>
       </c>
@@ -5695,7 +5839,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="116">
       <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
@@ -5703,7 +5847,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="101.5">
       <c r="A39" s="5" t="s">
         <v>119</v>
       </c>
@@ -5711,7 +5855,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="116">
       <c r="A40" s="5" t="s">
         <v>120</v>
       </c>
@@ -5719,7 +5863,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="116">
       <c r="A41" s="5" t="s">
         <v>123</v>
       </c>
@@ -5727,7 +5871,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="116">
       <c r="A42" s="5" t="s">
         <v>124</v>
       </c>
@@ -5741,7 +5885,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="174">
       <c r="A43" s="5" t="s">
         <v>126</v>
       </c>
@@ -5752,7 +5896,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="174">
       <c r="A44" s="5" t="s">
         <v>127</v>
       </c>
@@ -5763,7 +5907,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="101.5">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -5774,7 +5918,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="159.5">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -5785,7 +5929,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="174">
       <c r="A47" s="5" t="s">
         <v>130</v>
       </c>
@@ -5796,7 +5940,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="174">
       <c r="A48" s="5" t="s">
         <v>131</v>
       </c>
@@ -5807,7 +5951,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="101.5">
       <c r="A49" s="5" t="s">
         <v>132</v>
       </c>
@@ -5818,7 +5962,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="130.5">
       <c r="A50" s="5" t="s">
         <v>133</v>
       </c>
@@ -5829,7 +5973,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="101.5">
       <c r="A51" s="5" t="s">
         <v>134</v>
       </c>
@@ -5840,7 +5984,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="130.5">
       <c r="A52" s="5" t="s">
         <v>135</v>
       </c>
@@ -5851,7 +5995,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="116">
       <c r="A53" s="5" t="s">
         <v>136</v>
       </c>
@@ -5862,7 +6006,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="101.5">
       <c r="A54" s="5" t="s">
         <v>137</v>
       </c>
@@ -5870,7 +6014,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="116">
       <c r="A55" s="5" t="s">
         <v>139</v>
       </c>
@@ -5881,7 +6025,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="116">
       <c r="A56" s="5" t="s">
         <v>140</v>
       </c>
@@ -5889,7 +6033,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="159.5">
       <c r="A57" s="5" t="s">
         <v>146</v>
       </c>
@@ -5900,7 +6044,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="159.5">
       <c r="A58" s="5" t="s">
         <v>147</v>
       </c>
@@ -5908,7 +6052,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="145">
       <c r="A59" s="5" t="s">
         <v>151</v>
       </c>
@@ -5919,7 +6063,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="159.5">
       <c r="A60" s="5" t="s">
         <v>153</v>
       </c>
@@ -5930,7 +6074,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="174">
       <c r="A61" s="5" t="s">
         <v>154</v>
       </c>
@@ -5941,7 +6085,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="116">
       <c r="A62" s="5" t="s">
         <v>155</v>
       </c>
@@ -5952,7 +6096,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="43.5">
       <c r="A63" s="5" t="s">
         <v>156</v>
       </c>
@@ -5960,7 +6104,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="130.5">
       <c r="A64" s="5" t="s">
         <v>175</v>
       </c>
@@ -5971,7 +6115,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="130.5">
       <c r="A65" s="5" t="s">
         <v>176</v>
       </c>
@@ -5982,7 +6126,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3">
       <c r="A66" s="5" t="s">
         <v>181</v>
       </c>
@@ -5990,7 +6134,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3">
       <c r="A67" s="5" t="s">
         <v>182</v>
       </c>
@@ -5998,7 +6142,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="409.5">
       <c r="A68" s="5" t="s">
         <v>183</v>
       </c>
@@ -6006,7 +6150,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="409.5">
       <c r="A69" s="5" t="s">
         <v>184</v>
       </c>
@@ -6014,7 +6158,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="145">
       <c r="A70" s="5" t="s">
         <v>192</v>
       </c>
@@ -6025,7 +6169,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="232">
       <c r="A71" s="5" t="s">
         <v>195</v>
       </c>
@@ -6036,7 +6180,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3">
       <c r="A72" s="5" t="s">
         <v>196</v>
       </c>
@@ -6044,7 +6188,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3">
       <c r="A73" s="5" t="s">
         <v>277</v>
       </c>
@@ -6052,7 +6196,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="29">
       <c r="A74" s="5" t="s">
         <v>278</v>
       </c>
@@ -6060,7 +6204,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="29">
       <c r="A75" s="5" t="s">
         <v>281</v>
       </c>
@@ -6068,7 +6212,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="29">
       <c r="A76" s="5" t="s">
         <v>283</v>
       </c>
@@ -6076,7 +6220,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
         <v>355</v>
       </c>
@@ -6084,7 +6228,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3">
       <c r="A78" s="5" t="s">
         <v>356</v>
       </c>
@@ -6092,7 +6236,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3">
       <c r="A79" s="5" t="s">
         <v>357</v>
       </c>
@@ -6100,7 +6244,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3">
       <c r="A80" s="5" t="s">
         <v>359</v>
       </c>
@@ -6108,7 +6252,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="29">
       <c r="A81" s="5" t="s">
         <v>360</v>
       </c>
@@ -6116,7 +6260,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2">
       <c r="A82" s="5" t="s">
         <v>362</v>
       </c>
@@ -6124,7 +6268,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2">
       <c r="A83" s="5" t="s">
         <v>364</v>
       </c>
@@ -6132,7 +6276,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="29">
       <c r="A84" s="5" t="s">
         <v>365</v>
       </c>
@@ -6140,7 +6284,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2">
       <c r="A85" s="5" t="s">
         <v>366</v>
       </c>
@@ -6148,7 +6292,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="29">
       <c r="A86" s="5" t="s">
         <v>367</v>
       </c>
@@ -6156,7 +6300,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2">
       <c r="A87" s="5" t="s">
         <v>369</v>
       </c>
@@ -6164,7 +6308,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="29">
       <c r="A88" s="5" t="s">
         <v>370</v>
       </c>
@@ -6172,7 +6316,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2">
       <c r="A89" s="5" t="s">
         <v>372</v>
       </c>
@@ -6180,7 +6324,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="29">
       <c r="A90" s="5" t="s">
         <v>383</v>
       </c>
@@ -6188,7 +6332,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2">
       <c r="A91" s="5" t="s">
         <v>384</v>
       </c>
@@ -6196,7 +6340,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2">
       <c r="A92" s="5" t="s">
         <v>386</v>
       </c>
@@ -6204,7 +6348,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2">
       <c r="A93" s="5" t="s">
         <v>389</v>
       </c>
@@ -6212,7 +6356,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2">
       <c r="A94" s="5" t="s">
         <v>391</v>
       </c>
@@ -6220,7 +6364,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2">
       <c r="A95" s="5" t="s">
         <v>393</v>
       </c>
@@ -6228,7 +6372,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="29">
       <c r="A96" s="5" t="s">
         <v>395</v>
       </c>
@@ -6236,7 +6380,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3">
       <c r="A97" s="5" t="s">
         <v>396</v>
       </c>
@@ -6244,7 +6388,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="29">
       <c r="A98" s="5" t="s">
         <v>399</v>
       </c>
@@ -6252,7 +6396,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3">
       <c r="A99" s="5" t="s">
         <v>404</v>
       </c>
@@ -6260,7 +6404,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3">
       <c r="A100" s="5" t="s">
         <v>405</v>
       </c>
@@ -6268,7 +6412,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3">
       <c r="A101" s="5" t="s">
         <v>406</v>
       </c>
@@ -6276,7 +6420,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3">
       <c r="A102" s="5" t="s">
         <v>407</v>
       </c>
@@ -6284,7 +6428,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="188.5">
       <c r="A103" s="5" t="s">
         <v>408</v>
       </c>
@@ -6295,7 +6439,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="275.5">
       <c r="A104" s="5" t="s">
         <v>409</v>
       </c>
@@ -6306,7 +6450,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="232">
       <c r="A105" s="5" t="s">
         <v>411</v>
       </c>
@@ -6317,7 +6461,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
         <v>414</v>
       </c>
@@ -6325,7 +6469,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="43.5">
       <c r="A107" s="5" t="s">
         <v>416</v>
       </c>
@@ -6333,7 +6477,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3">
       <c r="A108" s="5" t="s">
         <v>421</v>
       </c>
@@ -6341,7 +6485,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="116">
       <c r="A109" s="5" t="s">
         <v>423</v>
       </c>
@@ -6349,7 +6493,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3">
       <c r="A110" s="5" t="s">
         <v>424</v>
       </c>
@@ -6357,7 +6501,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3">
       <c r="A111" s="5" t="s">
         <v>425</v>
       </c>
@@ -6365,7 +6509,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3">
       <c r="A112" s="5" t="s">
         <v>448</v>
       </c>
@@ -6376,7 +6520,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3">
       <c r="A113" s="5" t="s">
         <v>449</v>
       </c>
@@ -6387,7 +6531,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3">
       <c r="A114" s="5" t="s">
         <v>450</v>
       </c>
@@ -6398,7 +6542,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3">
       <c r="A115" s="5" t="s">
         <v>451</v>
       </c>
@@ -6409,7 +6553,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3">
       <c r="A116" s="5" t="s">
         <v>452</v>
       </c>
@@ -6420,7 +6564,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3">
       <c r="A117" s="5" t="s">
         <v>453</v>
       </c>
@@ -6431,7 +6575,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3">
       <c r="A118" s="5" t="s">
         <v>454</v>
       </c>
@@ -6442,7 +6586,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3">
       <c r="A119" s="5" t="s">
         <v>455</v>
       </c>
@@ -6453,7 +6597,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3">
       <c r="A120" s="5" t="s">
         <v>456</v>
       </c>
@@ -6464,7 +6608,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3">
       <c r="A121" s="5" t="s">
         <v>457</v>
       </c>
@@ -6475,7 +6619,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3">
       <c r="A122" s="5" t="s">
         <v>458</v>
       </c>
@@ -6486,7 +6630,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3">
       <c r="A123" s="5" t="s">
         <v>459</v>
       </c>
@@ -6497,7 +6641,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3">
       <c r="A124" s="5" t="s">
         <v>460</v>
       </c>
@@ -6508,7 +6652,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3">
       <c r="A125" s="5" t="s">
         <v>462</v>
       </c>
@@ -6516,7 +6660,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3">
       <c r="A126" s="5" t="s">
         <v>461</v>
       </c>
@@ -6524,7 +6668,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="116">
       <c r="A127" s="5" t="s">
         <v>464</v>
       </c>
@@ -6535,7 +6679,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="116">
       <c r="A128" s="5" t="s">
         <v>465</v>
       </c>
@@ -6546,7 +6690,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3">
       <c r="A129" s="5" t="s">
         <v>467</v>
       </c>
@@ -6554,7 +6698,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="174">
       <c r="A130" s="5" t="s">
         <v>468</v>
       </c>
@@ -6565,7 +6709,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="145">
       <c r="A131" s="5" t="s">
         <v>472</v>
       </c>
@@ -6576,7 +6720,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="145">
       <c r="A132" s="5" t="s">
         <v>473</v>
       </c>
@@ -6587,7 +6731,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="130.5">
       <c r="A133" s="5" t="s">
         <v>476</v>
       </c>
@@ -6598,7 +6742,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="130.5">
       <c r="A134" s="5" t="s">
         <v>478</v>
       </c>
@@ -6609,7 +6753,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="130.5">
       <c r="A135" s="5" t="s">
         <v>479</v>
       </c>
@@ -6620,7 +6764,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="130.5">
       <c r="A136" s="5" t="s">
         <v>482</v>
       </c>
@@ -6631,7 +6775,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="130.5">
       <c r="A137" s="5" t="s">
         <v>484</v>
       </c>
@@ -6642,7 +6786,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="130.5">
       <c r="A138" s="5" t="s">
         <v>486</v>
       </c>
@@ -6653,7 +6797,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="130.5">
       <c r="A139" s="5" t="s">
         <v>487</v>
       </c>
@@ -6664,7 +6808,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="130.5">
       <c r="A140" s="5" t="s">
         <v>490</v>
       </c>
@@ -6675,7 +6819,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="130.5">
       <c r="A141" s="5" t="s">
         <v>492</v>
       </c>
@@ -6686,7 +6830,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="130.5">
       <c r="A142" s="5" t="s">
         <v>493</v>
       </c>
@@ -6697,7 +6841,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="116">
       <c r="A143" s="5" t="s">
         <v>499</v>
       </c>
@@ -6708,7 +6852,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="130.5">
       <c r="A144" s="5" t="s">
         <v>502</v>
       </c>
@@ -6719,7 +6863,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="130.5">
       <c r="A145" s="5" t="s">
         <v>503</v>
       </c>
@@ -6730,7 +6874,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="130.5">
       <c r="A146" s="5" t="s">
         <v>505</v>
       </c>
@@ -6741,7 +6885,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="130.5">
       <c r="A147" s="5" t="s">
         <v>508</v>
       </c>
@@ -6752,7 +6896,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="130.5">
       <c r="A148" s="5" t="s">
         <v>509</v>
       </c>
@@ -6763,7 +6907,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3">
       <c r="A149" s="5" t="s">
         <v>529</v>
       </c>
@@ -6774,7 +6918,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3">
       <c r="A150" s="5" t="s">
         <v>530</v>
       </c>
@@ -6785,7 +6929,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3">
       <c r="A151" s="5" t="s">
         <v>531</v>
       </c>
@@ -6796,7 +6940,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3">
       <c r="A152" s="5" t="s">
         <v>532</v>
       </c>
@@ -6807,7 +6951,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="29">
       <c r="A153" s="5" t="s">
         <v>533</v>
       </c>
@@ -6818,7 +6962,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3">
       <c r="A154" s="5" t="s">
         <v>534</v>
       </c>
@@ -6829,7 +6973,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="87">
       <c r="A155" s="5" t="s">
         <v>536</v>
       </c>
@@ -6840,7 +6984,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="43.5">
       <c r="A156" s="5" t="s">
         <v>538</v>
       </c>
@@ -6851,7 +6995,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="174">
       <c r="A157" s="5" t="s">
         <v>542</v>
       </c>
@@ -6862,7 +7006,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="159.5">
       <c r="A158" s="5" t="s">
         <v>543</v>
       </c>
@@ -6873,7 +7017,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3">
       <c r="A159" s="5" t="s">
         <v>548</v>
       </c>
@@ -6881,7 +7025,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" ht="72.5">
       <c r="A160" s="5" t="s">
         <v>549</v>
       </c>
@@ -6892,7 +7036,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="58">
       <c r="A161" s="5" t="s">
         <v>553</v>
       </c>
@@ -6900,7 +7044,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="43.5">
       <c r="A162" s="5" t="s">
         <v>554</v>
       </c>
@@ -6908,7 +7052,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3">
       <c r="A163" s="5" t="s">
         <v>557</v>
       </c>
@@ -6919,7 +7063,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="101.5">
       <c r="A164" s="5" t="s">
         <v>562</v>
       </c>
@@ -6927,7 +7071,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="101.5">
       <c r="A165" s="5" t="s">
         <v>563</v>
       </c>
@@ -6935,7 +7079,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3">
       <c r="A166" s="5" t="s">
         <v>566</v>
       </c>
@@ -6946,7 +7090,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3">
       <c r="A167" s="5" t="s">
         <v>567</v>
       </c>
@@ -6957,7 +7101,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3">
       <c r="A168" s="5" t="s">
         <v>568</v>
       </c>
@@ -6965,7 +7109,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3">
       <c r="A169" s="5" t="s">
         <v>569</v>
       </c>
@@ -6976,7 +7120,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3">
       <c r="A170" s="5" t="s">
         <v>570</v>
       </c>
@@ -6984,7 +7128,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3">
       <c r="A171" s="5" t="s">
         <v>571</v>
       </c>
@@ -6995,7 +7139,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3">
       <c r="A172" s="5" t="s">
         <v>572</v>
       </c>
@@ -7006,7 +7150,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3">
       <c r="A173" s="5" t="s">
         <v>573</v>
       </c>
@@ -7017,7 +7161,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3">
       <c r="A174" s="5" t="s">
         <v>574</v>
       </c>
@@ -7028,7 +7172,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3">
       <c r="A175" s="5" t="s">
         <v>575</v>
       </c>
@@ -7036,7 +7180,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3">
       <c r="A176" s="5" t="s">
         <v>576</v>
       </c>
@@ -7047,7 +7191,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3">
       <c r="A177" s="5" t="s">
         <v>577</v>
       </c>
@@ -7058,7 +7202,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3">
       <c r="A178" s="5" t="s">
         <v>578</v>
       </c>
@@ -7069,7 +7213,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3">
       <c r="A179" s="5" t="s">
         <v>579</v>
       </c>
@@ -7080,7 +7224,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="29">
       <c r="A180" s="5" t="s">
         <v>580</v>
       </c>
@@ -7091,7 +7235,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3">
       <c r="A181" s="5" t="s">
         <v>581</v>
       </c>
@@ -7102,7 +7246,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3">
       <c r="A182" s="5" t="s">
         <v>582</v>
       </c>
@@ -7113,7 +7257,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="116">
       <c r="A183" s="5" t="s">
         <v>583</v>
       </c>
@@ -7124,7 +7268,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3">
       <c r="A184" s="5" t="s">
         <v>584</v>
       </c>
@@ -7135,7 +7279,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3">
       <c r="A185" s="5" t="s">
         <v>585</v>
       </c>
@@ -7146,7 +7290,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3">
       <c r="A186" s="5" t="s">
         <v>586</v>
       </c>
@@ -7157,7 +7301,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3">
       <c r="A187" s="5" t="s">
         <v>587</v>
       </c>
@@ -7168,7 +7312,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="72.5">
       <c r="A188" s="5" t="s">
         <v>588</v>
       </c>
@@ -7179,7 +7323,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="101.5">
       <c r="A189" s="5" t="s">
         <v>589</v>
       </c>
@@ -7190,7 +7334,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="72.5">
       <c r="A190" s="5" t="s">
         <v>669</v>
       </c>
@@ -7201,7 +7345,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="87">
       <c r="A191" s="5" t="s">
         <v>670</v>
       </c>
@@ -7212,7 +7356,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="87">
       <c r="A192" s="5" t="s">
         <v>671</v>
       </c>
@@ -7223,7 +7367,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3">
       <c r="A193" s="5" t="s">
         <v>672</v>
       </c>
@@ -7234,7 +7378,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3">
       <c r="A194" s="5" t="s">
         <v>673</v>
       </c>
@@ -7245,7 +7389,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3">
       <c r="A195" s="5" t="s">
         <v>674</v>
       </c>
@@ -7256,7 +7400,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3">
       <c r="A196" s="5" t="s">
         <v>675</v>
       </c>
@@ -7267,7 +7411,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="29">
       <c r="A197" s="5" t="s">
         <v>676</v>
       </c>
@@ -7278,7 +7422,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="29">
       <c r="A198" s="5" t="s">
         <v>677</v>
       </c>
@@ -7289,7 +7433,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3">
       <c r="A199" s="5" t="s">
         <v>678</v>
       </c>
@@ -7300,7 +7444,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="29">
       <c r="A200" s="5" t="s">
         <v>679</v>
       </c>
@@ -7311,7 +7455,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" ht="87">
       <c r="A201" s="5" t="s">
         <v>680</v>
       </c>
@@ -7322,7 +7466,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" ht="72.5">
       <c r="A202" s="5" t="s">
         <v>681</v>
       </c>
@@ -7333,7 +7477,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" ht="87">
       <c r="A203" s="5" t="s">
         <v>682</v>
       </c>
@@ -7344,7 +7488,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" ht="29">
       <c r="A204" s="5" t="s">
         <v>683</v>
       </c>
@@ -7352,7 +7496,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" ht="409.5">
       <c r="A205" s="5" t="s">
         <v>684</v>
       </c>
@@ -7363,7 +7507,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" ht="217.5">
       <c r="A206" s="5" t="s">
         <v>685</v>
       </c>
@@ -7374,7 +7518,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3">
       <c r="A207" s="5" t="s">
         <v>686</v>
       </c>
@@ -7385,7 +7529,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" ht="43.5">
       <c r="A208" s="5" t="s">
         <v>687</v>
       </c>
@@ -7396,7 +7540,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="101.5">
       <c r="A209" s="5" t="s">
         <v>688</v>
       </c>
@@ -7407,7 +7551,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3">
       <c r="A210" s="5" t="s">
         <v>689</v>
       </c>
@@ -7418,7 +7562,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" ht="409.5">
       <c r="A211" s="5" t="s">
         <v>690</v>
       </c>
@@ -7429,7 +7573,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" ht="105" customHeight="1">
       <c r="A212" s="5" t="s">
         <v>691</v>
       </c>
@@ -7440,7 +7584,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" ht="29">
       <c r="A213" s="5" t="s">
         <v>692</v>
       </c>
@@ -7451,7 +7595,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" ht="72.5">
       <c r="A214" s="5" t="s">
         <v>693</v>
       </c>
@@ -7462,7 +7606,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" ht="87">
       <c r="A215" s="5" t="s">
         <v>694</v>
       </c>
@@ -7473,7 +7617,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" ht="72.5">
       <c r="A216" s="5" t="s">
         <v>695</v>
       </c>
@@ -7484,7 +7628,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" ht="87">
       <c r="A217" s="5" t="s">
         <v>696</v>
       </c>
@@ -7495,7 +7639,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" ht="217.5">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -7506,7 +7650,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" ht="409.5">
       <c r="A219" s="5" t="s">
         <v>697</v>
       </c>
@@ -7517,7 +7661,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" ht="203">
       <c r="A220" s="5" t="s">
         <v>698</v>
       </c>
@@ -7528,7 +7672,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" ht="159.5">
       <c r="A221" s="5" t="s">
         <v>699</v>
       </c>
@@ -7536,7 +7680,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3">
       <c r="A222" s="5" t="s">
         <v>700</v>
       </c>
@@ -7544,7 +7688,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" ht="101.5">
       <c r="A223" s="5" t="s">
         <v>701</v>
       </c>
@@ -7555,7 +7699,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" ht="101.5">
       <c r="A224" s="5" t="s">
         <v>702</v>
       </c>
@@ -7566,7 +7710,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" ht="101.5">
       <c r="A225" s="5" t="s">
         <v>703</v>
       </c>
@@ -7577,17 +7721,17 @@
         <v>774</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3">
       <c r="A226" s="5" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3">
       <c r="A227" s="5" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3">
       <c r="A228" s="5" t="s">
         <v>706</v>
       </c>
@@ -7595,7 +7739,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3">
       <c r="A229" s="5" t="s">
         <v>707</v>
       </c>
@@ -7603,7 +7747,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3">
       <c r="A230" s="5" t="s">
         <v>708</v>
       </c>
@@ -7611,7 +7755,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3">
       <c r="A231" s="5" t="s">
         <v>709</v>
       </c>
@@ -7619,7 +7763,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3">
       <c r="A232" s="5" t="s">
         <v>710</v>
       </c>
@@ -7630,7 +7774,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3">
       <c r="A233" s="5" t="s">
         <v>711</v>
       </c>
@@ -7641,7 +7785,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" ht="87">
       <c r="A234" s="5" t="s">
         <v>712</v>
       </c>
@@ -7649,7 +7793,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3">
       <c r="A235" s="5" t="s">
         <v>713</v>
       </c>
@@ -7660,7 +7804,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" ht="87">
       <c r="A236" s="5" t="s">
         <v>714</v>
       </c>
@@ -7671,7 +7815,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3">
       <c r="A237" s="5" t="s">
         <v>715</v>
       </c>
@@ -7682,7 +7826,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3">
       <c r="A238" s="5" t="s">
         <v>716</v>
       </c>
@@ -7693,7 +7837,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" ht="130.5">
       <c r="A239" s="5" t="s">
         <v>717</v>
       </c>
@@ -7704,7 +7848,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" ht="29">
       <c r="A240" s="5" t="s">
         <v>718</v>
       </c>
@@ -7715,7 +7859,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3">
       <c r="A241" s="5" t="s">
         <v>719</v>
       </c>
@@ -7726,7 +7870,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" ht="101.5">
       <c r="A242" s="5" t="s">
         <v>787</v>
       </c>
@@ -7737,7 +7881,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" ht="43.5">
       <c r="A243" s="5" t="s">
         <v>788</v>
       </c>
@@ -7748,7 +7892,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" ht="174">
       <c r="A244" s="5" t="s">
         <v>789</v>
       </c>
@@ -7759,7 +7903,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" ht="217.5">
       <c r="A245" s="5" t="s">
         <v>791</v>
       </c>
@@ -7770,7 +7914,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" ht="174">
       <c r="A246" s="5" t="s">
         <v>796</v>
       </c>
@@ -7781,7 +7925,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" ht="188.5">
       <c r="A247" s="5" t="s">
         <v>801</v>
       </c>
@@ -7792,7 +7936,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" ht="188.5">
       <c r="A248" s="5" t="s">
         <v>804</v>
       </c>
@@ -7803,7 +7947,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" ht="217.5">
       <c r="A249" s="5" t="s">
         <v>807</v>
       </c>
@@ -7814,7 +7958,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" ht="116">
       <c r="A250" s="5" t="s">
         <v>827</v>
       </c>
@@ -7825,7 +7969,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" ht="145">
       <c r="A251" s="5" t="s">
         <v>830</v>
       </c>
@@ -7836,7 +7980,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" ht="116">
       <c r="A252" s="5" t="s">
         <v>833</v>
       </c>
@@ -7847,7 +7991,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:3">
       <c r="A253" s="5" t="s">
         <v>840</v>
       </c>
@@ -7858,7 +8002,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" ht="29">
       <c r="A254" s="5" t="s">
         <v>841</v>
       </c>
@@ -7869,7 +8013,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:3" ht="72.5">
       <c r="A255" s="5" t="s">
         <v>842</v>
       </c>
@@ -7880,7 +8024,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" ht="29">
       <c r="A256" s="5" t="s">
         <v>843</v>
       </c>
@@ -7891,7 +8035,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:3" ht="72.5">
       <c r="A257" s="5" t="s">
         <v>844</v>
       </c>
@@ -7902,7 +8046,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:3" ht="145">
       <c r="A258" s="5" t="s">
         <v>851</v>
       </c>
@@ -7913,23 +8057,34 @@
         <v>850</v>
       </c>
     </row>
-    <row r="259" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:3" ht="29">
       <c r="A259" s="5">
         <v>258</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>859</v>
+        <v>872</v>
       </c>
       <c r="C259" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="72.5">
       <c r="A260" s="5">
         <v>259</v>
       </c>
       <c r="B260" s="7" t="s">
-        <v>860</v>
+        <v>874</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="C261" t="s">
+        <v>875</v>
       </c>
     </row>
   </sheetData>
@@ -7946,16 +8101,16 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7975,7 +8130,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -7998,7 +8153,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -8021,7 +8176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -8041,7 +8196,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -8055,7 +8210,7 @@
         <v>656565</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -8069,7 +8224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -8092,7 +8247,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -8132,13 +8287,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="68.21875" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
         <v>197</v>
       </c>
@@ -8146,7 +8301,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="13" t="s">
         <v>199</v>
       </c>
@@ -8154,7 +8309,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
         <v>201</v>
       </c>
@@ -8162,55 +8317,55 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="13" t="s">
         <v>203</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="13" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="13" t="s">
         <v>205</v>
       </c>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="13" t="s">
         <v>206</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="13" t="s">
         <v>208</v>
       </c>
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="13" t="s">
         <v>210</v>
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="13" t="s">
         <v>211</v>
       </c>
@@ -8218,7 +8373,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="13" t="s">
         <v>213</v>
       </c>
@@ -8226,7 +8381,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="13" t="s">
         <v>215</v>
       </c>
@@ -8234,7 +8389,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="13" t="s">
         <v>44</v>
       </c>
@@ -8242,7 +8397,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="13" t="s">
         <v>218</v>
       </c>
@@ -8250,7 +8405,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="13" t="s">
         <v>220</v>
       </c>
@@ -8258,7 +8413,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="13" t="s">
         <v>222</v>
       </c>
@@ -8266,7 +8421,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="13" t="s">
         <v>224</v>
       </c>
@@ -8274,7 +8429,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="13" t="s">
         <v>226</v>
       </c>
@@ -8282,7 +8437,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="13" t="s">
         <v>228</v>
       </c>
@@ -8290,7 +8445,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="13" t="s">
         <v>230</v>
       </c>
@@ -8298,31 +8453,31 @@
         <v>231</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="22"/>
       <c r="B23" s="21" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" s="22"/>
       <c r="B26" s="15" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="13" t="s">
         <v>235</v>
       </c>
@@ -8330,7 +8485,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" s="13" t="s">
         <v>237</v>
       </c>
@@ -8338,7 +8493,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="13" t="s">
         <v>239</v>
       </c>
@@ -8346,7 +8501,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" s="13" t="s">
         <v>241</v>
       </c>
@@ -8354,7 +8509,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" s="13" t="s">
         <v>242</v>
       </c>
@@ -8362,7 +8517,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" s="13" t="s">
         <v>244</v>
       </c>
@@ -8370,7 +8525,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" s="13" t="s">
         <v>246</v>
       </c>
@@ -8378,7 +8533,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" s="13" t="s">
         <v>248</v>
       </c>
@@ -8386,7 +8541,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35" s="13" t="s">
         <v>249</v>
       </c>
@@ -8394,7 +8549,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36" s="13" t="s">
         <v>250</v>
       </c>
@@ -8402,7 +8557,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37" s="13" t="s">
         <v>252</v>
       </c>
@@ -8410,7 +8565,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38" s="13" t="s">
         <v>254</v>
       </c>
@@ -8418,7 +8573,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39" s="13" t="s">
         <v>256</v>
       </c>
@@ -8426,7 +8581,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40" s="13" t="s">
         <v>258</v>
       </c>
@@ -8434,7 +8589,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41" s="13" t="s">
         <v>260</v>
       </c>
@@ -8442,7 +8597,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42" s="13" t="s">
         <v>262</v>
       </c>
@@ -8450,7 +8605,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43" s="13" t="s">
         <v>264</v>
       </c>
@@ -8458,7 +8613,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="16">
       <c r="A44" s="13" t="s">
         <v>265</v>
       </c>
@@ -8466,7 +8621,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45" s="13" t="s">
         <v>266</v>
       </c>
@@ -8474,7 +8629,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46" s="13" t="s">
         <v>268</v>
       </c>
@@ -8482,7 +8637,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47" s="13" t="s">
         <v>269</v>
       </c>
@@ -8490,7 +8645,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" s="13" t="s">
         <v>270</v>
       </c>
@@ -8498,7 +8653,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2">
       <c r="A49" s="13" t="s">
         <v>272</v>
       </c>
@@ -8506,7 +8661,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50" s="13" t="s">
         <v>273</v>
       </c>
@@ -8514,7 +8669,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2">
       <c r="A51" s="13" t="s">
         <v>275</v>
       </c>
@@ -8548,13 +8703,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="85.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="85.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>285</v>
       </c>
@@ -8562,7 +8717,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="15" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>287</v>
       </c>
@@ -8570,7 +8725,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>289</v>
       </c>
@@ -8578,7 +8733,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15" thickBot="1">
       <c r="A4" s="25" t="s">
         <v>291</v>
       </c>
@@ -8586,7 +8741,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15" thickBot="1">
       <c r="A5" s="25" t="s">
         <v>293</v>
       </c>
@@ -8594,7 +8749,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15" thickBot="1">
       <c r="A6" s="25" t="s">
         <v>295</v>
       </c>
@@ -8602,7 +8757,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="15" thickBot="1">
       <c r="A7" s="25" t="s">
         <v>297</v>
       </c>
@@ -8610,7 +8765,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15" thickBot="1">
       <c r="A8" s="25" t="s">
         <v>299</v>
       </c>
@@ -8618,7 +8773,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15" thickBot="1">
       <c r="A9" s="25" t="s">
         <v>301</v>
       </c>
@@ -8626,7 +8781,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="15" thickBot="1">
       <c r="A10" s="25" t="s">
         <v>303</v>
       </c>
@@ -8634,7 +8789,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="15" thickBot="1">
       <c r="A11" s="25" t="s">
         <v>305</v>
       </c>
@@ -8642,7 +8797,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15" thickBot="1">
       <c r="A12" s="25" t="s">
         <v>307</v>
       </c>
@@ -8650,7 +8805,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15" thickBot="1">
       <c r="A13" s="25" t="s">
         <v>309</v>
       </c>
@@ -8658,7 +8813,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="15" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>311</v>
       </c>
@@ -8666,7 +8821,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="15" thickBot="1">
       <c r="A15" s="25" t="s">
         <v>313</v>
       </c>
@@ -8674,7 +8829,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="15" thickBot="1">
       <c r="A16" s="25" t="s">
         <v>315</v>
       </c>
@@ -8682,7 +8837,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="15" thickBot="1">
       <c r="A17" s="25" t="s">
         <v>317</v>
       </c>
@@ -8690,7 +8845,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>319</v>
       </c>
@@ -8698,7 +8853,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="15" thickBot="1">
       <c r="A19" s="25" t="s">
         <v>321</v>
       </c>
@@ -8706,7 +8861,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="15" thickBot="1">
       <c r="A20" s="25" t="s">
         <v>323</v>
       </c>
@@ -8714,7 +8869,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="15" thickBot="1">
       <c r="A21" s="25" t="s">
         <v>325</v>
       </c>
@@ -8722,7 +8877,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="15" thickBot="1">
       <c r="A22" s="25" t="s">
         <v>327</v>
       </c>
@@ -8730,7 +8885,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="15" thickBot="1">
       <c r="A23" s="25" t="s">
         <v>329</v>
       </c>
@@ -8738,7 +8893,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="15" thickBot="1">
       <c r="A24" s="25" t="s">
         <v>331</v>
       </c>
@@ -8746,7 +8901,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="15" thickBot="1">
       <c r="A25" s="25" t="s">
         <v>333</v>
       </c>
@@ -8754,7 +8909,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="15" thickBot="1">
       <c r="A26" s="25" t="s">
         <v>335</v>
       </c>
@@ -8762,7 +8917,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="15" thickBot="1">
       <c r="A27" s="25" t="s">
         <v>337</v>
       </c>
@@ -8770,7 +8925,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="15" thickBot="1">
       <c r="A28" s="25" t="s">
         <v>339</v>
       </c>
@@ -8778,7 +8933,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="15" thickBot="1">
       <c r="A29" s="25" t="s">
         <v>341</v>
       </c>
@@ -8786,7 +8941,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="15" thickBot="1">
       <c r="A30" s="25" t="s">
         <v>343</v>
       </c>
@@ -8794,7 +8949,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="15" thickBot="1">
       <c r="A31" s="25" t="s">
         <v>345</v>
       </c>
@@ -8802,7 +8957,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="15" thickBot="1">
       <c r="A32" s="25" t="s">
         <v>347</v>
       </c>
@@ -8810,7 +8965,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="15" thickBot="1">
       <c r="A33" s="25" t="s">
         <v>349</v>
       </c>
@@ -8818,7 +8973,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="15" thickBot="1">
       <c r="A34" s="25" t="s">
         <v>351</v>
       </c>
@@ -8826,7 +8981,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="15" thickBot="1">
       <c r="A35" s="25" t="s">
         <v>353</v>
       </c>
@@ -8838,47 +8993,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16592FEF-48E9-415D-9DDC-007B8657F147}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="47.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>852</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>853</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>855</v>
-      </c>
-      <c r="B2" t="s">
-        <v>856</v>
-      </c>
-      <c r="C2" t="s">
-        <v>857</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Manage User Portal experience US changes
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrish38\Documents\GitCucumber\RB-113.x\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrish38\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8176FE7C-6CAC-4DB6-B2C6-0993F5BB5352}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB427780-6931-4DE0-B658-528A817BCF10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="2259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2443" uniqueCount="2273">
   <si>
     <t>City</t>
   </si>
@@ -8496,6 +8496,60 @@
   </si>
   <si>
     <t>Colored columns and rowsAdded by Rahul</t>
+  </si>
+  <si>
+    <t>select * from ole.product_selection where PRTL_PRDCT_SELECTED_GRP_NM='Premium' and PRTL_PRDCT_SELECTED_STS_CD='A' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>Premium Provider TIN for Adding in BS admin User</t>
+  </si>
+  <si>
+    <t>select * from OLE.ENROLLED_PROVIDER where ENRL_STS_CD='A' and PAY_METH_TYP_CD='VO' order by CREAT_DTTM desc FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>VCP TIN for Adding in BS admin User</t>
+  </si>
+  <si>
+    <t>SELECT * FROM OLE.PORTAL_USER pu 
+INNER JOIN OLE.PORTAL_USER_BS_TIN pubst ON pubst.PORTAL_USER_ID = pu.PORTAL_USER_ID
+INNER JOIN OLE.BILLING_SERVICE bs ON bs.BILLING_SERVICE_ID = pubst.BILLING_SERVICE_ID
+WHERE pu.STS_CD ='A' AND pu.USER_TYP='BS' AND pu.SSO_ID='{$id}'</t>
+  </si>
+  <si>
+    <t>BS Active Tins</t>
+  </si>
+  <si>
+    <t>Select count(*) as TIN_COUNT from ole.PORTAL_USER pu, ole.PORTAL_USER_BS_TIN bs, ole.BILLING_SERVICE_PROVIDER bsp
+where pu.PORTAL_USER_ID=bs.PORTAL_USER_ID and bs.BILLING_SERVICE_ID=bsp.BILLING_SERVICE_ID and pu.SSO_ID='{$id}' and bsp.PROV_TIN_NBR='{$tin}' and bsp.STS_CD='A' with ur</t>
+  </si>
+  <si>
+    <t>select ps.PROV_TIN_NBR as PROV_TAX_ID_NBR from
+ole.product_selection ps join ole.enrolled_provider ep
+on ps.PROV_TIN_NBR=ep.PROV_TIN_NBR 
+where ps.PRTL_PRDCT_SELECTED_GRP_NM='{$prdctSelected}' and ps.PRTL_PRDCT_SELECTED_STS_CD='A'
+and ep.PAY_METH_TYP_CD='{$tinType}' and ep.ENRL_STS_CD='A'
+order by ps.LST_CHG_BY_DTTM desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Provider TINs for Legacy,Standard and Premium Tins</t>
+  </si>
+  <si>
+    <t>select * from ole.system_configuration  WHERE PROC_CD='SYSTEM_MODE'</t>
+  </si>
+  <si>
+    <t>System Mode FEEBASED or LEGACY</t>
+  </si>
+  <si>
+    <t>update ole.system_configuration  set PROC_DATA='{$sysMode}' WHERE PROC_CD='SYSTEM_MODE'</t>
+  </si>
+  <si>
+    <t>SELECT count(*) as TotalActPR
+ FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_TIN pt ON  pt.PORTAL_USER_ID = pu.PORTAL_USER_ID 
+WHERE pt.PROV_TIN_NBR = '{$tin}' and pu.STS_CD in ('A','PR','P')</t>
+  </si>
+  <si>
+    <t>No of User entry in PORTAL_USER Table</t>
   </si>
 </sst>
 </file>
@@ -9207,7 +9261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -9758,10 +9812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1606"/>
+  <dimension ref="A1:D1609"/>
   <sheetViews>
-    <sheetView topLeftCell="A272" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B273" sqref="B273"/>
+    <sheetView tabSelected="1" topLeftCell="A1605" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1609" sqref="A1609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -19143,34 +19197,91 @@
         <v>2217</v>
       </c>
     </row>
-    <row r="1601" spans="1:1">
+    <row r="1601" spans="1:3">
       <c r="A1601" s="5" t="s">
         <v>2218</v>
       </c>
     </row>
-    <row r="1602" spans="1:1">
+    <row r="1602" spans="1:3" ht="29">
       <c r="A1602" s="5" t="s">
         <v>2219</v>
       </c>
-    </row>
-    <row r="1603" spans="1:1">
+      <c r="B1602" s="7" t="s">
+        <v>2259</v>
+      </c>
+      <c r="C1602" t="s">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:3">
       <c r="A1603" s="5" t="s">
         <v>2220</v>
       </c>
-    </row>
-    <row r="1604" spans="1:1">
+      <c r="B1603" s="7" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C1603" t="s">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:3" ht="58">
       <c r="A1604" s="5" t="s">
         <v>2221</v>
       </c>
-    </row>
-    <row r="1605" spans="1:1">
+      <c r="B1604" s="7" t="s">
+        <v>2263</v>
+      </c>
+      <c r="C1604" t="s">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:3" ht="43.5">
       <c r="A1605" s="5" t="s">
         <v>2222</v>
       </c>
-    </row>
-    <row r="1606" spans="1:1">
+      <c r="B1605" s="7" t="s">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:3" ht="101.5">
       <c r="A1606" s="5" t="s">
         <v>2223</v>
+      </c>
+      <c r="B1606" s="7" t="s">
+        <v>2266</v>
+      </c>
+      <c r="C1606" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:3">
+      <c r="A1607" s="2">
+        <v>1606</v>
+      </c>
+      <c r="B1607" t="s">
+        <v>2268</v>
+      </c>
+      <c r="C1607" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:3">
+      <c r="A1608">
+        <v>1607</v>
+      </c>
+      <c r="B1608" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:3" ht="43.5">
+      <c r="A1609">
+        <v>1608</v>
+      </c>
+      <c r="B1609" s="7" t="s">
+        <v>2271</v>
+      </c>
+      <c r="C1609" t="s">
+        <v>2272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remit Detail Code Changes
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tathyush\Desktop\Team Members Autmation\Master Branch\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53198F8-CBED-4BB5-8749-67EA93E7C41E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB2C6F3-7EB1-41FF-89AF-92AA163B3A93}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="2783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="2789">
   <si>
     <t>City</t>
   </si>
@@ -10032,9 +10032,6 @@
     <t>2119</t>
   </si>
   <si>
-    <t>TIN for Remittance Detail - CSR</t>
-  </si>
-  <si>
     <t>SELECT PROV_TAX_ID_NBR FROM OLE.SRCH_CONSOL_TBL WHERE CP_PAY_METH_CD = 'ACH' 
 ORDER BY CP_SETL_DT DESC 
 FETCH FIRST 1 ROWS ONLY</t>
@@ -10106,6 +10103,52 @@
 GROUP BY CONSL_PAY_NBR
 HAVING COUNT(*) = 2
 ORDER BY CONSL_PAY_NBR ASC LIMIT 1)</t>
+  </si>
+  <si>
+    <t>TIN for Remittance Detail - CSR, Provider</t>
+  </si>
+  <si>
+    <t>Get TIN for BS Remit Detail</t>
+  </si>
+  <si>
+    <t>SELECT BSP.PROV_TIN_NBR AS PROV_TAX_ID_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+FROM OLE.PORTAL_USER PU 
+LEFT JOIN OLE.PORTAL_USER_BS_TIN PUB ON PUB.PORTAL_USER_ID = PU.PORTAL_USER_ID
+LEFT JOIN OLE.BILLING_SERVICE_PROVIDER BSP ON BSP.BILLING_SERVICE_ID = PUB.BILLING_SERVICE_ID
+LEFT JOIN OLE.SRCH_CONSOL_TBL SCL ON SCL.PROV_TAX_ID_NBR = BSP.PROV_TIN_NBR
+WHERE SCL.CP_PAY_METH_CD = 'ACH' AND PU.SSO_ID='{$id}'
+ORDER BY SCL.CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>SELECT BSP.PROV_TIN_NBR AS PROV_TAX_ID_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+FROM OLE.PORTAL_USER PU 
+LEFT JOIN OLE.PORTAL_USER_BS_TIN PUB ON PUB.PORTAL_USER_ID = PU.PORTAL_USER_ID
+LEFT JOIN OLE.BILLING_SERVICE_PROVIDER BSP ON BSP.BILLING_SERVICE_ID = PUB.BILLING_SERVICE_ID
+LEFT JOIN OLE.SRCH_CONSOL_TBL SCL ON SCL.PROV_TAX_ID_NBR = BSP.PROV_TIN_NBR
+WHERE SCL.CP_PAY_METH_CD = 'ACH' AND PU.SSO_ID='{$id}'
+GROUP BY BSP.PROV_TIN_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+HAVING COUNT(*) = 4
+ORDER BY SCL.CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Get TIN and electronic payment number for BS Remit Detail for Multiple PLB</t>
+  </si>
+  <si>
+    <t>Get TIN and electronic payment number for BS Remit Detail for PLB</t>
+  </si>
+  <si>
+    <t>SELECT BSP.PROV_TIN_NBR AS PROV_TAX_ID_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+FROM OLE.PORTAL_USER PU 
+LEFT JOIN OLE.PORTAL_USER_BS_TIN PUB ON PUB.PORTAL_USER_ID = PU.PORTAL_USER_ID
+LEFT JOIN OLE.BILLING_SERVICE_PROVIDER BSP ON BSP.BILLING_SERVICE_ID = PUB.BILLING_SERVICE_ID
+LEFT JOIN OLE.SRCH_CONSOL_TBL SCL ON SCL.PROV_TAX_ID_NBR = BSP.PROV_TIN_NBR
+WHERE SCL.CP_PAY_METH_CD = 'ACH' AND PU.SSO_ID='{$id}'
+GROUP BY BSP.PROV_TIN_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+HAVING COUNT(*) = 2
+ORDER BY SCL.CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
   </si>
 </sst>
 </file>
@@ -11370,8 +11413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B203" sqref="B203"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B215" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13353,7 +13396,7 @@
         <v>680</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="C203" t="s">
         <v>656</v>
@@ -22263,10 +22306,10 @@
         <v>2553</v>
       </c>
       <c r="B1902" s="7" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="C1902" t="s">
-        <v>2772</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="1903" spans="1:3" ht="90">
@@ -22274,10 +22317,10 @@
         <v>2554</v>
       </c>
       <c r="B1903" s="7" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="C1903" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="1904" spans="1:3" ht="225">
@@ -22285,10 +22328,10 @@
         <v>2555</v>
       </c>
       <c r="B1904" s="7" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="C1904" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="1905" spans="1:3" ht="150">
@@ -22296,10 +22339,10 @@
         <v>2556</v>
       </c>
       <c r="B1905" s="7" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="C1905" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="1906" spans="1:3" ht="150">
@@ -22307,25 +22350,43 @@
         <v>2557</v>
       </c>
       <c r="B1906" s="7" t="s">
+        <v>2779</v>
+      </c>
+      <c r="C1906" t="s">
         <v>2780</v>
       </c>
-      <c r="C1906" t="s">
-        <v>2781</v>
-      </c>
-    </row>
-    <row r="1907" spans="1:3">
+    </row>
+    <row r="1907" spans="1:3" ht="120">
       <c r="A1907" s="5" t="s">
         <v>2558</v>
       </c>
-    </row>
-    <row r="1908" spans="1:3">
+      <c r="B1907" s="7" t="s">
+        <v>2784</v>
+      </c>
+      <c r="C1907" t="s">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:3" ht="150">
       <c r="A1908" s="5" t="s">
         <v>2559</v>
       </c>
-    </row>
-    <row r="1909" spans="1:3">
+      <c r="B1908" s="7" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C1908" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="1909" spans="1:3" ht="150">
       <c r="A1909" s="5" t="s">
         <v>2560</v>
+      </c>
+      <c r="B1909" s="7" t="s">
+        <v>2788</v>
+      </c>
+      <c r="C1909" t="s">
+        <v>2787</v>
       </c>
     </row>
     <row r="1910" spans="1:3">

</xml_diff>

<commit_message>
Commiting Manage Users Code - Priyanka's
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tathyush\Desktop\Team Members Autmation\Master Branch\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367B6B2C-82A3-43D6-9129-41456123922D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A8434C-18BC-48AE-93B7-3CAE8468A552}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2970" uniqueCount="2800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="2816">
   <si>
     <t>City</t>
   </si>
@@ -10217,12 +10217,95 @@
   <si>
     <t>SELECT MOD_TYP_CD FROM OLE.PORTAL_USER_HISTORY  WHERE  PORTAL_USER_ID = '{$portalUserID}' and  EMAIL_ADR_TXT='{$email}' ORDER BY LST_CHG_BY_DTTM DESC  FETCH FIRST 1 ROW ONLY</t>
   </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_PAYER_TIN py on p.PORTAL_USER_ID=py.PORTAL_USER_ID where  py.PAYR_TIN_NBR=(select PAYR_TIN_NBR FROM OLE.PAYER WHERE PAYR_NM ='{$tin}') and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.PAYER_ENROLLED_PROVIDER where PAYR_835_ID in (select distinct PAYR_835_ID from ole.CTL_GRP_PAYER where CTL_GRP_ID in (select distinct CTL_GRP_ID from ole.CTL_GRP ))  and ENRL_STS_CD='{$enrollmentStatusCode}' and pay_meth_cd = '{$payMethodCode}' and PROV_TIN_NBR in (select distinct prov_tin_nbr from ole.enrolled_provider where enrl_sts_cd = '{$enrollmentStatusCode}' and PAY_METH_TYP_CD='{$tinType}') FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.PAYER_ENROLLED_PROVIDER where PAYR_835_ID in (select distinct PAYR_835_ID from ole.CTL_GRP_PAYER where CTL_GRP_ID in (select distinct CTL_GRP_ID from ole.CTL_GRP where PAYR_GRPNG_CD ='U' ))  and PROV_TIN_NBR = '{$tin}'</t>
+  </si>
+  <si>
+    <t>SELECT MOD_TYP_CD, * FROM OLE.PORTAL_USER_HISTORY WHERE PORTAL_USER_ID = (Select Portal_user_id from ole.portal_user where sso_id = '{$id}') order by lst_chg_by_dttm desc</t>
+  </si>
+  <si>
+    <t>select * from ole.PAYER_ENROLLED_PROVIDER where PAYR_835_ID in (select distinct PAYR_835_ID from ole.CTL_GRP_PAYER where CTL_GRP_ID in (select distinct CTL_GRP_ID from ole.CTL_GRP ))  and ENRL_STS_CD='{$enrollmentStatusCode}' and pay_meth_cd is null and PROV_TIN_NBR in (select distinct prov_tin_nbr from ole.enrolled_provider where enrl_sts_cd = '{$enrollmentStatusCode}' and PAY_METH_TYP_CD='{$tinType}') FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select PORTAL_USER_HISTORY_ID, SSO_ID,UUID,TEL_NBR,TXT_ALERT_IND,LST_SPLASH_IND,LST_SPLASH_ID from OLE.PORTAL_USER_HISTORY order by lst_chg_by_dttm desc </t>
+  </si>
+  <si>
+    <t>select ucp.UCONSL_PAY_NBR from PP054.PROVIDER p, PP054.UNCONSOLIDATED_PAYMENT ucp,PP054.CONSOLIDATED_PAYMENT cp,OLE.PROC_CTL pc where cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR and p.PROV_KEY_ID =ucp.PROV_KEY_ID  and cp.PROC_CTL_ID=pc.PROC_CTL_ID and p.PROV_TAX_ID_NBR='{$tin}'and pc.EXTRACT_STS_CD='C' and cp.setl_dt between current date - 6 MONTHS and current date fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select prov_tax_id_nbr from PP054.provider p, PP054.CONSOLIDATED_PAYMENT cp where p.prov_key_id in (select prov_key_id from pp054.consolidated_payment where pay_meth_cd = 'ACH') and prov_tax_id_nbr in(Select prov_tin_nbr from provider_payment_unit group by prov_tin_nbr having count(prov_tin_nbr) = 1) and cp.prov_key_id = p.prov_key_id and cp.setl_dt &gt; current date - 90 days fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.PAYER where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sts_cd = 'PU' and USER_TYP = 'PA')) Limit 1</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.PAYER where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sts_cd not in( 'PU') and USER_TYP = 'PA')) Limit 1</t>
+  </si>
+  <si>
+    <t>Select p.prov_tin_nbr from ole.ENROLLED_PROVIDER p join ole.portal_user_tin put on p.prov_tin_nbr = put.prov_tin_nbr where p.ENRL_STS_CD='A' and put.ACCESS_LVL='G' Group By p.prov_tin_nbr HAVING COUNT(PUT.ACCESS_LVL = 'G') = 1 fetch first row only</t>
+  </si>
+  <si>
+    <t>select * from 
+(SELECT DISTINCT pu.PORTAL_USER_ID ,pu.STS_CD, pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT , 
+CASE WHEN length(lower(pu.MIDDLE_INIT)) &gt; 0
+THEN
+trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) || ' ' || lower(pu.MIDDLE_INIT)) 
+ELSE trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) ) 
+END as FullName 
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID
+WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}') and pu.USER_TYP='PA'
+ORDER BY FullName asc)</t>
+  </si>
+  <si>
+    <t>select * from 
+(SELECT DISTINCT pu.PORTAL_USER_ID ,pu.STS_CD, pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT , 
+CASE WHEN length(lower(pu.MIDDLE_INIT)) &gt; 0
+THEN
+trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) || ' ' || lower(pu.MIDDLE_INIT)) 
+ELSE trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) ) 
+END as FullName 
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID
+WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
+and pu.STS_CD not in('PU')
+ORDER BY FullName asc)</t>
+  </si>
+  <si>
+    <t>SELECT pu.PORTAL_USER_ID , pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT, pu.USERNAME,pu.LST_CHG_BY_ID,pu.LST_CHG_BY_DTTM
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID 
+WHERE pt.PAYR_TIN_NBR in(select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
+and pu.STS_CD = 'PU'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in( '{$id}' ) and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.CREAT_DTTM ASC
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select t.PROV_TIN_NBR,t.PORTAL_USER_ID from OLE.PORTAL_USER_TIN t 
+join OLE.PORTAL_USER u 
+on t.PORTAL_USER_ID=u.PORTAL_USER_ID 
+join OLE.ENROLLED_PROVIDER e 
+on e.PROV_TIN_NBR=t.PROV_TIN_NBR                                                                                                                                               
+where u.SSO_ID='{$id}'
+and e.ENRL_STS_CD='A'
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10308,8 +10391,15 @@
       <color rgb="FF333333"/>
       <name val="Frutiger"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10338,6 +10428,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -10393,7 +10489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -10472,6 +10568,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11480,8 +11583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1286" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1302" sqref="B1302"/>
+    <sheetView tabSelected="1" topLeftCell="A416" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C417" sqref="C417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14836,322 +14939,406 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="401" spans="1:1">
+    <row r="401" spans="1:2">
       <c r="A401" s="5" t="s">
         <v>1016</v>
       </c>
-    </row>
-    <row r="402" spans="1:1">
+      <c r="B401" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2">
       <c r="A402" s="5" t="s">
         <v>1017</v>
       </c>
-    </row>
-    <row r="403" spans="1:1">
+      <c r="B402" t="s">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2">
       <c r="A403" s="5" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="404" spans="1:1">
+      <c r="B403" t="s">
+        <v>2801</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2">
       <c r="A404" s="5" t="s">
         <v>1019</v>
       </c>
-    </row>
-    <row r="405" spans="1:1">
+      <c r="B404" t="s">
+        <v>2802</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2">
       <c r="A405" s="5" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="406" spans="1:1">
+      <c r="B405" t="s">
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2">
       <c r="A406" s="5" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="407" spans="1:1">
+      <c r="B406" t="s">
+        <v>2804</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2">
       <c r="A407" s="5" t="s">
         <v>1022</v>
       </c>
-    </row>
-    <row r="408" spans="1:1">
+      <c r="B407" t="s">
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2">
       <c r="A408" s="5" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="409" spans="1:1">
+      <c r="B408" t="s">
+        <v>2806</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2">
       <c r="A409" s="5" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="410" spans="1:1">
+      <c r="B409" t="s">
+        <v>2807</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2">
       <c r="A410" s="5" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="411" spans="1:1">
+      <c r="B410" t="s">
+        <v>2808</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2">
       <c r="A411" s="5" t="s">
         <v>1026</v>
       </c>
-    </row>
-    <row r="412" spans="1:1">
+      <c r="B411" t="s">
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" ht="165">
       <c r="A412" s="5" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="413" spans="1:1">
+      <c r="B412" s="7" t="s">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" ht="180">
       <c r="A413" s="5" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="414" spans="1:1">
+      <c r="B413" s="7" t="s">
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" ht="75">
       <c r="A414" s="5" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="415" spans="1:1">
+      <c r="B414" s="7" t="s">
+        <v>2813</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2">
       <c r="A415" s="5" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="416" spans="1:1">
+      <c r="B415" t="s">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" ht="75">
       <c r="A416" s="5" t="s">
         <v>1031</v>
       </c>
-    </row>
-    <row r="417" spans="1:1">
+      <c r="B416" s="7" t="s">
+        <v>2814</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" ht="120">
       <c r="A417" s="5" t="s">
         <v>1032</v>
       </c>
-    </row>
-    <row r="418" spans="1:1">
+      <c r="B417" s="7" t="s">
+        <v>2815</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2">
       <c r="A418" s="5" t="s">
         <v>1033</v>
       </c>
-    </row>
-    <row r="419" spans="1:1">
+      <c r="B418" s="45"/>
+    </row>
+    <row r="419" spans="1:2">
       <c r="A419" s="5" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="420" spans="1:1">
+      <c r="B419" s="45"/>
+    </row>
+    <row r="420" spans="1:2">
       <c r="A420" s="5" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="421" spans="1:1">
+      <c r="B420" s="45"/>
+    </row>
+    <row r="421" spans="1:2">
       <c r="A421" s="5" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="422" spans="1:1">
+      <c r="B421" s="45"/>
+    </row>
+    <row r="422" spans="1:2">
       <c r="A422" s="5" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="423" spans="1:1">
+      <c r="B422" s="45"/>
+    </row>
+    <row r="423" spans="1:2">
       <c r="A423" s="5" t="s">
         <v>1038</v>
       </c>
-    </row>
-    <row r="424" spans="1:1">
+      <c r="B423" s="45"/>
+    </row>
+    <row r="424" spans="1:2">
       <c r="A424" s="5" t="s">
         <v>1039</v>
       </c>
-    </row>
-    <row r="425" spans="1:1">
+      <c r="B424" s="45"/>
+    </row>
+    <row r="425" spans="1:2">
       <c r="A425" s="5" t="s">
         <v>1040</v>
       </c>
-    </row>
-    <row r="426" spans="1:1">
+      <c r="B425" s="45"/>
+    </row>
+    <row r="426" spans="1:2">
       <c r="A426" s="5" t="s">
         <v>1041</v>
       </c>
-    </row>
-    <row r="427" spans="1:1">
+      <c r="B426" s="45"/>
+    </row>
+    <row r="427" spans="1:2">
       <c r="A427" s="5" t="s">
         <v>1042</v>
       </c>
-    </row>
-    <row r="428" spans="1:1">
+      <c r="B427" s="45"/>
+    </row>
+    <row r="428" spans="1:2">
       <c r="A428" s="5" t="s">
         <v>1043</v>
       </c>
-    </row>
-    <row r="429" spans="1:1">
+      <c r="B428" s="45"/>
+    </row>
+    <row r="429" spans="1:2">
       <c r="A429" s="5" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="430" spans="1:1">
+      <c r="B429" s="45"/>
+    </row>
+    <row r="430" spans="1:2">
       <c r="A430" s="5" t="s">
         <v>1045</v>
       </c>
-    </row>
-    <row r="431" spans="1:1">
+      <c r="B430" s="45"/>
+    </row>
+    <row r="431" spans="1:2">
       <c r="A431" s="5" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="432" spans="1:1">
+      <c r="B431" s="45"/>
+    </row>
+    <row r="432" spans="1:2">
       <c r="A432" s="5" t="s">
         <v>1047</v>
       </c>
-    </row>
-    <row r="433" spans="1:1">
+      <c r="B432" s="45"/>
+    </row>
+    <row r="433" spans="1:2">
       <c r="A433" s="5" t="s">
         <v>1048</v>
       </c>
-    </row>
-    <row r="434" spans="1:1">
+      <c r="B433" s="45"/>
+    </row>
+    <row r="434" spans="1:2">
       <c r="A434" s="5" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="435" spans="1:1">
+      <c r="B434" s="45"/>
+    </row>
+    <row r="435" spans="1:2">
       <c r="A435" s="5" t="s">
         <v>1050</v>
       </c>
-    </row>
-    <row r="436" spans="1:1">
+      <c r="B435" s="45"/>
+    </row>
+    <row r="436" spans="1:2">
       <c r="A436" s="5" t="s">
         <v>1051</v>
       </c>
-    </row>
-    <row r="437" spans="1:1">
+      <c r="B436" s="45"/>
+    </row>
+    <row r="437" spans="1:2">
       <c r="A437" s="5" t="s">
         <v>1052</v>
       </c>
-    </row>
-    <row r="438" spans="1:1">
+      <c r="B437" s="45"/>
+    </row>
+    <row r="438" spans="1:2">
       <c r="A438" s="5" t="s">
         <v>1053</v>
       </c>
-    </row>
-    <row r="439" spans="1:1">
+      <c r="B438" s="45"/>
+    </row>
+    <row r="439" spans="1:2">
       <c r="A439" s="5" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="440" spans="1:1">
+      <c r="B439" s="45"/>
+    </row>
+    <row r="440" spans="1:2">
       <c r="A440" s="5" t="s">
         <v>1055</v>
       </c>
-    </row>
-    <row r="441" spans="1:1">
+      <c r="B440" s="44"/>
+    </row>
+    <row r="441" spans="1:2">
       <c r="A441" s="5" t="s">
         <v>1056</v>
       </c>
-    </row>
-    <row r="442" spans="1:1">
+      <c r="B441" s="43"/>
+    </row>
+    <row r="442" spans="1:2">
       <c r="A442" s="5" t="s">
         <v>1057</v>
       </c>
-    </row>
-    <row r="443" spans="1:1">
+      <c r="B442" s="43"/>
+    </row>
+    <row r="443" spans="1:2">
       <c r="A443" s="5" t="s">
         <v>1058</v>
       </c>
-    </row>
-    <row r="444" spans="1:1">
+      <c r="B443" s="43"/>
+    </row>
+    <row r="444" spans="1:2">
       <c r="A444" s="5" t="s">
         <v>1059</v>
       </c>
-    </row>
-    <row r="445" spans="1:1">
+      <c r="B444" s="43"/>
+    </row>
+    <row r="445" spans="1:2">
       <c r="A445" s="5" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="446" spans="1:1">
+      <c r="B445" s="43"/>
+    </row>
+    <row r="446" spans="1:2">
       <c r="A446" s="5" t="s">
         <v>1061</v>
       </c>
-    </row>
-    <row r="447" spans="1:1">
+      <c r="B446" s="43"/>
+    </row>
+    <row r="447" spans="1:2">
       <c r="A447" s="5" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="448" spans="1:1">
+      <c r="B447" s="43"/>
+    </row>
+    <row r="448" spans="1:2">
       <c r="A448" s="5" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="449" spans="1:1">
+      <c r="B448" s="43"/>
+    </row>
+    <row r="449" spans="1:2">
       <c r="A449" s="5" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="450" spans="1:1">
+      <c r="B449" s="43"/>
+    </row>
+    <row r="450" spans="1:2">
       <c r="A450" s="5" t="s">
         <v>1065</v>
       </c>
-    </row>
-    <row r="451" spans="1:1">
+      <c r="B450" s="43"/>
+    </row>
+    <row r="451" spans="1:2">
       <c r="A451" s="5" t="s">
         <v>1066</v>
       </c>
     </row>
-    <row r="452" spans="1:1">
+    <row r="452" spans="1:2">
       <c r="A452" s="5" t="s">
         <v>1067</v>
       </c>
     </row>
-    <row r="453" spans="1:1">
+    <row r="453" spans="1:2">
       <c r="A453" s="5" t="s">
         <v>1068</v>
       </c>
     </row>
-    <row r="454" spans="1:1">
+    <row r="454" spans="1:2">
       <c r="A454" s="5" t="s">
         <v>1069</v>
       </c>
     </row>
-    <row r="455" spans="1:1">
+    <row r="455" spans="1:2">
       <c r="A455" s="5" t="s">
         <v>1070</v>
       </c>
     </row>
-    <row r="456" spans="1:1">
+    <row r="456" spans="1:2">
       <c r="A456" s="5" t="s">
         <v>1071</v>
       </c>
     </row>
-    <row r="457" spans="1:1">
+    <row r="457" spans="1:2">
       <c r="A457" s="5" t="s">
         <v>1072</v>
       </c>
     </row>
-    <row r="458" spans="1:1">
+    <row r="458" spans="1:2">
       <c r="A458" s="5" t="s">
         <v>1073</v>
       </c>
     </row>
-    <row r="459" spans="1:1">
+    <row r="459" spans="1:2">
       <c r="A459" s="5" t="s">
         <v>1074</v>
       </c>
     </row>
-    <row r="460" spans="1:1">
+    <row r="460" spans="1:2">
       <c r="A460" s="5" t="s">
         <v>1075</v>
       </c>
     </row>
-    <row r="461" spans="1:1">
+    <row r="461" spans="1:2">
       <c r="A461" s="5" t="s">
         <v>1076</v>
       </c>
     </row>
-    <row r="462" spans="1:1">
+    <row r="462" spans="1:2">
       <c r="A462" s="5" t="s">
         <v>1077</v>
       </c>
     </row>
-    <row r="463" spans="1:1">
+    <row r="463" spans="1:2">
       <c r="A463" s="5" t="s">
         <v>1078</v>
       </c>
     </row>
-    <row r="464" spans="1:1">
+    <row r="464" spans="1:2">
       <c r="A464" s="5" t="s">
         <v>1079</v>
       </c>

</xml_diff>

<commit_message>
data file changes for oct
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrish38\Documents\GitCucumber\RB-113.x\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LatestMAster29Sep\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0E07C7-B38C-4EFE-932D-40482E967312}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A5F458-EECF-4211-94A2-1A6614C5B117}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,6 @@
     <definedName name="URL">[1]Sheet2!$E:$E</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2446" uniqueCount="2276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="2287">
   <si>
     <t>City</t>
   </si>
@@ -8582,6 +8581,58 @@
 ORDER BY SETL_DT DESC
 fetch first row only with ur</t>
   </si>
+  <si>
+    <t>1606</t>
+  </si>
+  <si>
+    <t>1607</t>
+  </si>
+  <si>
+    <t>1608</t>
+  </si>
+  <si>
+    <t>1609</t>
+  </si>
+  <si>
+    <t>1610</t>
+  </si>
+  <si>
+    <t>1611</t>
+  </si>
+  <si>
+    <t>select py.PAYR_SCHM_NM from ole.PAYER py, ole.CTL_GRP_PAYER cg
+ where cg.PAYR_835_ID=py.PAYR_835_ID
+ and py.PAYR_835_ID='87726' with ur</t>
+  </si>
+  <si>
+    <t>Amit-Oct release</t>
+  </si>
+  <si>
+    <t>select * from {$schema}.CONSOLIDATED_PAYMENT cp
+where cp.DSPL_CONSL_PAY_NBR='{$ELECTRONIC_PAYMENT_NUMBER}'
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr,cp.DSPL_CONSL_PAY_NBR from {$schema}.CONSOLIDATED_PAYMENT cp,
+{$schema}.PROVIDER p,ole.product_selection ps,ole.enrolled_provider ep,ole.PRODUCT_CONFIGURATION pc ,OLE.PROC_CTL PC
+where cp.prov_key_id = p.prov_key_id
+and PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and p.prov_tax_id_nbr=ps.PROV_TIN_NBR
+and ps.PROV_TIN_NBR=ep.PROV_TIN_NBR
+and pc.GROUP_NM=ps.PRTL_PRDCT_SELECTED_GRP_NM
+AND PC.EXTRACT_STS_CD = 'C'
+and ps.PRTL_PRDCT_SELECTED_GRP_NM='{$portalAccess}'
+and ps.PRTL_PRDCT_SELECTED_STS_CD='A' and (cp.ARCHV_IND is null or cp.ARCHV_IND='N')
+and ep.PAY_METH_TYP_CD='{$tinType}' and ep.ENRL_STS_CD='A'
+and cp.setl_dt between '{$fromDate}' and '{$toDate}'
+group by p.prov_tax_id_nbr,cp.DSPL_CONSL_PAY_NBR
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>Priyanka-Oct Release</t>
+  </si>
 </sst>
 </file>
 
@@ -8674,7 +8725,7 @@
       <name val="Frutiger"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8702,6 +8753,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8758,7 +8815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -8837,6 +8894,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9843,10 +9910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1611"/>
+  <dimension ref="A1:D1612"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1611" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1611" sqref="B1611"/>
+    <sheetView tabSelected="1" topLeftCell="A1612" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1612" sqref="B1612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -18758,14 +18825,26 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="1507" spans="1:3">
-      <c r="A1507" s="5" t="s">
+    <row r="1507" spans="1:3" ht="43.5">
+      <c r="A1507" s="47" t="s">
         <v>2124</v>
       </c>
-    </row>
-    <row r="1508" spans="1:3">
-      <c r="A1508" s="5" t="s">
+      <c r="B1507" s="48" t="s">
+        <v>2284</v>
+      </c>
+      <c r="C1507" s="46" t="s">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:3" ht="43.5">
+      <c r="A1508" s="44" t="s">
         <v>2125</v>
+      </c>
+      <c r="B1508" s="45" t="s">
+        <v>2282</v>
+      </c>
+      <c r="C1508" s="46" t="s">
+        <v>2283</v>
       </c>
     </row>
     <row r="1509" spans="1:3">
@@ -19286,8 +19365,8 @@
       </c>
     </row>
     <row r="1607" spans="1:3">
-      <c r="A1607" s="2">
-        <v>1606</v>
+      <c r="A1607" s="43" t="s">
+        <v>2276</v>
       </c>
       <c r="B1607" t="s">
         <v>2267</v>
@@ -19297,16 +19376,16 @@
       </c>
     </row>
     <row r="1608" spans="1:3">
-      <c r="A1608">
-        <v>1607</v>
+      <c r="A1608" s="5" t="s">
+        <v>2277</v>
       </c>
       <c r="B1608" t="s">
         <v>2269</v>
       </c>
     </row>
     <row r="1609" spans="1:3" ht="43.5">
-      <c r="A1609">
-        <v>1608</v>
+      <c r="A1609" s="5" t="s">
+        <v>2278</v>
       </c>
       <c r="B1609" s="7" t="s">
         <v>2270</v>
@@ -19316,22 +19395,33 @@
       </c>
     </row>
     <row r="1610" spans="1:3" ht="29">
-      <c r="A1610">
-        <v>1609</v>
+      <c r="A1610" s="5" t="s">
+        <v>2279</v>
       </c>
       <c r="B1610" s="7" t="s">
         <v>2272</v>
       </c>
     </row>
     <row r="1611" spans="1:3" ht="391.5">
-      <c r="A1611">
-        <v>1610</v>
+      <c r="A1611" s="5" t="s">
+        <v>2280</v>
       </c>
       <c r="B1611" s="7" t="s">
         <v>2275</v>
       </c>
       <c r="C1611" t="s">
         <v>2273</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:3" ht="232">
+      <c r="A1612" s="44" t="s">
+        <v>2281</v>
+      </c>
+      <c r="B1612" s="45" t="s">
+        <v>2285</v>
+      </c>
+      <c r="C1612" s="46" t="s">
+        <v>2286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added rows in data file
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LatestMAster29Sep\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A5F458-EECF-4211-94A2-1A6614C5B117}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C44C7E2-3E81-4CF4-B84C-D1BB827A72C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="2287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2516" uniqueCount="2315">
   <si>
     <t>City</t>
   </si>
@@ -8633,6 +8633,143 @@
   <si>
     <t>Priyanka-Oct Release</t>
   </si>
+  <si>
+    <t>select * from ole.PAYER_ENROLLED_PROVIDER where PAYR_835_ID in (select distinct PAYR_835_ID from ole.CTL_GRP_PAYER where CTL_GRP_ID in (select distinct CTL_GRP_ID from ole.CTL_GRP ))  and ENRL_STS_CD='{$enrollmentStatusCode}' and pay_meth_cd = '{$payMethodCode}' and PROV_TIN_NBR in (select distinct prov_tin_nbr from ole.enrolled_provider where enrl_sts_cd = '{$enrollmentStatusCode}' and PAY_METH_TYP_CD='{$tinType}') FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t>select * from ole.PAYER_ENROLLED_PROVIDER where PAYR_835_ID in (select distinct PAYR_835_ID from ole.CTL_GRP_PAYER where CTL_GRP_ID in (select distinct CTL_GRP_ID from ole.CTL_GRP where PAYR_GRPNG_CD ='U' ))  and PROV_TIN_NBR = '{$tin}'</t>
+  </si>
+  <si>
+    <t>SELECT MOD_TYP_CD, * FROM OLE.PORTAL_USER_HISTORY WHERE PORTAL_USER_ID = (Select Portal_user_id from ole.portal_user where sso_id = '{$id}') order by lst_chg_by_dttm desc</t>
+  </si>
+  <si>
+    <t>select * from ole.PAYER_ENROLLED_PROVIDER where PAYR_835_ID in (select distinct PAYR_835_ID from ole.CTL_GRP_PAYER where CTL_GRP_ID in (select distinct CTL_GRP_ID from ole.CTL_GRP ))  and ENRL_STS_CD='{$enrollmentStatusCode}' and pay_meth_cd is null and PROV_TIN_NBR in (select distinct prov_tin_nbr from ole.enrolled_provider where enrl_sts_cd = '{$enrollmentStatusCode}' and PAY_METH_TYP_CD='{$tinType}') FETCH FIRST 1 ROW ONLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select PORTAL_USER_HISTORY_ID, SSO_ID,UUID,TEL_NBR,TXT_ALERT_IND,LST_SPLASH_IND,LST_SPLASH_ID from OLE.PORTAL_USER_HISTORY order by lst_chg_by_dttm desc </t>
+  </si>
+  <si>
+    <t>select ucp.UCONSL_PAY_NBR
+from PP054.PROVIDER p, PP054.UNCONSOLIDATED_PAYMENT ucp,PP054.CONSOLIDATED_PAYMENT cp,OLE.PROC_CTL pc
+where cp.CONSL_PAY_NBR = ucp.CONSL_PAY_NBR
+and p.PROV_KEY_ID =ucp.PROV_KEY_ID 
+and cp.PROC_CTL_ID=pc.PROC_CTL_ID 
+and p.PROV_TAX_ID_NBR='{$tin}'
+and pc.EXTRACT_STS_CD='C'
+and cp.setl_dt between current date - 6 MONTHS and current date
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>Select prov_tax_id_nbr from PP054.provider p, PP054.CONSOLIDATED_PAYMENT cp where p.prov_key_id in (select prov_key_id from pp054.consolidated_payment where pay_meth_cd = 'ACH') and prov_tax_id_nbr in(Select prov_tin_nbr from provider_payment_unit group by prov_tin_nbr having count(prov_tin_nbr) = 1) and cp.prov_key_id = p.prov_key_id and cp.setl_dt &gt; current date - 90 days fetch first row only with ur</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.PAYER where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sts_cd = 'PU' and USER_TYP = 'PA')) Limit 1</t>
+  </si>
+  <si>
+    <t>select PAYR_DSPL_NM from ole.PAYER where PAYR_TIN_NBR in (select PAYR_TIN_NBR from ole.PORTAL_USER_PAYER_TIN where PORTAL_USER_ID in (select PORTAL_USER_ID from ole.PORTAL_USER where sts_cd not in( 'PU') and USER_TYP = 'PA')) Limit 1</t>
+  </si>
+  <si>
+    <t>select * from 
+(SELECT DISTINCT pu.PORTAL_USER_ID ,pu.STS_CD, pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT , 
+CASE WHEN length(lower(pu.MIDDLE_INIT)) &gt; 0
+THEN
+trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) || ' ' || lower(pu.MIDDLE_INIT)) 
+ELSE trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) ) 
+END as FullName 
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID
+WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}') and pu.USER_TYP='PA'
+ORDER BY FullName asc)</t>
+  </si>
+  <si>
+    <t>select * from 
+(SELECT DISTINCT pu.PORTAL_USER_ID ,pu.STS_CD, pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT , 
+CASE WHEN length(lower(pu.MIDDLE_INIT)) &gt; 0
+THEN
+trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) || ' ' || lower(pu.MIDDLE_INIT)) 
+ELSE trim(lower(pu.LST_NM) || ', ' || lower(pu.FST_NM) ) 
+END as FullName 
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID
+WHERE pt.PAYR_TIN_NBR IN (select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
+and pu.STS_CD not in('PU')
+ORDER BY FullName asc)</t>
+  </si>
+  <si>
+    <t>SELECT pu.PORTAL_USER_ID , pu.LST_NM , pu.FST_NM , pu.MIDDLE_INIT, pu.USERNAME,pu.LST_CHG_BY_ID,pu.LST_CHG_BY_DTTM
+FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_PAYER_TIN pt
+ON  pu.PORTAL_USER_ID = pt.PORTAL_USER_ID 
+WHERE pt.PAYR_TIN_NBR in(select paa.PAYR_TIN_NBR from ole.PAYER paa WHERE paa.PAYR_DSPL_NM='{$tin}')
+and pu.STS_CD = 'PU'</t>
+  </si>
+  <si>
+    <t>Select p.prov_tin_nbr from ole.ENROLLED_PROVIDER p join ole.portal_user_tin put on p.prov_tin_nbr = put.prov_tin_nbr where p.ENRL_STS_CD='A' and put.ACCESS_LVL='G' Group By p.prov_tin_nbr HAVING COUNT(PUT.ACCESS_LVL = 'G') = 1 fetch first row only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in( '{$id}' ) and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.CREAT_DTTM ASC
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select t.PROV_TIN_NBR,t.PORTAL_USER_ID from OLE.PORTAL_USER_TIN t 
+join OLE.PORTAL_USER u 
+on t.PORTAL_USER_ID=u.PORTAL_USER_ID 
+join OLE.ENROLLED_PROVIDER e 
+on e.PROV_TIN_NBR=t.PROV_TIN_NBR                                                                                                                                               
+where u.SSO_ID='{$id}'
+and e.ENRL_STS_CD='A'
+</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr
+from PP054.CONSOLIDATED_PAYMENT cp, PP054.PROVIDER p, OLE.PROC_CTL PC ,OLE.ENROLLED_PROVIDER ep WHERE p.PROV_TAX_ID_NBR=ep.PROV_TIN_NBR and PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and cp.prov_key_id = p.prov_key_id AND  ep.ENRL_STS_CD='A' and PC.EXTRACT_STS_CD = 'C'
+and cp.setl_dt &gt; current date - 90 days and p.PROV_NPI_NBR is null
+group by p.prov_tax_id_nbr
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only with ur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Select * From pp054.consolidated_payment where prov_key_id in (Select prov_key_id from pp054.provider where prov_tax_id_nbr = '{$tin}') order by setl_dt desc fetch first row only</t>
+  </si>
+  <si>
+    <t>select PROV_TIN_NBR from OLE.ENROLLED_PROVIDER e where e.PAY_METH_TYP_CD='AV' FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>select PROV_TIN_NBR from OLE.ENROLLED_PROVIDER e where e.PAY_METH_TYP_CD='VO' FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>select PROV_TIN_NBR from OLE.ENROLLED_PROVIDER e where e.PAY_METH_TYP_CD='AO' FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Select * from OLE.PAYER_ENROLLED_PROVIDER_HISTORY eh where eh.PROV_TIN_NBR = '{$tin}' order by eh.LST_CHG_BY_DTTM desc FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.ENROLLED_PROVIDER p where p.ENRL_STS_CD='A'  FETCH FIRST 1 ROW ONLY </t>
+  </si>
+  <si>
+    <t>select * from ole.PORTAL_USER_HISTORY where PROV_TIN_NBR = '{$tin}' order by LST_CHG_BY_DTTM desc FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>select count(*) as rowcount from ole.PORTAL_USER_HISTORY</t>
+  </si>
+  <si>
+    <t>select * from ole.PORTAL_USER_HISTORY order by LST_CHG_BY_DTTM desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.BILLING_SERVICE_PROVIDER bs where bs.STS_CD='A'  order by bs.LST_CHG_BY_DTTM desc FETCH FIRST 1 ROW ONLY </t>
+  </si>
+  <si>
+    <t>select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
+on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
+ on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
+where  bs.IDENTIFIER_NBR='200045122'  and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Added by Pranav</t>
+  </si>
 </sst>
 </file>
 
@@ -8815,7 +8952,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -8905,6 +9042,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9912,8 +10050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1612"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1612" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1612" sqref="B1612"/>
+    <sheetView tabSelected="1" topLeftCell="C393" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C401" sqref="C401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13268,162 +13406,336 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="401" spans="1:1">
-      <c r="A401" s="5" t="s">
+    <row r="401" spans="1:3" ht="29">
+      <c r="A401" s="2" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="402" spans="1:1">
-      <c r="A402" s="5" t="s">
+      <c r="B401" s="48" t="s">
+        <v>2233</v>
+      </c>
+      <c r="C401" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" ht="72.5">
+      <c r="A402" s="2" t="s">
         <v>1019</v>
       </c>
-    </row>
-    <row r="403" spans="1:1">
-      <c r="A403" s="5" t="s">
+      <c r="B402" s="48" t="s">
+        <v>2235</v>
+      </c>
+      <c r="C402" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" ht="58">
+      <c r="A403" s="2" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="404" spans="1:1">
-      <c r="A404" s="5" t="s">
+      <c r="B403" s="48" t="s">
+        <v>2287</v>
+      </c>
+      <c r="C403" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" ht="29">
+      <c r="A404" s="2" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="405" spans="1:1">
-      <c r="A405" s="5" t="s">
+      <c r="B404" s="48" t="s">
+        <v>2288</v>
+      </c>
+      <c r="C404" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" ht="29">
+      <c r="A405" s="2" t="s">
         <v>1022</v>
       </c>
-    </row>
-    <row r="406" spans="1:1">
-      <c r="A406" s="5" t="s">
+      <c r="B405" s="48" t="s">
+        <v>2289</v>
+      </c>
+      <c r="C405" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" ht="43.5">
+      <c r="A406" s="2" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="407" spans="1:1">
-      <c r="A407" s="5" t="s">
+      <c r="B406" s="48" t="s">
+        <v>2290</v>
+      </c>
+      <c r="C406" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" ht="29">
+      <c r="A407" s="2" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="408" spans="1:1">
-      <c r="A408" s="5" t="s">
+      <c r="B407" s="48" t="s">
+        <v>2291</v>
+      </c>
+      <c r="C407" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" ht="130.5">
+      <c r="A408" s="2" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="409" spans="1:1">
-      <c r="A409" s="5" t="s">
+      <c r="B408" s="48" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C408" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" ht="43.5">
+      <c r="A409" s="2" t="s">
         <v>1026</v>
       </c>
-    </row>
-    <row r="410" spans="1:1">
-      <c r="A410" s="5" t="s">
+      <c r="B409" s="48" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C409" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" ht="29">
+      <c r="A410" s="2" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="411" spans="1:1">
-      <c r="A411" s="5" t="s">
+      <c r="B410" s="27" t="s">
+        <v>2294</v>
+      </c>
+      <c r="C410" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" ht="29">
+      <c r="A411" s="2" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="412" spans="1:1">
-      <c r="A412" s="5" t="s">
+      <c r="B411" s="27" t="s">
+        <v>2295</v>
+      </c>
+      <c r="C411" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" ht="159.5">
+      <c r="A412" s="2" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="413" spans="1:1">
-      <c r="A413" s="5" t="s">
+      <c r="B412" s="27" t="s">
+        <v>2296</v>
+      </c>
+      <c r="C412" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" ht="174">
+      <c r="A413" s="2" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="414" spans="1:1">
-      <c r="A414" s="5" t="s">
+      <c r="B413" s="27" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C413" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" ht="72.5">
+      <c r="A414" s="2" t="s">
         <v>1031</v>
       </c>
-    </row>
-    <row r="415" spans="1:1">
-      <c r="A415" s="5" t="s">
+      <c r="B414" s="27" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C414" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3">
+      <c r="A415" s="2" t="s">
         <v>1032</v>
       </c>
-    </row>
-    <row r="416" spans="1:1">
-      <c r="A416" s="5" t="s">
+      <c r="B415" t="s">
+        <v>2299</v>
+      </c>
+      <c r="C415" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" ht="72.5">
+      <c r="A416" s="2" t="s">
         <v>1033</v>
       </c>
-    </row>
-    <row r="417" spans="1:1">
-      <c r="A417" s="5" t="s">
+      <c r="B416" s="48" t="s">
+        <v>2300</v>
+      </c>
+      <c r="C416" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" ht="116">
+      <c r="A417" s="2" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="418" spans="1:1">
-      <c r="A418" s="5" t="s">
+      <c r="B417" s="48" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C417" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" ht="130.5">
+      <c r="A418" s="2" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="419" spans="1:1">
-      <c r="A419" s="5" t="s">
+      <c r="B418" s="48" t="s">
+        <v>2302</v>
+      </c>
+      <c r="C418" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" ht="29">
+      <c r="A419" s="2" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="420" spans="1:1">
-      <c r="A420" s="5" t="s">
+      <c r="B419" s="48" t="s">
+        <v>2303</v>
+      </c>
+      <c r="C419" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3">
+      <c r="A420" s="2" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="421" spans="1:1">
-      <c r="A421" s="5" t="s">
+      <c r="B420" t="s">
+        <v>2304</v>
+      </c>
+      <c r="C420" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3">
+      <c r="A421" s="2" t="s">
         <v>1038</v>
       </c>
-    </row>
-    <row r="422" spans="1:1">
-      <c r="A422" s="5" t="s">
+      <c r="B421" t="s">
+        <v>2305</v>
+      </c>
+      <c r="C421" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3">
+      <c r="A422" s="2" t="s">
         <v>1039</v>
       </c>
-    </row>
-    <row r="423" spans="1:1">
-      <c r="A423" s="5" t="s">
+      <c r="B422" t="s">
+        <v>2306</v>
+      </c>
+      <c r="C422" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3">
+      <c r="A423" s="2" t="s">
         <v>1040</v>
       </c>
-    </row>
-    <row r="424" spans="1:1">
-      <c r="A424" s="5" t="s">
+      <c r="B423" t="s">
+        <v>2307</v>
+      </c>
+      <c r="C423" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3">
+      <c r="A424" s="2" t="s">
         <v>1041</v>
       </c>
-    </row>
-    <row r="425" spans="1:1">
-      <c r="A425" s="5" t="s">
+      <c r="B424" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C424" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3">
+      <c r="A425" s="2" t="s">
         <v>1042</v>
       </c>
-    </row>
-    <row r="426" spans="1:1">
-      <c r="A426" s="5" t="s">
+      <c r="B425" t="s">
+        <v>2309</v>
+      </c>
+      <c r="C425" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3">
+      <c r="A426" s="2" t="s">
         <v>1043</v>
       </c>
-    </row>
-    <row r="427" spans="1:1">
-      <c r="A427" s="5" t="s">
+      <c r="B426" t="s">
+        <v>2310</v>
+      </c>
+      <c r="C426" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3">
+      <c r="A427" s="2" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="428" spans="1:1">
-      <c r="A428" s="5" t="s">
+      <c r="B427" t="s">
+        <v>2311</v>
+      </c>
+      <c r="C427" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3">
+      <c r="A428" s="2" t="s">
         <v>1045</v>
       </c>
-    </row>
-    <row r="429" spans="1:1">
-      <c r="A429" s="5" t="s">
+      <c r="B428" t="s">
+        <v>2312</v>
+      </c>
+      <c r="C428" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" ht="72.5">
+      <c r="A429" s="2" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="430" spans="1:1">
+      <c r="B429" s="48" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C429" s="49" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3">
       <c r="A430" s="5" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="431" spans="1:1">
+    <row r="431" spans="1:3">
       <c r="A431" s="5" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="432" spans="1:1">
+    <row r="432" spans="1:3">
       <c r="A432" s="5" t="s">
         <v>1049</v>
       </c>

</xml_diff>

<commit_message>
Updating Few queries from line 1901
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LatestMAster29Sep\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tathyush\Desktop\Team Members Autmation\updated master\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C44C7E2-3E81-4CF4-B84C-D1BB827A72C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE2C517-EED4-4F83-A655-081A5AB86E3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2516" uniqueCount="2315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="2337">
   <si>
     <t>City</t>
   </si>
@@ -8769,6 +8769,140 @@
   </si>
   <si>
     <t>Added by Pranav</t>
+  </si>
+  <si>
+    <t>SELECT PROV_TAX_ID_NBR FROM OLE.SRCH_CONSOL_TBL WHERE CP_PAY_METH_CD = 'ACH' 
+ORDER BY CP_SETL_DT DESC 
+FETCH FIRST 1 ROWS ONLY</t>
+  </si>
+  <si>
+    <t>TIN for Remittance Detail - CSR, Provider</t>
+  </si>
+  <si>
+    <t>SELECT SC.CP_DSPL_CONSL_PAY_NBR, PA.CONSL_PAY_NBR
+FROM OLE.SRCH_CONSOL_TBL SC
+LEFT JOIN PP001.PROVIDER_PAYOR_ADJUSTMENT PA ON SC.UCP_CONSL_PAY_NBR = PA.CONSL_PAY_NBR
+WHERE PROV_TAX_ID_NBR = '{$tin}'
+ORDER BY SC.CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Get CONSL_PAY_NBR for Remittance Detail</t>
+  </si>
+  <si>
+    <t>SELECT SC.CP_DSPL_CONSL_PAY_NBR AS DSPL_CONSL_PAY_NBR, SC.UCP_CONSL_PAY_NBR AS CONSL_PAY_NBR,SC.CP_SETL_DT,
+SCL.RP_UPPER_LST_NM as LST_NM,SCL.CLM_PTNT_FST_NM as PTNT_FST_NM, SCL.CLM_PTNT_LST_NM as PTNT_LST_NM
+FROM OLE.PORTAL_USER PU, OLE.PORTAL_USER_TIN PUT, OLE.SRCH_CONSOL_TBL SC, OLE.SRCH_CLAIM_TBL SCL
+WHERE PU.PORTAL_USER_ID = PUT.PORTAL_USER_ID 
+AND PUT.PROV_TIN_NBR=SC.PROV_TAX_ID_NBR
+AND SC.UCP_UCONSL_PAY_KEY_ID = SCL.CUP_UCONSL_PAY_KEY_ID
+AND SC.PAYR_SCHM_NM=SCL.PAYR_SCHM_NM
+AND PU.STS_CD='A'
+AND PU.USER_TYP='P'
+AND SCL.RP_UPPER_LST_NM != '' 
+AND SCL.PROV_TAX_ID_NBR = '{$tin}'
+GROUP BY SC.CP_DSPL_CONSL_PAY_NBR, SC.UCP_CONSL_PAY_NBR,
+SCL.RP_UPPER_LST_NM ,SCL.CLM_PTNT_FST_NM, SCL.CLM_PTNT_LST_NM,SC.CP_SETL_DT
+ORDER BY SC.CP_SETL_DT DESC
+FETCH FIRST  ROW ONLY</t>
+  </si>
+  <si>
+    <t>Get Electronic Payment Number for checking Rendering Provider for Provider</t>
+  </si>
+  <si>
+    <t>Select DISTINCT PROV_TAX_ID_NBR,CP_DSPL_CONSL_PAY_NBR,UCP_CONSL_PAY_NBR,CP_SETL_DT from OLE.SRCH_CONSOL_TBL where CP_DSPL_CONSL_PAY_NBR IN
+(Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 4
+ORDER BY CONSL_PAY_NBR ASC))
+GROUP BY PROV_TAX_ID_NBR,CP_DSPL_CONSL_PAY_NBR,UCP_CONSL_PAY_NBR,CP_SETL_DT
+ORDER BY CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Get TIN and Electronic Payment Number for Multiple PLB</t>
+  </si>
+  <si>
+    <t>Select DISTINCT PROV_TAX_ID_NBR,CP_DSPL_CONSL_PAY_NBR,UCP_CONSL_PAY_NBR,CP_SETL_DT from OLE.SRCH_CONSOL_TBL where CP_DSPL_CONSL_PAY_NBR IN
+(Select DISTINCT CP_DSPL_CONSL_PAY_NBR from OLE.SRCH_CONSOL_TBL where UCP_CONSL_PAY_NBR in (SELECT CONSL_PAY_NBR
+FROM PP001.PROVIDER_PAYOR_ADJUSTMENT 
+GROUP BY CONSL_PAY_NBR
+HAVING COUNT(*) = 2
+ORDER BY CONSL_PAY_NBR ASC))
+GROUP BY PROV_TAX_ID_NBR,CP_DSPL_CONSL_PAY_NBR,UCP_CONSL_PAY_NBR,CP_SETL_DT
+ORDER BY CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Get TIN and Electronic Payment Number for PLB</t>
+  </si>
+  <si>
+    <t>SELECT BSP.PROV_TIN_NBR AS PROV_TAX_ID_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+FROM OLE.PORTAL_USER PU 
+LEFT JOIN OLE.PORTAL_USER_BS_TIN PUB ON PUB.PORTAL_USER_ID = PU.PORTAL_USER_ID
+LEFT JOIN OLE.BILLING_SERVICE_PROVIDER BSP ON BSP.BILLING_SERVICE_ID = PUB.BILLING_SERVICE_ID
+LEFT JOIN OLE.SRCH_CONSOL_TBL SCL ON SCL.PROV_TAX_ID_NBR = BSP.PROV_TIN_NBR
+WHERE SCL.CP_PAY_METH_CD = 'ACH' AND PU.SSO_ID='{$id}'
+ORDER BY SCL.CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Get TIN for BS Remit Detail</t>
+  </si>
+  <si>
+    <t>SELECT BSP.PROV_TIN_NBR AS PROV_TAX_ID_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+FROM OLE.PORTAL_USER PU 
+LEFT JOIN OLE.PORTAL_USER_BS_TIN PUB ON PUB.PORTAL_USER_ID = PU.PORTAL_USER_ID
+LEFT JOIN OLE.BILLING_SERVICE_PROVIDER BSP ON BSP.BILLING_SERVICE_ID = PUB.BILLING_SERVICE_ID
+LEFT JOIN OLE.SRCH_CONSOL_TBL SCL ON SCL.PROV_TAX_ID_NBR = BSP.PROV_TIN_NBR
+WHERE SCL.CP_PAY_METH_CD = 'ACH' AND PU.SSO_ID='{$id}'
+GROUP BY BSP.PROV_TIN_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+HAVING COUNT(*) = 4
+ORDER BY SCL.CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Get TIN and electronic payment number for BS Remit Detail for Multiple PLB</t>
+  </si>
+  <si>
+    <t>SELECT BSP.PROV_TIN_NBR AS PROV_TAX_ID_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+FROM OLE.PORTAL_USER PU 
+LEFT JOIN OLE.PORTAL_USER_BS_TIN PUB ON PUB.PORTAL_USER_ID = PU.PORTAL_USER_ID
+LEFT JOIN OLE.BILLING_SERVICE_PROVIDER BSP ON BSP.BILLING_SERVICE_ID = PUB.BILLING_SERVICE_ID
+LEFT JOIN OLE.SRCH_CONSOL_TBL SCL ON SCL.PROV_TAX_ID_NBR = BSP.PROV_TIN_NBR
+WHERE SCL.CP_PAY_METH_CD = 'ACH' AND PU.SSO_ID='{$id}'
+GROUP BY BSP.PROV_TIN_NBR,SCL.CP_DSPL_CONSL_PAY_NBR, SCL.UCP_CONSL_PAY_NBR, SCL.CP_SETL_DT
+HAVING COUNT(*) = 2
+ORDER BY SCL.CP_SETL_DT DESC
+FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>Get TIN and electronic payment number for BS Remit Detail for PLB</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT BS.IDENTIFIER_NBR, BSP.PROV_TIN_NBR AS PROV_TAX_ID_NBR,BS.BS_NM,BSP.REQ_DT,BSP.EFF_DT,BSP.LST_CHG_BY_DTTM
+FROM OLE.BILLING_SERVICE_PROVIDER BSP
+LEFT JOIN OLE.BILLING_SERVICE BS ON BS.BILLING_SERVICE_ID != BSP.BILLING_SERVICE_ID
+LEFT JOIN OLE.ENROLLED_PROVIDER EP ON EP.PROV_TIN_NBR = BSP.PROV_TIN_NBR
+WHERE BSP.STS_CD = 'A' AND BS.ENRL_STS_CD = 'A' AND EP.ENRL_STS_CD = 'A'
+GROUP BY BS.IDENTIFIER_NBR, BSP.PROV_TIN_NBR,BS.BS_NM,BSP.REQ_DT,BSP.EFF_DT,BSP.LST_CHG_BY_DTTM 
+ORDER BY BSP.LST_CHG_BY_DTTM DESC</t>
+  </si>
+  <si>
+    <t>Get TIN for BS and Prov for BS Info Tab</t>
+  </si>
+  <si>
+    <t>SELECT current date AS CURRENT_DATE FROM sysibm.sysdummy1</t>
+  </si>
+  <si>
+    <t>Get Current Date</t>
+  </si>
+  <si>
+    <t>DELETE FROM OLE.BILLING_SERVICE_PROVIDER WHERE PROV_TIN_NBR = '{$tin}'  AND REQ_DT IN (SELECT current date AS CURRENT_DATE FROM sysibm.sysdummy1)</t>
+  </si>
+  <si>
+    <t>Delete Prov Assoc after script run</t>
   </si>
 </sst>
 </file>
@@ -9501,20 +9635,20 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="18.26953125" customWidth="1"/>
-    <col min="12" max="12" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1796875" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -10048,17 +10182,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1612"/>
+  <dimension ref="A1:D1912"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C393" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C401" sqref="C401"/>
+    <sheetView tabSelected="1" topLeftCell="A1885" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1902" sqref="B1902"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="136.54296875" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="136.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -10094,7 +10228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="58">
+    <row r="4" spans="1:3" ht="60">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -10102,7 +10236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -10137,7 +10271,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="29">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -10145,7 +10279,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="87">
+    <row r="10" spans="1:3" ht="90">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -10153,7 +10287,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72.5">
+    <row r="11" spans="1:3" ht="75">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -10161,7 +10295,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.5">
+    <row r="12" spans="1:3" ht="45">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -10169,7 +10303,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="58">
+    <row r="13" spans="1:3" ht="60">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -10185,7 +10319,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="58">
+    <row r="15" spans="1:3" ht="60">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -10193,7 +10327,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29">
+    <row r="16" spans="1:3" ht="30">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -10201,7 +10335,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="30">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -10209,7 +10343,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29">
+    <row r="18" spans="1:3" ht="30">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -10217,7 +10351,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="87">
+    <row r="19" spans="1:3" ht="90">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -10225,7 +10359,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="72.5">
+    <row r="20" spans="1:3" ht="75">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -10233,7 +10367,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29">
+    <row r="21" spans="1:3" ht="30">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
@@ -10241,7 +10375,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5">
+    <row r="22" spans="1:3" ht="75">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -10249,7 +10383,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29">
+    <row r="23" spans="1:3" ht="30">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -10257,7 +10391,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.5">
+    <row r="24" spans="1:3" ht="45">
       <c r="A24" s="5" t="s">
         <v>88</v>
       </c>
@@ -10268,7 +10402,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72.5">
+    <row r="25" spans="1:3" ht="75">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -10284,7 +10418,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="130.5">
+    <row r="27" spans="1:3" ht="135">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -10292,7 +10426,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="87">
+    <row r="28" spans="1:3" ht="90">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
@@ -10300,7 +10434,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="29">
+    <row r="29" spans="1:3" ht="30">
       <c r="A29" s="5" t="s">
         <v>94</v>
       </c>
@@ -10308,7 +10442,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="145">
+    <row r="30" spans="1:3" ht="150">
       <c r="A30" s="5" t="s">
         <v>95</v>
       </c>
@@ -10319,7 +10453,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="159.5">
+    <row r="31" spans="1:3" ht="165">
       <c r="A31" s="5" t="s">
         <v>98</v>
       </c>
@@ -10330,7 +10464,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="159.5">
+    <row r="32" spans="1:3" ht="165">
       <c r="A32" s="5" t="s">
         <v>101</v>
       </c>
@@ -10341,7 +10475,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="188.5">
+    <row r="33" spans="1:4" ht="195">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -10352,7 +10486,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="116">
+    <row r="34" spans="1:4" ht="120">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -10360,7 +10494,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.5">
+    <row r="35" spans="1:4" ht="45">
       <c r="A35" s="5" t="s">
         <v>108</v>
       </c>
@@ -10368,7 +10502,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="116">
+    <row r="36" spans="1:4" ht="120">
       <c r="A36" s="5" t="s">
         <v>113</v>
       </c>
@@ -10379,7 +10513,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="101.5">
+    <row r="37" spans="1:4" ht="105">
       <c r="A37" s="5" t="s">
         <v>112</v>
       </c>
@@ -10390,7 +10524,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="116">
+    <row r="38" spans="1:4" ht="120">
       <c r="A38" s="5" t="s">
         <v>114</v>
       </c>
@@ -10398,7 +10532,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="101.5">
+    <row r="39" spans="1:4" ht="105">
       <c r="A39" s="5" t="s">
         <v>117</v>
       </c>
@@ -10406,7 +10540,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="116">
+    <row r="40" spans="1:4" ht="120">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -10414,7 +10548,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="116">
+    <row r="41" spans="1:4" ht="120">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -10422,7 +10556,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="116">
+    <row r="42" spans="1:4" ht="120">
       <c r="A42" s="5" t="s">
         <v>122</v>
       </c>
@@ -10436,7 +10570,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="174">
+    <row r="43" spans="1:4" ht="180">
       <c r="A43" s="5" t="s">
         <v>124</v>
       </c>
@@ -10447,7 +10581,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="174">
+    <row r="44" spans="1:4" ht="180">
       <c r="A44" s="5" t="s">
         <v>125</v>
       </c>
@@ -10458,7 +10592,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="101.5">
+    <row r="45" spans="1:4" ht="105">
       <c r="A45" s="5" t="s">
         <v>126</v>
       </c>
@@ -10469,7 +10603,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="159.5">
+    <row r="46" spans="1:4" ht="165">
       <c r="A46" s="5" t="s">
         <v>127</v>
       </c>
@@ -10480,7 +10614,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="174">
+    <row r="47" spans="1:4" ht="180">
       <c r="A47" s="5" t="s">
         <v>128</v>
       </c>
@@ -10491,7 +10625,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="174">
+    <row r="48" spans="1:4" ht="180">
       <c r="A48" s="5" t="s">
         <v>129</v>
       </c>
@@ -10502,7 +10636,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="101.5">
+    <row r="49" spans="1:3" ht="105">
       <c r="A49" s="5" t="s">
         <v>130</v>
       </c>
@@ -10513,7 +10647,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="130.5">
+    <row r="50" spans="1:3" ht="135">
       <c r="A50" s="5" t="s">
         <v>131</v>
       </c>
@@ -10524,7 +10658,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="101.5">
+    <row r="51" spans="1:3" ht="105">
       <c r="A51" s="5" t="s">
         <v>132</v>
       </c>
@@ -10535,7 +10669,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="130.5">
+    <row r="52" spans="1:3" ht="135">
       <c r="A52" s="5" t="s">
         <v>133</v>
       </c>
@@ -10546,7 +10680,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="116">
+    <row r="53" spans="1:3" ht="120">
       <c r="A53" s="5" t="s">
         <v>134</v>
       </c>
@@ -10557,7 +10691,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="101.5">
+    <row r="54" spans="1:3" ht="105">
       <c r="A54" s="5" t="s">
         <v>135</v>
       </c>
@@ -10565,7 +10699,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="116">
+    <row r="55" spans="1:3" ht="120">
       <c r="A55" s="5" t="s">
         <v>137</v>
       </c>
@@ -10576,7 +10710,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="116">
+    <row r="56" spans="1:3" ht="120">
       <c r="A56" s="5" t="s">
         <v>138</v>
       </c>
@@ -10584,7 +10718,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="159.5">
+    <row r="57" spans="1:3" ht="165">
       <c r="A57" s="5" t="s">
         <v>144</v>
       </c>
@@ -10595,7 +10729,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="159.5">
+    <row r="58" spans="1:3" ht="165">
       <c r="A58" s="5" t="s">
         <v>145</v>
       </c>
@@ -10603,7 +10737,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="145">
+    <row r="59" spans="1:3" ht="150">
       <c r="A59" s="5" t="s">
         <v>149</v>
       </c>
@@ -10614,7 +10748,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="159.5">
+    <row r="60" spans="1:3" ht="165">
       <c r="A60" s="5" t="s">
         <v>151</v>
       </c>
@@ -10625,7 +10759,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="174">
+    <row r="61" spans="1:3" ht="180">
       <c r="A61" s="5" t="s">
         <v>152</v>
       </c>
@@ -10636,7 +10770,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="116">
+    <row r="62" spans="1:3" ht="120">
       <c r="A62" s="5" t="s">
         <v>153</v>
       </c>
@@ -10647,7 +10781,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.5">
+    <row r="63" spans="1:3" ht="45">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -10655,7 +10789,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="130.5">
+    <row r="64" spans="1:3" ht="135">
       <c r="A64" s="5" t="s">
         <v>173</v>
       </c>
@@ -10666,7 +10800,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="130.5">
+    <row r="65" spans="1:3" ht="135">
       <c r="A65" s="5" t="s">
         <v>174</v>
       </c>
@@ -10709,7 +10843,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="145">
+    <row r="70" spans="1:3" ht="150">
       <c r="A70" s="5" t="s">
         <v>190</v>
       </c>
@@ -10720,7 +10854,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="232">
+    <row r="71" spans="1:3" ht="240">
       <c r="A71" s="5" t="s">
         <v>193</v>
       </c>
@@ -10747,7 +10881,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="29">
+    <row r="74" spans="1:3" ht="30">
       <c r="A74" s="5" t="s">
         <v>276</v>
       </c>
@@ -10755,7 +10889,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="29">
+    <row r="75" spans="1:3" ht="30">
       <c r="A75" s="5" t="s">
         <v>279</v>
       </c>
@@ -10763,7 +10897,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="29">
+    <row r="76" spans="1:3" ht="30">
       <c r="A76" s="5" t="s">
         <v>281</v>
       </c>
@@ -10771,7 +10905,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" ht="30">
       <c r="A77" s="5" t="s">
         <v>353</v>
       </c>
@@ -10803,7 +10937,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="29">
+    <row r="81" spans="1:2" ht="30">
       <c r="A81" s="5" t="s">
         <v>358</v>
       </c>
@@ -10827,7 +10961,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="29">
+    <row r="84" spans="1:2" ht="30">
       <c r="A84" s="5" t="s">
         <v>363</v>
       </c>
@@ -10835,7 +10969,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" ht="30">
       <c r="A85" s="5" t="s">
         <v>364</v>
       </c>
@@ -10843,7 +10977,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="29">
+    <row r="86" spans="1:2" ht="30">
       <c r="A86" s="5" t="s">
         <v>365</v>
       </c>
@@ -10859,7 +10993,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="29">
+    <row r="88" spans="1:2" ht="30">
       <c r="A88" s="5" t="s">
         <v>368</v>
       </c>
@@ -10875,7 +11009,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="29">
+    <row r="90" spans="1:2" ht="30">
       <c r="A90" s="5" t="s">
         <v>381</v>
       </c>
@@ -10923,7 +11057,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="29">
+    <row r="96" spans="1:2" ht="45">
       <c r="A96" s="5" t="s">
         <v>393</v>
       </c>
@@ -10939,7 +11073,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="29">
+    <row r="98" spans="1:3" ht="30">
       <c r="A98" s="5" t="s">
         <v>397</v>
       </c>
@@ -10979,7 +11113,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="188.5">
+    <row r="103" spans="1:3" ht="195">
       <c r="A103" s="5" t="s">
         <v>406</v>
       </c>
@@ -10990,7 +11124,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="275.5">
+    <row r="104" spans="1:3" ht="285">
       <c r="A104" s="5" t="s">
         <v>407</v>
       </c>
@@ -11001,7 +11135,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="232">
+    <row r="105" spans="1:3" ht="240">
       <c r="A105" s="5" t="s">
         <v>409</v>
       </c>
@@ -11012,7 +11146,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" ht="30">
       <c r="A106" s="5" t="s">
         <v>412</v>
       </c>
@@ -11020,7 +11154,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.5">
+    <row r="107" spans="1:3" ht="45">
       <c r="A107" s="5" t="s">
         <v>414</v>
       </c>
@@ -11036,7 +11170,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="116">
+    <row r="109" spans="1:3" ht="120">
       <c r="A109" s="5" t="s">
         <v>421</v>
       </c>
@@ -11219,7 +11353,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="116">
+    <row r="127" spans="1:3" ht="120">
       <c r="A127" s="5" t="s">
         <v>462</v>
       </c>
@@ -11230,7 +11364,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="116">
+    <row r="128" spans="1:3" ht="120">
       <c r="A128" s="5" t="s">
         <v>463</v>
       </c>
@@ -11249,7 +11383,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="174">
+    <row r="130" spans="1:3" ht="180">
       <c r="A130" s="5" t="s">
         <v>466</v>
       </c>
@@ -11260,7 +11394,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="145">
+    <row r="131" spans="1:3" ht="150">
       <c r="A131" s="5" t="s">
         <v>470</v>
       </c>
@@ -11271,7 +11405,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="145">
+    <row r="132" spans="1:3" ht="150">
       <c r="A132" s="5" t="s">
         <v>471</v>
       </c>
@@ -11282,7 +11416,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="130.5">
+    <row r="133" spans="1:3" ht="135">
       <c r="A133" s="5" t="s">
         <v>474</v>
       </c>
@@ -11293,7 +11427,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="130.5">
+    <row r="134" spans="1:3" ht="135">
       <c r="A134" s="5" t="s">
         <v>476</v>
       </c>
@@ -11304,7 +11438,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="130.5">
+    <row r="135" spans="1:3" ht="135">
       <c r="A135" s="5" t="s">
         <v>477</v>
       </c>
@@ -11315,7 +11449,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="130.5">
+    <row r="136" spans="1:3" ht="135">
       <c r="A136" s="5" t="s">
         <v>480</v>
       </c>
@@ -11326,7 +11460,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="130.5">
+    <row r="137" spans="1:3" ht="135">
       <c r="A137" s="5" t="s">
         <v>482</v>
       </c>
@@ -11337,7 +11471,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="130.5">
+    <row r="138" spans="1:3" ht="135">
       <c r="A138" s="5" t="s">
         <v>484</v>
       </c>
@@ -11348,7 +11482,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="130.5">
+    <row r="139" spans="1:3" ht="135">
       <c r="A139" s="5" t="s">
         <v>485</v>
       </c>
@@ -11359,7 +11493,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="130.5">
+    <row r="140" spans="1:3" ht="135">
       <c r="A140" s="5" t="s">
         <v>488</v>
       </c>
@@ -11370,7 +11504,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="130.5">
+    <row r="141" spans="1:3" ht="135">
       <c r="A141" s="5" t="s">
         <v>490</v>
       </c>
@@ -11381,7 +11515,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="130.5">
+    <row r="142" spans="1:3" ht="135">
       <c r="A142" s="5" t="s">
         <v>491</v>
       </c>
@@ -11392,7 +11526,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="116">
+    <row r="143" spans="1:3" ht="120">
       <c r="A143" s="5" t="s">
         <v>497</v>
       </c>
@@ -11403,7 +11537,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="130.5">
+    <row r="144" spans="1:3" ht="135">
       <c r="A144" s="5" t="s">
         <v>500</v>
       </c>
@@ -11414,7 +11548,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="130.5">
+    <row r="145" spans="1:3" ht="135">
       <c r="A145" s="5" t="s">
         <v>501</v>
       </c>
@@ -11425,7 +11559,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="130.5">
+    <row r="146" spans="1:3" ht="135">
       <c r="A146" s="5" t="s">
         <v>503</v>
       </c>
@@ -11436,7 +11570,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="130.5">
+    <row r="147" spans="1:3" ht="135">
       <c r="A147" s="5" t="s">
         <v>506</v>
       </c>
@@ -11447,7 +11581,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="130.5">
+    <row r="148" spans="1:3" ht="135">
       <c r="A148" s="5" t="s">
         <v>507</v>
       </c>
@@ -11502,7 +11636,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="29">
+    <row r="153" spans="1:3" ht="30">
       <c r="A153" s="5" t="s">
         <v>531</v>
       </c>
@@ -11513,7 +11647,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" ht="30">
       <c r="A154" s="5" t="s">
         <v>532</v>
       </c>
@@ -11524,7 +11658,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="87">
+    <row r="155" spans="1:3" ht="90">
       <c r="A155" s="5" t="s">
         <v>534</v>
       </c>
@@ -11535,7 +11669,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.5">
+    <row r="156" spans="1:3" ht="45">
       <c r="A156" s="5" t="s">
         <v>536</v>
       </c>
@@ -11546,7 +11680,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="174">
+    <row r="157" spans="1:3" ht="180">
       <c r="A157" s="5" t="s">
         <v>540</v>
       </c>
@@ -11557,7 +11691,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="159.5">
+    <row r="158" spans="1:3" ht="165">
       <c r="A158" s="5" t="s">
         <v>541</v>
       </c>
@@ -11576,7 +11710,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="72.5">
+    <row r="160" spans="1:3" ht="75">
       <c r="A160" s="5" t="s">
         <v>547</v>
       </c>
@@ -11587,7 +11721,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="58">
+    <row r="161" spans="1:3" ht="60">
       <c r="A161" s="5" t="s">
         <v>551</v>
       </c>
@@ -11595,7 +11729,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.5">
+    <row r="162" spans="1:3" ht="45">
       <c r="A162" s="5" t="s">
         <v>552</v>
       </c>
@@ -11614,7 +11748,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="101.5">
+    <row r="164" spans="1:3" ht="105">
       <c r="A164" s="5" t="s">
         <v>560</v>
       </c>
@@ -11622,7 +11756,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="101.5">
+    <row r="165" spans="1:3" ht="105">
       <c r="A165" s="5" t="s">
         <v>561</v>
       </c>
@@ -11701,7 +11835,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" ht="30">
       <c r="A173" s="5" t="s">
         <v>571</v>
       </c>
@@ -11764,7 +11898,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" ht="30">
       <c r="A179" s="5" t="s">
         <v>577</v>
       </c>
@@ -11775,7 +11909,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="29">
+    <row r="180" spans="1:3" ht="30">
       <c r="A180" s="5" t="s">
         <v>578</v>
       </c>
@@ -11797,7 +11931,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" ht="30">
       <c r="A182" s="5" t="s">
         <v>580</v>
       </c>
@@ -11808,7 +11942,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="116">
+    <row r="183" spans="1:3" ht="120">
       <c r="A183" s="5" t="s">
         <v>581</v>
       </c>
@@ -11863,7 +11997,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="72.5">
+    <row r="188" spans="1:3" ht="75">
       <c r="A188" s="5" t="s">
         <v>586</v>
       </c>
@@ -11874,7 +12008,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="101.5">
+    <row r="189" spans="1:3" ht="105">
       <c r="A189" s="5" t="s">
         <v>587</v>
       </c>
@@ -11885,7 +12019,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="72.5">
+    <row r="190" spans="1:3" ht="75">
       <c r="A190" s="5" t="s">
         <v>667</v>
       </c>
@@ -11896,7 +12030,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="87">
+    <row r="191" spans="1:3" ht="90">
       <c r="A191" s="5" t="s">
         <v>668</v>
       </c>
@@ -11907,7 +12041,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="87">
+    <row r="192" spans="1:3" ht="90">
       <c r="A192" s="5" t="s">
         <v>669</v>
       </c>
@@ -11962,7 +12096,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="29">
+    <row r="197" spans="1:3" ht="30">
       <c r="A197" s="5" t="s">
         <v>674</v>
       </c>
@@ -11973,7 +12107,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="29">
+    <row r="198" spans="1:3" ht="30">
       <c r="A198" s="5" t="s">
         <v>675</v>
       </c>
@@ -11995,7 +12129,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="29">
+    <row r="200" spans="1:3" ht="30">
       <c r="A200" s="5" t="s">
         <v>677</v>
       </c>
@@ -12006,7 +12140,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="87">
+    <row r="201" spans="1:3" ht="90">
       <c r="A201" s="5" t="s">
         <v>678</v>
       </c>
@@ -12017,7 +12151,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72.5">
+    <row r="202" spans="1:3" ht="75">
       <c r="A202" s="5" t="s">
         <v>679</v>
       </c>
@@ -12028,7 +12162,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="87">
+    <row r="203" spans="1:3" ht="90">
       <c r="A203" s="5" t="s">
         <v>680</v>
       </c>
@@ -12039,7 +12173,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29">
+    <row r="204" spans="1:3" ht="30">
       <c r="A204" s="5" t="s">
         <v>681</v>
       </c>
@@ -12058,7 +12192,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="217.5">
+    <row r="206" spans="1:3" ht="240">
       <c r="A206" s="5" t="s">
         <v>683</v>
       </c>
@@ -12080,7 +12214,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="43.5">
+    <row r="208" spans="1:3" ht="45">
       <c r="A208" s="5" t="s">
         <v>685</v>
       </c>
@@ -12091,7 +12225,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="101.5">
+    <row r="209" spans="1:3" ht="105">
       <c r="A209" s="5" t="s">
         <v>686</v>
       </c>
@@ -12135,7 +12269,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="29">
+    <row r="213" spans="1:3" ht="30">
       <c r="A213" s="5" t="s">
         <v>690</v>
       </c>
@@ -12146,7 +12280,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72.5">
+    <row r="214" spans="1:3" ht="75">
       <c r="A214" s="5" t="s">
         <v>691</v>
       </c>
@@ -12157,7 +12291,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="87">
+    <row r="215" spans="1:3" ht="90">
       <c r="A215" s="5" t="s">
         <v>692</v>
       </c>
@@ -12168,7 +12302,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72.5">
+    <row r="216" spans="1:3" ht="75">
       <c r="A216" s="5" t="s">
         <v>693</v>
       </c>
@@ -12179,7 +12313,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="87">
+    <row r="217" spans="1:3" ht="90">
       <c r="A217" s="5" t="s">
         <v>694</v>
       </c>
@@ -12190,7 +12324,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="217.5">
+    <row r="218" spans="1:3" ht="240">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -12212,7 +12346,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="203">
+    <row r="220" spans="1:3" ht="240">
       <c r="A220" s="5" t="s">
         <v>696</v>
       </c>
@@ -12223,7 +12357,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="159.5">
+    <row r="221" spans="1:3" ht="180">
       <c r="A221" s="5" t="s">
         <v>697</v>
       </c>
@@ -12239,7 +12373,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="101.5">
+    <row r="223" spans="1:3" ht="105">
       <c r="A223" s="5" t="s">
         <v>699</v>
       </c>
@@ -12250,7 +12384,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="101.5">
+    <row r="224" spans="1:3" ht="105">
       <c r="A224" s="5" t="s">
         <v>700</v>
       </c>
@@ -12261,7 +12395,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="101.5">
+    <row r="225" spans="1:3" ht="105">
       <c r="A225" s="5" t="s">
         <v>701</v>
       </c>
@@ -12336,7 +12470,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="87">
+    <row r="234" spans="1:3" ht="105">
       <c r="A234" s="5" t="s">
         <v>710</v>
       </c>
@@ -12355,7 +12489,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="87">
+    <row r="236" spans="1:3" ht="90">
       <c r="A236" s="5" t="s">
         <v>712</v>
       </c>
@@ -12388,7 +12522,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="130.5">
+    <row r="239" spans="1:3" ht="135">
       <c r="A239" s="5" t="s">
         <v>715</v>
       </c>
@@ -12399,7 +12533,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="29">
+    <row r="240" spans="1:3" ht="30">
       <c r="A240" s="5" t="s">
         <v>716</v>
       </c>
@@ -12421,7 +12555,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="101.5">
+    <row r="242" spans="1:3" ht="105">
       <c r="A242" s="5" t="s">
         <v>785</v>
       </c>
@@ -12432,7 +12566,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="43.5">
+    <row r="243" spans="1:3" ht="45">
       <c r="A243" s="5" t="s">
         <v>786</v>
       </c>
@@ -12443,7 +12577,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="174">
+    <row r="244" spans="1:3" ht="180">
       <c r="A244" s="5" t="s">
         <v>787</v>
       </c>
@@ -12454,7 +12588,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="217.5">
+    <row r="245" spans="1:3" ht="225">
       <c r="A245" s="5" t="s">
         <v>789</v>
       </c>
@@ -12465,7 +12599,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="174">
+    <row r="246" spans="1:3" ht="180">
       <c r="A246" s="5" t="s">
         <v>794</v>
       </c>
@@ -12476,7 +12610,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="188.5">
+    <row r="247" spans="1:3" ht="195">
       <c r="A247" s="5" t="s">
         <v>799</v>
       </c>
@@ -12487,7 +12621,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="188.5">
+    <row r="248" spans="1:3" ht="195">
       <c r="A248" s="5" t="s">
         <v>802</v>
       </c>
@@ -12498,7 +12632,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="217.5">
+    <row r="249" spans="1:3" ht="225">
       <c r="A249" s="5" t="s">
         <v>805</v>
       </c>
@@ -12509,7 +12643,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="116">
+    <row r="250" spans="1:3" ht="120">
       <c r="A250" s="5" t="s">
         <v>825</v>
       </c>
@@ -12520,7 +12654,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="145">
+    <row r="251" spans="1:3" ht="150">
       <c r="A251" s="5" t="s">
         <v>828</v>
       </c>
@@ -12531,7 +12665,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="116">
+    <row r="252" spans="1:3" ht="120">
       <c r="A252" s="5" t="s">
         <v>831</v>
       </c>
@@ -12553,7 +12687,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="29">
+    <row r="254" spans="1:3" ht="30">
       <c r="A254" s="5" t="s">
         <v>839</v>
       </c>
@@ -12564,7 +12698,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="72.5">
+    <row r="255" spans="1:3" ht="75">
       <c r="A255" s="5" t="s">
         <v>840</v>
       </c>
@@ -12575,7 +12709,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="29">
+    <row r="256" spans="1:3" ht="30">
       <c r="A256" s="5" t="s">
         <v>841</v>
       </c>
@@ -12586,7 +12720,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="72.5">
+    <row r="257" spans="1:3" ht="75">
       <c r="A257" s="5" t="s">
         <v>842</v>
       </c>
@@ -12597,7 +12731,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="145">
+    <row r="258" spans="1:3" ht="150">
       <c r="A258" s="5" t="s">
         <v>848</v>
       </c>
@@ -12619,7 +12753,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="43.5">
+    <row r="260" spans="1:3" ht="45">
       <c r="A260" s="5" t="s">
         <v>852</v>
       </c>
@@ -12630,7 +12764,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="58">
+    <row r="261" spans="1:3" ht="60">
       <c r="A261" s="5" t="s">
         <v>855</v>
       </c>
@@ -12641,7 +12775,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="87">
+    <row r="262" spans="1:3" ht="90">
       <c r="A262" s="5" t="s">
         <v>858</v>
       </c>
@@ -12660,7 +12794,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="58">
+    <row r="264" spans="1:3" ht="60">
       <c r="A264" s="5" t="s">
         <v>863</v>
       </c>
@@ -12671,7 +12805,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="87">
+    <row r="265" spans="1:3" ht="90">
       <c r="A265" s="5" t="s">
         <v>866</v>
       </c>
@@ -12682,7 +12816,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="72.5">
+    <row r="266" spans="1:3" ht="75">
       <c r="A266" s="5" t="s">
         <v>869</v>
       </c>
@@ -12717,7 +12851,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="29">
+    <row r="270" spans="1:3" ht="30">
       <c r="A270" s="5" t="s">
         <v>883</v>
       </c>
@@ -12725,7 +12859,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="101.5">
+    <row r="271" spans="1:3" ht="120">
       <c r="A271" s="5" t="s">
         <v>884</v>
       </c>
@@ -12736,7 +12870,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="43.5">
+    <row r="272" spans="1:3" ht="45">
       <c r="A272" s="5" t="s">
         <v>885</v>
       </c>
@@ -12747,7 +12881,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="29">
+    <row r="273" spans="1:4" ht="30">
       <c r="A273" s="5" t="s">
         <v>886</v>
       </c>
@@ -12758,7 +12892,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="72.5">
+    <row r="274" spans="1:4" ht="75">
       <c r="A274" s="5" t="s">
         <v>890</v>
       </c>
@@ -13406,7 +13540,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="401" spans="1:3" ht="29">
+    <row r="401" spans="1:3" ht="30">
       <c r="A401" s="2" t="s">
         <v>1018</v>
       </c>
@@ -13417,7 +13551,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="402" spans="1:3" ht="72.5">
+    <row r="402" spans="1:3" ht="75">
       <c r="A402" s="2" t="s">
         <v>1019</v>
       </c>
@@ -13428,7 +13562,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="58">
+    <row r="403" spans="1:3" ht="60">
       <c r="A403" s="2" t="s">
         <v>1020</v>
       </c>
@@ -13439,7 +13573,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="29">
+    <row r="404" spans="1:3" ht="30">
       <c r="A404" s="2" t="s">
         <v>1021</v>
       </c>
@@ -13450,7 +13584,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="29">
+    <row r="405" spans="1:3" ht="30">
       <c r="A405" s="2" t="s">
         <v>1022</v>
       </c>
@@ -13461,7 +13595,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="43.5">
+    <row r="406" spans="1:3" ht="60">
       <c r="A406" s="2" t="s">
         <v>1023</v>
       </c>
@@ -13472,7 +13606,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="407" spans="1:3" ht="29">
+    <row r="407" spans="1:3" ht="30">
       <c r="A407" s="2" t="s">
         <v>1024</v>
       </c>
@@ -13483,7 +13617,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="130.5">
+    <row r="408" spans="1:3" ht="135">
       <c r="A408" s="2" t="s">
         <v>1025</v>
       </c>
@@ -13494,7 +13628,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="409" spans="1:3" ht="43.5">
+    <row r="409" spans="1:3" ht="45">
       <c r="A409" s="2" t="s">
         <v>1026</v>
       </c>
@@ -13505,7 +13639,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="410" spans="1:3" ht="29">
+    <row r="410" spans="1:3" ht="30">
       <c r="A410" s="2" t="s">
         <v>1027</v>
       </c>
@@ -13516,7 +13650,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="29">
+    <row r="411" spans="1:3" ht="30">
       <c r="A411" s="2" t="s">
         <v>1028</v>
       </c>
@@ -13527,7 +13661,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="159.5">
+    <row r="412" spans="1:3" ht="165">
       <c r="A412" s="2" t="s">
         <v>1029</v>
       </c>
@@ -13538,7 +13672,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="174">
+    <row r="413" spans="1:3" ht="180">
       <c r="A413" s="2" t="s">
         <v>1030</v>
       </c>
@@ -13549,7 +13683,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="72.5">
+    <row r="414" spans="1:3" ht="75">
       <c r="A414" s="2" t="s">
         <v>1031</v>
       </c>
@@ -13571,7 +13705,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="72.5">
+    <row r="416" spans="1:3" ht="75">
       <c r="A416" s="2" t="s">
         <v>1033</v>
       </c>
@@ -13582,7 +13716,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="116">
+    <row r="417" spans="1:3" ht="120">
       <c r="A417" s="2" t="s">
         <v>1034</v>
       </c>
@@ -13593,7 +13727,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="130.5">
+    <row r="418" spans="1:3" ht="135">
       <c r="A418" s="2" t="s">
         <v>1035</v>
       </c>
@@ -13604,7 +13738,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="29">
+    <row r="419" spans="1:3" ht="30">
       <c r="A419" s="2" t="s">
         <v>1036</v>
       </c>
@@ -13714,7 +13848,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="72.5">
+    <row r="429" spans="1:3" ht="75">
       <c r="A429" s="2" t="s">
         <v>1046</v>
       </c>
@@ -19085,7 +19219,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="1502" spans="1:3" ht="87">
+    <row r="1502" spans="1:3" ht="90">
       <c r="A1502" s="5" t="s">
         <v>2119</v>
       </c>
@@ -19096,7 +19230,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="1503" spans="1:3" ht="87">
+    <row r="1503" spans="1:3" ht="90">
       <c r="A1503" s="5" t="s">
         <v>2120</v>
       </c>
@@ -19107,7 +19241,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="1504" spans="1:3" ht="145">
+    <row r="1504" spans="1:3" ht="150">
       <c r="A1504" s="5" t="s">
         <v>2121</v>
       </c>
@@ -19118,7 +19252,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="1505" spans="1:3" ht="145">
+    <row r="1505" spans="1:3" ht="150">
       <c r="A1505" s="5" t="s">
         <v>2122</v>
       </c>
@@ -19129,7 +19263,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1506" spans="1:3" ht="72.5">
+    <row r="1506" spans="1:3" ht="75">
       <c r="A1506" s="5" t="s">
         <v>2123</v>
       </c>
@@ -19137,7 +19271,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="1507" spans="1:3" ht="43.5">
+    <row r="1507" spans="1:3" ht="45">
       <c r="A1507" s="47" t="s">
         <v>2124</v>
       </c>
@@ -19148,7 +19282,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1508" spans="1:3" ht="43.5">
+    <row r="1508" spans="1:3" ht="45">
       <c r="A1508" s="44" t="s">
         <v>2125</v>
       </c>
@@ -19624,7 +19758,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="1602" spans="1:3" ht="29">
+    <row r="1602" spans="1:3" ht="30">
       <c r="A1602" s="5" t="s">
         <v>2219</v>
       </c>
@@ -19646,7 +19780,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="1604" spans="1:3" ht="58">
+    <row r="1604" spans="1:3" ht="60">
       <c r="A1604" s="5" t="s">
         <v>2221</v>
       </c>
@@ -19657,7 +19791,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="1605" spans="1:3" ht="43.5">
+    <row r="1605" spans="1:3" ht="45">
       <c r="A1605" s="5" t="s">
         <v>2222</v>
       </c>
@@ -19665,7 +19799,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="1606" spans="1:3" ht="101.5">
+    <row r="1606" spans="1:3" ht="105">
       <c r="A1606" s="5" t="s">
         <v>2223</v>
       </c>
@@ -19695,7 +19829,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="1609" spans="1:3" ht="43.5">
+    <row r="1609" spans="1:3" ht="45">
       <c r="A1609" s="5" t="s">
         <v>2278</v>
       </c>
@@ -19706,7 +19840,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="1610" spans="1:3" ht="29">
+    <row r="1610" spans="1:3" ht="30">
       <c r="A1610" s="5" t="s">
         <v>2279</v>
       </c>
@@ -19714,7 +19848,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="1611" spans="1:3" ht="391.5">
+    <row r="1611" spans="1:3" ht="409.5">
       <c r="A1611" s="5" t="s">
         <v>2280</v>
       </c>
@@ -19725,7 +19859,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="1612" spans="1:3" ht="232">
+    <row r="1612" spans="1:3" ht="240">
       <c r="A1612" s="44" t="s">
         <v>2281</v>
       </c>
@@ -19734,6 +19868,130 @@
       </c>
       <c r="C1612" s="46" t="s">
         <v>2286</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:3">
+      <c r="B1901" s="48"/>
+    </row>
+    <row r="1902" spans="1:3" ht="45">
+      <c r="A1902">
+        <v>1901</v>
+      </c>
+      <c r="B1902" s="48" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C1902" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:3" ht="90">
+      <c r="A1903">
+        <v>1902</v>
+      </c>
+      <c r="B1903" s="48" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1903" t="s">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="1904" spans="1:3" ht="225">
+      <c r="A1904">
+        <v>1903</v>
+      </c>
+      <c r="B1904" s="48" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1904" t="s">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="1905" spans="1:3" ht="150">
+      <c r="A1905">
+        <v>1904</v>
+      </c>
+      <c r="B1905" s="48" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C1905" t="s">
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="1906" spans="1:3" ht="150">
+      <c r="A1906">
+        <v>1905</v>
+      </c>
+      <c r="B1906" s="48" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C1906" t="s">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="1907" spans="1:3" ht="120">
+      <c r="A1907">
+        <v>1906</v>
+      </c>
+      <c r="B1907" s="48" t="s">
+        <v>2325</v>
+      </c>
+      <c r="C1907" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:3" ht="150">
+      <c r="A1908">
+        <v>1907</v>
+      </c>
+      <c r="B1908" s="48" t="s">
+        <v>2327</v>
+      </c>
+      <c r="C1908" t="s">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="1909" spans="1:3" ht="150">
+      <c r="A1909">
+        <v>1908</v>
+      </c>
+      <c r="B1909" s="48" t="s">
+        <v>2329</v>
+      </c>
+      <c r="C1909" t="s">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="1910" spans="1:3" ht="105">
+      <c r="A1910">
+        <v>1909</v>
+      </c>
+      <c r="B1910" s="48" t="s">
+        <v>2331</v>
+      </c>
+      <c r="C1910" t="s">
+        <v>2332</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:3">
+      <c r="A1911">
+        <v>1910</v>
+      </c>
+      <c r="B1911" t="s">
+        <v>2333</v>
+      </c>
+      <c r="C1911" t="s">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:3">
+      <c r="A1912">
+        <v>1911</v>
+      </c>
+      <c r="B1912" t="s">
+        <v>2335</v>
+      </c>
+      <c r="C1912" t="s">
+        <v>2336</v>
       </c>
     </row>
   </sheetData>
@@ -19751,13 +20009,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -19937,10 +20195,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -20263,7 +20521,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16">
+    <row r="44" spans="1:2">
       <c r="A44" s="13" t="s">
         <v>263</v>
       </c>
@@ -20353,13 +20611,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="85.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>283</v>
       </c>
@@ -20367,7 +20625,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>285</v>
       </c>
@@ -20375,7 +20633,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>287</v>
       </c>
@@ -20383,7 +20641,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
       <c r="A4" s="25" t="s">
         <v>289</v>
       </c>
@@ -20391,7 +20649,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
       <c r="A5" s="25" t="s">
         <v>291</v>
       </c>
@@ -20399,7 +20657,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1">
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
       <c r="A6" s="25" t="s">
         <v>293</v>
       </c>
@@ -20407,7 +20665,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1">
       <c r="A7" s="25" t="s">
         <v>295</v>
       </c>
@@ -20415,7 +20673,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1">
       <c r="A8" s="25" t="s">
         <v>297</v>
       </c>
@@ -20423,7 +20681,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1">
       <c r="A9" s="25" t="s">
         <v>299</v>
       </c>
@@ -20431,7 +20689,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1">
       <c r="A10" s="25" t="s">
         <v>301</v>
       </c>
@@ -20439,7 +20697,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1">
       <c r="A11" s="25" t="s">
         <v>303</v>
       </c>
@@ -20447,7 +20705,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1">
       <c r="A12" s="25" t="s">
         <v>305</v>
       </c>
@@ -20455,7 +20713,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1">
       <c r="A13" s="25" t="s">
         <v>307</v>
       </c>
@@ -20463,7 +20721,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>309</v>
       </c>
@@ -20471,7 +20729,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1">
       <c r="A15" s="25" t="s">
         <v>311</v>
       </c>
@@ -20479,7 +20737,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1">
+    <row r="16" spans="1:2" ht="15.75" thickBot="1">
       <c r="A16" s="25" t="s">
         <v>313</v>
       </c>
@@ -20487,7 +20745,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1">
       <c r="A17" s="25" t="s">
         <v>315</v>
       </c>
@@ -20495,7 +20753,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1">
+    <row r="18" spans="1:2" ht="15.75" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>317</v>
       </c>
@@ -20503,7 +20761,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1">
       <c r="A19" s="25" t="s">
         <v>319</v>
       </c>
@@ -20511,7 +20769,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1">
+    <row r="20" spans="1:2" ht="15.75" thickBot="1">
       <c r="A20" s="25" t="s">
         <v>321</v>
       </c>
@@ -20519,7 +20777,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1">
       <c r="A21" s="25" t="s">
         <v>323</v>
       </c>
@@ -20527,7 +20785,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1">
+    <row r="22" spans="1:2" ht="15.75" thickBot="1">
       <c r="A22" s="25" t="s">
         <v>325</v>
       </c>
@@ -20535,7 +20793,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1">
+    <row r="23" spans="1:2" ht="15.75" thickBot="1">
       <c r="A23" s="25" t="s">
         <v>327</v>
       </c>
@@ -20543,7 +20801,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1">
+    <row r="24" spans="1:2" ht="15.75" thickBot="1">
       <c r="A24" s="25" t="s">
         <v>329</v>
       </c>
@@ -20551,7 +20809,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1">
       <c r="A25" s="25" t="s">
         <v>331</v>
       </c>
@@ -20559,7 +20817,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1">
+    <row r="26" spans="1:2" ht="15.75" thickBot="1">
       <c r="A26" s="25" t="s">
         <v>333</v>
       </c>
@@ -20567,7 +20825,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1">
+    <row r="27" spans="1:2" ht="15.75" thickBot="1">
       <c r="A27" s="25" t="s">
         <v>335</v>
       </c>
@@ -20575,7 +20833,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1">
+    <row r="28" spans="1:2" ht="15.75" thickBot="1">
       <c r="A28" s="25" t="s">
         <v>337</v>
       </c>
@@ -20583,7 +20841,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1">
+    <row r="29" spans="1:2" ht="15.75" thickBot="1">
       <c r="A29" s="25" t="s">
         <v>339</v>
       </c>
@@ -20591,7 +20849,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1">
+    <row r="30" spans="1:2" ht="15.75" thickBot="1">
       <c r="A30" s="25" t="s">
         <v>341</v>
       </c>
@@ -20599,7 +20857,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1">
+    <row r="31" spans="1:2" ht="15.75" thickBot="1">
       <c r="A31" s="25" t="s">
         <v>343</v>
       </c>
@@ -20607,7 +20865,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1">
+    <row r="32" spans="1:2" ht="15.75" thickBot="1">
       <c r="A32" s="25" t="s">
         <v>345</v>
       </c>
@@ -20615,7 +20873,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1">
+    <row r="33" spans="1:2" ht="15.75" thickBot="1">
       <c r="A33" s="25" t="s">
         <v>347</v>
       </c>
@@ -20623,7 +20881,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1">
+    <row r="34" spans="1:2" ht="15.75" thickBot="1">
       <c r="A34" s="25" t="s">
         <v>349</v>
       </c>
@@ -20631,7 +20889,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1">
+    <row r="35" spans="1:2" ht="15.75" thickBot="1">
       <c r="A35" s="25" t="s">
         <v>351</v>
       </c>

</xml_diff>

<commit_message>
Optum Pay Solution changes
Optum Pay Solution changes and Before you begin Enrollment change,FII -RTN header title validations
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tathyush\Desktop\Team Members Autmation\updated master\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrish38\Documents\GitCucumber\RB-116.x\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE2C517-EED4-4F83-A655-081A5AB86E3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3455A05-C367-4FC7-8E81-17A236125220}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="2337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="2346">
   <si>
     <t>City</t>
   </si>
@@ -8903,6 +8905,37 @@
   </si>
   <si>
     <t>Delete Prov Assoc after script run</t>
+  </si>
+  <si>
+    <t>select cast(CLOB_VAL as varchar(32000)) as clobvalfrom,TEXT_VAL from ole.content where CONT_NM like '%BeginEnrollmentPage%' order by CREAT_DTTM desc</t>
+  </si>
+  <si>
+    <t>BeginEnrollment page</t>
+  </si>
+  <si>
+    <t>1612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select TEXT_VAL from OLE.CONTENT where CONT_NM like '%Text for Authorized Agent%' </t>
+  </si>
+  <si>
+    <t>FII-RTN Bank header text</t>
+  </si>
+  <si>
+    <t>select * from OLE.PRODUCT_SELECTION where PROV_TIN_NBR='{$Prov_Tin}'</t>
+  </si>
+  <si>
+    <t>TIN whose debit fee is not null</t>
+  </si>
+  <si>
+    <t>SELECT dfa.PROV_TIN_NBR as PROV_TAX_ID_NBR 
+FROM OLE.DEBIT_FEE_ACCRD dfa,OLE.PRODUCT_SELECTION ps
+WHERE ps.PROV_TIN_NBR=dfa.PROV_TIN_NBR AND
+ps.PRTL_PRDCT_SELECTED_GRP_NM='Premium' AND
+dfa.DBT_FEE_ACCRD_AMT {$nullStatus} AND dfa.PROC_DT between CURRENT_DATE - (DAY(CURRENT_DATE)-1) DAYS and LAST_DAY(CURRENT DATE) order by dfa.PROV_TIN_NBR desc fetch first 1 rows only with ur</t>
+  </si>
+  <si>
+    <t>Select SUM(DBT_FEE_ACCRD_AMT) as ACCRDFEE from OLE.DEBIT_FEE_ACCRD dfa where PROV_TIN_NBR='{$tin}' AND dfa.PROC_DT between CURRENT_DATE - (DAY(CURRENT_DATE)-1) DAYS and LAST_DAY(CURRENT DATE)</t>
   </si>
 </sst>
 </file>
@@ -9635,20 +9668,20 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.26953125" customWidth="1"/>
+    <col min="12" max="12" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -10184,15 +10217,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1912"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1885" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1902" sqref="B1902"/>
+    <sheetView tabSelected="1" topLeftCell="A1613" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1616" sqref="B1616"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="136.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="136.54296875" customWidth="1"/>
+    <col min="3" max="3" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -10228,7 +10261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60">
+    <row r="4" spans="1:3" ht="58">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -10236,7 +10269,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="29">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -10271,7 +10304,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="29">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -10279,7 +10312,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="90">
+    <row r="10" spans="1:3" ht="87">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -10287,7 +10320,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="75">
+    <row r="11" spans="1:3" ht="72.5">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -10295,7 +10328,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="43.5">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -10303,7 +10336,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60">
+    <row r="13" spans="1:3" ht="58">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -10319,7 +10352,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60">
+    <row r="15" spans="1:3" ht="58">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -10327,7 +10360,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30">
+    <row r="16" spans="1:3" ht="29">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -10335,7 +10368,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -10343,7 +10376,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -10351,7 +10384,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90">
+    <row r="19" spans="1:3" ht="87">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -10359,7 +10392,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75">
+    <row r="20" spans="1:3" ht="72.5">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -10367,7 +10400,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="29">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
@@ -10375,7 +10408,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -10383,7 +10416,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="29">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -10391,7 +10424,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="45">
+    <row r="24" spans="1:3" ht="43.5">
       <c r="A24" s="5" t="s">
         <v>88</v>
       </c>
@@ -10402,7 +10435,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="75">
+    <row r="25" spans="1:3" ht="72.5">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -10418,7 +10451,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="135">
+    <row r="27" spans="1:3" ht="130.5">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -10426,7 +10459,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="90">
+    <row r="28" spans="1:3" ht="87">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
@@ -10434,7 +10467,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="29">
       <c r="A29" s="5" t="s">
         <v>94</v>
       </c>
@@ -10442,7 +10475,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="150">
+    <row r="30" spans="1:3" ht="145">
       <c r="A30" s="5" t="s">
         <v>95</v>
       </c>
@@ -10453,7 +10486,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="165">
+    <row r="31" spans="1:3" ht="159.5">
       <c r="A31" s="5" t="s">
         <v>98</v>
       </c>
@@ -10464,7 +10497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="165">
+    <row r="32" spans="1:3" ht="159.5">
       <c r="A32" s="5" t="s">
         <v>101</v>
       </c>
@@ -10475,7 +10508,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="195">
+    <row r="33" spans="1:4" ht="188.5">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -10486,7 +10519,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="120">
+    <row r="34" spans="1:4" ht="116">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -10494,7 +10527,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45">
+    <row r="35" spans="1:4" ht="43.5">
       <c r="A35" s="5" t="s">
         <v>108</v>
       </c>
@@ -10502,7 +10535,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="120">
+    <row r="36" spans="1:4" ht="116">
       <c r="A36" s="5" t="s">
         <v>113</v>
       </c>
@@ -10513,7 +10546,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="105">
+    <row r="37" spans="1:4" ht="101.5">
       <c r="A37" s="5" t="s">
         <v>112</v>
       </c>
@@ -10524,7 +10557,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="120">
+    <row r="38" spans="1:4" ht="116">
       <c r="A38" s="5" t="s">
         <v>114</v>
       </c>
@@ -10532,7 +10565,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="105">
+    <row r="39" spans="1:4" ht="101.5">
       <c r="A39" s="5" t="s">
         <v>117</v>
       </c>
@@ -10540,7 +10573,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="120">
+    <row r="40" spans="1:4" ht="116">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -10548,7 +10581,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="120">
+    <row r="41" spans="1:4" ht="116">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -10556,7 +10589,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="120">
+    <row r="42" spans="1:4" ht="116">
       <c r="A42" s="5" t="s">
         <v>122</v>
       </c>
@@ -10570,7 +10603,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="180">
+    <row r="43" spans="1:4" ht="174">
       <c r="A43" s="5" t="s">
         <v>124</v>
       </c>
@@ -10581,7 +10614,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="180">
+    <row r="44" spans="1:4" ht="174">
       <c r="A44" s="5" t="s">
         <v>125</v>
       </c>
@@ -10592,7 +10625,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="105">
+    <row r="45" spans="1:4" ht="101.5">
       <c r="A45" s="5" t="s">
         <v>126</v>
       </c>
@@ -10603,7 +10636,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="165">
+    <row r="46" spans="1:4" ht="159.5">
       <c r="A46" s="5" t="s">
         <v>127</v>
       </c>
@@ -10614,7 +10647,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="180">
+    <row r="47" spans="1:4" ht="174">
       <c r="A47" s="5" t="s">
         <v>128</v>
       </c>
@@ -10625,7 +10658,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="180">
+    <row r="48" spans="1:4" ht="174">
       <c r="A48" s="5" t="s">
         <v>129</v>
       </c>
@@ -10636,7 +10669,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="105">
+    <row r="49" spans="1:3" ht="101.5">
       <c r="A49" s="5" t="s">
         <v>130</v>
       </c>
@@ -10647,7 +10680,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="135">
+    <row r="50" spans="1:3" ht="130.5">
       <c r="A50" s="5" t="s">
         <v>131</v>
       </c>
@@ -10658,7 +10691,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="105">
+    <row r="51" spans="1:3" ht="101.5">
       <c r="A51" s="5" t="s">
         <v>132</v>
       </c>
@@ -10669,7 +10702,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="135">
+    <row r="52" spans="1:3" ht="130.5">
       <c r="A52" s="5" t="s">
         <v>133</v>
       </c>
@@ -10680,7 +10713,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="120">
+    <row r="53" spans="1:3" ht="116">
       <c r="A53" s="5" t="s">
         <v>134</v>
       </c>
@@ -10691,7 +10724,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="105">
+    <row r="54" spans="1:3" ht="101.5">
       <c r="A54" s="5" t="s">
         <v>135</v>
       </c>
@@ -10699,7 +10732,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="120">
+    <row r="55" spans="1:3" ht="116">
       <c r="A55" s="5" t="s">
         <v>137</v>
       </c>
@@ -10710,7 +10743,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="120">
+    <row r="56" spans="1:3" ht="116">
       <c r="A56" s="5" t="s">
         <v>138</v>
       </c>
@@ -10718,7 +10751,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="165">
+    <row r="57" spans="1:3" ht="159.5">
       <c r="A57" s="5" t="s">
         <v>144</v>
       </c>
@@ -10729,7 +10762,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="165">
+    <row r="58" spans="1:3" ht="159.5">
       <c r="A58" s="5" t="s">
         <v>145</v>
       </c>
@@ -10737,7 +10770,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="150">
+    <row r="59" spans="1:3" ht="145">
       <c r="A59" s="5" t="s">
         <v>149</v>
       </c>
@@ -10748,7 +10781,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="165">
+    <row r="60" spans="1:3" ht="159.5">
       <c r="A60" s="5" t="s">
         <v>151</v>
       </c>
@@ -10759,7 +10792,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="180">
+    <row r="61" spans="1:3" ht="174">
       <c r="A61" s="5" t="s">
         <v>152</v>
       </c>
@@ -10770,7 +10803,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="120">
+    <row r="62" spans="1:3" ht="116">
       <c r="A62" s="5" t="s">
         <v>153</v>
       </c>
@@ -10781,7 +10814,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="45">
+    <row r="63" spans="1:3" ht="43.5">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -10789,7 +10822,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="135">
+    <row r="64" spans="1:3" ht="130.5">
       <c r="A64" s="5" t="s">
         <v>173</v>
       </c>
@@ -10800,7 +10833,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="135">
+    <row r="65" spans="1:3" ht="130.5">
       <c r="A65" s="5" t="s">
         <v>174</v>
       </c>
@@ -10843,7 +10876,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="150">
+    <row r="70" spans="1:3" ht="145">
       <c r="A70" s="5" t="s">
         <v>190</v>
       </c>
@@ -10854,7 +10887,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="240">
+    <row r="71" spans="1:3" ht="232">
       <c r="A71" s="5" t="s">
         <v>193</v>
       </c>
@@ -10881,7 +10914,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="30">
+    <row r="74" spans="1:3" ht="29">
       <c r="A74" s="5" t="s">
         <v>276</v>
       </c>
@@ -10889,7 +10922,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="30">
+    <row r="75" spans="1:3" ht="29">
       <c r="A75" s="5" t="s">
         <v>279</v>
       </c>
@@ -10897,7 +10930,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="30">
+    <row r="76" spans="1:3" ht="29">
       <c r="A76" s="5" t="s">
         <v>281</v>
       </c>
@@ -10905,7 +10938,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="30">
+    <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
         <v>353</v>
       </c>
@@ -10937,7 +10970,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="30">
+    <row r="81" spans="1:2" ht="29">
       <c r="A81" s="5" t="s">
         <v>358</v>
       </c>
@@ -10961,7 +10994,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="30">
+    <row r="84" spans="1:2" ht="29">
       <c r="A84" s="5" t="s">
         <v>363</v>
       </c>
@@ -10969,7 +11002,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="30">
+    <row r="85" spans="1:2">
       <c r="A85" s="5" t="s">
         <v>364</v>
       </c>
@@ -10977,7 +11010,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30">
+    <row r="86" spans="1:2" ht="29">
       <c r="A86" s="5" t="s">
         <v>365</v>
       </c>
@@ -10993,7 +11026,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="30">
+    <row r="88" spans="1:2" ht="29">
       <c r="A88" s="5" t="s">
         <v>368</v>
       </c>
@@ -11009,7 +11042,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="30">
+    <row r="90" spans="1:2" ht="29">
       <c r="A90" s="5" t="s">
         <v>381</v>
       </c>
@@ -11057,7 +11090,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="45">
+    <row r="96" spans="1:2" ht="29">
       <c r="A96" s="5" t="s">
         <v>393</v>
       </c>
@@ -11073,7 +11106,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="30">
+    <row r="98" spans="1:3" ht="29">
       <c r="A98" s="5" t="s">
         <v>397</v>
       </c>
@@ -11113,7 +11146,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="195">
+    <row r="103" spans="1:3" ht="188.5">
       <c r="A103" s="5" t="s">
         <v>406</v>
       </c>
@@ -11124,7 +11157,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="285">
+    <row r="104" spans="1:3" ht="275.5">
       <c r="A104" s="5" t="s">
         <v>407</v>
       </c>
@@ -11135,7 +11168,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="240">
+    <row r="105" spans="1:3" ht="232">
       <c r="A105" s="5" t="s">
         <v>409</v>
       </c>
@@ -11146,7 +11179,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="30">
+    <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
         <v>412</v>
       </c>
@@ -11154,7 +11187,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="45">
+    <row r="107" spans="1:3" ht="43.5">
       <c r="A107" s="5" t="s">
         <v>414</v>
       </c>
@@ -11170,7 +11203,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="120">
+    <row r="109" spans="1:3" ht="116">
       <c r="A109" s="5" t="s">
         <v>421</v>
       </c>
@@ -11353,7 +11386,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="120">
+    <row r="127" spans="1:3" ht="116">
       <c r="A127" s="5" t="s">
         <v>462</v>
       </c>
@@ -11364,7 +11397,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="120">
+    <row r="128" spans="1:3" ht="116">
       <c r="A128" s="5" t="s">
         <v>463</v>
       </c>
@@ -11383,7 +11416,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="180">
+    <row r="130" spans="1:3" ht="174">
       <c r="A130" s="5" t="s">
         <v>466</v>
       </c>
@@ -11394,7 +11427,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="150">
+    <row r="131" spans="1:3" ht="145">
       <c r="A131" s="5" t="s">
         <v>470</v>
       </c>
@@ -11405,7 +11438,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="150">
+    <row r="132" spans="1:3" ht="145">
       <c r="A132" s="5" t="s">
         <v>471</v>
       </c>
@@ -11416,7 +11449,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="135">
+    <row r="133" spans="1:3" ht="130.5">
       <c r="A133" s="5" t="s">
         <v>474</v>
       </c>
@@ -11427,7 +11460,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="135">
+    <row r="134" spans="1:3" ht="130.5">
       <c r="A134" s="5" t="s">
         <v>476</v>
       </c>
@@ -11438,7 +11471,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="135">
+    <row r="135" spans="1:3" ht="130.5">
       <c r="A135" s="5" t="s">
         <v>477</v>
       </c>
@@ -11449,7 +11482,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="135">
+    <row r="136" spans="1:3" ht="130.5">
       <c r="A136" s="5" t="s">
         <v>480</v>
       </c>
@@ -11460,7 +11493,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="135">
+    <row r="137" spans="1:3" ht="130.5">
       <c r="A137" s="5" t="s">
         <v>482</v>
       </c>
@@ -11471,7 +11504,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="135">
+    <row r="138" spans="1:3" ht="130.5">
       <c r="A138" s="5" t="s">
         <v>484</v>
       </c>
@@ -11482,7 +11515,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="135">
+    <row r="139" spans="1:3" ht="130.5">
       <c r="A139" s="5" t="s">
         <v>485</v>
       </c>
@@ -11493,7 +11526,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="135">
+    <row r="140" spans="1:3" ht="130.5">
       <c r="A140" s="5" t="s">
         <v>488</v>
       </c>
@@ -11504,7 +11537,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="135">
+    <row r="141" spans="1:3" ht="130.5">
       <c r="A141" s="5" t="s">
         <v>490</v>
       </c>
@@ -11515,7 +11548,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="135">
+    <row r="142" spans="1:3" ht="130.5">
       <c r="A142" s="5" t="s">
         <v>491</v>
       </c>
@@ -11526,7 +11559,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="120">
+    <row r="143" spans="1:3" ht="116">
       <c r="A143" s="5" t="s">
         <v>497</v>
       </c>
@@ -11537,7 +11570,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="135">
+    <row r="144" spans="1:3" ht="130.5">
       <c r="A144" s="5" t="s">
         <v>500</v>
       </c>
@@ -11548,7 +11581,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="135">
+    <row r="145" spans="1:3" ht="130.5">
       <c r="A145" s="5" t="s">
         <v>501</v>
       </c>
@@ -11559,7 +11592,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="135">
+    <row r="146" spans="1:3" ht="130.5">
       <c r="A146" s="5" t="s">
         <v>503</v>
       </c>
@@ -11570,7 +11603,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="135">
+    <row r="147" spans="1:3" ht="130.5">
       <c r="A147" s="5" t="s">
         <v>506</v>
       </c>
@@ -11581,7 +11614,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="135">
+    <row r="148" spans="1:3" ht="130.5">
       <c r="A148" s="5" t="s">
         <v>507</v>
       </c>
@@ -11636,7 +11669,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="30">
+    <row r="153" spans="1:3" ht="29">
       <c r="A153" s="5" t="s">
         <v>531</v>
       </c>
@@ -11647,7 +11680,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="30">
+    <row r="154" spans="1:3">
       <c r="A154" s="5" t="s">
         <v>532</v>
       </c>
@@ -11658,7 +11691,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="90">
+    <row r="155" spans="1:3" ht="87">
       <c r="A155" s="5" t="s">
         <v>534</v>
       </c>
@@ -11669,7 +11702,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="45">
+    <row r="156" spans="1:3" ht="43.5">
       <c r="A156" s="5" t="s">
         <v>536</v>
       </c>
@@ -11680,7 +11713,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="180">
+    <row r="157" spans="1:3" ht="174">
       <c r="A157" s="5" t="s">
         <v>540</v>
       </c>
@@ -11691,7 +11724,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="165">
+    <row r="158" spans="1:3" ht="159.5">
       <c r="A158" s="5" t="s">
         <v>541</v>
       </c>
@@ -11710,7 +11743,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="75">
+    <row r="160" spans="1:3" ht="72.5">
       <c r="A160" s="5" t="s">
         <v>547</v>
       </c>
@@ -11721,7 +11754,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="60">
+    <row r="161" spans="1:3" ht="58">
       <c r="A161" s="5" t="s">
         <v>551</v>
       </c>
@@ -11729,7 +11762,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="45">
+    <row r="162" spans="1:3" ht="43.5">
       <c r="A162" s="5" t="s">
         <v>552</v>
       </c>
@@ -11748,7 +11781,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="105">
+    <row r="164" spans="1:3" ht="101.5">
       <c r="A164" s="5" t="s">
         <v>560</v>
       </c>
@@ -11756,7 +11789,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="105">
+    <row r="165" spans="1:3" ht="101.5">
       <c r="A165" s="5" t="s">
         <v>561</v>
       </c>
@@ -11835,7 +11868,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="30">
+    <row r="173" spans="1:3">
       <c r="A173" s="5" t="s">
         <v>571</v>
       </c>
@@ -11898,7 +11931,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="30">
+    <row r="179" spans="1:3">
       <c r="A179" s="5" t="s">
         <v>577</v>
       </c>
@@ -11909,7 +11942,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="30">
+    <row r="180" spans="1:3" ht="29">
       <c r="A180" s="5" t="s">
         <v>578</v>
       </c>
@@ -11931,7 +11964,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="30">
+    <row r="182" spans="1:3">
       <c r="A182" s="5" t="s">
         <v>580</v>
       </c>
@@ -11942,7 +11975,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="120">
+    <row r="183" spans="1:3" ht="116">
       <c r="A183" s="5" t="s">
         <v>581</v>
       </c>
@@ -11997,7 +12030,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="75">
+    <row r="188" spans="1:3" ht="72.5">
       <c r="A188" s="5" t="s">
         <v>586</v>
       </c>
@@ -12008,7 +12041,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="105">
+    <row r="189" spans="1:3" ht="101.5">
       <c r="A189" s="5" t="s">
         <v>587</v>
       </c>
@@ -12019,7 +12052,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="75">
+    <row r="190" spans="1:3" ht="72.5">
       <c r="A190" s="5" t="s">
         <v>667</v>
       </c>
@@ -12030,7 +12063,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="90">
+    <row r="191" spans="1:3" ht="87">
       <c r="A191" s="5" t="s">
         <v>668</v>
       </c>
@@ -12041,7 +12074,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="90">
+    <row r="192" spans="1:3" ht="87">
       <c r="A192" s="5" t="s">
         <v>669</v>
       </c>
@@ -12096,7 +12129,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="30">
+    <row r="197" spans="1:3" ht="29">
       <c r="A197" s="5" t="s">
         <v>674</v>
       </c>
@@ -12107,7 +12140,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="30">
+    <row r="198" spans="1:3" ht="29">
       <c r="A198" s="5" t="s">
         <v>675</v>
       </c>
@@ -12129,7 +12162,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="30">
+    <row r="200" spans="1:3" ht="29">
       <c r="A200" s="5" t="s">
         <v>677</v>
       </c>
@@ -12140,7 +12173,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="90">
+    <row r="201" spans="1:3" ht="87">
       <c r="A201" s="5" t="s">
         <v>678</v>
       </c>
@@ -12151,7 +12184,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="75">
+    <row r="202" spans="1:3" ht="72.5">
       <c r="A202" s="5" t="s">
         <v>679</v>
       </c>
@@ -12162,7 +12195,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="90">
+    <row r="203" spans="1:3" ht="87">
       <c r="A203" s="5" t="s">
         <v>680</v>
       </c>
@@ -12173,7 +12206,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="30">
+    <row r="204" spans="1:3" ht="29">
       <c r="A204" s="5" t="s">
         <v>681</v>
       </c>
@@ -12192,7 +12225,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="240">
+    <row r="206" spans="1:3" ht="217.5">
       <c r="A206" s="5" t="s">
         <v>683</v>
       </c>
@@ -12214,7 +12247,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="45">
+    <row r="208" spans="1:3" ht="43.5">
       <c r="A208" s="5" t="s">
         <v>685</v>
       </c>
@@ -12225,7 +12258,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="105">
+    <row r="209" spans="1:3" ht="101.5">
       <c r="A209" s="5" t="s">
         <v>686</v>
       </c>
@@ -12269,7 +12302,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="30">
+    <row r="213" spans="1:3" ht="29">
       <c r="A213" s="5" t="s">
         <v>690</v>
       </c>
@@ -12280,7 +12313,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="75">
+    <row r="214" spans="1:3" ht="72.5">
       <c r="A214" s="5" t="s">
         <v>691</v>
       </c>
@@ -12291,7 +12324,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="90">
+    <row r="215" spans="1:3" ht="87">
       <c r="A215" s="5" t="s">
         <v>692</v>
       </c>
@@ -12302,7 +12335,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="75">
+    <row r="216" spans="1:3" ht="72.5">
       <c r="A216" s="5" t="s">
         <v>693</v>
       </c>
@@ -12313,7 +12346,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="90">
+    <row r="217" spans="1:3" ht="87">
       <c r="A217" s="5" t="s">
         <v>694</v>
       </c>
@@ -12324,7 +12357,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="240">
+    <row r="218" spans="1:3" ht="217.5">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -12346,7 +12379,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="240">
+    <row r="220" spans="1:3" ht="203">
       <c r="A220" s="5" t="s">
         <v>696</v>
       </c>
@@ -12357,7 +12390,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="180">
+    <row r="221" spans="1:3" ht="159.5">
       <c r="A221" s="5" t="s">
         <v>697</v>
       </c>
@@ -12373,7 +12406,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="105">
+    <row r="223" spans="1:3" ht="101.5">
       <c r="A223" s="5" t="s">
         <v>699</v>
       </c>
@@ -12384,7 +12417,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="105">
+    <row r="224" spans="1:3" ht="101.5">
       <c r="A224" s="5" t="s">
         <v>700</v>
       </c>
@@ -12395,7 +12428,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="105">
+    <row r="225" spans="1:3" ht="101.5">
       <c r="A225" s="5" t="s">
         <v>701</v>
       </c>
@@ -12470,7 +12503,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="105">
+    <row r="234" spans="1:3" ht="87">
       <c r="A234" s="5" t="s">
         <v>710</v>
       </c>
@@ -12489,7 +12522,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="90">
+    <row r="236" spans="1:3" ht="87">
       <c r="A236" s="5" t="s">
         <v>712</v>
       </c>
@@ -12522,7 +12555,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="135">
+    <row r="239" spans="1:3" ht="130.5">
       <c r="A239" s="5" t="s">
         <v>715</v>
       </c>
@@ -12533,7 +12566,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="30">
+    <row r="240" spans="1:3" ht="29">
       <c r="A240" s="5" t="s">
         <v>716</v>
       </c>
@@ -12555,7 +12588,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="105">
+    <row r="242" spans="1:3" ht="101.5">
       <c r="A242" s="5" t="s">
         <v>785</v>
       </c>
@@ -12566,7 +12599,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="45">
+    <row r="243" spans="1:3" ht="43.5">
       <c r="A243" s="5" t="s">
         <v>786</v>
       </c>
@@ -12577,7 +12610,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="180">
+    <row r="244" spans="1:3" ht="174">
       <c r="A244" s="5" t="s">
         <v>787</v>
       </c>
@@ -12588,7 +12621,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="225">
+    <row r="245" spans="1:3" ht="217.5">
       <c r="A245" s="5" t="s">
         <v>789</v>
       </c>
@@ -12599,7 +12632,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="180">
+    <row r="246" spans="1:3" ht="174">
       <c r="A246" s="5" t="s">
         <v>794</v>
       </c>
@@ -12610,7 +12643,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="195">
+    <row r="247" spans="1:3" ht="188.5">
       <c r="A247" s="5" t="s">
         <v>799</v>
       </c>
@@ -12621,7 +12654,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="195">
+    <row r="248" spans="1:3" ht="188.5">
       <c r="A248" s="5" t="s">
         <v>802</v>
       </c>
@@ -12632,7 +12665,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="225">
+    <row r="249" spans="1:3" ht="217.5">
       <c r="A249" s="5" t="s">
         <v>805</v>
       </c>
@@ -12643,7 +12676,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="120">
+    <row r="250" spans="1:3" ht="116">
       <c r="A250" s="5" t="s">
         <v>825</v>
       </c>
@@ -12654,7 +12687,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="150">
+    <row r="251" spans="1:3" ht="145">
       <c r="A251" s="5" t="s">
         <v>828</v>
       </c>
@@ -12665,7 +12698,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="120">
+    <row r="252" spans="1:3" ht="116">
       <c r="A252" s="5" t="s">
         <v>831</v>
       </c>
@@ -12687,7 +12720,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="30">
+    <row r="254" spans="1:3" ht="29">
       <c r="A254" s="5" t="s">
         <v>839</v>
       </c>
@@ -12698,7 +12731,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="75">
+    <row r="255" spans="1:3" ht="72.5">
       <c r="A255" s="5" t="s">
         <v>840</v>
       </c>
@@ -12709,7 +12742,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="30">
+    <row r="256" spans="1:3" ht="29">
       <c r="A256" s="5" t="s">
         <v>841</v>
       </c>
@@ -12720,7 +12753,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="75">
+    <row r="257" spans="1:3" ht="72.5">
       <c r="A257" s="5" t="s">
         <v>842</v>
       </c>
@@ -12731,7 +12764,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="150">
+    <row r="258" spans="1:3" ht="145">
       <c r="A258" s="5" t="s">
         <v>848</v>
       </c>
@@ -12753,7 +12786,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="45">
+    <row r="260" spans="1:3" ht="43.5">
       <c r="A260" s="5" t="s">
         <v>852</v>
       </c>
@@ -12764,7 +12797,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="60">
+    <row r="261" spans="1:3" ht="58">
       <c r="A261" s="5" t="s">
         <v>855</v>
       </c>
@@ -12775,7 +12808,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="90">
+    <row r="262" spans="1:3" ht="87">
       <c r="A262" s="5" t="s">
         <v>858</v>
       </c>
@@ -12794,7 +12827,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="60">
+    <row r="264" spans="1:3" ht="58">
       <c r="A264" s="5" t="s">
         <v>863</v>
       </c>
@@ -12805,7 +12838,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="90">
+    <row r="265" spans="1:3" ht="87">
       <c r="A265" s="5" t="s">
         <v>866</v>
       </c>
@@ -12816,7 +12849,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="75">
+    <row r="266" spans="1:3" ht="72.5">
       <c r="A266" s="5" t="s">
         <v>869</v>
       </c>
@@ -12851,7 +12884,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="30">
+    <row r="270" spans="1:3" ht="29">
       <c r="A270" s="5" t="s">
         <v>883</v>
       </c>
@@ -12859,7 +12892,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="120">
+    <row r="271" spans="1:3" ht="101.5">
       <c r="A271" s="5" t="s">
         <v>884</v>
       </c>
@@ -12870,7 +12903,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="45">
+    <row r="272" spans="1:3" ht="43.5">
       <c r="A272" s="5" t="s">
         <v>885</v>
       </c>
@@ -12881,7 +12914,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="30">
+    <row r="273" spans="1:4" ht="29">
       <c r="A273" s="5" t="s">
         <v>886</v>
       </c>
@@ -12892,7 +12925,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="75">
+    <row r="274" spans="1:4" ht="72.5">
       <c r="A274" s="5" t="s">
         <v>890</v>
       </c>
@@ -13540,7 +13573,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="401" spans="1:3" ht="30">
+    <row r="401" spans="1:3" ht="29">
       <c r="A401" s="2" t="s">
         <v>1018</v>
       </c>
@@ -13551,7 +13584,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="402" spans="1:3" ht="75">
+    <row r="402" spans="1:3" ht="72.5">
       <c r="A402" s="2" t="s">
         <v>1019</v>
       </c>
@@ -13562,7 +13595,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="60">
+    <row r="403" spans="1:3" ht="58">
       <c r="A403" s="2" t="s">
         <v>1020</v>
       </c>
@@ -13573,7 +13606,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="30">
+    <row r="404" spans="1:3" ht="29">
       <c r="A404" s="2" t="s">
         <v>1021</v>
       </c>
@@ -13584,7 +13617,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="30">
+    <row r="405" spans="1:3" ht="29">
       <c r="A405" s="2" t="s">
         <v>1022</v>
       </c>
@@ -13595,7 +13628,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="60">
+    <row r="406" spans="1:3" ht="43.5">
       <c r="A406" s="2" t="s">
         <v>1023</v>
       </c>
@@ -13606,7 +13639,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="407" spans="1:3" ht="30">
+    <row r="407" spans="1:3" ht="29">
       <c r="A407" s="2" t="s">
         <v>1024</v>
       </c>
@@ -13617,7 +13650,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="135">
+    <row r="408" spans="1:3" ht="130.5">
       <c r="A408" s="2" t="s">
         <v>1025</v>
       </c>
@@ -13628,7 +13661,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="409" spans="1:3" ht="45">
+    <row r="409" spans="1:3" ht="43.5">
       <c r="A409" s="2" t="s">
         <v>1026</v>
       </c>
@@ -13639,7 +13672,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="410" spans="1:3" ht="30">
+    <row r="410" spans="1:3" ht="29">
       <c r="A410" s="2" t="s">
         <v>1027</v>
       </c>
@@ -13650,7 +13683,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="30">
+    <row r="411" spans="1:3" ht="29">
       <c r="A411" s="2" t="s">
         <v>1028</v>
       </c>
@@ -13661,7 +13694,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="165">
+    <row r="412" spans="1:3" ht="159.5">
       <c r="A412" s="2" t="s">
         <v>1029</v>
       </c>
@@ -13672,7 +13705,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="180">
+    <row r="413" spans="1:3" ht="174">
       <c r="A413" s="2" t="s">
         <v>1030</v>
       </c>
@@ -13683,7 +13716,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="75">
+    <row r="414" spans="1:3" ht="72.5">
       <c r="A414" s="2" t="s">
         <v>1031</v>
       </c>
@@ -13705,7 +13738,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="75">
+    <row r="416" spans="1:3" ht="72.5">
       <c r="A416" s="2" t="s">
         <v>1033</v>
       </c>
@@ -13716,7 +13749,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="120">
+    <row r="417" spans="1:3" ht="116">
       <c r="A417" s="2" t="s">
         <v>1034</v>
       </c>
@@ -13727,7 +13760,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="135">
+    <row r="418" spans="1:3" ht="130.5">
       <c r="A418" s="2" t="s">
         <v>1035</v>
       </c>
@@ -13738,7 +13771,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="30">
+    <row r="419" spans="1:3" ht="29">
       <c r="A419" s="2" t="s">
         <v>1036</v>
       </c>
@@ -13848,7 +13881,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="75">
+    <row r="429" spans="1:3" ht="72.5">
       <c r="A429" s="2" t="s">
         <v>1046</v>
       </c>
@@ -19219,7 +19252,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="1502" spans="1:3" ht="90">
+    <row r="1502" spans="1:3" ht="87">
       <c r="A1502" s="5" t="s">
         <v>2119</v>
       </c>
@@ -19230,7 +19263,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="1503" spans="1:3" ht="90">
+    <row r="1503" spans="1:3" ht="87">
       <c r="A1503" s="5" t="s">
         <v>2120</v>
       </c>
@@ -19241,7 +19274,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="1504" spans="1:3" ht="150">
+    <row r="1504" spans="1:3" ht="145">
       <c r="A1504" s="5" t="s">
         <v>2121</v>
       </c>
@@ -19252,7 +19285,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="1505" spans="1:3" ht="150">
+    <row r="1505" spans="1:3" ht="145">
       <c r="A1505" s="5" t="s">
         <v>2122</v>
       </c>
@@ -19263,7 +19296,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1506" spans="1:3" ht="75">
+    <row r="1506" spans="1:3" ht="72.5">
       <c r="A1506" s="5" t="s">
         <v>2123</v>
       </c>
@@ -19271,7 +19304,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="1507" spans="1:3" ht="45">
+    <row r="1507" spans="1:3" ht="43.5">
       <c r="A1507" s="47" t="s">
         <v>2124</v>
       </c>
@@ -19282,7 +19315,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1508" spans="1:3" ht="45">
+    <row r="1508" spans="1:3" ht="43.5">
       <c r="A1508" s="44" t="s">
         <v>2125</v>
       </c>
@@ -19758,7 +19791,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="1602" spans="1:3" ht="30">
+    <row r="1602" spans="1:3" ht="29">
       <c r="A1602" s="5" t="s">
         <v>2219</v>
       </c>
@@ -19780,7 +19813,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="1604" spans="1:3" ht="60">
+    <row r="1604" spans="1:3" ht="58">
       <c r="A1604" s="5" t="s">
         <v>2221</v>
       </c>
@@ -19791,7 +19824,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="1605" spans="1:3" ht="45">
+    <row r="1605" spans="1:3" ht="43.5">
       <c r="A1605" s="5" t="s">
         <v>2222</v>
       </c>
@@ -19799,7 +19832,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="1606" spans="1:3" ht="105">
+    <row r="1606" spans="1:3" ht="101.5">
       <c r="A1606" s="5" t="s">
         <v>2223</v>
       </c>
@@ -19829,7 +19862,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="1609" spans="1:3" ht="45">
+    <row r="1609" spans="1:3" ht="43.5">
       <c r="A1609" s="5" t="s">
         <v>2278</v>
       </c>
@@ -19840,7 +19873,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="1610" spans="1:3" ht="30">
+    <row r="1610" spans="1:3" ht="29">
       <c r="A1610" s="5" t="s">
         <v>2279</v>
       </c>
@@ -19848,7 +19881,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="1611" spans="1:3" ht="409.5">
+    <row r="1611" spans="1:3" ht="391.5">
       <c r="A1611" s="5" t="s">
         <v>2280</v>
       </c>
@@ -19859,7 +19892,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="1612" spans="1:3" ht="240">
+    <row r="1612" spans="1:3" ht="232">
       <c r="A1612" s="44" t="s">
         <v>2281</v>
       </c>
@@ -19870,10 +19903,59 @@
         <v>2286</v>
       </c>
     </row>
+    <row r="1613" spans="1:3">
+      <c r="A1613" s="44" t="s">
+        <v>2339</v>
+      </c>
+      <c r="B1613" s="48" t="s">
+        <v>2337</v>
+      </c>
+      <c r="C1613" t="s">
+        <v>2338</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:3">
+      <c r="A1614">
+        <v>1613</v>
+      </c>
+      <c r="B1614" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C1614" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:3">
+      <c r="A1615">
+        <v>1614</v>
+      </c>
+      <c r="B1615" s="48" t="s">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:3" ht="87">
+      <c r="A1616">
+        <v>1615</v>
+      </c>
+      <c r="B1616" s="48" t="s">
+        <v>2344</v>
+      </c>
+      <c r="C1616" t="s">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:2" ht="29">
+      <c r="A1617">
+        <v>1616</v>
+      </c>
+      <c r="B1617" s="48" t="s">
+        <v>2345</v>
+      </c>
+    </row>
     <row r="1901" spans="1:3">
       <c r="B1901" s="48"/>
     </row>
-    <row r="1902" spans="1:3" ht="45">
+    <row r="1902" spans="1:3" ht="43.5">
       <c r="A1902">
         <v>1901</v>
       </c>
@@ -19884,7 +19966,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="1903" spans="1:3" ht="90">
+    <row r="1903" spans="1:3" ht="87">
       <c r="A1903">
         <v>1902</v>
       </c>
@@ -19895,7 +19977,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="1904" spans="1:3" ht="225">
+    <row r="1904" spans="1:3" ht="217.5">
       <c r="A1904">
         <v>1903</v>
       </c>
@@ -19906,7 +19988,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="1905" spans="1:3" ht="150">
+    <row r="1905" spans="1:3" ht="145">
       <c r="A1905">
         <v>1904</v>
       </c>
@@ -19917,7 +19999,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="1906" spans="1:3" ht="150">
+    <row r="1906" spans="1:3" ht="145">
       <c r="A1906">
         <v>1905</v>
       </c>
@@ -19928,7 +20010,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="1907" spans="1:3" ht="120">
+    <row r="1907" spans="1:3" ht="116">
       <c r="A1907">
         <v>1906</v>
       </c>
@@ -19939,7 +20021,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="1908" spans="1:3" ht="150">
+    <row r="1908" spans="1:3" ht="145">
       <c r="A1908">
         <v>1907</v>
       </c>
@@ -19950,7 +20032,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="1909" spans="1:3" ht="150">
+    <row r="1909" spans="1:3" ht="145">
       <c r="A1909">
         <v>1908</v>
       </c>
@@ -19961,7 +20043,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="1910" spans="1:3" ht="105">
+    <row r="1910" spans="1:3" ht="101.5">
       <c r="A1910">
         <v>1909</v>
       </c>
@@ -20009,13 +20091,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -20195,10 +20277,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -20521,7 +20603,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" ht="16">
       <c r="A44" s="13" t="s">
         <v>263</v>
       </c>
@@ -20611,13 +20693,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="85.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+    <row r="1" spans="1:2" ht="15" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>283</v>
       </c>
@@ -20625,7 +20707,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+    <row r="2" spans="1:2" ht="15" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>285</v>
       </c>
@@ -20633,7 +20715,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+    <row r="3" spans="1:2" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>287</v>
       </c>
@@ -20641,7 +20723,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+    <row r="4" spans="1:2" ht="15" thickBot="1">
       <c r="A4" s="25" t="s">
         <v>289</v>
       </c>
@@ -20649,7 +20731,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+    <row r="5" spans="1:2" ht="15" thickBot="1">
       <c r="A5" s="25" t="s">
         <v>291</v>
       </c>
@@ -20657,7 +20739,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+    <row r="6" spans="1:2" ht="15" thickBot="1">
       <c r="A6" s="25" t="s">
         <v>293</v>
       </c>
@@ -20665,7 +20747,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1">
+    <row r="7" spans="1:2" ht="15" thickBot="1">
       <c r="A7" s="25" t="s">
         <v>295</v>
       </c>
@@ -20673,7 +20755,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+    <row r="8" spans="1:2" ht="15" thickBot="1">
       <c r="A8" s="25" t="s">
         <v>297</v>
       </c>
@@ -20681,7 +20763,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1">
+    <row r="9" spans="1:2" ht="15" thickBot="1">
       <c r="A9" s="25" t="s">
         <v>299</v>
       </c>
@@ -20689,7 +20771,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1">
+    <row r="10" spans="1:2" ht="15" thickBot="1">
       <c r="A10" s="25" t="s">
         <v>301</v>
       </c>
@@ -20697,7 +20779,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1">
+    <row r="11" spans="1:2" ht="15" thickBot="1">
       <c r="A11" s="25" t="s">
         <v>303</v>
       </c>
@@ -20705,7 +20787,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+    <row r="12" spans="1:2" ht="15" thickBot="1">
       <c r="A12" s="25" t="s">
         <v>305</v>
       </c>
@@ -20713,7 +20795,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1">
+    <row r="13" spans="1:2" ht="15" thickBot="1">
       <c r="A13" s="25" t="s">
         <v>307</v>
       </c>
@@ -20721,7 +20803,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1">
+    <row r="14" spans="1:2" ht="15" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>309</v>
       </c>
@@ -20729,7 +20811,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1">
+    <row r="15" spans="1:2" ht="15" thickBot="1">
       <c r="A15" s="25" t="s">
         <v>311</v>
       </c>
@@ -20737,7 +20819,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1">
+    <row r="16" spans="1:2" ht="15" thickBot="1">
       <c r="A16" s="25" t="s">
         <v>313</v>
       </c>
@@ -20745,7 +20827,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1">
+    <row r="17" spans="1:2" ht="15" thickBot="1">
       <c r="A17" s="25" t="s">
         <v>315</v>
       </c>
@@ -20753,7 +20835,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1">
+    <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>317</v>
       </c>
@@ -20761,7 +20843,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1">
+    <row r="19" spans="1:2" ht="15" thickBot="1">
       <c r="A19" s="25" t="s">
         <v>319</v>
       </c>
@@ -20769,7 +20851,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1">
+    <row r="20" spans="1:2" ht="15" thickBot="1">
       <c r="A20" s="25" t="s">
         <v>321</v>
       </c>
@@ -20777,7 +20859,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1">
+    <row r="21" spans="1:2" ht="15" thickBot="1">
       <c r="A21" s="25" t="s">
         <v>323</v>
       </c>
@@ -20785,7 +20867,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1">
+    <row r="22" spans="1:2" ht="15" thickBot="1">
       <c r="A22" s="25" t="s">
         <v>325</v>
       </c>
@@ -20793,7 +20875,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1">
+    <row r="23" spans="1:2" ht="15" thickBot="1">
       <c r="A23" s="25" t="s">
         <v>327</v>
       </c>
@@ -20801,7 +20883,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1">
+    <row r="24" spans="1:2" ht="15" thickBot="1">
       <c r="A24" s="25" t="s">
         <v>329</v>
       </c>
@@ -20809,7 +20891,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1">
+    <row r="25" spans="1:2" ht="15" thickBot="1">
       <c r="A25" s="25" t="s">
         <v>331</v>
       </c>
@@ -20817,7 +20899,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1">
+    <row r="26" spans="1:2" ht="15" thickBot="1">
       <c r="A26" s="25" t="s">
         <v>333</v>
       </c>
@@ -20825,7 +20907,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1">
+    <row r="27" spans="1:2" ht="15" thickBot="1">
       <c r="A27" s="25" t="s">
         <v>335</v>
       </c>
@@ -20833,7 +20915,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1">
+    <row r="28" spans="1:2" ht="15" thickBot="1">
       <c r="A28" s="25" t="s">
         <v>337</v>
       </c>
@@ -20841,7 +20923,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1">
+    <row r="29" spans="1:2" ht="15" thickBot="1">
       <c r="A29" s="25" t="s">
         <v>339</v>
       </c>
@@ -20849,7 +20931,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1">
+    <row r="30" spans="1:2" ht="15" thickBot="1">
       <c r="A30" s="25" t="s">
         <v>341</v>
       </c>
@@ -20857,7 +20939,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1">
+    <row r="31" spans="1:2" ht="15" thickBot="1">
       <c r="A31" s="25" t="s">
         <v>343</v>
       </c>
@@ -20865,7 +20947,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1">
+    <row r="32" spans="1:2" ht="15" thickBot="1">
       <c r="A32" s="25" t="s">
         <v>345</v>
       </c>
@@ -20873,7 +20955,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1">
+    <row r="33" spans="1:2" ht="15" thickBot="1">
       <c r="A33" s="25" t="s">
         <v>347</v>
       </c>
@@ -20881,7 +20963,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1">
+    <row r="34" spans="1:2" ht="15" thickBot="1">
       <c r="A34" s="25" t="s">
         <v>349</v>
       </c>
@@ -20889,7 +20971,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1">
+    <row r="35" spans="1:2" ht="15" thickBot="1">
       <c r="A35" s="25" t="s">
         <v>351</v>
       </c>

</xml_diff>

<commit_message>
Billing Service Information script fix
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tathyush\Desktop\Team Members Autmation\updated master\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsunand1\Desktop\OPP_Eclipse\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE2C517-EED4-4F83-A655-081A5AB86E3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90C2702-7887-40AC-A3CF-3593B53BB7F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -26,20 +26,12 @@
     <definedName name="Platform">[1]Sheet2!$A$1:$A$11</definedName>
     <definedName name="URL">[1]Sheet2!$E:$E</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="2337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="2629">
   <si>
     <t>City</t>
   </si>
@@ -8904,6 +8896,890 @@
   <si>
     <t>Delete Prov Assoc after script run</t>
   </si>
+  <si>
+    <t>1612</t>
+  </si>
+  <si>
+    <t>1613</t>
+  </si>
+  <si>
+    <t>1614</t>
+  </si>
+  <si>
+    <t>1615</t>
+  </si>
+  <si>
+    <t>1616</t>
+  </si>
+  <si>
+    <t>1617</t>
+  </si>
+  <si>
+    <t>1618</t>
+  </si>
+  <si>
+    <t>1619</t>
+  </si>
+  <si>
+    <t>1620</t>
+  </si>
+  <si>
+    <t>1621</t>
+  </si>
+  <si>
+    <t>1622</t>
+  </si>
+  <si>
+    <t>1623</t>
+  </si>
+  <si>
+    <t>1624</t>
+  </si>
+  <si>
+    <t>1625</t>
+  </si>
+  <si>
+    <t>1626</t>
+  </si>
+  <si>
+    <t>1627</t>
+  </si>
+  <si>
+    <t>1628</t>
+  </si>
+  <si>
+    <t>1629</t>
+  </si>
+  <si>
+    <t>1630</t>
+  </si>
+  <si>
+    <t>1631</t>
+  </si>
+  <si>
+    <t>1632</t>
+  </si>
+  <si>
+    <t>1633</t>
+  </si>
+  <si>
+    <t>1634</t>
+  </si>
+  <si>
+    <t>1635</t>
+  </si>
+  <si>
+    <t>1636</t>
+  </si>
+  <si>
+    <t>1637</t>
+  </si>
+  <si>
+    <t>1638</t>
+  </si>
+  <si>
+    <t>1639</t>
+  </si>
+  <si>
+    <t>1640</t>
+  </si>
+  <si>
+    <t>1641</t>
+  </si>
+  <si>
+    <t>1642</t>
+  </si>
+  <si>
+    <t>1643</t>
+  </si>
+  <si>
+    <t>1644</t>
+  </si>
+  <si>
+    <t>1645</t>
+  </si>
+  <si>
+    <t>1646</t>
+  </si>
+  <si>
+    <t>1647</t>
+  </si>
+  <si>
+    <t>1648</t>
+  </si>
+  <si>
+    <t>1649</t>
+  </si>
+  <si>
+    <t>1650</t>
+  </si>
+  <si>
+    <t>1651</t>
+  </si>
+  <si>
+    <t>1652</t>
+  </si>
+  <si>
+    <t>1653</t>
+  </si>
+  <si>
+    <t>1654</t>
+  </si>
+  <si>
+    <t>1655</t>
+  </si>
+  <si>
+    <t>1656</t>
+  </si>
+  <si>
+    <t>1657</t>
+  </si>
+  <si>
+    <t>1658</t>
+  </si>
+  <si>
+    <t>1659</t>
+  </si>
+  <si>
+    <t>1660</t>
+  </si>
+  <si>
+    <t>1661</t>
+  </si>
+  <si>
+    <t>1662</t>
+  </si>
+  <si>
+    <t>1663</t>
+  </si>
+  <si>
+    <t>1664</t>
+  </si>
+  <si>
+    <t>1665</t>
+  </si>
+  <si>
+    <t>1666</t>
+  </si>
+  <si>
+    <t>1667</t>
+  </si>
+  <si>
+    <t>1668</t>
+  </si>
+  <si>
+    <t>1669</t>
+  </si>
+  <si>
+    <t>1670</t>
+  </si>
+  <si>
+    <t>1671</t>
+  </si>
+  <si>
+    <t>1672</t>
+  </si>
+  <si>
+    <t>1673</t>
+  </si>
+  <si>
+    <t>1674</t>
+  </si>
+  <si>
+    <t>1675</t>
+  </si>
+  <si>
+    <t>1676</t>
+  </si>
+  <si>
+    <t>1677</t>
+  </si>
+  <si>
+    <t>1678</t>
+  </si>
+  <si>
+    <t>1679</t>
+  </si>
+  <si>
+    <t>1680</t>
+  </si>
+  <si>
+    <t>1681</t>
+  </si>
+  <si>
+    <t>1682</t>
+  </si>
+  <si>
+    <t>1683</t>
+  </si>
+  <si>
+    <t>1684</t>
+  </si>
+  <si>
+    <t>1685</t>
+  </si>
+  <si>
+    <t>1686</t>
+  </si>
+  <si>
+    <t>1687</t>
+  </si>
+  <si>
+    <t>1688</t>
+  </si>
+  <si>
+    <t>1689</t>
+  </si>
+  <si>
+    <t>1690</t>
+  </si>
+  <si>
+    <t>1691</t>
+  </si>
+  <si>
+    <t>1692</t>
+  </si>
+  <si>
+    <t>1693</t>
+  </si>
+  <si>
+    <t>1694</t>
+  </si>
+  <si>
+    <t>1695</t>
+  </si>
+  <si>
+    <t>1696</t>
+  </si>
+  <si>
+    <t>1697</t>
+  </si>
+  <si>
+    <t>1698</t>
+  </si>
+  <si>
+    <t>1699</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>1701</t>
+  </si>
+  <si>
+    <t>1702</t>
+  </si>
+  <si>
+    <t>1703</t>
+  </si>
+  <si>
+    <t>1704</t>
+  </si>
+  <si>
+    <t>1705</t>
+  </si>
+  <si>
+    <t>1706</t>
+  </si>
+  <si>
+    <t>1707</t>
+  </si>
+  <si>
+    <t>1708</t>
+  </si>
+  <si>
+    <t>1709</t>
+  </si>
+  <si>
+    <t>1710</t>
+  </si>
+  <si>
+    <t>1711</t>
+  </si>
+  <si>
+    <t>1712</t>
+  </si>
+  <si>
+    <t>1713</t>
+  </si>
+  <si>
+    <t>1714</t>
+  </si>
+  <si>
+    <t>1715</t>
+  </si>
+  <si>
+    <t>1716</t>
+  </si>
+  <si>
+    <t>1717</t>
+  </si>
+  <si>
+    <t>1718</t>
+  </si>
+  <si>
+    <t>1719</t>
+  </si>
+  <si>
+    <t>1720</t>
+  </si>
+  <si>
+    <t>1721</t>
+  </si>
+  <si>
+    <t>1722</t>
+  </si>
+  <si>
+    <t>1723</t>
+  </si>
+  <si>
+    <t>1724</t>
+  </si>
+  <si>
+    <t>1725</t>
+  </si>
+  <si>
+    <t>1726</t>
+  </si>
+  <si>
+    <t>1727</t>
+  </si>
+  <si>
+    <t>1728</t>
+  </si>
+  <si>
+    <t>1729</t>
+  </si>
+  <si>
+    <t>1730</t>
+  </si>
+  <si>
+    <t>1731</t>
+  </si>
+  <si>
+    <t>1732</t>
+  </si>
+  <si>
+    <t>1733</t>
+  </si>
+  <si>
+    <t>1734</t>
+  </si>
+  <si>
+    <t>1735</t>
+  </si>
+  <si>
+    <t>1736</t>
+  </si>
+  <si>
+    <t>1737</t>
+  </si>
+  <si>
+    <t>1738</t>
+  </si>
+  <si>
+    <t>1739</t>
+  </si>
+  <si>
+    <t>1740</t>
+  </si>
+  <si>
+    <t>1741</t>
+  </si>
+  <si>
+    <t>1742</t>
+  </si>
+  <si>
+    <t>1743</t>
+  </si>
+  <si>
+    <t>1744</t>
+  </si>
+  <si>
+    <t>1745</t>
+  </si>
+  <si>
+    <t>1746</t>
+  </si>
+  <si>
+    <t>1747</t>
+  </si>
+  <si>
+    <t>1748</t>
+  </si>
+  <si>
+    <t>1749</t>
+  </si>
+  <si>
+    <t>1750</t>
+  </si>
+  <si>
+    <t>1751</t>
+  </si>
+  <si>
+    <t>1752</t>
+  </si>
+  <si>
+    <t>1753</t>
+  </si>
+  <si>
+    <t>1754</t>
+  </si>
+  <si>
+    <t>1755</t>
+  </si>
+  <si>
+    <t>1756</t>
+  </si>
+  <si>
+    <t>1757</t>
+  </si>
+  <si>
+    <t>1758</t>
+  </si>
+  <si>
+    <t>1759</t>
+  </si>
+  <si>
+    <t>1760</t>
+  </si>
+  <si>
+    <t>1761</t>
+  </si>
+  <si>
+    <t>1762</t>
+  </si>
+  <si>
+    <t>1763</t>
+  </si>
+  <si>
+    <t>1764</t>
+  </si>
+  <si>
+    <t>1765</t>
+  </si>
+  <si>
+    <t>1766</t>
+  </si>
+  <si>
+    <t>1767</t>
+  </si>
+  <si>
+    <t>1768</t>
+  </si>
+  <si>
+    <t>1769</t>
+  </si>
+  <si>
+    <t>1770</t>
+  </si>
+  <si>
+    <t>1771</t>
+  </si>
+  <si>
+    <t>1772</t>
+  </si>
+  <si>
+    <t>1773</t>
+  </si>
+  <si>
+    <t>1774</t>
+  </si>
+  <si>
+    <t>1775</t>
+  </si>
+  <si>
+    <t>1776</t>
+  </si>
+  <si>
+    <t>1777</t>
+  </si>
+  <si>
+    <t>1778</t>
+  </si>
+  <si>
+    <t>1779</t>
+  </si>
+  <si>
+    <t>1780</t>
+  </si>
+  <si>
+    <t>1781</t>
+  </si>
+  <si>
+    <t>1782</t>
+  </si>
+  <si>
+    <t>1783</t>
+  </si>
+  <si>
+    <t>1784</t>
+  </si>
+  <si>
+    <t>1785</t>
+  </si>
+  <si>
+    <t>1786</t>
+  </si>
+  <si>
+    <t>1787</t>
+  </si>
+  <si>
+    <t>1788</t>
+  </si>
+  <si>
+    <t>1789</t>
+  </si>
+  <si>
+    <t>1790</t>
+  </si>
+  <si>
+    <t>1791</t>
+  </si>
+  <si>
+    <t>1792</t>
+  </si>
+  <si>
+    <t>1793</t>
+  </si>
+  <si>
+    <t>1794</t>
+  </si>
+  <si>
+    <t>1795</t>
+  </si>
+  <si>
+    <t>1796</t>
+  </si>
+  <si>
+    <t>1797</t>
+  </si>
+  <si>
+    <t>1798</t>
+  </si>
+  <si>
+    <t>1799</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>1801</t>
+  </si>
+  <si>
+    <t>1802</t>
+  </si>
+  <si>
+    <t>1803</t>
+  </si>
+  <si>
+    <t>1804</t>
+  </si>
+  <si>
+    <t>1805</t>
+  </si>
+  <si>
+    <t>1806</t>
+  </si>
+  <si>
+    <t>1807</t>
+  </si>
+  <si>
+    <t>1808</t>
+  </si>
+  <si>
+    <t>1809</t>
+  </si>
+  <si>
+    <t>1810</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>1812</t>
+  </si>
+  <si>
+    <t>1813</t>
+  </si>
+  <si>
+    <t>1814</t>
+  </si>
+  <si>
+    <t>1815</t>
+  </si>
+  <si>
+    <t>1816</t>
+  </si>
+  <si>
+    <t>1817</t>
+  </si>
+  <si>
+    <t>1818</t>
+  </si>
+  <si>
+    <t>1819</t>
+  </si>
+  <si>
+    <t>1820</t>
+  </si>
+  <si>
+    <t>1821</t>
+  </si>
+  <si>
+    <t>1822</t>
+  </si>
+  <si>
+    <t>1823</t>
+  </si>
+  <si>
+    <t>1824</t>
+  </si>
+  <si>
+    <t>1825</t>
+  </si>
+  <si>
+    <t>1826</t>
+  </si>
+  <si>
+    <t>1827</t>
+  </si>
+  <si>
+    <t>1828</t>
+  </si>
+  <si>
+    <t>1829</t>
+  </si>
+  <si>
+    <t>1830</t>
+  </si>
+  <si>
+    <t>1831</t>
+  </si>
+  <si>
+    <t>1832</t>
+  </si>
+  <si>
+    <t>1833</t>
+  </si>
+  <si>
+    <t>1834</t>
+  </si>
+  <si>
+    <t>1835</t>
+  </si>
+  <si>
+    <t>1836</t>
+  </si>
+  <si>
+    <t>1837</t>
+  </si>
+  <si>
+    <t>1838</t>
+  </si>
+  <si>
+    <t>1839</t>
+  </si>
+  <si>
+    <t>1840</t>
+  </si>
+  <si>
+    <t>1841</t>
+  </si>
+  <si>
+    <t>1842</t>
+  </si>
+  <si>
+    <t>1843</t>
+  </si>
+  <si>
+    <t>1844</t>
+  </si>
+  <si>
+    <t>1845</t>
+  </si>
+  <si>
+    <t>1846</t>
+  </si>
+  <si>
+    <t>1847</t>
+  </si>
+  <si>
+    <t>1848</t>
+  </si>
+  <si>
+    <t>1849</t>
+  </si>
+  <si>
+    <t>1850</t>
+  </si>
+  <si>
+    <t>1851</t>
+  </si>
+  <si>
+    <t>1852</t>
+  </si>
+  <si>
+    <t>1853</t>
+  </si>
+  <si>
+    <t>1854</t>
+  </si>
+  <si>
+    <t>1855</t>
+  </si>
+  <si>
+    <t>1856</t>
+  </si>
+  <si>
+    <t>1857</t>
+  </si>
+  <si>
+    <t>1858</t>
+  </si>
+  <si>
+    <t>1859</t>
+  </si>
+  <si>
+    <t>1860</t>
+  </si>
+  <si>
+    <t>1861</t>
+  </si>
+  <si>
+    <t>1862</t>
+  </si>
+  <si>
+    <t>1863</t>
+  </si>
+  <si>
+    <t>1864</t>
+  </si>
+  <si>
+    <t>1865</t>
+  </si>
+  <si>
+    <t>1866</t>
+  </si>
+  <si>
+    <t>1867</t>
+  </si>
+  <si>
+    <t>1868</t>
+  </si>
+  <si>
+    <t>1869</t>
+  </si>
+  <si>
+    <t>1870</t>
+  </si>
+  <si>
+    <t>1871</t>
+  </si>
+  <si>
+    <t>1872</t>
+  </si>
+  <si>
+    <t>1873</t>
+  </si>
+  <si>
+    <t>1874</t>
+  </si>
+  <si>
+    <t>1875</t>
+  </si>
+  <si>
+    <t>1876</t>
+  </si>
+  <si>
+    <t>1877</t>
+  </si>
+  <si>
+    <t>1878</t>
+  </si>
+  <si>
+    <t>1879</t>
+  </si>
+  <si>
+    <t>1880</t>
+  </si>
+  <si>
+    <t>1881</t>
+  </si>
+  <si>
+    <t>1882</t>
+  </si>
+  <si>
+    <t>1883</t>
+  </si>
+  <si>
+    <t>1884</t>
+  </si>
+  <si>
+    <t>1885</t>
+  </si>
+  <si>
+    <t>1886</t>
+  </si>
+  <si>
+    <t>1887</t>
+  </si>
+  <si>
+    <t>1888</t>
+  </si>
+  <si>
+    <t>1889</t>
+  </si>
+  <si>
+    <t>1890</t>
+  </si>
+  <si>
+    <t>1891</t>
+  </si>
+  <si>
+    <t>1892</t>
+  </si>
+  <si>
+    <t>1893</t>
+  </si>
+  <si>
+    <t>1894</t>
+  </si>
+  <si>
+    <t>1895</t>
+  </si>
+  <si>
+    <t>1896</t>
+  </si>
+  <si>
+    <t>1897</t>
+  </si>
+  <si>
+    <t>1898</t>
+  </si>
+  <si>
+    <t>1899</t>
+  </si>
+  <si>
+    <t>1900</t>
+  </si>
+  <si>
+    <t>select * from OLE.SYSTEM_CONFIGURATION where PROC_TYP_DESC='RollOut_Trial_End_DT'</t>
+  </si>
+  <si>
+    <t>UPDATE OLE.SYSTEM_CONFIGURATION SET PROC_DATA ='{$currentDate}'  where PROC_TYP_DESC='RollOut_Trial_End_DT' AND SYS_CNFG_ID='4187940'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+select * from ole.enrolled_provider ep where ep.enrl_sts_cd='A' and ep.PROV_TIN_NBR NOT IN(
+select ep.PROV_TIN_NBR from ole.billing_service bs 
+join ole.billing_service_provider bsp on bs.billing_service_id=bsp.billing_service_id
+join ole.enrolled_provider ep on bsp.prov_tin_nbr=ep.prov_tin_nbr
+where bs.billing_service_id in(select bs.billing_service_id from ole.billing_service bs 
+join ole.billing_service_provider bsp on bs.billing_service_id=bsp.billing_service_id
+join ole.enrolled_provider ep on bsp.prov_tin_nbr=ep.prov_tin_nbr
+where ep.enrl_STS_CD='A' and bs.identifier_nbr='{$bsTIN}')) fetch first row only</t>
+  </si>
 </sst>
 </file>
 
@@ -9086,7 +9962,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -9177,6 +10053,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9635,20 +10512,20 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="26.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -10184,15 +11061,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1912"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1885" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1902" sqref="B1902"/>
+    <sheetView tabSelected="1" topLeftCell="A1339" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1341" sqref="B1341"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="136.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="136.5546875" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -10228,7 +11105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60">
+    <row r="4" spans="1:3" ht="57.6">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -10236,7 +11113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="28.8">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -10271,7 +11148,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="28.8">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -10279,7 +11156,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="90">
+    <row r="10" spans="1:3" ht="86.4">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -10287,7 +11164,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="75">
+    <row r="11" spans="1:3" ht="72">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -10295,7 +11172,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="43.2">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -10303,7 +11180,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60">
+    <row r="13" spans="1:3" ht="57.6">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -10319,7 +11196,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60">
+    <row r="15" spans="1:3" ht="57.6">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -10327,7 +11204,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30">
+    <row r="16" spans="1:3" ht="28.8">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -10335,7 +11212,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -10343,7 +11220,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="28.8">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -10351,7 +11228,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90">
+    <row r="19" spans="1:3" ht="86.4">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -10359,7 +11236,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75">
+    <row r="20" spans="1:3" ht="72">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -10367,7 +11244,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="28.8">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
@@ -10375,7 +11252,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -10383,7 +11260,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="28.8">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -10391,7 +11268,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="45">
+    <row r="24" spans="1:3" ht="43.2">
       <c r="A24" s="5" t="s">
         <v>88</v>
       </c>
@@ -10402,7 +11279,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="75">
+    <row r="25" spans="1:3" ht="72">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -10418,7 +11295,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="135">
+    <row r="27" spans="1:3" ht="129.6">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -10426,7 +11303,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="90">
+    <row r="28" spans="1:3" ht="86.4">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
@@ -10434,7 +11311,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="28.8">
       <c r="A29" s="5" t="s">
         <v>94</v>
       </c>
@@ -10442,7 +11319,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="150">
+    <row r="30" spans="1:3" ht="144">
       <c r="A30" s="5" t="s">
         <v>95</v>
       </c>
@@ -10453,7 +11330,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="165">
+    <row r="31" spans="1:3" ht="158.4">
       <c r="A31" s="5" t="s">
         <v>98</v>
       </c>
@@ -10464,7 +11341,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="165">
+    <row r="32" spans="1:3" ht="158.4">
       <c r="A32" s="5" t="s">
         <v>101</v>
       </c>
@@ -10475,7 +11352,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="195">
+    <row r="33" spans="1:4" ht="187.2">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -10486,7 +11363,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="120">
+    <row r="34" spans="1:4" ht="115.2">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -10494,7 +11371,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45">
+    <row r="35" spans="1:4" ht="43.2">
       <c r="A35" s="5" t="s">
         <v>108</v>
       </c>
@@ -10502,7 +11379,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="120">
+    <row r="36" spans="1:4" ht="115.2">
       <c r="A36" s="5" t="s">
         <v>113</v>
       </c>
@@ -10513,7 +11390,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="105">
+    <row r="37" spans="1:4" ht="100.8">
       <c r="A37" s="5" t="s">
         <v>112</v>
       </c>
@@ -10524,7 +11401,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="120">
+    <row r="38" spans="1:4" ht="115.2">
       <c r="A38" s="5" t="s">
         <v>114</v>
       </c>
@@ -10532,7 +11409,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="105">
+    <row r="39" spans="1:4" ht="100.8">
       <c r="A39" s="5" t="s">
         <v>117</v>
       </c>
@@ -10540,7 +11417,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="120">
+    <row r="40" spans="1:4" ht="115.2">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -10548,7 +11425,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="120">
+    <row r="41" spans="1:4" ht="115.2">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -10556,7 +11433,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="120">
+    <row r="42" spans="1:4" ht="115.2">
       <c r="A42" s="5" t="s">
         <v>122</v>
       </c>
@@ -10570,7 +11447,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="180">
+    <row r="43" spans="1:4" ht="172.8">
       <c r="A43" s="5" t="s">
         <v>124</v>
       </c>
@@ -10581,7 +11458,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="180">
+    <row r="44" spans="1:4" ht="172.8">
       <c r="A44" s="5" t="s">
         <v>125</v>
       </c>
@@ -10592,7 +11469,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="105">
+    <row r="45" spans="1:4" ht="100.8">
       <c r="A45" s="5" t="s">
         <v>126</v>
       </c>
@@ -10603,7 +11480,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="165">
+    <row r="46" spans="1:4" ht="158.4">
       <c r="A46" s="5" t="s">
         <v>127</v>
       </c>
@@ -10614,7 +11491,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="180">
+    <row r="47" spans="1:4" ht="172.8">
       <c r="A47" s="5" t="s">
         <v>128</v>
       </c>
@@ -10625,7 +11502,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="180">
+    <row r="48" spans="1:4" ht="172.8">
       <c r="A48" s="5" t="s">
         <v>129</v>
       </c>
@@ -10636,7 +11513,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="105">
+    <row r="49" spans="1:3" ht="100.8">
       <c r="A49" s="5" t="s">
         <v>130</v>
       </c>
@@ -10647,7 +11524,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="135">
+    <row r="50" spans="1:3" ht="129.6">
       <c r="A50" s="5" t="s">
         <v>131</v>
       </c>
@@ -10658,7 +11535,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="105">
+    <row r="51" spans="1:3" ht="100.8">
       <c r="A51" s="5" t="s">
         <v>132</v>
       </c>
@@ -10669,7 +11546,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="135">
+    <row r="52" spans="1:3" ht="129.6">
       <c r="A52" s="5" t="s">
         <v>133</v>
       </c>
@@ -10680,7 +11557,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="120">
+    <row r="53" spans="1:3" ht="115.2">
       <c r="A53" s="5" t="s">
         <v>134</v>
       </c>
@@ -10691,7 +11568,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="105">
+    <row r="54" spans="1:3" ht="100.8">
       <c r="A54" s="5" t="s">
         <v>135</v>
       </c>
@@ -10699,7 +11576,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="120">
+    <row r="55" spans="1:3" ht="115.2">
       <c r="A55" s="5" t="s">
         <v>137</v>
       </c>
@@ -10710,7 +11587,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="120">
+    <row r="56" spans="1:3" ht="115.2">
       <c r="A56" s="5" t="s">
         <v>138</v>
       </c>
@@ -10718,7 +11595,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="165">
+    <row r="57" spans="1:3" ht="158.4">
       <c r="A57" s="5" t="s">
         <v>144</v>
       </c>
@@ -10729,7 +11606,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="165">
+    <row r="58" spans="1:3" ht="158.4">
       <c r="A58" s="5" t="s">
         <v>145</v>
       </c>
@@ -10737,7 +11614,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="150">
+    <row r="59" spans="1:3" ht="144">
       <c r="A59" s="5" t="s">
         <v>149</v>
       </c>
@@ -10748,7 +11625,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="165">
+    <row r="60" spans="1:3" ht="158.4">
       <c r="A60" s="5" t="s">
         <v>151</v>
       </c>
@@ -10759,7 +11636,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="180">
+    <row r="61" spans="1:3" ht="172.8">
       <c r="A61" s="5" t="s">
         <v>152</v>
       </c>
@@ -10770,7 +11647,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="120">
+    <row r="62" spans="1:3" ht="115.2">
       <c r="A62" s="5" t="s">
         <v>153</v>
       </c>
@@ -10781,7 +11658,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="45">
+    <row r="63" spans="1:3" ht="43.2">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -10789,7 +11666,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="135">
+    <row r="64" spans="1:3" ht="129.6">
       <c r="A64" s="5" t="s">
         <v>173</v>
       </c>
@@ -10800,7 +11677,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="135">
+    <row r="65" spans="1:3" ht="129.6">
       <c r="A65" s="5" t="s">
         <v>174</v>
       </c>
@@ -10827,7 +11704,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.5">
+    <row r="68" spans="1:3" ht="409.6">
       <c r="A68" s="5" t="s">
         <v>181</v>
       </c>
@@ -10835,7 +11712,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.5">
+    <row r="69" spans="1:3" ht="409.6">
       <c r="A69" s="5" t="s">
         <v>182</v>
       </c>
@@ -10843,7 +11720,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="150">
+    <row r="70" spans="1:3" ht="144">
       <c r="A70" s="5" t="s">
         <v>190</v>
       </c>
@@ -10854,7 +11731,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="240">
+    <row r="71" spans="1:3" ht="230.4">
       <c r="A71" s="5" t="s">
         <v>193</v>
       </c>
@@ -10881,7 +11758,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="30">
+    <row r="74" spans="1:3" ht="28.8">
       <c r="A74" s="5" t="s">
         <v>276</v>
       </c>
@@ -10889,7 +11766,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="30">
+    <row r="75" spans="1:3" ht="28.8">
       <c r="A75" s="5" t="s">
         <v>279</v>
       </c>
@@ -10897,7 +11774,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="30">
+    <row r="76" spans="1:3" ht="28.8">
       <c r="A76" s="5" t="s">
         <v>281</v>
       </c>
@@ -10905,7 +11782,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="30">
+    <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
         <v>353</v>
       </c>
@@ -10937,7 +11814,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="30">
+    <row r="81" spans="1:2" ht="28.8">
       <c r="A81" s="5" t="s">
         <v>358</v>
       </c>
@@ -10961,7 +11838,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="30">
+    <row r="84" spans="1:2" ht="28.8">
       <c r="A84" s="5" t="s">
         <v>363</v>
       </c>
@@ -10969,7 +11846,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="30">
+    <row r="85" spans="1:2">
       <c r="A85" s="5" t="s">
         <v>364</v>
       </c>
@@ -10977,7 +11854,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30">
+    <row r="86" spans="1:2" ht="28.8">
       <c r="A86" s="5" t="s">
         <v>365</v>
       </c>
@@ -10993,7 +11870,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="30">
+    <row r="88" spans="1:2" ht="28.8">
       <c r="A88" s="5" t="s">
         <v>368</v>
       </c>
@@ -11009,7 +11886,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="30">
+    <row r="90" spans="1:2" ht="28.8">
       <c r="A90" s="5" t="s">
         <v>381</v>
       </c>
@@ -11057,7 +11934,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="45">
+    <row r="96" spans="1:2" ht="28.8">
       <c r="A96" s="5" t="s">
         <v>393</v>
       </c>
@@ -11073,7 +11950,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="30">
+    <row r="98" spans="1:3" ht="28.8">
       <c r="A98" s="5" t="s">
         <v>397</v>
       </c>
@@ -11113,7 +11990,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="195">
+    <row r="103" spans="1:3" ht="187.2">
       <c r="A103" s="5" t="s">
         <v>406</v>
       </c>
@@ -11124,7 +12001,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="285">
+    <row r="104" spans="1:3" ht="273.60000000000002">
       <c r="A104" s="5" t="s">
         <v>407</v>
       </c>
@@ -11135,7 +12012,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="240">
+    <row r="105" spans="1:3" ht="230.4">
       <c r="A105" s="5" t="s">
         <v>409</v>
       </c>
@@ -11146,7 +12023,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="30">
+    <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
         <v>412</v>
       </c>
@@ -11154,7 +12031,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="45">
+    <row r="107" spans="1:3" ht="43.2">
       <c r="A107" s="5" t="s">
         <v>414</v>
       </c>
@@ -11170,7 +12047,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="120">
+    <row r="109" spans="1:3" ht="115.2">
       <c r="A109" s="5" t="s">
         <v>421</v>
       </c>
@@ -11353,7 +12230,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="120">
+    <row r="127" spans="1:3" ht="115.2">
       <c r="A127" s="5" t="s">
         <v>462</v>
       </c>
@@ -11364,7 +12241,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="120">
+    <row r="128" spans="1:3" ht="115.2">
       <c r="A128" s="5" t="s">
         <v>463</v>
       </c>
@@ -11383,7 +12260,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="180">
+    <row r="130" spans="1:3" ht="172.8">
       <c r="A130" s="5" t="s">
         <v>466</v>
       </c>
@@ -11394,7 +12271,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="150">
+    <row r="131" spans="1:3" ht="144">
       <c r="A131" s="5" t="s">
         <v>470</v>
       </c>
@@ -11405,7 +12282,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="150">
+    <row r="132" spans="1:3" ht="144">
       <c r="A132" s="5" t="s">
         <v>471</v>
       </c>
@@ -11416,7 +12293,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="135">
+    <row r="133" spans="1:3" ht="129.6">
       <c r="A133" s="5" t="s">
         <v>474</v>
       </c>
@@ -11427,7 +12304,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="135">
+    <row r="134" spans="1:3" ht="129.6">
       <c r="A134" s="5" t="s">
         <v>476</v>
       </c>
@@ -11438,7 +12315,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="135">
+    <row r="135" spans="1:3" ht="129.6">
       <c r="A135" s="5" t="s">
         <v>477</v>
       </c>
@@ -11449,7 +12326,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="135">
+    <row r="136" spans="1:3" ht="129.6">
       <c r="A136" s="5" t="s">
         <v>480</v>
       </c>
@@ -11460,7 +12337,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="135">
+    <row r="137" spans="1:3" ht="129.6">
       <c r="A137" s="5" t="s">
         <v>482</v>
       </c>
@@ -11471,7 +12348,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="135">
+    <row r="138" spans="1:3" ht="129.6">
       <c r="A138" s="5" t="s">
         <v>484</v>
       </c>
@@ -11482,7 +12359,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="135">
+    <row r="139" spans="1:3" ht="129.6">
       <c r="A139" s="5" t="s">
         <v>485</v>
       </c>
@@ -11493,7 +12370,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="135">
+    <row r="140" spans="1:3" ht="129.6">
       <c r="A140" s="5" t="s">
         <v>488</v>
       </c>
@@ -11504,7 +12381,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="135">
+    <row r="141" spans="1:3" ht="129.6">
       <c r="A141" s="5" t="s">
         <v>490</v>
       </c>
@@ -11515,7 +12392,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="135">
+    <row r="142" spans="1:3" ht="129.6">
       <c r="A142" s="5" t="s">
         <v>491</v>
       </c>
@@ -11526,7 +12403,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="120">
+    <row r="143" spans="1:3" ht="115.2">
       <c r="A143" s="5" t="s">
         <v>497</v>
       </c>
@@ -11537,7 +12414,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="135">
+    <row r="144" spans="1:3" ht="129.6">
       <c r="A144" s="5" t="s">
         <v>500</v>
       </c>
@@ -11548,7 +12425,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="135">
+    <row r="145" spans="1:3" ht="129.6">
       <c r="A145" s="5" t="s">
         <v>501</v>
       </c>
@@ -11559,7 +12436,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="135">
+    <row r="146" spans="1:3" ht="129.6">
       <c r="A146" s="5" t="s">
         <v>503</v>
       </c>
@@ -11570,7 +12447,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="135">
+    <row r="147" spans="1:3" ht="129.6">
       <c r="A147" s="5" t="s">
         <v>506</v>
       </c>
@@ -11581,7 +12458,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="135">
+    <row r="148" spans="1:3" ht="129.6">
       <c r="A148" s="5" t="s">
         <v>507</v>
       </c>
@@ -11636,7 +12513,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="30">
+    <row r="153" spans="1:3" ht="28.8">
       <c r="A153" s="5" t="s">
         <v>531</v>
       </c>
@@ -11647,7 +12524,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="30">
+    <row r="154" spans="1:3">
       <c r="A154" s="5" t="s">
         <v>532</v>
       </c>
@@ -11658,7 +12535,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="90">
+    <row r="155" spans="1:3" ht="86.4">
       <c r="A155" s="5" t="s">
         <v>534</v>
       </c>
@@ -11669,7 +12546,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="45">
+    <row r="156" spans="1:3" ht="43.2">
       <c r="A156" s="5" t="s">
         <v>536</v>
       </c>
@@ -11680,7 +12557,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="180">
+    <row r="157" spans="1:3" ht="172.8">
       <c r="A157" s="5" t="s">
         <v>540</v>
       </c>
@@ -11691,7 +12568,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="165">
+    <row r="158" spans="1:3" ht="158.4">
       <c r="A158" s="5" t="s">
         <v>541</v>
       </c>
@@ -11710,7 +12587,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="75">
+    <row r="160" spans="1:3" ht="72">
       <c r="A160" s="5" t="s">
         <v>547</v>
       </c>
@@ -11721,7 +12598,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="60">
+    <row r="161" spans="1:3" ht="57.6">
       <c r="A161" s="5" t="s">
         <v>551</v>
       </c>
@@ -11729,7 +12606,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="45">
+    <row r="162" spans="1:3" ht="43.2">
       <c r="A162" s="5" t="s">
         <v>552</v>
       </c>
@@ -11748,7 +12625,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="105">
+    <row r="164" spans="1:3" ht="100.8">
       <c r="A164" s="5" t="s">
         <v>560</v>
       </c>
@@ -11756,7 +12633,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="105">
+    <row r="165" spans="1:3" ht="100.8">
       <c r="A165" s="5" t="s">
         <v>561</v>
       </c>
@@ -11835,7 +12712,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="30">
+    <row r="173" spans="1:3">
       <c r="A173" s="5" t="s">
         <v>571</v>
       </c>
@@ -11898,7 +12775,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="30">
+    <row r="179" spans="1:3">
       <c r="A179" s="5" t="s">
         <v>577</v>
       </c>
@@ -11909,7 +12786,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="30">
+    <row r="180" spans="1:3" ht="28.8">
       <c r="A180" s="5" t="s">
         <v>578</v>
       </c>
@@ -11931,7 +12808,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="30">
+    <row r="182" spans="1:3">
       <c r="A182" s="5" t="s">
         <v>580</v>
       </c>
@@ -11942,7 +12819,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="120">
+    <row r="183" spans="1:3" ht="115.2">
       <c r="A183" s="5" t="s">
         <v>581</v>
       </c>
@@ -11997,7 +12874,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="75">
+    <row r="188" spans="1:3" ht="72">
       <c r="A188" s="5" t="s">
         <v>586</v>
       </c>
@@ -12008,7 +12885,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="105">
+    <row r="189" spans="1:3" ht="100.8">
       <c r="A189" s="5" t="s">
         <v>587</v>
       </c>
@@ -12019,7 +12896,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="75">
+    <row r="190" spans="1:3" ht="72">
       <c r="A190" s="5" t="s">
         <v>667</v>
       </c>
@@ -12030,7 +12907,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="90">
+    <row r="191" spans="1:3" ht="86.4">
       <c r="A191" s="5" t="s">
         <v>668</v>
       </c>
@@ -12041,7 +12918,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="90">
+    <row r="192" spans="1:3" ht="86.4">
       <c r="A192" s="5" t="s">
         <v>669</v>
       </c>
@@ -12096,7 +12973,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="30">
+    <row r="197" spans="1:3" ht="28.8">
       <c r="A197" s="5" t="s">
         <v>674</v>
       </c>
@@ -12107,7 +12984,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="30">
+    <row r="198" spans="1:3" ht="28.8">
       <c r="A198" s="5" t="s">
         <v>675</v>
       </c>
@@ -12129,7 +13006,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="30">
+    <row r="200" spans="1:3" ht="28.8">
       <c r="A200" s="5" t="s">
         <v>677</v>
       </c>
@@ -12140,7 +13017,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="90">
+    <row r="201" spans="1:3" ht="86.4">
       <c r="A201" s="5" t="s">
         <v>678</v>
       </c>
@@ -12151,7 +13028,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="75">
+    <row r="202" spans="1:3" ht="72">
       <c r="A202" s="5" t="s">
         <v>679</v>
       </c>
@@ -12162,7 +13039,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="90">
+    <row r="203" spans="1:3" ht="86.4">
       <c r="A203" s="5" t="s">
         <v>680</v>
       </c>
@@ -12173,7 +13050,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="30">
+    <row r="204" spans="1:3" ht="28.8">
       <c r="A204" s="5" t="s">
         <v>681</v>
       </c>
@@ -12181,7 +13058,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="409.5">
+    <row r="205" spans="1:3" ht="409.6">
       <c r="A205" s="5" t="s">
         <v>682</v>
       </c>
@@ -12192,7 +13069,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="240">
+    <row r="206" spans="1:3" ht="216">
       <c r="A206" s="5" t="s">
         <v>683</v>
       </c>
@@ -12214,7 +13091,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="45">
+    <row r="208" spans="1:3" ht="43.2">
       <c r="A208" s="5" t="s">
         <v>685</v>
       </c>
@@ -12225,7 +13102,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="105">
+    <row r="209" spans="1:3" ht="100.8">
       <c r="A209" s="5" t="s">
         <v>686</v>
       </c>
@@ -12247,7 +13124,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="409.5">
+    <row r="211" spans="1:3" ht="409.6">
       <c r="A211" s="5" t="s">
         <v>688</v>
       </c>
@@ -12269,7 +13146,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="30">
+    <row r="213" spans="1:3" ht="28.8">
       <c r="A213" s="5" t="s">
         <v>690</v>
       </c>
@@ -12280,7 +13157,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="75">
+    <row r="214" spans="1:3" ht="72">
       <c r="A214" s="5" t="s">
         <v>691</v>
       </c>
@@ -12291,7 +13168,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="90">
+    <row r="215" spans="1:3" ht="86.4">
       <c r="A215" s="5" t="s">
         <v>692</v>
       </c>
@@ -12302,7 +13179,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="75">
+    <row r="216" spans="1:3" ht="72">
       <c r="A216" s="5" t="s">
         <v>693</v>
       </c>
@@ -12313,7 +13190,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="90">
+    <row r="217" spans="1:3" ht="86.4">
       <c r="A217" s="5" t="s">
         <v>694</v>
       </c>
@@ -12324,7 +13201,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="240">
+    <row r="218" spans="1:3" ht="216">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -12335,7 +13212,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="409.5">
+    <row r="219" spans="1:3" ht="409.6">
       <c r="A219" s="5" t="s">
         <v>695</v>
       </c>
@@ -12346,7 +13223,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="240">
+    <row r="220" spans="1:3" ht="216">
       <c r="A220" s="5" t="s">
         <v>696</v>
       </c>
@@ -12357,7 +13234,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="180">
+    <row r="221" spans="1:3" ht="158.4">
       <c r="A221" s="5" t="s">
         <v>697</v>
       </c>
@@ -12373,7 +13250,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="105">
+    <row r="223" spans="1:3" ht="100.8">
       <c r="A223" s="5" t="s">
         <v>699</v>
       </c>
@@ -12384,7 +13261,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="105">
+    <row r="224" spans="1:3" ht="100.8">
       <c r="A224" s="5" t="s">
         <v>700</v>
       </c>
@@ -12395,7 +13272,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="105">
+    <row r="225" spans="1:3" ht="100.8">
       <c r="A225" s="5" t="s">
         <v>701</v>
       </c>
@@ -12470,7 +13347,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="105">
+    <row r="234" spans="1:3" ht="86.4">
       <c r="A234" s="5" t="s">
         <v>710</v>
       </c>
@@ -12489,7 +13366,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="90">
+    <row r="236" spans="1:3" ht="86.4">
       <c r="A236" s="5" t="s">
         <v>712</v>
       </c>
@@ -12522,7 +13399,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="135">
+    <row r="239" spans="1:3" ht="129.6">
       <c r="A239" s="5" t="s">
         <v>715</v>
       </c>
@@ -12533,7 +13410,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="30">
+    <row r="240" spans="1:3" ht="28.8">
       <c r="A240" s="5" t="s">
         <v>716</v>
       </c>
@@ -12555,7 +13432,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="105">
+    <row r="242" spans="1:3" ht="100.8">
       <c r="A242" s="5" t="s">
         <v>785</v>
       </c>
@@ -12566,7 +13443,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="45">
+    <row r="243" spans="1:3" ht="43.2">
       <c r="A243" s="5" t="s">
         <v>786</v>
       </c>
@@ -12577,7 +13454,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="180">
+    <row r="244" spans="1:3" ht="172.8">
       <c r="A244" s="5" t="s">
         <v>787</v>
       </c>
@@ -12588,7 +13465,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="225">
+    <row r="245" spans="1:3" ht="216">
       <c r="A245" s="5" t="s">
         <v>789</v>
       </c>
@@ -12599,7 +13476,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="180">
+    <row r="246" spans="1:3" ht="172.8">
       <c r="A246" s="5" t="s">
         <v>794</v>
       </c>
@@ -12610,7 +13487,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="195">
+    <row r="247" spans="1:3" ht="187.2">
       <c r="A247" s="5" t="s">
         <v>799</v>
       </c>
@@ -12621,7 +13498,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="195">
+    <row r="248" spans="1:3" ht="187.2">
       <c r="A248" s="5" t="s">
         <v>802</v>
       </c>
@@ -12632,7 +13509,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="225">
+    <row r="249" spans="1:3" ht="216">
       <c r="A249" s="5" t="s">
         <v>805</v>
       </c>
@@ -12643,7 +13520,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="120">
+    <row r="250" spans="1:3" ht="115.2">
       <c r="A250" s="5" t="s">
         <v>825</v>
       </c>
@@ -12654,7 +13531,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="150">
+    <row r="251" spans="1:3" ht="144">
       <c r="A251" s="5" t="s">
         <v>828</v>
       </c>
@@ -12665,7 +13542,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="120">
+    <row r="252" spans="1:3" ht="115.2">
       <c r="A252" s="5" t="s">
         <v>831</v>
       </c>
@@ -12687,7 +13564,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="30">
+    <row r="254" spans="1:3" ht="28.8">
       <c r="A254" s="5" t="s">
         <v>839</v>
       </c>
@@ -12698,7 +13575,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="75">
+    <row r="255" spans="1:3" ht="72">
       <c r="A255" s="5" t="s">
         <v>840</v>
       </c>
@@ -12709,7 +13586,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="30">
+    <row r="256" spans="1:3" ht="28.8">
       <c r="A256" s="5" t="s">
         <v>841</v>
       </c>
@@ -12720,7 +13597,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="75">
+    <row r="257" spans="1:3" ht="72">
       <c r="A257" s="5" t="s">
         <v>842</v>
       </c>
@@ -12731,7 +13608,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="150">
+    <row r="258" spans="1:3" ht="144">
       <c r="A258" s="5" t="s">
         <v>848</v>
       </c>
@@ -12753,7 +13630,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="45">
+    <row r="260" spans="1:3" ht="43.2">
       <c r="A260" s="5" t="s">
         <v>852</v>
       </c>
@@ -12764,7 +13641,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="60">
+    <row r="261" spans="1:3" ht="57.6">
       <c r="A261" s="5" t="s">
         <v>855</v>
       </c>
@@ -12775,7 +13652,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="90">
+    <row r="262" spans="1:3" ht="86.4">
       <c r="A262" s="5" t="s">
         <v>858</v>
       </c>
@@ -12794,7 +13671,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="60">
+    <row r="264" spans="1:3" ht="57.6">
       <c r="A264" s="5" t="s">
         <v>863</v>
       </c>
@@ -12805,7 +13682,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="90">
+    <row r="265" spans="1:3" ht="86.4">
       <c r="A265" s="5" t="s">
         <v>866</v>
       </c>
@@ -12816,7 +13693,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="75">
+    <row r="266" spans="1:3" ht="72">
       <c r="A266" s="5" t="s">
         <v>869</v>
       </c>
@@ -12851,7 +13728,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="30">
+    <row r="270" spans="1:3" ht="28.8">
       <c r="A270" s="5" t="s">
         <v>883</v>
       </c>
@@ -12859,7 +13736,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="120">
+    <row r="271" spans="1:3" ht="100.8">
       <c r="A271" s="5" t="s">
         <v>884</v>
       </c>
@@ -12870,7 +13747,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="45">
+    <row r="272" spans="1:3" ht="43.2">
       <c r="A272" s="5" t="s">
         <v>885</v>
       </c>
@@ -12881,7 +13758,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="30">
+    <row r="273" spans="1:4" ht="28.8">
       <c r="A273" s="5" t="s">
         <v>886</v>
       </c>
@@ -12892,7 +13769,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="75">
+    <row r="274" spans="1:4" ht="72">
       <c r="A274" s="5" t="s">
         <v>890</v>
       </c>
@@ -13540,7 +14417,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="401" spans="1:3" ht="30">
+    <row r="401" spans="1:3" ht="28.8">
       <c r="A401" s="2" t="s">
         <v>1018</v>
       </c>
@@ -13551,7 +14428,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="402" spans="1:3" ht="75">
+    <row r="402" spans="1:3" ht="72">
       <c r="A402" s="2" t="s">
         <v>1019</v>
       </c>
@@ -13562,7 +14439,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="60">
+    <row r="403" spans="1:3" ht="43.2">
       <c r="A403" s="2" t="s">
         <v>1020</v>
       </c>
@@ -13573,7 +14450,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="30">
+    <row r="404" spans="1:3" ht="28.8">
       <c r="A404" s="2" t="s">
         <v>1021</v>
       </c>
@@ -13584,7 +14461,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="30">
+    <row r="405" spans="1:3" ht="28.8">
       <c r="A405" s="2" t="s">
         <v>1022</v>
       </c>
@@ -13595,7 +14472,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="60">
+    <row r="406" spans="1:3" ht="43.2">
       <c r="A406" s="2" t="s">
         <v>1023</v>
       </c>
@@ -13606,7 +14483,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="407" spans="1:3" ht="30">
+    <row r="407" spans="1:3" ht="28.8">
       <c r="A407" s="2" t="s">
         <v>1024</v>
       </c>
@@ -13617,7 +14494,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="135">
+    <row r="408" spans="1:3" ht="129.6">
       <c r="A408" s="2" t="s">
         <v>1025</v>
       </c>
@@ -13628,7 +14505,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="409" spans="1:3" ht="45">
+    <row r="409" spans="1:3" ht="43.2">
       <c r="A409" s="2" t="s">
         <v>1026</v>
       </c>
@@ -13639,7 +14516,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="410" spans="1:3" ht="30">
+    <row r="410" spans="1:3" ht="28.8">
       <c r="A410" s="2" t="s">
         <v>1027</v>
       </c>
@@ -13650,7 +14527,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="30">
+    <row r="411" spans="1:3" ht="28.8">
       <c r="A411" s="2" t="s">
         <v>1028</v>
       </c>
@@ -13661,7 +14538,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="165">
+    <row r="412" spans="1:3" ht="158.4">
       <c r="A412" s="2" t="s">
         <v>1029</v>
       </c>
@@ -13672,7 +14549,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="180">
+    <row r="413" spans="1:3" ht="172.8">
       <c r="A413" s="2" t="s">
         <v>1030</v>
       </c>
@@ -13683,7 +14560,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="75">
+    <row r="414" spans="1:3" ht="72">
       <c r="A414" s="2" t="s">
         <v>1031</v>
       </c>
@@ -13705,7 +14582,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="75">
+    <row r="416" spans="1:3" ht="72">
       <c r="A416" s="2" t="s">
         <v>1033</v>
       </c>
@@ -13716,7 +14593,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="120">
+    <row r="417" spans="1:3" ht="115.2">
       <c r="A417" s="2" t="s">
         <v>1034</v>
       </c>
@@ -13727,7 +14604,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="135">
+    <row r="418" spans="1:3" ht="129.6">
       <c r="A418" s="2" t="s">
         <v>1035</v>
       </c>
@@ -13738,7 +14615,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="30">
+    <row r="419" spans="1:3" ht="28.8">
       <c r="A419" s="2" t="s">
         <v>1036</v>
       </c>
@@ -13848,7 +14725,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="75">
+    <row r="429" spans="1:3" ht="72">
       <c r="A429" s="2" t="s">
         <v>1046</v>
       </c>
@@ -18354,82 +19231,91 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="1329" spans="1:1">
+    <row r="1329" spans="1:2">
       <c r="A1329" s="5" t="s">
         <v>1946</v>
       </c>
     </row>
-    <row r="1330" spans="1:1">
+    <row r="1330" spans="1:2">
       <c r="A1330" s="5" t="s">
         <v>1947</v>
       </c>
     </row>
-    <row r="1331" spans="1:1">
+    <row r="1331" spans="1:2">
       <c r="A1331" s="5" t="s">
         <v>1948</v>
       </c>
     </row>
-    <row r="1332" spans="1:1">
+    <row r="1332" spans="1:2">
       <c r="A1332" s="5" t="s">
         <v>1949</v>
       </c>
     </row>
-    <row r="1333" spans="1:1">
+    <row r="1333" spans="1:2">
       <c r="A1333" s="5" t="s">
         <v>1950</v>
       </c>
     </row>
-    <row r="1334" spans="1:1">
+    <row r="1334" spans="1:2">
       <c r="A1334" s="5" t="s">
         <v>1951</v>
       </c>
     </row>
-    <row r="1335" spans="1:1">
+    <row r="1335" spans="1:2">
       <c r="A1335" s="5" t="s">
         <v>1952</v>
       </c>
     </row>
-    <row r="1336" spans="1:1">
+    <row r="1336" spans="1:2">
       <c r="A1336" s="5" t="s">
         <v>1953</v>
       </c>
     </row>
-    <row r="1337" spans="1:1">
+    <row r="1337" spans="1:2">
       <c r="A1337" s="5" t="s">
         <v>1954</v>
       </c>
     </row>
-    <row r="1338" spans="1:1">
+    <row r="1338" spans="1:2">
       <c r="A1338" s="5" t="s">
         <v>1955</v>
       </c>
     </row>
-    <row r="1339" spans="1:1">
+    <row r="1339" spans="1:2">
       <c r="A1339" s="5" t="s">
         <v>1956</v>
       </c>
     </row>
-    <row r="1340" spans="1:1">
-      <c r="A1340" s="5" t="s">
+    <row r="1340" spans="1:2">
+      <c r="A1340" s="47" t="s">
         <v>1957</v>
       </c>
     </row>
-    <row r="1341" spans="1:1">
-      <c r="A1341" s="5" t="s">
+    <row r="1341" spans="1:2" ht="129.6">
+      <c r="A1341" s="47" t="s">
         <v>1958</v>
       </c>
-    </row>
-    <row r="1342" spans="1:1">
-      <c r="A1342" s="5" t="s">
+      <c r="B1341" s="48" t="s">
+        <v>2628</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:2">
+      <c r="A1342" s="47" t="s">
         <v>1959</v>
       </c>
-    </row>
-    <row r="1343" spans="1:1">
+      <c r="B1342" t="s">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:2">
       <c r="A1343" s="5" t="s">
         <v>1960</v>
       </c>
-    </row>
-    <row r="1344" spans="1:1">
+      <c r="B1343" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:2">
       <c r="A1344" s="5" t="s">
         <v>1961</v>
       </c>
@@ -19219,7 +20105,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="1502" spans="1:3" ht="90">
+    <row r="1502" spans="1:3" ht="86.4">
       <c r="A1502" s="5" t="s">
         <v>2119</v>
       </c>
@@ -19230,7 +20116,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="1503" spans="1:3" ht="90">
+    <row r="1503" spans="1:3" ht="86.4">
       <c r="A1503" s="5" t="s">
         <v>2120</v>
       </c>
@@ -19241,7 +20127,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="1504" spans="1:3" ht="150">
+    <row r="1504" spans="1:3" ht="144">
       <c r="A1504" s="5" t="s">
         <v>2121</v>
       </c>
@@ -19252,7 +20138,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="1505" spans="1:3" ht="150">
+    <row r="1505" spans="1:3" ht="144">
       <c r="A1505" s="5" t="s">
         <v>2122</v>
       </c>
@@ -19263,7 +20149,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1506" spans="1:3" ht="75">
+    <row r="1506" spans="1:3" ht="72">
       <c r="A1506" s="5" t="s">
         <v>2123</v>
       </c>
@@ -19271,7 +20157,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="1507" spans="1:3" ht="45">
+    <row r="1507" spans="1:3" ht="43.2">
       <c r="A1507" s="47" t="s">
         <v>2124</v>
       </c>
@@ -19282,7 +20168,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1508" spans="1:3" ht="45">
+    <row r="1508" spans="1:3" ht="43.2">
       <c r="A1508" s="44" t="s">
         <v>2125</v>
       </c>
@@ -19758,7 +20644,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="1602" spans="1:3" ht="30">
+    <row r="1602" spans="1:3" ht="28.8">
       <c r="A1602" s="5" t="s">
         <v>2219</v>
       </c>
@@ -19780,7 +20666,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="1604" spans="1:3" ht="60">
+    <row r="1604" spans="1:3" ht="57.6">
       <c r="A1604" s="5" t="s">
         <v>2221</v>
       </c>
@@ -19791,7 +20677,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="1605" spans="1:3" ht="45">
+    <row r="1605" spans="1:3" ht="43.2">
       <c r="A1605" s="5" t="s">
         <v>2222</v>
       </c>
@@ -19799,7 +20685,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="1606" spans="1:3" ht="105">
+    <row r="1606" spans="1:3" ht="100.8">
       <c r="A1606" s="5" t="s">
         <v>2223</v>
       </c>
@@ -19829,7 +20715,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="1609" spans="1:3" ht="45">
+    <row r="1609" spans="1:3" ht="43.2">
       <c r="A1609" s="5" t="s">
         <v>2278</v>
       </c>
@@ -19840,7 +20726,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="1610" spans="1:3" ht="30">
+    <row r="1610" spans="1:3" ht="28.8">
       <c r="A1610" s="5" t="s">
         <v>2279</v>
       </c>
@@ -19848,7 +20734,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="1611" spans="1:3" ht="409.5">
+    <row r="1611" spans="1:3" ht="388.8">
       <c r="A1611" s="5" t="s">
         <v>2280</v>
       </c>
@@ -19859,7 +20745,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="1612" spans="1:3" ht="240">
+    <row r="1612" spans="1:3" ht="230.4">
       <c r="A1612" s="44" t="s">
         <v>2281</v>
       </c>
@@ -19870,10 +20756,1453 @@
         <v>2286</v>
       </c>
     </row>
+    <row r="1613" spans="1:3">
+      <c r="A1613" s="50" t="s">
+        <v>2337</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:3">
+      <c r="A1614" s="50" t="s">
+        <v>2338</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:3">
+      <c r="A1615" s="50" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:3">
+      <c r="A1616" s="50" t="s">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:1">
+      <c r="A1617" s="50" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:1">
+      <c r="A1618" s="50" t="s">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:1">
+      <c r="A1619" s="50" t="s">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:1">
+      <c r="A1620" s="50" t="s">
+        <v>2344</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:1">
+      <c r="A1621" s="50" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:1">
+      <c r="A1622" s="50" t="s">
+        <v>2346</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:1">
+      <c r="A1623" s="50" t="s">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:1">
+      <c r="A1624" s="50" t="s">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:1">
+      <c r="A1625" s="50" t="s">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:1">
+      <c r="A1626" s="50" t="s">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:1">
+      <c r="A1627" s="50" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:1">
+      <c r="A1628" s="50" t="s">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:1">
+      <c r="A1629" s="50" t="s">
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:1">
+      <c r="A1630" s="50" t="s">
+        <v>2354</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:1">
+      <c r="A1631" s="50" t="s">
+        <v>2355</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:1">
+      <c r="A1632" s="50" t="s">
+        <v>2356</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:1">
+      <c r="A1633" s="50" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:1">
+      <c r="A1634" s="50" t="s">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:1">
+      <c r="A1635" s="50" t="s">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:1">
+      <c r="A1636" s="50" t="s">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:1">
+      <c r="A1637" s="50" t="s">
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:1">
+      <c r="A1638" s="50" t="s">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:1">
+      <c r="A1639" s="50" t="s">
+        <v>2363</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:1">
+      <c r="A1640" s="50" t="s">
+        <v>2364</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:1">
+      <c r="A1641" s="50" t="s">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:1">
+      <c r="A1642" s="50" t="s">
+        <v>2366</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:1">
+      <c r="A1643" s="50" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:1">
+      <c r="A1644" s="50" t="s">
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:1">
+      <c r="A1645" s="50" t="s">
+        <v>2369</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:1">
+      <c r="A1646" s="50" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:1">
+      <c r="A1647" s="50" t="s">
+        <v>2371</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:1">
+      <c r="A1648" s="50" t="s">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:1">
+      <c r="A1649" s="50" t="s">
+        <v>2373</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:1">
+      <c r="A1650" s="50" t="s">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:1">
+      <c r="A1651" s="50" t="s">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:1">
+      <c r="A1652" s="50" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:1">
+      <c r="A1653" s="50" t="s">
+        <v>2377</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:1">
+      <c r="A1654" s="50" t="s">
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:1">
+      <c r="A1655" s="50" t="s">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:1">
+      <c r="A1656" s="50" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:1">
+      <c r="A1657" s="50" t="s">
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:1">
+      <c r="A1658" s="50" t="s">
+        <v>2382</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:1">
+      <c r="A1659" s="50" t="s">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:1">
+      <c r="A1660" s="50" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:1">
+      <c r="A1661" s="50" t="s">
+        <v>2385</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:1">
+      <c r="A1662" s="50" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:1">
+      <c r="A1663" s="50" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:1">
+      <c r="A1664" s="50" t="s">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:1">
+      <c r="A1665" s="50" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:1">
+      <c r="A1666" s="50" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:1">
+      <c r="A1667" s="50" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:1">
+      <c r="A1668" s="50" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:1">
+      <c r="A1669" s="50" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:1">
+      <c r="A1670" s="50" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:1">
+      <c r="A1671" s="50" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:1">
+      <c r="A1672" s="50" t="s">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:1">
+      <c r="A1673" s="50" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:1">
+      <c r="A1674" s="50" t="s">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:1">
+      <c r="A1675" s="50" t="s">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:1">
+      <c r="A1676" s="50" t="s">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:1">
+      <c r="A1677" s="50" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:1">
+      <c r="A1678" s="50" t="s">
+        <v>2402</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:1">
+      <c r="A1679" s="50" t="s">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:1">
+      <c r="A1680" s="50" t="s">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:1">
+      <c r="A1681" s="50" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:1">
+      <c r="A1682" s="50" t="s">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:1">
+      <c r="A1683" s="50" t="s">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:1">
+      <c r="A1684" s="50" t="s">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:1">
+      <c r="A1685" s="50" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:1">
+      <c r="A1686" s="50" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:1">
+      <c r="A1687" s="50" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:1">
+      <c r="A1688" s="50" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:1">
+      <c r="A1689" s="50" t="s">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:1">
+      <c r="A1690" s="50" t="s">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:1">
+      <c r="A1691" s="50" t="s">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:1">
+      <c r="A1692" s="50" t="s">
+        <v>2416</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:1">
+      <c r="A1693" s="50" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:1">
+      <c r="A1694" s="50" t="s">
+        <v>2418</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:1">
+      <c r="A1695" s="50" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:1">
+      <c r="A1696" s="50" t="s">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:1">
+      <c r="A1697" s="50" t="s">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:1">
+      <c r="A1698" s="50" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:1">
+      <c r="A1699" s="50" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:1">
+      <c r="A1700" s="50" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:1">
+      <c r="A1701" s="50" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:1">
+      <c r="A1702" s="50" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:1">
+      <c r="A1703" s="50" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:1">
+      <c r="A1704" s="50" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:1">
+      <c r="A1705" s="50" t="s">
+        <v>2429</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:1">
+      <c r="A1706" s="50" t="s">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:1">
+      <c r="A1707" s="50" t="s">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:1">
+      <c r="A1708" s="50" t="s">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:1">
+      <c r="A1709" s="50" t="s">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:1">
+      <c r="A1710" s="50" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:1">
+      <c r="A1711" s="50" t="s">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:1">
+      <c r="A1712" s="50" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:1">
+      <c r="A1713" s="50" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:1">
+      <c r="A1714" s="50" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:1">
+      <c r="A1715" s="50" t="s">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:1">
+      <c r="A1716" s="50" t="s">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:1">
+      <c r="A1717" s="50" t="s">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:1">
+      <c r="A1718" s="50" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:1">
+      <c r="A1719" s="50" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:1">
+      <c r="A1720" s="50" t="s">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:1">
+      <c r="A1721" s="50" t="s">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:1">
+      <c r="A1722" s="50" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:1">
+      <c r="A1723" s="50" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:1">
+      <c r="A1724" s="50" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:1">
+      <c r="A1725" s="50" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:1">
+      <c r="A1726" s="50" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:1">
+      <c r="A1727" s="50" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:1">
+      <c r="A1728" s="50" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:1">
+      <c r="A1729" s="50" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:1">
+      <c r="A1730" s="50" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:1">
+      <c r="A1731" s="50" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:1">
+      <c r="A1732" s="50" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:1">
+      <c r="A1733" s="50" t="s">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:1">
+      <c r="A1734" s="50" t="s">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:1">
+      <c r="A1735" s="50" t="s">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:1">
+      <c r="A1736" s="50" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:1">
+      <c r="A1737" s="50" t="s">
+        <v>2461</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:1">
+      <c r="A1738" s="50" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:1">
+      <c r="A1739" s="50" t="s">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:1">
+      <c r="A1740" s="50" t="s">
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:1">
+      <c r="A1741" s="50" t="s">
+        <v>2465</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:1">
+      <c r="A1742" s="50" t="s">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:1">
+      <c r="A1743" s="50" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:1">
+      <c r="A1744" s="50" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:1">
+      <c r="A1745" s="50" t="s">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:1">
+      <c r="A1746" s="50" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:1">
+      <c r="A1747" s="50" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:1">
+      <c r="A1748" s="50" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:1">
+      <c r="A1749" s="50" t="s">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:1">
+      <c r="A1750" s="50" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:1">
+      <c r="A1751" s="50" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:1">
+      <c r="A1752" s="50" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:1">
+      <c r="A1753" s="50" t="s">
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:1">
+      <c r="A1754" s="50" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:1">
+      <c r="A1755" s="50" t="s">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:1">
+      <c r="A1756" s="50" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:1">
+      <c r="A1757" s="50" t="s">
+        <v>2481</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:1">
+      <c r="A1758" s="50" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:1">
+      <c r="A1759" s="50" t="s">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:1">
+      <c r="A1760" s="50" t="s">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:1">
+      <c r="A1761" s="50" t="s">
+        <v>2485</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:1">
+      <c r="A1762" s="50" t="s">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:1">
+      <c r="A1763" s="50" t="s">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:1">
+      <c r="A1764" s="50" t="s">
+        <v>2488</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:1">
+      <c r="A1765" s="50" t="s">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:1">
+      <c r="A1766" s="50" t="s">
+        <v>2490</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:1">
+      <c r="A1767" s="50" t="s">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:1">
+      <c r="A1768" s="50" t="s">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:1">
+      <c r="A1769" s="50" t="s">
+        <v>2493</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:1">
+      <c r="A1770" s="50" t="s">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:1">
+      <c r="A1771" s="50" t="s">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:1">
+      <c r="A1772" s="50" t="s">
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:1">
+      <c r="A1773" s="50" t="s">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:1">
+      <c r="A1774" s="50" t="s">
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:1">
+      <c r="A1775" s="50" t="s">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:1">
+      <c r="A1776" s="50" t="s">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:1">
+      <c r="A1777" s="50" t="s">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:1">
+      <c r="A1778" s="50" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:1">
+      <c r="A1779" s="50" t="s">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:1">
+      <c r="A1780" s="50" t="s">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:1">
+      <c r="A1781" s="50" t="s">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:1">
+      <c r="A1782" s="50" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:1">
+      <c r="A1783" s="50" t="s">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:1">
+      <c r="A1784" s="50" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:1">
+      <c r="A1785" s="50" t="s">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:1">
+      <c r="A1786" s="50" t="s">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:1">
+      <c r="A1787" s="50" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:1">
+      <c r="A1788" s="50" t="s">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:1">
+      <c r="A1789" s="50" t="s">
+        <v>2513</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:1">
+      <c r="A1790" s="50" t="s">
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:1">
+      <c r="A1791" s="50" t="s">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:1">
+      <c r="A1792" s="50" t="s">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:1">
+      <c r="A1793" s="50" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:1">
+      <c r="A1794" s="50" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:1">
+      <c r="A1795" s="50" t="s">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:1">
+      <c r="A1796" s="50" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:1">
+      <c r="A1797" s="50" t="s">
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:1">
+      <c r="A1798" s="50" t="s">
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:1">
+      <c r="A1799" s="50" t="s">
+        <v>2523</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:1">
+      <c r="A1800" s="50" t="s">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:1">
+      <c r="A1801" s="50" t="s">
+        <v>2525</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:1">
+      <c r="A1802" s="50" t="s">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:1">
+      <c r="A1803" s="50" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:1">
+      <c r="A1804" s="50" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:1">
+      <c r="A1805" s="50" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:1">
+      <c r="A1806" s="50" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:1">
+      <c r="A1807" s="50" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:1">
+      <c r="A1808" s="50" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:1">
+      <c r="A1809" s="50" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:1">
+      <c r="A1810" s="50" t="s">
+        <v>2534</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:1">
+      <c r="A1811" s="50" t="s">
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:1">
+      <c r="A1812" s="50" t="s">
+        <v>2536</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:1">
+      <c r="A1813" s="50" t="s">
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:1">
+      <c r="A1814" s="50" t="s">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:1">
+      <c r="A1815" s="50" t="s">
+        <v>2539</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:1">
+      <c r="A1816" s="50" t="s">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:1">
+      <c r="A1817" s="50" t="s">
+        <v>2541</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:1">
+      <c r="A1818" s="50" t="s">
+        <v>2542</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:1">
+      <c r="A1819" s="50" t="s">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:1">
+      <c r="A1820" s="50" t="s">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:1">
+      <c r="A1821" s="50" t="s">
+        <v>2545</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:1">
+      <c r="A1822" s="50" t="s">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:1">
+      <c r="A1823" s="50" t="s">
+        <v>2547</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:1">
+      <c r="A1824" s="50" t="s">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:1">
+      <c r="A1825" s="50" t="s">
+        <v>2549</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:1">
+      <c r="A1826" s="50" t="s">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:1">
+      <c r="A1827" s="50" t="s">
+        <v>2551</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:1">
+      <c r="A1828" s="50" t="s">
+        <v>2552</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:1">
+      <c r="A1829" s="50" t="s">
+        <v>2553</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:1">
+      <c r="A1830" s="50" t="s">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:1">
+      <c r="A1831" s="50" t="s">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:1">
+      <c r="A1832" s="50" t="s">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="1833" spans="1:1">
+      <c r="A1833" s="50" t="s">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:1">
+      <c r="A1834" s="50" t="s">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:1">
+      <c r="A1835" s="50" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:1">
+      <c r="A1836" s="50" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:1">
+      <c r="A1837" s="50" t="s">
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:1">
+      <c r="A1838" s="50" t="s">
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:1">
+      <c r="A1839" s="50" t="s">
+        <v>2563</v>
+      </c>
+    </row>
+    <row r="1840" spans="1:1">
+      <c r="A1840" s="50" t="s">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:1">
+      <c r="A1841" s="50" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:1">
+      <c r="A1842" s="50" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:1">
+      <c r="A1843" s="50" t="s">
+        <v>2567</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:1">
+      <c r="A1844" s="50" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:1">
+      <c r="A1845" s="50" t="s">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:1">
+      <c r="A1846" s="50" t="s">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:1">
+      <c r="A1847" s="50" t="s">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:1">
+      <c r="A1848" s="50" t="s">
+        <v>2572</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:1">
+      <c r="A1849" s="50" t="s">
+        <v>2573</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:1">
+      <c r="A1850" s="50" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:1">
+      <c r="A1851" s="50" t="s">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:1">
+      <c r="A1852" s="50" t="s">
+        <v>2576</v>
+      </c>
+    </row>
+    <row r="1853" spans="1:1">
+      <c r="A1853" s="50" t="s">
+        <v>2577</v>
+      </c>
+    </row>
+    <row r="1854" spans="1:1">
+      <c r="A1854" s="50" t="s">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="1855" spans="1:1">
+      <c r="A1855" s="50" t="s">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="1856" spans="1:1">
+      <c r="A1856" s="50" t="s">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:1">
+      <c r="A1857" s="50" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:1">
+      <c r="A1858" s="50" t="s">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="1859" spans="1:1">
+      <c r="A1859" s="50" t="s">
+        <v>2583</v>
+      </c>
+    </row>
+    <row r="1860" spans="1:1">
+      <c r="A1860" s="50" t="s">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="1861" spans="1:1">
+      <c r="A1861" s="50" t="s">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:1">
+      <c r="A1862" s="50" t="s">
+        <v>2586</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:1">
+      <c r="A1863" s="50" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:1">
+      <c r="A1864" s="50" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:1">
+      <c r="A1865" s="50" t="s">
+        <v>2589</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:1">
+      <c r="A1866" s="50" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:1">
+      <c r="A1867" s="50" t="s">
+        <v>2591</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:1">
+      <c r="A1868" s="50" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:1">
+      <c r="A1869" s="50" t="s">
+        <v>2593</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:1">
+      <c r="A1870" s="50" t="s">
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:1">
+      <c r="A1871" s="50" t="s">
+        <v>2595</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:1">
+      <c r="A1872" s="50" t="s">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:1">
+      <c r="A1873" s="50" t="s">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:1">
+      <c r="A1874" s="50" t="s">
+        <v>2598</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:1">
+      <c r="A1875" s="50" t="s">
+        <v>2599</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:1">
+      <c r="A1876" s="50" t="s">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:1">
+      <c r="A1877" s="50" t="s">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:1">
+      <c r="A1878" s="50" t="s">
+        <v>2602</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:1">
+      <c r="A1879" s="50" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:1">
+      <c r="A1880" s="50" t="s">
+        <v>2604</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:1">
+      <c r="A1881" s="50" t="s">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:1">
+      <c r="A1882" s="50" t="s">
+        <v>2606</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:1">
+      <c r="A1883" s="50" t="s">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:1">
+      <c r="A1884" s="50" t="s">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:1">
+      <c r="A1885" s="50" t="s">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:1">
+      <c r="A1886" s="50" t="s">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:1">
+      <c r="A1887" s="50" t="s">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:1">
+      <c r="A1888" s="50" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:3">
+      <c r="A1889" s="50" t="s">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="1890" spans="1:3">
+      <c r="A1890" s="50" t="s">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="1891" spans="1:3">
+      <c r="A1891" s="50" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:3">
+      <c r="A1892" s="50" t="s">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:3">
+      <c r="A1893" s="50" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:3">
+      <c r="A1894" s="50" t="s">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:3">
+      <c r="A1895" s="50" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:3">
+      <c r="A1896" s="50" t="s">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:3">
+      <c r="A1897" s="50" t="s">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:3">
+      <c r="A1898" s="50" t="s">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="1899" spans="1:3">
+      <c r="A1899" s="50" t="s">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:3">
+      <c r="A1900" s="50" t="s">
+        <v>2624</v>
+      </c>
+    </row>
     <row r="1901" spans="1:3">
+      <c r="A1901" s="50" t="s">
+        <v>2625</v>
+      </c>
       <c r="B1901" s="48"/>
     </row>
-    <row r="1902" spans="1:3" ht="45">
+    <row r="1902" spans="1:3" ht="43.2">
       <c r="A1902">
         <v>1901</v>
       </c>
@@ -19884,7 +22213,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="1903" spans="1:3" ht="90">
+    <row r="1903" spans="1:3" ht="86.4">
       <c r="A1903">
         <v>1902</v>
       </c>
@@ -19895,7 +22224,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="1904" spans="1:3" ht="225">
+    <row r="1904" spans="1:3" ht="216">
       <c r="A1904">
         <v>1903</v>
       </c>
@@ -19906,7 +22235,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="1905" spans="1:3" ht="150">
+    <row r="1905" spans="1:3" ht="144">
       <c r="A1905">
         <v>1904</v>
       </c>
@@ -19917,7 +22246,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="1906" spans="1:3" ht="150">
+    <row r="1906" spans="1:3" ht="144">
       <c r="A1906">
         <v>1905</v>
       </c>
@@ -19928,7 +22257,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="1907" spans="1:3" ht="120">
+    <row r="1907" spans="1:3" ht="115.2">
       <c r="A1907">
         <v>1906</v>
       </c>
@@ -19939,7 +22268,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="1908" spans="1:3" ht="150">
+    <row r="1908" spans="1:3" ht="144">
       <c r="A1908">
         <v>1907</v>
       </c>
@@ -19950,7 +22279,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="1909" spans="1:3" ht="150">
+    <row r="1909" spans="1:3" ht="144">
       <c r="A1909">
         <v>1908</v>
       </c>
@@ -19961,7 +22290,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="1910" spans="1:3" ht="105">
+    <row r="1910" spans="1:3" ht="100.8">
       <c r="A1910">
         <v>1909</v>
       </c>
@@ -20009,13 +22338,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -20195,10 +22524,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -20521,7 +22850,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" ht="15">
       <c r="A44" s="13" t="s">
         <v>263</v>
       </c>
@@ -20611,13 +22940,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="85.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+    <row r="1" spans="1:2" ht="15" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>283</v>
       </c>
@@ -20625,7 +22954,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+    <row r="2" spans="1:2" ht="15" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>285</v>
       </c>
@@ -20633,7 +22962,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+    <row r="3" spans="1:2" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>287</v>
       </c>
@@ -20641,7 +22970,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+    <row r="4" spans="1:2" ht="15" thickBot="1">
       <c r="A4" s="25" t="s">
         <v>289</v>
       </c>
@@ -20649,7 +22978,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+    <row r="5" spans="1:2" ht="15" thickBot="1">
       <c r="A5" s="25" t="s">
         <v>291</v>
       </c>
@@ -20657,7 +22986,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+    <row r="6" spans="1:2" ht="15" thickBot="1">
       <c r="A6" s="25" t="s">
         <v>293</v>
       </c>
@@ -20665,7 +22994,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1">
+    <row r="7" spans="1:2" ht="15" thickBot="1">
       <c r="A7" s="25" t="s">
         <v>295</v>
       </c>
@@ -20673,7 +23002,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+    <row r="8" spans="1:2" ht="15" thickBot="1">
       <c r="A8" s="25" t="s">
         <v>297</v>
       </c>
@@ -20681,7 +23010,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1">
+    <row r="9" spans="1:2" ht="15" thickBot="1">
       <c r="A9" s="25" t="s">
         <v>299</v>
       </c>
@@ -20689,7 +23018,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1">
+    <row r="10" spans="1:2" ht="15" thickBot="1">
       <c r="A10" s="25" t="s">
         <v>301</v>
       </c>
@@ -20697,7 +23026,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1">
+    <row r="11" spans="1:2" ht="15" thickBot="1">
       <c r="A11" s="25" t="s">
         <v>303</v>
       </c>
@@ -20705,7 +23034,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+    <row r="12" spans="1:2" ht="15" thickBot="1">
       <c r="A12" s="25" t="s">
         <v>305</v>
       </c>
@@ -20713,7 +23042,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1">
+    <row r="13" spans="1:2" ht="15" thickBot="1">
       <c r="A13" s="25" t="s">
         <v>307</v>
       </c>
@@ -20721,7 +23050,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1">
+    <row r="14" spans="1:2" ht="15" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>309</v>
       </c>
@@ -20729,7 +23058,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1">
+    <row r="15" spans="1:2" ht="15" thickBot="1">
       <c r="A15" s="25" t="s">
         <v>311</v>
       </c>
@@ -20737,7 +23066,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1">
+    <row r="16" spans="1:2" ht="15" thickBot="1">
       <c r="A16" s="25" t="s">
         <v>313</v>
       </c>
@@ -20745,7 +23074,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1">
+    <row r="17" spans="1:2" ht="15" thickBot="1">
       <c r="A17" s="25" t="s">
         <v>315</v>
       </c>
@@ -20753,7 +23082,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1">
+    <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>317</v>
       </c>
@@ -20761,7 +23090,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1">
+    <row r="19" spans="1:2" ht="15" thickBot="1">
       <c r="A19" s="25" t="s">
         <v>319</v>
       </c>
@@ -20769,7 +23098,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1">
+    <row r="20" spans="1:2" ht="15" thickBot="1">
       <c r="A20" s="25" t="s">
         <v>321</v>
       </c>
@@ -20777,7 +23106,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1">
+    <row r="21" spans="1:2" ht="15" thickBot="1">
       <c r="A21" s="25" t="s">
         <v>323</v>
       </c>
@@ -20785,7 +23114,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1">
+    <row r="22" spans="1:2" ht="15" thickBot="1">
       <c r="A22" s="25" t="s">
         <v>325</v>
       </c>
@@ -20793,7 +23122,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1">
+    <row r="23" spans="1:2" ht="15" thickBot="1">
       <c r="A23" s="25" t="s">
         <v>327</v>
       </c>
@@ -20801,7 +23130,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1">
+    <row r="24" spans="1:2" ht="15" thickBot="1">
       <c r="A24" s="25" t="s">
         <v>329</v>
       </c>
@@ -20809,7 +23138,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1">
+    <row r="25" spans="1:2" ht="15" thickBot="1">
       <c r="A25" s="25" t="s">
         <v>331</v>
       </c>
@@ -20817,7 +23146,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1">
+    <row r="26" spans="1:2" ht="15" thickBot="1">
       <c r="A26" s="25" t="s">
         <v>333</v>
       </c>
@@ -20825,7 +23154,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1">
+    <row r="27" spans="1:2" ht="15" thickBot="1">
       <c r="A27" s="25" t="s">
         <v>335</v>
       </c>
@@ -20833,7 +23162,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1">
+    <row r="28" spans="1:2" ht="15" thickBot="1">
       <c r="A28" s="25" t="s">
         <v>337</v>
       </c>
@@ -20841,7 +23170,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1">
+    <row r="29" spans="1:2" ht="15" thickBot="1">
       <c r="A29" s="25" t="s">
         <v>339</v>
       </c>
@@ -20849,7 +23178,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1">
+    <row r="30" spans="1:2" ht="15" thickBot="1">
       <c r="A30" s="25" t="s">
         <v>341</v>
       </c>
@@ -20857,7 +23186,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1">
+    <row r="31" spans="1:2" ht="15" thickBot="1">
       <c r="A31" s="25" t="s">
         <v>343</v>
       </c>
@@ -20865,7 +23194,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1">
+    <row r="32" spans="1:2" ht="15" thickBot="1">
       <c r="A32" s="25" t="s">
         <v>345</v>
       </c>
@@ -20873,7 +23202,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1">
+    <row r="33" spans="1:2" ht="15" thickBot="1">
       <c r="A33" s="25" t="s">
         <v>347</v>
       </c>
@@ -20881,7 +23210,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1">
+    <row r="34" spans="1:2" ht="15" thickBot="1">
       <c r="A34" s="25" t="s">
         <v>349</v>
       </c>
@@ -20889,7 +23218,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1">
+    <row r="35" spans="1:2" ht="15" thickBot="1">
       <c r="A35" s="25" t="s">
         <v>351</v>
       </c>

</xml_diff>

<commit_message>
Updating data file -Sunanda
Updating data file -Sunanda
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1058\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsunand1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0A9ABB-5941-4EA4-973D-5B2E88BF50BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF3976F4-58F7-4DE6-8D46-054D3E34CE5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="2639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2853" uniqueCount="2648">
   <si>
     <t>City</t>
   </si>
@@ -9813,6 +9813,53 @@
   </si>
   <si>
     <t>BeginEnrollment page-Rahul</t>
+  </si>
+  <si>
+    <t>Amit-Jan-release</t>
+  </si>
+  <si>
+    <t>select * from ole.product_selection where prov_tin_nbr='{$tin}' and PRTL_PRDCT_REC_STS_CD='PS' and PRTL_PRDCT_SELECTED_GRP_NM='Premium'</t>
+  </si>
+  <si>
+    <t>select * from ole.DEBIT_FEE_ACCRD where PROV_TIN_NBR='{$tin}' and CONSL_PAY_NBR='{$conslpaynbr}'</t>
+  </si>
+  <si>
+    <t>Amit-Feb-release</t>
+  </si>
+  <si>
+    <t>Select p.prov_tax_id_nbr,cp.SETL_DT,cp.DSPL_CONSL_PAY_NBR from {$schema}.CONSOLIDATED_PAYMENT cp,
+{$schema}.PROVIDER p,ole.product_selection ps,ole.enrolled_provider ep,ole.PRODUCT_CONFIGURATION pc ,OLE.PROC_CTL PC
+where cp.prov_key_id = p.prov_key_id
+and PC.PROC_CTL_ID = CP.PROC_CTL_ID
+and p.prov_tax_id_nbr=ps.PROV_TIN_NBR
+and ps.PROV_TIN_NBR=ep.PROV_TIN_NBR
+and pc.GROUP_NM=ps.PRTL_PRDCT_SELECTED_GRP_NM
+AND PC.EXTRACT_STS_CD = 'C'
+and ps.PRTL_PRDCT_SELECTED_STS_CD='A' 
+and ep.ENRL_STS_CD='A'
+and cp.setl_dt between current date-18 months and current date - 13 months
+group by p.prov_tax_id_nbr,cp.DSPL_CONSL_PAY_NBR,cp.SETL_DT
+having count(*) between 1 and 30
+order by count(*) desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>select ps.prov_tin_nbr as PROV_TAX_ID_NBR, ps.PRTL_PRDCT_REC_STS_CD, ps.PRTL_PRDCT_SELECTED_STS_CD from ole.product_selection ps
+join ole.enrolled_provider ep on  ps.prov_tin_nbr=ep.prov_tin_nbr
+where ep.enrl_sts_cd='A' and ep.pay_meth_typ_cd='{$tinType}'
+and (PRTL_PRDCT_REC_STS_CD='TR' and PRTL_PRDCT_SELECTED_STS_CD='{$trialStatus}')
+and ps.PROV_TIN_NBR in (select PROV_TIN_NBR from ole.PRODUCT_SELECTION where PRTL_PRDCT_REC_STS_CD='{$SelectedOrDefault}' and PRTL_PRDCT_SELECTED_STS_CD='{$statusOfStandardRecd}' and PRTL_PRDCT_SELECTED_GRP_NM='{$portalAccess}')
+and ps.PROV_TIN_NBR in (select PROV_TIN_NBR from ole.PORTAL_USER_TIN where portal_user_id in (select portal_user_id from ole.PORTAL_USER where SSO_ID = '{$id}'))
+fetch first row only</t>
+  </si>
+  <si>
+    <t>SELECT PRTL_PRDCT_SELECT_DTTM, PRTL_PRDCT_SELECT_USER_FULLNAME FROM ole.PRODUCT_SELECTION  WHERE PRTL_PRDCT_SELECTED_STS_CD='{$statusOfStandardRecd}' AND PRTL_PRDCT_REC_STS_CD='{$SelectedOrDefault}' AND PROV_TIN_NBR='{$tin}'</t>
+  </si>
+  <si>
+    <t>Added by sunanda 27/1</t>
+  </si>
+  <si>
+    <t>US2955579, US3069345 and US2955579 During or post Trial for Standard TIN- Sunanda 27/1</t>
   </si>
 </sst>
 </file>
@@ -10557,20 +10604,20 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="17.08984375" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.90625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.90625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.08984375" customWidth="1"/>
-    <col min="8" max="8" width="26.90625" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="26.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="18.36328125" customWidth="1"/>
-    <col min="12" max="12" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.08984375" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -11106,15 +11153,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1912"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1613" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1617" sqref="C1617"/>
+    <sheetView tabSelected="1" topLeftCell="A1344" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1344" sqref="C1344"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="136.54296875" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="136.5546875" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -11150,7 +11197,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="58">
+    <row r="4" spans="1:3" ht="57.6">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -11158,7 +11205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29">
+    <row r="5" spans="1:3" ht="28.8">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -11193,7 +11240,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="29">
+    <row r="9" spans="1:3" ht="28.8">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -11201,7 +11248,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="87">
+    <row r="10" spans="1:3" ht="86.4">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -11209,7 +11256,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72.5">
+    <row r="11" spans="1:3" ht="72">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -11217,7 +11264,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.5">
+    <row r="12" spans="1:3" ht="43.2">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -11225,7 +11272,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="58">
+    <row r="13" spans="1:3" ht="57.6">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -11241,7 +11288,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="58">
+    <row r="15" spans="1:3" ht="57.6">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -11249,7 +11296,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29">
+    <row r="16" spans="1:3" ht="28.8">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -11257,7 +11304,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -11265,7 +11312,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29">
+    <row r="18" spans="1:3" ht="28.8">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -11273,7 +11320,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="87">
+    <row r="19" spans="1:3" ht="86.4">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -11281,7 +11328,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="72.5">
+    <row r="20" spans="1:3" ht="72">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -11289,7 +11336,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29">
+    <row r="21" spans="1:3" ht="28.8">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
@@ -11297,7 +11344,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5">
+    <row r="22" spans="1:3" ht="72">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -11305,7 +11352,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29">
+    <row r="23" spans="1:3" ht="28.8">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -11313,7 +11360,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.5">
+    <row r="24" spans="1:3" ht="43.2">
       <c r="A24" s="5" t="s">
         <v>88</v>
       </c>
@@ -11324,7 +11371,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72.5">
+    <row r="25" spans="1:3" ht="72">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -11340,7 +11387,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="130.5">
+    <row r="27" spans="1:3" ht="129.6">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -11348,7 +11395,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="87">
+    <row r="28" spans="1:3" ht="86.4">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
@@ -11356,7 +11403,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="29">
+    <row r="29" spans="1:3" ht="28.8">
       <c r="A29" s="5" t="s">
         <v>94</v>
       </c>
@@ -11364,7 +11411,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="145">
+    <row r="30" spans="1:3" ht="144">
       <c r="A30" s="5" t="s">
         <v>95</v>
       </c>
@@ -11375,7 +11422,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="159.5">
+    <row r="31" spans="1:3" ht="158.4">
       <c r="A31" s="5" t="s">
         <v>98</v>
       </c>
@@ -11386,7 +11433,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="159.5">
+    <row r="32" spans="1:3" ht="158.4">
       <c r="A32" s="5" t="s">
         <v>101</v>
       </c>
@@ -11397,7 +11444,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="188.5">
+    <row r="33" spans="1:4" ht="187.2">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -11408,7 +11455,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="116">
+    <row r="34" spans="1:4" ht="115.2">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -11416,7 +11463,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.5">
+    <row r="35" spans="1:4" ht="43.2">
       <c r="A35" s="5" t="s">
         <v>108</v>
       </c>
@@ -11424,7 +11471,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="116">
+    <row r="36" spans="1:4" ht="115.2">
       <c r="A36" s="5" t="s">
         <v>113</v>
       </c>
@@ -11435,7 +11482,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="101.5">
+    <row r="37" spans="1:4" ht="100.8">
       <c r="A37" s="5" t="s">
         <v>112</v>
       </c>
@@ -11446,7 +11493,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="116">
+    <row r="38" spans="1:4" ht="115.2">
       <c r="A38" s="5" t="s">
         <v>114</v>
       </c>
@@ -11454,7 +11501,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="101.5">
+    <row r="39" spans="1:4" ht="100.8">
       <c r="A39" s="5" t="s">
         <v>117</v>
       </c>
@@ -11462,7 +11509,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="116">
+    <row r="40" spans="1:4" ht="115.2">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -11470,7 +11517,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="116">
+    <row r="41" spans="1:4" ht="115.2">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -11478,7 +11525,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="116">
+    <row r="42" spans="1:4" ht="115.2">
       <c r="A42" s="5" t="s">
         <v>122</v>
       </c>
@@ -11492,7 +11539,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="174">
+    <row r="43" spans="1:4" ht="172.8">
       <c r="A43" s="5" t="s">
         <v>124</v>
       </c>
@@ -11503,7 +11550,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="174">
+    <row r="44" spans="1:4" ht="172.8">
       <c r="A44" s="5" t="s">
         <v>125</v>
       </c>
@@ -11514,7 +11561,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="101.5">
+    <row r="45" spans="1:4" ht="100.8">
       <c r="A45" s="5" t="s">
         <v>126</v>
       </c>
@@ -11525,7 +11572,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="159.5">
+    <row r="46" spans="1:4" ht="158.4">
       <c r="A46" s="5" t="s">
         <v>127</v>
       </c>
@@ -11536,7 +11583,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="174">
+    <row r="47" spans="1:4" ht="172.8">
       <c r="A47" s="5" t="s">
         <v>128</v>
       </c>
@@ -11547,7 +11594,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="174">
+    <row r="48" spans="1:4" ht="172.8">
       <c r="A48" s="5" t="s">
         <v>129</v>
       </c>
@@ -11558,7 +11605,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="101.5">
+    <row r="49" spans="1:3" ht="100.8">
       <c r="A49" s="5" t="s">
         <v>130</v>
       </c>
@@ -11569,7 +11616,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="130.5">
+    <row r="50" spans="1:3" ht="129.6">
       <c r="A50" s="5" t="s">
         <v>131</v>
       </c>
@@ -11580,7 +11627,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="101.5">
+    <row r="51" spans="1:3" ht="100.8">
       <c r="A51" s="5" t="s">
         <v>132</v>
       </c>
@@ -11591,7 +11638,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="130.5">
+    <row r="52" spans="1:3" ht="129.6">
       <c r="A52" s="5" t="s">
         <v>133</v>
       </c>
@@ -11602,7 +11649,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="116">
+    <row r="53" spans="1:3" ht="115.2">
       <c r="A53" s="5" t="s">
         <v>134</v>
       </c>
@@ -11613,7 +11660,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="101.5">
+    <row r="54" spans="1:3" ht="100.8">
       <c r="A54" s="5" t="s">
         <v>135</v>
       </c>
@@ -11621,7 +11668,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="116">
+    <row r="55" spans="1:3" ht="115.2">
       <c r="A55" s="5" t="s">
         <v>137</v>
       </c>
@@ -11632,7 +11679,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="116">
+    <row r="56" spans="1:3" ht="115.2">
       <c r="A56" s="5" t="s">
         <v>138</v>
       </c>
@@ -11640,7 +11687,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="159.5">
+    <row r="57" spans="1:3" ht="158.4">
       <c r="A57" s="5" t="s">
         <v>144</v>
       </c>
@@ -11651,7 +11698,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="159.5">
+    <row r="58" spans="1:3" ht="158.4">
       <c r="A58" s="5" t="s">
         <v>145</v>
       </c>
@@ -11659,7 +11706,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="145">
+    <row r="59" spans="1:3" ht="144">
       <c r="A59" s="5" t="s">
         <v>149</v>
       </c>
@@ -11670,7 +11717,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="159.5">
+    <row r="60" spans="1:3" ht="158.4">
       <c r="A60" s="5" t="s">
         <v>151</v>
       </c>
@@ -11681,7 +11728,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="174">
+    <row r="61" spans="1:3" ht="172.8">
       <c r="A61" s="5" t="s">
         <v>152</v>
       </c>
@@ -11692,7 +11739,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="116">
+    <row r="62" spans="1:3" ht="115.2">
       <c r="A62" s="5" t="s">
         <v>153</v>
       </c>
@@ -11703,7 +11750,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.5">
+    <row r="63" spans="1:3" ht="43.2">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -11711,7 +11758,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="130.5">
+    <row r="64" spans="1:3" ht="129.6">
       <c r="A64" s="5" t="s">
         <v>173</v>
       </c>
@@ -11722,7 +11769,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="130.5">
+    <row r="65" spans="1:3" ht="129.6">
       <c r="A65" s="5" t="s">
         <v>174</v>
       </c>
@@ -11749,7 +11796,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.5">
+    <row r="68" spans="1:3" ht="409.6">
       <c r="A68" s="5" t="s">
         <v>181</v>
       </c>
@@ -11757,7 +11804,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.5">
+    <row r="69" spans="1:3" ht="409.6">
       <c r="A69" s="5" t="s">
         <v>182</v>
       </c>
@@ -11765,7 +11812,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="145">
+    <row r="70" spans="1:3" ht="144">
       <c r="A70" s="5" t="s">
         <v>190</v>
       </c>
@@ -11776,7 +11823,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="232">
+    <row r="71" spans="1:3" ht="230.4">
       <c r="A71" s="5" t="s">
         <v>193</v>
       </c>
@@ -11803,7 +11850,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="29">
+    <row r="74" spans="1:3" ht="28.8">
       <c r="A74" s="5" t="s">
         <v>276</v>
       </c>
@@ -11811,7 +11858,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="29">
+    <row r="75" spans="1:3" ht="28.8">
       <c r="A75" s="5" t="s">
         <v>279</v>
       </c>
@@ -11819,7 +11866,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="29">
+    <row r="76" spans="1:3" ht="28.8">
       <c r="A76" s="5" t="s">
         <v>281</v>
       </c>
@@ -11859,7 +11906,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="29">
+    <row r="81" spans="1:2" ht="28.8">
       <c r="A81" s="5" t="s">
         <v>358</v>
       </c>
@@ -11883,7 +11930,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="29">
+    <row r="84" spans="1:2" ht="28.8">
       <c r="A84" s="5" t="s">
         <v>363</v>
       </c>
@@ -11899,7 +11946,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="29">
+    <row r="86" spans="1:2" ht="28.8">
       <c r="A86" s="5" t="s">
         <v>365</v>
       </c>
@@ -11915,7 +11962,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="29">
+    <row r="88" spans="1:2" ht="28.8">
       <c r="A88" s="5" t="s">
         <v>368</v>
       </c>
@@ -11931,7 +11978,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="29">
+    <row r="90" spans="1:2" ht="28.8">
       <c r="A90" s="5" t="s">
         <v>381</v>
       </c>
@@ -11979,7 +12026,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="29">
+    <row r="96" spans="1:2" ht="28.8">
       <c r="A96" s="5" t="s">
         <v>393</v>
       </c>
@@ -11995,7 +12042,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="29">
+    <row r="98" spans="1:3" ht="28.8">
       <c r="A98" s="5" t="s">
         <v>397</v>
       </c>
@@ -12035,7 +12082,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="188.5">
+    <row r="103" spans="1:3" ht="187.2">
       <c r="A103" s="5" t="s">
         <v>406</v>
       </c>
@@ -12046,7 +12093,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="275.5">
+    <row r="104" spans="1:3" ht="273.60000000000002">
       <c r="A104" s="5" t="s">
         <v>407</v>
       </c>
@@ -12057,7 +12104,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="232">
+    <row r="105" spans="1:3" ht="230.4">
       <c r="A105" s="5" t="s">
         <v>409</v>
       </c>
@@ -12076,7 +12123,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.5">
+    <row r="107" spans="1:3" ht="43.2">
       <c r="A107" s="5" t="s">
         <v>414</v>
       </c>
@@ -12092,7 +12139,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="116">
+    <row r="109" spans="1:3" ht="115.2">
       <c r="A109" s="5" t="s">
         <v>421</v>
       </c>
@@ -12275,7 +12322,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="116">
+    <row r="127" spans="1:3" ht="115.2">
       <c r="A127" s="5" t="s">
         <v>462</v>
       </c>
@@ -12286,7 +12333,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="116">
+    <row r="128" spans="1:3" ht="115.2">
       <c r="A128" s="5" t="s">
         <v>463</v>
       </c>
@@ -12305,7 +12352,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="174">
+    <row r="130" spans="1:3" ht="172.8">
       <c r="A130" s="5" t="s">
         <v>466</v>
       </c>
@@ -12316,7 +12363,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="145">
+    <row r="131" spans="1:3" ht="144">
       <c r="A131" s="5" t="s">
         <v>470</v>
       </c>
@@ -12327,7 +12374,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="145">
+    <row r="132" spans="1:3" ht="144">
       <c r="A132" s="5" t="s">
         <v>471</v>
       </c>
@@ -12338,7 +12385,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="130.5">
+    <row r="133" spans="1:3" ht="129.6">
       <c r="A133" s="5" t="s">
         <v>474</v>
       </c>
@@ -12349,7 +12396,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="130.5">
+    <row r="134" spans="1:3" ht="129.6">
       <c r="A134" s="5" t="s">
         <v>476</v>
       </c>
@@ -12360,7 +12407,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="130.5">
+    <row r="135" spans="1:3" ht="129.6">
       <c r="A135" s="5" t="s">
         <v>477</v>
       </c>
@@ -12371,7 +12418,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="130.5">
+    <row r="136" spans="1:3" ht="129.6">
       <c r="A136" s="5" t="s">
         <v>480</v>
       </c>
@@ -12382,7 +12429,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="130.5">
+    <row r="137" spans="1:3" ht="129.6">
       <c r="A137" s="5" t="s">
         <v>482</v>
       </c>
@@ -12393,7 +12440,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="130.5">
+    <row r="138" spans="1:3" ht="129.6">
       <c r="A138" s="5" t="s">
         <v>484</v>
       </c>
@@ -12404,7 +12451,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="130.5">
+    <row r="139" spans="1:3" ht="129.6">
       <c r="A139" s="5" t="s">
         <v>485</v>
       </c>
@@ -12415,7 +12462,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="130.5">
+    <row r="140" spans="1:3" ht="129.6">
       <c r="A140" s="5" t="s">
         <v>488</v>
       </c>
@@ -12426,7 +12473,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="130.5">
+    <row r="141" spans="1:3" ht="129.6">
       <c r="A141" s="5" t="s">
         <v>490</v>
       </c>
@@ -12437,7 +12484,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="130.5">
+    <row r="142" spans="1:3" ht="129.6">
       <c r="A142" s="5" t="s">
         <v>491</v>
       </c>
@@ -12448,7 +12495,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="116">
+    <row r="143" spans="1:3" ht="115.2">
       <c r="A143" s="5" t="s">
         <v>497</v>
       </c>
@@ -12459,7 +12506,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="130.5">
+    <row r="144" spans="1:3" ht="129.6">
       <c r="A144" s="5" t="s">
         <v>500</v>
       </c>
@@ -12470,7 +12517,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="130.5">
+    <row r="145" spans="1:3" ht="129.6">
       <c r="A145" s="5" t="s">
         <v>501</v>
       </c>
@@ -12481,7 +12528,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="130.5">
+    <row r="146" spans="1:3" ht="129.6">
       <c r="A146" s="5" t="s">
         <v>503</v>
       </c>
@@ -12492,7 +12539,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="130.5">
+    <row r="147" spans="1:3" ht="129.6">
       <c r="A147" s="5" t="s">
         <v>506</v>
       </c>
@@ -12503,7 +12550,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="130.5">
+    <row r="148" spans="1:3" ht="129.6">
       <c r="A148" s="5" t="s">
         <v>507</v>
       </c>
@@ -12558,7 +12605,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="29">
+    <row r="153" spans="1:3" ht="28.8">
       <c r="A153" s="5" t="s">
         <v>531</v>
       </c>
@@ -12580,7 +12627,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="87">
+    <row r="155" spans="1:3" ht="86.4">
       <c r="A155" s="5" t="s">
         <v>534</v>
       </c>
@@ -12591,7 +12638,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.5">
+    <row r="156" spans="1:3" ht="43.2">
       <c r="A156" s="5" t="s">
         <v>536</v>
       </c>
@@ -12602,7 +12649,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="174">
+    <row r="157" spans="1:3" ht="172.8">
       <c r="A157" s="5" t="s">
         <v>540</v>
       </c>
@@ -12613,7 +12660,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="159.5">
+    <row r="158" spans="1:3" ht="158.4">
       <c r="A158" s="5" t="s">
         <v>541</v>
       </c>
@@ -12632,7 +12679,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="72.5">
+    <row r="160" spans="1:3" ht="72">
       <c r="A160" s="5" t="s">
         <v>547</v>
       </c>
@@ -12643,7 +12690,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="58">
+    <row r="161" spans="1:3" ht="57.6">
       <c r="A161" s="5" t="s">
         <v>551</v>
       </c>
@@ -12651,7 +12698,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.5">
+    <row r="162" spans="1:3" ht="43.2">
       <c r="A162" s="5" t="s">
         <v>552</v>
       </c>
@@ -12670,7 +12717,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="101.5">
+    <row r="164" spans="1:3" ht="100.8">
       <c r="A164" s="5" t="s">
         <v>560</v>
       </c>
@@ -12678,7 +12725,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="101.5">
+    <row r="165" spans="1:3" ht="100.8">
       <c r="A165" s="5" t="s">
         <v>561</v>
       </c>
@@ -12831,7 +12878,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="29">
+    <row r="180" spans="1:3" ht="28.8">
       <c r="A180" s="5" t="s">
         <v>578</v>
       </c>
@@ -12864,7 +12911,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="116">
+    <row r="183" spans="1:3" ht="115.2">
       <c r="A183" s="5" t="s">
         <v>581</v>
       </c>
@@ -12919,7 +12966,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="72.5">
+    <row r="188" spans="1:3" ht="72">
       <c r="A188" s="5" t="s">
         <v>586</v>
       </c>
@@ -12930,7 +12977,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="101.5">
+    <row r="189" spans="1:3" ht="100.8">
       <c r="A189" s="5" t="s">
         <v>587</v>
       </c>
@@ -12941,7 +12988,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="72.5">
+    <row r="190" spans="1:3" ht="72">
       <c r="A190" s="5" t="s">
         <v>667</v>
       </c>
@@ -12952,7 +12999,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="87">
+    <row r="191" spans="1:3" ht="86.4">
       <c r="A191" s="5" t="s">
         <v>668</v>
       </c>
@@ -12963,7 +13010,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="87">
+    <row r="192" spans="1:3" ht="86.4">
       <c r="A192" s="5" t="s">
         <v>669</v>
       </c>
@@ -13018,7 +13065,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="29">
+    <row r="197" spans="1:3" ht="28.8">
       <c r="A197" s="5" t="s">
         <v>674</v>
       </c>
@@ -13029,7 +13076,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="29">
+    <row r="198" spans="1:3" ht="28.8">
       <c r="A198" s="5" t="s">
         <v>675</v>
       </c>
@@ -13051,7 +13098,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="29">
+    <row r="200" spans="1:3" ht="28.8">
       <c r="A200" s="5" t="s">
         <v>677</v>
       </c>
@@ -13062,7 +13109,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="87">
+    <row r="201" spans="1:3" ht="86.4">
       <c r="A201" s="5" t="s">
         <v>678</v>
       </c>
@@ -13073,7 +13120,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72.5">
+    <row r="202" spans="1:3" ht="72">
       <c r="A202" s="5" t="s">
         <v>679</v>
       </c>
@@ -13084,7 +13131,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="87">
+    <row r="203" spans="1:3" ht="86.4">
       <c r="A203" s="5" t="s">
         <v>680</v>
       </c>
@@ -13095,7 +13142,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29">
+    <row r="204" spans="1:3" ht="28.8">
       <c r="A204" s="5" t="s">
         <v>681</v>
       </c>
@@ -13103,7 +13150,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="409.5">
+    <row r="205" spans="1:3" ht="409.6">
       <c r="A205" s="5" t="s">
         <v>682</v>
       </c>
@@ -13114,7 +13161,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="217.5">
+    <row r="206" spans="1:3" ht="216">
       <c r="A206" s="5" t="s">
         <v>683</v>
       </c>
@@ -13136,7 +13183,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="43.5">
+    <row r="208" spans="1:3" ht="43.2">
       <c r="A208" s="5" t="s">
         <v>685</v>
       </c>
@@ -13147,7 +13194,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="101.5">
+    <row r="209" spans="1:3" ht="100.8">
       <c r="A209" s="5" t="s">
         <v>686</v>
       </c>
@@ -13169,7 +13216,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="409.5">
+    <row r="211" spans="1:3" ht="409.6">
       <c r="A211" s="5" t="s">
         <v>688</v>
       </c>
@@ -13191,7 +13238,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="29">
+    <row r="213" spans="1:3" ht="28.8">
       <c r="A213" s="5" t="s">
         <v>690</v>
       </c>
@@ -13202,7 +13249,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72.5">
+    <row r="214" spans="1:3" ht="72">
       <c r="A214" s="5" t="s">
         <v>691</v>
       </c>
@@ -13213,7 +13260,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="87">
+    <row r="215" spans="1:3" ht="86.4">
       <c r="A215" s="5" t="s">
         <v>692</v>
       </c>
@@ -13224,7 +13271,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72.5">
+    <row r="216" spans="1:3" ht="72">
       <c r="A216" s="5" t="s">
         <v>693</v>
       </c>
@@ -13235,7 +13282,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="87">
+    <row r="217" spans="1:3" ht="86.4">
       <c r="A217" s="5" t="s">
         <v>694</v>
       </c>
@@ -13246,7 +13293,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="217.5">
+    <row r="218" spans="1:3" ht="216">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -13257,7 +13304,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="409.5">
+    <row r="219" spans="1:3" ht="409.6">
       <c r="A219" s="5" t="s">
         <v>695</v>
       </c>
@@ -13268,7 +13315,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="203">
+    <row r="220" spans="1:3" ht="216">
       <c r="A220" s="5" t="s">
         <v>696</v>
       </c>
@@ -13279,7 +13326,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="159.5">
+    <row r="221" spans="1:3" ht="158.4">
       <c r="A221" s="5" t="s">
         <v>697</v>
       </c>
@@ -13295,7 +13342,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="101.5">
+    <row r="223" spans="1:3" ht="100.8">
       <c r="A223" s="5" t="s">
         <v>699</v>
       </c>
@@ -13306,7 +13353,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="101.5">
+    <row r="224" spans="1:3" ht="100.8">
       <c r="A224" s="5" t="s">
         <v>700</v>
       </c>
@@ -13317,7 +13364,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="101.5">
+    <row r="225" spans="1:3" ht="100.8">
       <c r="A225" s="5" t="s">
         <v>701</v>
       </c>
@@ -13392,7 +13439,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="87">
+    <row r="234" spans="1:3" ht="86.4">
       <c r="A234" s="5" t="s">
         <v>710</v>
       </c>
@@ -13411,7 +13458,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="87">
+    <row r="236" spans="1:3" ht="86.4">
       <c r="A236" s="5" t="s">
         <v>712</v>
       </c>
@@ -13444,7 +13491,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="130.5">
+    <row r="239" spans="1:3" ht="129.6">
       <c r="A239" s="5" t="s">
         <v>715</v>
       </c>
@@ -13455,7 +13502,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="29">
+    <row r="240" spans="1:3" ht="28.8">
       <c r="A240" s="5" t="s">
         <v>716</v>
       </c>
@@ -13477,7 +13524,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="101.5">
+    <row r="242" spans="1:3" ht="100.8">
       <c r="A242" s="5" t="s">
         <v>785</v>
       </c>
@@ -13488,7 +13535,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="43.5">
+    <row r="243" spans="1:3" ht="43.2">
       <c r="A243" s="5" t="s">
         <v>786</v>
       </c>
@@ -13499,7 +13546,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="174">
+    <row r="244" spans="1:3" ht="172.8">
       <c r="A244" s="5" t="s">
         <v>787</v>
       </c>
@@ -13510,7 +13557,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="217.5">
+    <row r="245" spans="1:3" ht="216">
       <c r="A245" s="5" t="s">
         <v>789</v>
       </c>
@@ -13521,7 +13568,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="174">
+    <row r="246" spans="1:3" ht="172.8">
       <c r="A246" s="5" t="s">
         <v>794</v>
       </c>
@@ -13532,7 +13579,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="188.5">
+    <row r="247" spans="1:3" ht="187.2">
       <c r="A247" s="5" t="s">
         <v>799</v>
       </c>
@@ -13543,7 +13590,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="188.5">
+    <row r="248" spans="1:3" ht="187.2">
       <c r="A248" s="5" t="s">
         <v>802</v>
       </c>
@@ -13554,7 +13601,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="217.5">
+    <row r="249" spans="1:3" ht="216">
       <c r="A249" s="5" t="s">
         <v>805</v>
       </c>
@@ -13565,7 +13612,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="116">
+    <row r="250" spans="1:3" ht="115.2">
       <c r="A250" s="5" t="s">
         <v>825</v>
       </c>
@@ -13576,7 +13623,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="145">
+    <row r="251" spans="1:3" ht="144">
       <c r="A251" s="5" t="s">
         <v>828</v>
       </c>
@@ -13587,7 +13634,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="116">
+    <row r="252" spans="1:3" ht="115.2">
       <c r="A252" s="5" t="s">
         <v>831</v>
       </c>
@@ -13609,7 +13656,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="29">
+    <row r="254" spans="1:3" ht="28.8">
       <c r="A254" s="5" t="s">
         <v>839</v>
       </c>
@@ -13620,7 +13667,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="72.5">
+    <row r="255" spans="1:3" ht="72">
       <c r="A255" s="5" t="s">
         <v>840</v>
       </c>
@@ -13631,7 +13678,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="29">
+    <row r="256" spans="1:3" ht="28.8">
       <c r="A256" s="5" t="s">
         <v>841</v>
       </c>
@@ -13642,7 +13689,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="72.5">
+    <row r="257" spans="1:3" ht="72">
       <c r="A257" s="5" t="s">
         <v>842</v>
       </c>
@@ -13653,7 +13700,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="145">
+    <row r="258" spans="1:3" ht="144">
       <c r="A258" s="5" t="s">
         <v>848</v>
       </c>
@@ -13675,7 +13722,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="43.5">
+    <row r="260" spans="1:3" ht="43.2">
       <c r="A260" s="5" t="s">
         <v>852</v>
       </c>
@@ -13686,7 +13733,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="58">
+    <row r="261" spans="1:3" ht="57.6">
       <c r="A261" s="5" t="s">
         <v>855</v>
       </c>
@@ -13697,7 +13744,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="87">
+    <row r="262" spans="1:3" ht="86.4">
       <c r="A262" s="5" t="s">
         <v>858</v>
       </c>
@@ -13716,7 +13763,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="58">
+    <row r="264" spans="1:3" ht="57.6">
       <c r="A264" s="5" t="s">
         <v>863</v>
       </c>
@@ -13727,7 +13774,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="87">
+    <row r="265" spans="1:3" ht="86.4">
       <c r="A265" s="5" t="s">
         <v>866</v>
       </c>
@@ -13738,7 +13785,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="72.5">
+    <row r="266" spans="1:3" ht="72">
       <c r="A266" s="5" t="s">
         <v>869</v>
       </c>
@@ -13773,7 +13820,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="29">
+    <row r="270" spans="1:3" ht="28.8">
       <c r="A270" s="5" t="s">
         <v>883</v>
       </c>
@@ -13781,7 +13828,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="101.5">
+    <row r="271" spans="1:3" ht="100.8">
       <c r="A271" s="5" t="s">
         <v>884</v>
       </c>
@@ -13792,7 +13839,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="43.5">
+    <row r="272" spans="1:3" ht="43.2">
       <c r="A272" s="5" t="s">
         <v>885</v>
       </c>
@@ -13803,7 +13850,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="29">
+    <row r="273" spans="1:4" ht="28.8">
       <c r="A273" s="5" t="s">
         <v>886</v>
       </c>
@@ -13814,7 +13861,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="72.5">
+    <row r="274" spans="1:4" ht="72">
       <c r="A274" s="5" t="s">
         <v>890</v>
       </c>
@@ -14462,7 +14509,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="401" spans="1:3" ht="29">
+    <row r="401" spans="1:3" ht="28.8">
       <c r="A401" s="2" t="s">
         <v>1018</v>
       </c>
@@ -14473,7 +14520,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="402" spans="1:3" ht="72.5">
+    <row r="402" spans="1:3" ht="72">
       <c r="A402" s="2" t="s">
         <v>1019</v>
       </c>
@@ -14484,7 +14531,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="58">
+    <row r="403" spans="1:3" ht="43.2">
       <c r="A403" s="2" t="s">
         <v>1020</v>
       </c>
@@ -14495,7 +14542,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="29">
+    <row r="404" spans="1:3" ht="28.8">
       <c r="A404" s="2" t="s">
         <v>1021</v>
       </c>
@@ -14506,7 +14553,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="29">
+    <row r="405" spans="1:3" ht="28.8">
       <c r="A405" s="2" t="s">
         <v>1022</v>
       </c>
@@ -14517,7 +14564,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="43.5">
+    <row r="406" spans="1:3" ht="43.2">
       <c r="A406" s="2" t="s">
         <v>1023</v>
       </c>
@@ -14528,7 +14575,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="407" spans="1:3" ht="29">
+    <row r="407" spans="1:3" ht="28.8">
       <c r="A407" s="2" t="s">
         <v>1024</v>
       </c>
@@ -14539,7 +14586,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="130.5">
+    <row r="408" spans="1:3" ht="129.6">
       <c r="A408" s="2" t="s">
         <v>1025</v>
       </c>
@@ -14550,7 +14597,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="409" spans="1:3" ht="43.5">
+    <row r="409" spans="1:3" ht="43.2">
       <c r="A409" s="2" t="s">
         <v>1026</v>
       </c>
@@ -14561,7 +14608,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="410" spans="1:3" ht="29">
+    <row r="410" spans="1:3" ht="28.8">
       <c r="A410" s="2" t="s">
         <v>1027</v>
       </c>
@@ -14572,7 +14619,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="29">
+    <row r="411" spans="1:3" ht="28.8">
       <c r="A411" s="2" t="s">
         <v>1028</v>
       </c>
@@ -14583,7 +14630,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="159.5">
+    <row r="412" spans="1:3" ht="158.4">
       <c r="A412" s="2" t="s">
         <v>1029</v>
       </c>
@@ -14594,7 +14641,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="174">
+    <row r="413" spans="1:3" ht="172.8">
       <c r="A413" s="2" t="s">
         <v>1030</v>
       </c>
@@ -14605,7 +14652,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="72.5">
+    <row r="414" spans="1:3" ht="72">
       <c r="A414" s="2" t="s">
         <v>1031</v>
       </c>
@@ -14627,7 +14674,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="72.5">
+    <row r="416" spans="1:3" ht="72">
       <c r="A416" s="2" t="s">
         <v>1033</v>
       </c>
@@ -14638,7 +14685,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="116">
+    <row r="417" spans="1:3" ht="115.2">
       <c r="A417" s="2" t="s">
         <v>1034</v>
       </c>
@@ -14649,7 +14696,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="130.5">
+    <row r="418" spans="1:3" ht="129.6">
       <c r="A418" s="2" t="s">
         <v>1035</v>
       </c>
@@ -14660,7 +14707,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="29">
+    <row r="419" spans="1:3" ht="28.8">
       <c r="A419" s="2" t="s">
         <v>1036</v>
       </c>
@@ -14770,7 +14817,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="72.5">
+    <row r="429" spans="1:3" ht="72">
       <c r="A429" s="2" t="s">
         <v>1046</v>
       </c>
@@ -19336,7 +19383,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="1341" spans="1:3" ht="130.5">
+    <row r="1341" spans="1:3" ht="129.6">
       <c r="A1341" s="51" t="s">
         <v>1958</v>
       </c>
@@ -19369,87 +19416,99 @@
         <v>2629</v>
       </c>
     </row>
-    <row r="1344" spans="1:3">
+    <row r="1344" spans="1:3" ht="129.6">
       <c r="A1344" s="5" t="s">
         <v>1961</v>
       </c>
-    </row>
-    <row r="1345" spans="1:1">
+      <c r="B1344" s="52" t="s">
+        <v>2644</v>
+      </c>
+      <c r="C1344" s="52" t="s">
+        <v>2647</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:3" ht="28.8">
       <c r="A1345" s="5" t="s">
         <v>1962</v>
       </c>
-    </row>
-    <row r="1346" spans="1:1">
+      <c r="B1345" s="52" t="s">
+        <v>2645</v>
+      </c>
+      <c r="C1345" s="52" t="s">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:3">
       <c r="A1346" s="5" t="s">
         <v>1963</v>
       </c>
     </row>
-    <row r="1347" spans="1:1">
+    <row r="1347" spans="1:3">
       <c r="A1347" s="5" t="s">
         <v>1964</v>
       </c>
     </row>
-    <row r="1348" spans="1:1">
+    <row r="1348" spans="1:3">
       <c r="A1348" s="5" t="s">
         <v>1965</v>
       </c>
     </row>
-    <row r="1349" spans="1:1">
+    <row r="1349" spans="1:3">
       <c r="A1349" s="5" t="s">
         <v>1966</v>
       </c>
     </row>
-    <row r="1350" spans="1:1">
+    <row r="1350" spans="1:3">
       <c r="A1350" s="5" t="s">
         <v>1967</v>
       </c>
     </row>
-    <row r="1351" spans="1:1">
+    <row r="1351" spans="1:3">
       <c r="A1351" s="5" t="s">
         <v>1968</v>
       </c>
     </row>
-    <row r="1352" spans="1:1">
+    <row r="1352" spans="1:3">
       <c r="A1352" s="5" t="s">
         <v>1969</v>
       </c>
     </row>
-    <row r="1353" spans="1:1">
+    <row r="1353" spans="1:3">
       <c r="A1353" s="5" t="s">
         <v>1970</v>
       </c>
     </row>
-    <row r="1354" spans="1:1">
+    <row r="1354" spans="1:3">
       <c r="A1354" s="5" t="s">
         <v>1971</v>
       </c>
     </row>
-    <row r="1355" spans="1:1">
+    <row r="1355" spans="1:3">
       <c r="A1355" s="5" t="s">
         <v>1972</v>
       </c>
     </row>
-    <row r="1356" spans="1:1">
+    <row r="1356" spans="1:3">
       <c r="A1356" s="5" t="s">
         <v>1973</v>
       </c>
     </row>
-    <row r="1357" spans="1:1">
+    <row r="1357" spans="1:3">
       <c r="A1357" s="5" t="s">
         <v>1974</v>
       </c>
     </row>
-    <row r="1358" spans="1:1">
+    <row r="1358" spans="1:3">
       <c r="A1358" s="5" t="s">
         <v>1975</v>
       </c>
     </row>
-    <row r="1359" spans="1:1">
+    <row r="1359" spans="1:3">
       <c r="A1359" s="5" t="s">
         <v>1976</v>
       </c>
     </row>
-    <row r="1360" spans="1:1">
+    <row r="1360" spans="1:3">
       <c r="A1360" s="5" t="s">
         <v>1977</v>
       </c>
@@ -20159,7 +20218,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="1502" spans="1:3" ht="87">
+    <row r="1502" spans="1:3" ht="86.4">
       <c r="A1502" s="5" t="s">
         <v>2119</v>
       </c>
@@ -20170,7 +20229,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="1503" spans="1:3" ht="87">
+    <row r="1503" spans="1:3" ht="86.4">
       <c r="A1503" s="5" t="s">
         <v>2120</v>
       </c>
@@ -20181,7 +20240,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="1504" spans="1:3" ht="145">
+    <row r="1504" spans="1:3" ht="144">
       <c r="A1504" s="5" t="s">
         <v>2121</v>
       </c>
@@ -20192,7 +20251,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="1505" spans="1:3" ht="145">
+    <row r="1505" spans="1:3" ht="144">
       <c r="A1505" s="5" t="s">
         <v>2122</v>
       </c>
@@ -20203,7 +20262,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1506" spans="1:3" ht="72.5">
+    <row r="1506" spans="1:3" ht="72">
       <c r="A1506" s="5" t="s">
         <v>2123</v>
       </c>
@@ -20211,7 +20270,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="1507" spans="1:3" ht="43.5">
+    <row r="1507" spans="1:3" ht="43.2">
       <c r="A1507" s="47" t="s">
         <v>2124</v>
       </c>
@@ -20222,7 +20281,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1508" spans="1:3" ht="43.5">
+    <row r="1508" spans="1:3" ht="43.2">
       <c r="A1508" s="44" t="s">
         <v>2125</v>
       </c>
@@ -20233,20 +20292,38 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1509" spans="1:3">
+    <row r="1509" spans="1:3" ht="216">
       <c r="A1509" s="5" t="s">
         <v>2126</v>
+      </c>
+      <c r="B1509" s="48" t="s">
+        <v>2643</v>
+      </c>
+      <c r="C1509" t="s">
+        <v>2639</v>
       </c>
     </row>
     <row r="1510" spans="1:3">
       <c r="A1510" s="5" t="s">
         <v>2127</v>
       </c>
+      <c r="B1510" t="s">
+        <v>2640</v>
+      </c>
+      <c r="C1510" t="s">
+        <v>2639</v>
+      </c>
     </row>
     <row r="1511" spans="1:3">
       <c r="A1511" s="5" t="s">
         <v>2128</v>
       </c>
+      <c r="B1511" t="s">
+        <v>2641</v>
+      </c>
+      <c r="C1511" t="s">
+        <v>2642</v>
+      </c>
     </row>
     <row r="1512" spans="1:3">
       <c r="A1512" s="5" t="s">
@@ -20698,7 +20775,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="1602" spans="1:3" ht="29">
+    <row r="1602" spans="1:3" ht="28.8">
       <c r="A1602" s="5" t="s">
         <v>2219</v>
       </c>
@@ -20720,7 +20797,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="1604" spans="1:3" ht="58">
+    <row r="1604" spans="1:3" ht="57.6">
       <c r="A1604" s="5" t="s">
         <v>2221</v>
       </c>
@@ -20731,7 +20808,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="1605" spans="1:3" ht="43.5">
+    <row r="1605" spans="1:3" ht="43.2">
       <c r="A1605" s="5" t="s">
         <v>2222</v>
       </c>
@@ -20739,7 +20816,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="1606" spans="1:3" ht="101.5">
+    <row r="1606" spans="1:3" ht="100.8">
       <c r="A1606" s="5" t="s">
         <v>2223</v>
       </c>
@@ -20769,7 +20846,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="1609" spans="1:3" ht="43.5">
+    <row r="1609" spans="1:3" ht="43.2">
       <c r="A1609" s="5" t="s">
         <v>2278</v>
       </c>
@@ -20780,7 +20857,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="1610" spans="1:3" ht="29">
+    <row r="1610" spans="1:3" ht="28.8">
       <c r="A1610" s="5" t="s">
         <v>2279</v>
       </c>
@@ -20788,7 +20865,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="1611" spans="1:3" ht="391.5">
+    <row r="1611" spans="1:3" ht="388.8">
       <c r="A1611" s="5" t="s">
         <v>2280</v>
       </c>
@@ -20799,7 +20876,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="1612" spans="1:3" ht="232">
+    <row r="1612" spans="1:3" ht="230.4">
       <c r="A1612" s="44" t="s">
         <v>2281</v>
       </c>
@@ -20843,7 +20920,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="1616" spans="1:3" ht="87">
+    <row r="1616" spans="1:3" ht="86.4">
       <c r="A1616" s="47" t="s">
         <v>2340</v>
       </c>
@@ -20854,7 +20931,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="1617" spans="1:3" ht="29">
+    <row r="1617" spans="1:3" ht="28.8">
       <c r="A1617" s="47" t="s">
         <v>2341</v>
       </c>
@@ -22286,7 +22363,7 @@
       </c>
       <c r="B1901" s="48"/>
     </row>
-    <row r="1902" spans="1:3" ht="43.5">
+    <row r="1902" spans="1:3" ht="43.2">
       <c r="A1902">
         <v>1901</v>
       </c>
@@ -22297,7 +22374,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="1903" spans="1:3" ht="87">
+    <row r="1903" spans="1:3" ht="86.4">
       <c r="A1903">
         <v>1902</v>
       </c>
@@ -22308,7 +22385,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="1904" spans="1:3" ht="217.5">
+    <row r="1904" spans="1:3" ht="216">
       <c r="A1904">
         <v>1903</v>
       </c>
@@ -22319,7 +22396,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="1905" spans="1:3" ht="145">
+    <row r="1905" spans="1:3" ht="144">
       <c r="A1905">
         <v>1904</v>
       </c>
@@ -22330,7 +22407,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="1906" spans="1:3" ht="145">
+    <row r="1906" spans="1:3" ht="144">
       <c r="A1906">
         <v>1905</v>
       </c>
@@ -22341,7 +22418,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="1907" spans="1:3" ht="116">
+    <row r="1907" spans="1:3" ht="115.2">
       <c r="A1907">
         <v>1906</v>
       </c>
@@ -22352,7 +22429,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="1908" spans="1:3" ht="145">
+    <row r="1908" spans="1:3" ht="144">
       <c r="A1908">
         <v>1907</v>
       </c>
@@ -22363,7 +22440,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="1909" spans="1:3" ht="145">
+    <row r="1909" spans="1:3" ht="144">
       <c r="A1909">
         <v>1908</v>
       </c>
@@ -22374,7 +22451,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="1910" spans="1:3" ht="101.5">
+    <row r="1910" spans="1:3" ht="100.8">
       <c r="A1910">
         <v>1909</v>
       </c>
@@ -22422,13 +22499,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="4" max="4" width="21.08984375" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -22608,10 +22685,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="68.08984375" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -22934,7 +23011,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16">
+    <row r="44" spans="1:2" ht="15">
       <c r="A44" s="13" t="s">
         <v>263</v>
       </c>
@@ -23024,10 +23101,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="85.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="85.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">

</xml_diff>

<commit_message>
update in sata file-Sayonee
update in sata file-Sayonee
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsunand1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdassani\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF3976F4-58F7-4DE6-8D46-054D3E34CE5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D68645-20B4-4E64-9622-F15128A1A353}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2853" uniqueCount="2648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="2650">
   <si>
     <t>City</t>
   </si>
@@ -9861,6 +9861,12 @@
   <si>
     <t>US2955579, US3069345 and US2955579 During or post Trial for Standard TIN- Sunanda 27/1</t>
   </si>
+  <si>
+    <t>Sayonee 28/01/21</t>
+  </si>
+  <si>
+    <t>select PAY_PROC_ACPT_CD_VAL_DESC from OLE.PAY_PROC_VAL where PAY_PROC_CD = '{$pay_proc_cd}'</t>
+  </si>
 </sst>
 </file>
 
@@ -9953,7 +9959,7 @@
       <name val="Frutiger"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9993,6 +9999,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10049,7 +10061,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -10146,6 +10158,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10604,20 +10618,20 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="26.88671875" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -11153,15 +11167,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1912"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1344" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1344" sqref="C1344"/>
+    <sheetView tabSelected="1" topLeftCell="A1082" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1112" sqref="B1112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="136.5546875" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="136.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -11197,7 +11211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.6">
+    <row r="4" spans="1:3" ht="60">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -11205,7 +11219,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -11240,7 +11254,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -11248,7 +11262,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="86.4">
+    <row r="10" spans="1:3" ht="90">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -11256,7 +11270,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72">
+    <row r="11" spans="1:3" ht="75">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -11264,7 +11278,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2">
+    <row r="12" spans="1:3" ht="45">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -11272,7 +11286,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57.6">
+    <row r="13" spans="1:3" ht="60">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -11288,7 +11302,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.6">
+    <row r="15" spans="1:3" ht="60">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -11296,7 +11310,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8">
+    <row r="16" spans="1:3" ht="30">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -11304,7 +11318,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="30">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -11312,7 +11326,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8">
+    <row r="18" spans="1:3" ht="30">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -11320,7 +11334,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="86.4">
+    <row r="19" spans="1:3" ht="90">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -11328,7 +11342,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="72">
+    <row r="20" spans="1:3" ht="75">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -11336,7 +11350,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8">
+    <row r="21" spans="1:3" ht="30">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
@@ -11344,7 +11358,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72">
+    <row r="22" spans="1:3" ht="75">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -11352,7 +11366,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.8">
+    <row r="23" spans="1:3" ht="30">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -11360,7 +11374,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.2">
+    <row r="24" spans="1:3" ht="45">
       <c r="A24" s="5" t="s">
         <v>88</v>
       </c>
@@ -11371,7 +11385,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72">
+    <row r="25" spans="1:3" ht="75">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -11387,7 +11401,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="129.6">
+    <row r="27" spans="1:3" ht="135">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -11395,7 +11409,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="86.4">
+    <row r="28" spans="1:3" ht="90">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
@@ -11403,7 +11417,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.8">
+    <row r="29" spans="1:3" ht="30">
       <c r="A29" s="5" t="s">
         <v>94</v>
       </c>
@@ -11411,7 +11425,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="144">
+    <row r="30" spans="1:3" ht="150">
       <c r="A30" s="5" t="s">
         <v>95</v>
       </c>
@@ -11422,7 +11436,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="158.4">
+    <row r="31" spans="1:3" ht="165">
       <c r="A31" s="5" t="s">
         <v>98</v>
       </c>
@@ -11433,7 +11447,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="158.4">
+    <row r="32" spans="1:3" ht="165">
       <c r="A32" s="5" t="s">
         <v>101</v>
       </c>
@@ -11444,7 +11458,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="187.2">
+    <row r="33" spans="1:4" ht="195">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -11455,7 +11469,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="115.2">
+    <row r="34" spans="1:4" ht="120">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -11463,7 +11477,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.2">
+    <row r="35" spans="1:4" ht="45">
       <c r="A35" s="5" t="s">
         <v>108</v>
       </c>
@@ -11471,7 +11485,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="115.2">
+    <row r="36" spans="1:4" ht="120">
       <c r="A36" s="5" t="s">
         <v>113</v>
       </c>
@@ -11482,7 +11496,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="100.8">
+    <row r="37" spans="1:4" ht="105">
       <c r="A37" s="5" t="s">
         <v>112</v>
       </c>
@@ -11493,7 +11507,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="115.2">
+    <row r="38" spans="1:4" ht="120">
       <c r="A38" s="5" t="s">
         <v>114</v>
       </c>
@@ -11501,7 +11515,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="100.8">
+    <row r="39" spans="1:4" ht="105">
       <c r="A39" s="5" t="s">
         <v>117</v>
       </c>
@@ -11509,7 +11523,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="115.2">
+    <row r="40" spans="1:4" ht="120">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -11517,7 +11531,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="115.2">
+    <row r="41" spans="1:4" ht="120">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -11525,7 +11539,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="115.2">
+    <row r="42" spans="1:4" ht="120">
       <c r="A42" s="5" t="s">
         <v>122</v>
       </c>
@@ -11539,7 +11553,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="172.8">
+    <row r="43" spans="1:4" ht="180">
       <c r="A43" s="5" t="s">
         <v>124</v>
       </c>
@@ -11550,7 +11564,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="172.8">
+    <row r="44" spans="1:4" ht="180">
       <c r="A44" s="5" t="s">
         <v>125</v>
       </c>
@@ -11561,7 +11575,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="100.8">
+    <row r="45" spans="1:4" ht="105">
       <c r="A45" s="5" t="s">
         <v>126</v>
       </c>
@@ -11572,7 +11586,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="158.4">
+    <row r="46" spans="1:4" ht="165">
       <c r="A46" s="5" t="s">
         <v>127</v>
       </c>
@@ -11583,7 +11597,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="172.8">
+    <row r="47" spans="1:4" ht="180">
       <c r="A47" s="5" t="s">
         <v>128</v>
       </c>
@@ -11594,7 +11608,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="172.8">
+    <row r="48" spans="1:4" ht="180">
       <c r="A48" s="5" t="s">
         <v>129</v>
       </c>
@@ -11605,7 +11619,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="100.8">
+    <row r="49" spans="1:3" ht="105">
       <c r="A49" s="5" t="s">
         <v>130</v>
       </c>
@@ -11616,7 +11630,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="129.6">
+    <row r="50" spans="1:3" ht="135">
       <c r="A50" s="5" t="s">
         <v>131</v>
       </c>
@@ -11627,7 +11641,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="100.8">
+    <row r="51" spans="1:3" ht="105">
       <c r="A51" s="5" t="s">
         <v>132</v>
       </c>
@@ -11638,7 +11652,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="129.6">
+    <row r="52" spans="1:3" ht="135">
       <c r="A52" s="5" t="s">
         <v>133</v>
       </c>
@@ -11649,7 +11663,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="115.2">
+    <row r="53" spans="1:3" ht="120">
       <c r="A53" s="5" t="s">
         <v>134</v>
       </c>
@@ -11660,7 +11674,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="100.8">
+    <row r="54" spans="1:3" ht="105">
       <c r="A54" s="5" t="s">
         <v>135</v>
       </c>
@@ -11668,7 +11682,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="115.2">
+    <row r="55" spans="1:3" ht="120">
       <c r="A55" s="5" t="s">
         <v>137</v>
       </c>
@@ -11679,7 +11693,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="115.2">
+    <row r="56" spans="1:3" ht="120">
       <c r="A56" s="5" t="s">
         <v>138</v>
       </c>
@@ -11687,7 +11701,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="158.4">
+    <row r="57" spans="1:3" ht="165">
       <c r="A57" s="5" t="s">
         <v>144</v>
       </c>
@@ -11698,7 +11712,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="158.4">
+    <row r="58" spans="1:3" ht="165">
       <c r="A58" s="5" t="s">
         <v>145</v>
       </c>
@@ -11706,7 +11720,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="144">
+    <row r="59" spans="1:3" ht="150">
       <c r="A59" s="5" t="s">
         <v>149</v>
       </c>
@@ -11717,7 +11731,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="158.4">
+    <row r="60" spans="1:3" ht="165">
       <c r="A60" s="5" t="s">
         <v>151</v>
       </c>
@@ -11728,7 +11742,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="172.8">
+    <row r="61" spans="1:3" ht="180">
       <c r="A61" s="5" t="s">
         <v>152</v>
       </c>
@@ -11739,7 +11753,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="115.2">
+    <row r="62" spans="1:3" ht="120">
       <c r="A62" s="5" t="s">
         <v>153</v>
       </c>
@@ -11750,7 +11764,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.2">
+    <row r="63" spans="1:3" ht="45">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -11758,7 +11772,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="129.6">
+    <row r="64" spans="1:3" ht="135">
       <c r="A64" s="5" t="s">
         <v>173</v>
       </c>
@@ -11769,7 +11783,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="129.6">
+    <row r="65" spans="1:3" ht="135">
       <c r="A65" s="5" t="s">
         <v>174</v>
       </c>
@@ -11796,7 +11810,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="409.6">
+    <row r="68" spans="1:3" ht="409.5">
       <c r="A68" s="5" t="s">
         <v>181</v>
       </c>
@@ -11804,7 +11818,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="409.6">
+    <row r="69" spans="1:3" ht="409.5">
       <c r="A69" s="5" t="s">
         <v>182</v>
       </c>
@@ -11812,7 +11826,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="144">
+    <row r="70" spans="1:3" ht="150">
       <c r="A70" s="5" t="s">
         <v>190</v>
       </c>
@@ -11823,7 +11837,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="230.4">
+    <row r="71" spans="1:3" ht="240">
       <c r="A71" s="5" t="s">
         <v>193</v>
       </c>
@@ -11850,7 +11864,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="28.8">
+    <row r="74" spans="1:3" ht="30">
       <c r="A74" s="5" t="s">
         <v>276</v>
       </c>
@@ -11858,7 +11872,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.8">
+    <row r="75" spans="1:3" ht="30">
       <c r="A75" s="5" t="s">
         <v>279</v>
       </c>
@@ -11866,7 +11880,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="28.8">
+    <row r="76" spans="1:3" ht="30">
       <c r="A76" s="5" t="s">
         <v>281</v>
       </c>
@@ -11874,7 +11888,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" ht="30">
       <c r="A77" s="5" t="s">
         <v>353</v>
       </c>
@@ -11906,7 +11920,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.8">
+    <row r="81" spans="1:2" ht="30">
       <c r="A81" s="5" t="s">
         <v>358</v>
       </c>
@@ -11930,7 +11944,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="28.8">
+    <row r="84" spans="1:2" ht="30">
       <c r="A84" s="5" t="s">
         <v>363</v>
       </c>
@@ -11938,7 +11952,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" ht="30">
       <c r="A85" s="5" t="s">
         <v>364</v>
       </c>
@@ -11946,7 +11960,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.8">
+    <row r="86" spans="1:2" ht="30">
       <c r="A86" s="5" t="s">
         <v>365</v>
       </c>
@@ -11962,7 +11976,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.8">
+    <row r="88" spans="1:2" ht="30">
       <c r="A88" s="5" t="s">
         <v>368</v>
       </c>
@@ -11978,7 +11992,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="28.8">
+    <row r="90" spans="1:2" ht="30">
       <c r="A90" s="5" t="s">
         <v>381</v>
       </c>
@@ -12026,7 +12040,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.8">
+    <row r="96" spans="1:2" ht="45">
       <c r="A96" s="5" t="s">
         <v>393</v>
       </c>
@@ -12042,7 +12056,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="28.8">
+    <row r="98" spans="1:3" ht="30">
       <c r="A98" s="5" t="s">
         <v>397</v>
       </c>
@@ -12082,7 +12096,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="187.2">
+    <row r="103" spans="1:3" ht="195">
       <c r="A103" s="5" t="s">
         <v>406</v>
       </c>
@@ -12093,7 +12107,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="273.60000000000002">
+    <row r="104" spans="1:3" ht="285">
       <c r="A104" s="5" t="s">
         <v>407</v>
       </c>
@@ -12104,7 +12118,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="230.4">
+    <row r="105" spans="1:3" ht="240">
       <c r="A105" s="5" t="s">
         <v>409</v>
       </c>
@@ -12115,7 +12129,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" ht="30">
       <c r="A106" s="5" t="s">
         <v>412</v>
       </c>
@@ -12123,7 +12137,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="43.2">
+    <row r="107" spans="1:3" ht="45">
       <c r="A107" s="5" t="s">
         <v>414</v>
       </c>
@@ -12139,7 +12153,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="115.2">
+    <row r="109" spans="1:3" ht="120">
       <c r="A109" s="5" t="s">
         <v>421</v>
       </c>
@@ -12322,7 +12336,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="115.2">
+    <row r="127" spans="1:3" ht="120">
       <c r="A127" s="5" t="s">
         <v>462</v>
       </c>
@@ -12333,7 +12347,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="115.2">
+    <row r="128" spans="1:3" ht="120">
       <c r="A128" s="5" t="s">
         <v>463</v>
       </c>
@@ -12352,7 +12366,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="172.8">
+    <row r="130" spans="1:3" ht="180">
       <c r="A130" s="5" t="s">
         <v>466</v>
       </c>
@@ -12363,7 +12377,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="144">
+    <row r="131" spans="1:3" ht="150">
       <c r="A131" s="5" t="s">
         <v>470</v>
       </c>
@@ -12374,7 +12388,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="144">
+    <row r="132" spans="1:3" ht="150">
       <c r="A132" s="5" t="s">
         <v>471</v>
       </c>
@@ -12385,7 +12399,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="129.6">
+    <row r="133" spans="1:3" ht="135">
       <c r="A133" s="5" t="s">
         <v>474</v>
       </c>
@@ -12396,7 +12410,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="129.6">
+    <row r="134" spans="1:3" ht="135">
       <c r="A134" s="5" t="s">
         <v>476</v>
       </c>
@@ -12407,7 +12421,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="129.6">
+    <row r="135" spans="1:3" ht="135">
       <c r="A135" s="5" t="s">
         <v>477</v>
       </c>
@@ -12418,7 +12432,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="129.6">
+    <row r="136" spans="1:3" ht="135">
       <c r="A136" s="5" t="s">
         <v>480</v>
       </c>
@@ -12429,7 +12443,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="129.6">
+    <row r="137" spans="1:3" ht="135">
       <c r="A137" s="5" t="s">
         <v>482</v>
       </c>
@@ -12440,7 +12454,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="129.6">
+    <row r="138" spans="1:3" ht="135">
       <c r="A138" s="5" t="s">
         <v>484</v>
       </c>
@@ -12451,7 +12465,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="129.6">
+    <row r="139" spans="1:3" ht="135">
       <c r="A139" s="5" t="s">
         <v>485</v>
       </c>
@@ -12462,7 +12476,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="129.6">
+    <row r="140" spans="1:3" ht="135">
       <c r="A140" s="5" t="s">
         <v>488</v>
       </c>
@@ -12473,7 +12487,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="129.6">
+    <row r="141" spans="1:3" ht="135">
       <c r="A141" s="5" t="s">
         <v>490</v>
       </c>
@@ -12484,7 +12498,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="129.6">
+    <row r="142" spans="1:3" ht="135">
       <c r="A142" s="5" t="s">
         <v>491</v>
       </c>
@@ -12495,7 +12509,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="115.2">
+    <row r="143" spans="1:3" ht="120">
       <c r="A143" s="5" t="s">
         <v>497</v>
       </c>
@@ -12506,7 +12520,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="129.6">
+    <row r="144" spans="1:3" ht="135">
       <c r="A144" s="5" t="s">
         <v>500</v>
       </c>
@@ -12517,7 +12531,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="129.6">
+    <row r="145" spans="1:3" ht="135">
       <c r="A145" s="5" t="s">
         <v>501</v>
       </c>
@@ -12528,7 +12542,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="129.6">
+    <row r="146" spans="1:3" ht="135">
       <c r="A146" s="5" t="s">
         <v>503</v>
       </c>
@@ -12539,7 +12553,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="129.6">
+    <row r="147" spans="1:3" ht="135">
       <c r="A147" s="5" t="s">
         <v>506</v>
       </c>
@@ -12550,7 +12564,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="129.6">
+    <row r="148" spans="1:3" ht="135">
       <c r="A148" s="5" t="s">
         <v>507</v>
       </c>
@@ -12605,7 +12619,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="28.8">
+    <row r="153" spans="1:3" ht="30">
       <c r="A153" s="5" t="s">
         <v>531</v>
       </c>
@@ -12616,7 +12630,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" ht="30">
       <c r="A154" s="5" t="s">
         <v>532</v>
       </c>
@@ -12627,7 +12641,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="86.4">
+    <row r="155" spans="1:3" ht="90">
       <c r="A155" s="5" t="s">
         <v>534</v>
       </c>
@@ -12638,7 +12652,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="43.2">
+    <row r="156" spans="1:3" ht="45">
       <c r="A156" s="5" t="s">
         <v>536</v>
       </c>
@@ -12649,7 +12663,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="172.8">
+    <row r="157" spans="1:3" ht="180">
       <c r="A157" s="5" t="s">
         <v>540</v>
       </c>
@@ -12660,7 +12674,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="158.4">
+    <row r="158" spans="1:3" ht="165">
       <c r="A158" s="5" t="s">
         <v>541</v>
       </c>
@@ -12679,7 +12693,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="72">
+    <row r="160" spans="1:3" ht="75">
       <c r="A160" s="5" t="s">
         <v>547</v>
       </c>
@@ -12690,7 +12704,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="57.6">
+    <row r="161" spans="1:3" ht="60">
       <c r="A161" s="5" t="s">
         <v>551</v>
       </c>
@@ -12698,7 +12712,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="43.2">
+    <row r="162" spans="1:3" ht="45">
       <c r="A162" s="5" t="s">
         <v>552</v>
       </c>
@@ -12717,7 +12731,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="100.8">
+    <row r="164" spans="1:3" ht="105">
       <c r="A164" s="5" t="s">
         <v>560</v>
       </c>
@@ -12725,7 +12739,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="100.8">
+    <row r="165" spans="1:3" ht="105">
       <c r="A165" s="5" t="s">
         <v>561</v>
       </c>
@@ -12804,7 +12818,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" ht="30">
       <c r="A173" s="5" t="s">
         <v>571</v>
       </c>
@@ -12867,7 +12881,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" ht="30">
       <c r="A179" s="5" t="s">
         <v>577</v>
       </c>
@@ -12878,7 +12892,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="28.8">
+    <row r="180" spans="1:3" ht="30">
       <c r="A180" s="5" t="s">
         <v>578</v>
       </c>
@@ -12900,7 +12914,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" ht="30">
       <c r="A182" s="5" t="s">
         <v>580</v>
       </c>
@@ -12911,7 +12925,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="115.2">
+    <row r="183" spans="1:3" ht="120">
       <c r="A183" s="5" t="s">
         <v>581</v>
       </c>
@@ -12966,7 +12980,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="72">
+    <row r="188" spans="1:3" ht="75">
       <c r="A188" s="5" t="s">
         <v>586</v>
       </c>
@@ -12977,7 +12991,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="100.8">
+    <row r="189" spans="1:3" ht="105">
       <c r="A189" s="5" t="s">
         <v>587</v>
       </c>
@@ -12988,7 +13002,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="72">
+    <row r="190" spans="1:3" ht="75">
       <c r="A190" s="5" t="s">
         <v>667</v>
       </c>
@@ -12999,7 +13013,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="86.4">
+    <row r="191" spans="1:3" ht="90">
       <c r="A191" s="5" t="s">
         <v>668</v>
       </c>
@@ -13010,7 +13024,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="86.4">
+    <row r="192" spans="1:3" ht="90">
       <c r="A192" s="5" t="s">
         <v>669</v>
       </c>
@@ -13065,7 +13079,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="28.8">
+    <row r="197" spans="1:3" ht="30">
       <c r="A197" s="5" t="s">
         <v>674</v>
       </c>
@@ -13076,7 +13090,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="28.8">
+    <row r="198" spans="1:3" ht="30">
       <c r="A198" s="5" t="s">
         <v>675</v>
       </c>
@@ -13098,7 +13112,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="28.8">
+    <row r="200" spans="1:3" ht="30">
       <c r="A200" s="5" t="s">
         <v>677</v>
       </c>
@@ -13109,7 +13123,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="86.4">
+    <row r="201" spans="1:3" ht="90">
       <c r="A201" s="5" t="s">
         <v>678</v>
       </c>
@@ -13120,7 +13134,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="72">
+    <row r="202" spans="1:3" ht="75">
       <c r="A202" s="5" t="s">
         <v>679</v>
       </c>
@@ -13131,7 +13145,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="86.4">
+    <row r="203" spans="1:3" ht="90">
       <c r="A203" s="5" t="s">
         <v>680</v>
       </c>
@@ -13142,7 +13156,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="28.8">
+    <row r="204" spans="1:3" ht="30">
       <c r="A204" s="5" t="s">
         <v>681</v>
       </c>
@@ -13150,7 +13164,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="409.6">
+    <row r="205" spans="1:3" ht="409.5">
       <c r="A205" s="5" t="s">
         <v>682</v>
       </c>
@@ -13161,7 +13175,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="216">
+    <row r="206" spans="1:3" ht="240">
       <c r="A206" s="5" t="s">
         <v>683</v>
       </c>
@@ -13183,7 +13197,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="43.2">
+    <row r="208" spans="1:3" ht="45">
       <c r="A208" s="5" t="s">
         <v>685</v>
       </c>
@@ -13194,7 +13208,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="100.8">
+    <row r="209" spans="1:3" ht="105">
       <c r="A209" s="5" t="s">
         <v>686</v>
       </c>
@@ -13216,7 +13230,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="409.6">
+    <row r="211" spans="1:3" ht="409.5">
       <c r="A211" s="5" t="s">
         <v>688</v>
       </c>
@@ -13238,7 +13252,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="28.8">
+    <row r="213" spans="1:3" ht="30">
       <c r="A213" s="5" t="s">
         <v>690</v>
       </c>
@@ -13249,7 +13263,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="72">
+    <row r="214" spans="1:3" ht="75">
       <c r="A214" s="5" t="s">
         <v>691</v>
       </c>
@@ -13260,7 +13274,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="86.4">
+    <row r="215" spans="1:3" ht="90">
       <c r="A215" s="5" t="s">
         <v>692</v>
       </c>
@@ -13271,7 +13285,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="72">
+    <row r="216" spans="1:3" ht="75">
       <c r="A216" s="5" t="s">
         <v>693</v>
       </c>
@@ -13282,7 +13296,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="86.4">
+    <row r="217" spans="1:3" ht="90">
       <c r="A217" s="5" t="s">
         <v>694</v>
       </c>
@@ -13293,7 +13307,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="216">
+    <row r="218" spans="1:3" ht="240">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -13304,7 +13318,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="409.6">
+    <row r="219" spans="1:3" ht="409.5">
       <c r="A219" s="5" t="s">
         <v>695</v>
       </c>
@@ -13315,7 +13329,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="216">
+    <row r="220" spans="1:3" ht="240">
       <c r="A220" s="5" t="s">
         <v>696</v>
       </c>
@@ -13326,7 +13340,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="158.4">
+    <row r="221" spans="1:3" ht="180">
       <c r="A221" s="5" t="s">
         <v>697</v>
       </c>
@@ -13342,7 +13356,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="100.8">
+    <row r="223" spans="1:3" ht="105">
       <c r="A223" s="5" t="s">
         <v>699</v>
       </c>
@@ -13353,7 +13367,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="100.8">
+    <row r="224" spans="1:3" ht="105">
       <c r="A224" s="5" t="s">
         <v>700</v>
       </c>
@@ -13364,7 +13378,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="100.8">
+    <row r="225" spans="1:3" ht="105">
       <c r="A225" s="5" t="s">
         <v>701</v>
       </c>
@@ -13439,7 +13453,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="86.4">
+    <row r="234" spans="1:3" ht="105">
       <c r="A234" s="5" t="s">
         <v>710</v>
       </c>
@@ -13458,7 +13472,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="86.4">
+    <row r="236" spans="1:3" ht="90">
       <c r="A236" s="5" t="s">
         <v>712</v>
       </c>
@@ -13491,7 +13505,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="129.6">
+    <row r="239" spans="1:3" ht="135">
       <c r="A239" s="5" t="s">
         <v>715</v>
       </c>
@@ -13502,7 +13516,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="28.8">
+    <row r="240" spans="1:3" ht="30">
       <c r="A240" s="5" t="s">
         <v>716</v>
       </c>
@@ -13524,7 +13538,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="100.8">
+    <row r="242" spans="1:3" ht="105">
       <c r="A242" s="5" t="s">
         <v>785</v>
       </c>
@@ -13535,7 +13549,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="43.2">
+    <row r="243" spans="1:3" ht="45">
       <c r="A243" s="5" t="s">
         <v>786</v>
       </c>
@@ -13546,7 +13560,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="172.8">
+    <row r="244" spans="1:3" ht="180">
       <c r="A244" s="5" t="s">
         <v>787</v>
       </c>
@@ -13557,7 +13571,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="216">
+    <row r="245" spans="1:3" ht="225">
       <c r="A245" s="5" t="s">
         <v>789</v>
       </c>
@@ -13568,7 +13582,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="172.8">
+    <row r="246" spans="1:3" ht="180">
       <c r="A246" s="5" t="s">
         <v>794</v>
       </c>
@@ -13579,7 +13593,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="187.2">
+    <row r="247" spans="1:3" ht="195">
       <c r="A247" s="5" t="s">
         <v>799</v>
       </c>
@@ -13590,7 +13604,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="187.2">
+    <row r="248" spans="1:3" ht="195">
       <c r="A248" s="5" t="s">
         <v>802</v>
       </c>
@@ -13601,7 +13615,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="216">
+    <row r="249" spans="1:3" ht="225">
       <c r="A249" s="5" t="s">
         <v>805</v>
       </c>
@@ -13612,7 +13626,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="115.2">
+    <row r="250" spans="1:3" ht="120">
       <c r="A250" s="5" t="s">
         <v>825</v>
       </c>
@@ -13623,7 +13637,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="144">
+    <row r="251" spans="1:3" ht="150">
       <c r="A251" s="5" t="s">
         <v>828</v>
       </c>
@@ -13634,7 +13648,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="115.2">
+    <row r="252" spans="1:3" ht="120">
       <c r="A252" s="5" t="s">
         <v>831</v>
       </c>
@@ -13656,7 +13670,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="28.8">
+    <row r="254" spans="1:3" ht="30">
       <c r="A254" s="5" t="s">
         <v>839</v>
       </c>
@@ -13667,7 +13681,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="72">
+    <row r="255" spans="1:3" ht="75">
       <c r="A255" s="5" t="s">
         <v>840</v>
       </c>
@@ -13678,7 +13692,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="28.8">
+    <row r="256" spans="1:3" ht="30">
       <c r="A256" s="5" t="s">
         <v>841</v>
       </c>
@@ -13689,7 +13703,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="72">
+    <row r="257" spans="1:3" ht="75">
       <c r="A257" s="5" t="s">
         <v>842</v>
       </c>
@@ -13700,7 +13714,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="144">
+    <row r="258" spans="1:3" ht="150">
       <c r="A258" s="5" t="s">
         <v>848</v>
       </c>
@@ -13722,7 +13736,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="43.2">
+    <row r="260" spans="1:3" ht="45">
       <c r="A260" s="5" t="s">
         <v>852</v>
       </c>
@@ -13733,7 +13747,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="57.6">
+    <row r="261" spans="1:3" ht="60">
       <c r="A261" s="5" t="s">
         <v>855</v>
       </c>
@@ -13744,7 +13758,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="86.4">
+    <row r="262" spans="1:3" ht="90">
       <c r="A262" s="5" t="s">
         <v>858</v>
       </c>
@@ -13763,7 +13777,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="57.6">
+    <row r="264" spans="1:3" ht="60">
       <c r="A264" s="5" t="s">
         <v>863</v>
       </c>
@@ -13774,7 +13788,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="86.4">
+    <row r="265" spans="1:3" ht="90">
       <c r="A265" s="5" t="s">
         <v>866</v>
       </c>
@@ -13785,7 +13799,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="72">
+    <row r="266" spans="1:3" ht="75">
       <c r="A266" s="5" t="s">
         <v>869</v>
       </c>
@@ -13820,7 +13834,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="28.8">
+    <row r="270" spans="1:3" ht="30">
       <c r="A270" s="5" t="s">
         <v>883</v>
       </c>
@@ -13828,7 +13842,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="100.8">
+    <row r="271" spans="1:3" ht="120">
       <c r="A271" s="5" t="s">
         <v>884</v>
       </c>
@@ -13839,7 +13853,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="43.2">
+    <row r="272" spans="1:3" ht="45">
       <c r="A272" s="5" t="s">
         <v>885</v>
       </c>
@@ -13850,7 +13864,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="28.8">
+    <row r="273" spans="1:4" ht="30">
       <c r="A273" s="5" t="s">
         <v>886</v>
       </c>
@@ -13861,7 +13875,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="72">
+    <row r="274" spans="1:4" ht="75">
       <c r="A274" s="5" t="s">
         <v>890</v>
       </c>
@@ -14509,7 +14523,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="401" spans="1:3" ht="28.8">
+    <row r="401" spans="1:3" ht="30">
       <c r="A401" s="2" t="s">
         <v>1018</v>
       </c>
@@ -14520,7 +14534,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="402" spans="1:3" ht="72">
+    <row r="402" spans="1:3" ht="75">
       <c r="A402" s="2" t="s">
         <v>1019</v>
       </c>
@@ -14531,7 +14545,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="43.2">
+    <row r="403" spans="1:3" ht="60">
       <c r="A403" s="2" t="s">
         <v>1020</v>
       </c>
@@ -14542,7 +14556,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="28.8">
+    <row r="404" spans="1:3" ht="30">
       <c r="A404" s="2" t="s">
         <v>1021</v>
       </c>
@@ -14553,7 +14567,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="28.8">
+    <row r="405" spans="1:3" ht="30">
       <c r="A405" s="2" t="s">
         <v>1022</v>
       </c>
@@ -14564,7 +14578,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="43.2">
+    <row r="406" spans="1:3" ht="60">
       <c r="A406" s="2" t="s">
         <v>1023</v>
       </c>
@@ -14575,7 +14589,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="407" spans="1:3" ht="28.8">
+    <row r="407" spans="1:3" ht="30">
       <c r="A407" s="2" t="s">
         <v>1024</v>
       </c>
@@ -14586,7 +14600,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="129.6">
+    <row r="408" spans="1:3" ht="135">
       <c r="A408" s="2" t="s">
         <v>1025</v>
       </c>
@@ -14597,7 +14611,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="409" spans="1:3" ht="43.2">
+    <row r="409" spans="1:3" ht="45">
       <c r="A409" s="2" t="s">
         <v>1026</v>
       </c>
@@ -14608,7 +14622,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="410" spans="1:3" ht="28.8">
+    <row r="410" spans="1:3" ht="30">
       <c r="A410" s="2" t="s">
         <v>1027</v>
       </c>
@@ -14619,7 +14633,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="28.8">
+    <row r="411" spans="1:3" ht="30">
       <c r="A411" s="2" t="s">
         <v>1028</v>
       </c>
@@ -14630,7 +14644,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="158.4">
+    <row r="412" spans="1:3" ht="165">
       <c r="A412" s="2" t="s">
         <v>1029</v>
       </c>
@@ -14641,7 +14655,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="172.8">
+    <row r="413" spans="1:3" ht="180">
       <c r="A413" s="2" t="s">
         <v>1030</v>
       </c>
@@ -14652,7 +14666,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="72">
+    <row r="414" spans="1:3" ht="75">
       <c r="A414" s="2" t="s">
         <v>1031</v>
       </c>
@@ -14674,7 +14688,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="72">
+    <row r="416" spans="1:3" ht="75">
       <c r="A416" s="2" t="s">
         <v>1033</v>
       </c>
@@ -14685,7 +14699,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="115.2">
+    <row r="417" spans="1:3" ht="120">
       <c r="A417" s="2" t="s">
         <v>1034</v>
       </c>
@@ -14696,7 +14710,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="129.6">
+    <row r="418" spans="1:3" ht="135">
       <c r="A418" s="2" t="s">
         <v>1035</v>
       </c>
@@ -14707,7 +14721,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="28.8">
+    <row r="419" spans="1:3" ht="30">
       <c r="A419" s="2" t="s">
         <v>1036</v>
       </c>
@@ -14817,7 +14831,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="72">
+    <row r="429" spans="1:3" ht="75">
       <c r="A429" s="2" t="s">
         <v>1046</v>
       </c>
@@ -18203,82 +18217,88 @@
         <v>1721</v>
       </c>
     </row>
-    <row r="1105" spans="1:1">
+    <row r="1105" spans="1:3">
       <c r="A1105" s="5" t="s">
         <v>1722</v>
       </c>
     </row>
-    <row r="1106" spans="1:1">
+    <row r="1106" spans="1:3">
       <c r="A1106" s="5" t="s">
         <v>1723</v>
       </c>
     </row>
-    <row r="1107" spans="1:1">
+    <row r="1107" spans="1:3">
       <c r="A1107" s="5" t="s">
         <v>1724</v>
       </c>
     </row>
-    <row r="1108" spans="1:1">
+    <row r="1108" spans="1:3">
       <c r="A1108" s="5" t="s">
         <v>1725</v>
       </c>
     </row>
-    <row r="1109" spans="1:1">
+    <row r="1109" spans="1:3">
       <c r="A1109" s="5" t="s">
         <v>1726</v>
       </c>
     </row>
-    <row r="1110" spans="1:1">
+    <row r="1110" spans="1:3">
       <c r="A1110" s="5" t="s">
         <v>1727</v>
       </c>
     </row>
-    <row r="1111" spans="1:1">
+    <row r="1111" spans="1:3">
       <c r="A1111" s="5" t="s">
         <v>1728</v>
       </c>
     </row>
-    <row r="1112" spans="1:1">
-      <c r="A1112" s="5" t="s">
+    <row r="1112" spans="1:3" s="55" customFormat="1">
+      <c r="A1112" s="54" t="s">
         <v>1729</v>
       </c>
-    </row>
-    <row r="1113" spans="1:1">
+      <c r="B1112" s="55" t="s">
+        <v>2649</v>
+      </c>
+      <c r="C1112" s="55" t="s">
+        <v>2648</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:3">
       <c r="A1113" s="5" t="s">
         <v>1730</v>
       </c>
     </row>
-    <row r="1114" spans="1:1">
+    <row r="1114" spans="1:3">
       <c r="A1114" s="5" t="s">
         <v>1731</v>
       </c>
     </row>
-    <row r="1115" spans="1:1">
+    <row r="1115" spans="1:3">
       <c r="A1115" s="5" t="s">
         <v>1732</v>
       </c>
     </row>
-    <row r="1116" spans="1:1">
+    <row r="1116" spans="1:3">
       <c r="A1116" s="5" t="s">
         <v>1733</v>
       </c>
     </row>
-    <row r="1117" spans="1:1">
+    <row r="1117" spans="1:3">
       <c r="A1117" s="5" t="s">
         <v>1734</v>
       </c>
     </row>
-    <row r="1118" spans="1:1">
+    <row r="1118" spans="1:3">
       <c r="A1118" s="5" t="s">
         <v>1735</v>
       </c>
     </row>
-    <row r="1119" spans="1:1">
+    <row r="1119" spans="1:3">
       <c r="A1119" s="5" t="s">
         <v>1736</v>
       </c>
     </row>
-    <row r="1120" spans="1:1">
+    <row r="1120" spans="1:3">
       <c r="A1120" s="5" t="s">
         <v>1737</v>
       </c>
@@ -19383,7 +19403,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="1341" spans="1:3" ht="129.6">
+    <row r="1341" spans="1:3" ht="135">
       <c r="A1341" s="51" t="s">
         <v>1958</v>
       </c>
@@ -19416,7 +19436,7 @@
         <v>2629</v>
       </c>
     </row>
-    <row r="1344" spans="1:3" ht="129.6">
+    <row r="1344" spans="1:3" ht="135">
       <c r="A1344" s="5" t="s">
         <v>1961</v>
       </c>
@@ -19427,7 +19447,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="1345" spans="1:3" ht="28.8">
+    <row r="1345" spans="1:3" ht="30">
       <c r="A1345" s="5" t="s">
         <v>1962</v>
       </c>
@@ -20218,7 +20238,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="1502" spans="1:3" ht="86.4">
+    <row r="1502" spans="1:3" ht="90">
       <c r="A1502" s="5" t="s">
         <v>2119</v>
       </c>
@@ -20229,7 +20249,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="1503" spans="1:3" ht="86.4">
+    <row r="1503" spans="1:3" ht="90">
       <c r="A1503" s="5" t="s">
         <v>2120</v>
       </c>
@@ -20240,7 +20260,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="1504" spans="1:3" ht="144">
+    <row r="1504" spans="1:3" ht="150">
       <c r="A1504" s="5" t="s">
         <v>2121</v>
       </c>
@@ -20251,7 +20271,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="1505" spans="1:3" ht="144">
+    <row r="1505" spans="1:3" ht="150">
       <c r="A1505" s="5" t="s">
         <v>2122</v>
       </c>
@@ -20262,7 +20282,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1506" spans="1:3" ht="72">
+    <row r="1506" spans="1:3" ht="75">
       <c r="A1506" s="5" t="s">
         <v>2123</v>
       </c>
@@ -20270,7 +20290,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="1507" spans="1:3" ht="43.2">
+    <row r="1507" spans="1:3" ht="45">
       <c r="A1507" s="47" t="s">
         <v>2124</v>
       </c>
@@ -20281,7 +20301,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1508" spans="1:3" ht="43.2">
+    <row r="1508" spans="1:3" ht="45">
       <c r="A1508" s="44" t="s">
         <v>2125</v>
       </c>
@@ -20292,7 +20312,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1509" spans="1:3" ht="216">
+    <row r="1509" spans="1:3" ht="225">
       <c r="A1509" s="5" t="s">
         <v>2126</v>
       </c>
@@ -20775,7 +20795,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="1602" spans="1:3" ht="28.8">
+    <row r="1602" spans="1:3" ht="30">
       <c r="A1602" s="5" t="s">
         <v>2219</v>
       </c>
@@ -20797,7 +20817,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="1604" spans="1:3" ht="57.6">
+    <row r="1604" spans="1:3" ht="60">
       <c r="A1604" s="5" t="s">
         <v>2221</v>
       </c>
@@ -20808,7 +20828,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="1605" spans="1:3" ht="43.2">
+    <row r="1605" spans="1:3" ht="45">
       <c r="A1605" s="5" t="s">
         <v>2222</v>
       </c>
@@ -20816,7 +20836,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="1606" spans="1:3" ht="100.8">
+    <row r="1606" spans="1:3" ht="105">
       <c r="A1606" s="5" t="s">
         <v>2223</v>
       </c>
@@ -20846,7 +20866,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="1609" spans="1:3" ht="43.2">
+    <row r="1609" spans="1:3" ht="45">
       <c r="A1609" s="5" t="s">
         <v>2278</v>
       </c>
@@ -20857,7 +20877,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="1610" spans="1:3" ht="28.8">
+    <row r="1610" spans="1:3" ht="30">
       <c r="A1610" s="5" t="s">
         <v>2279</v>
       </c>
@@ -20865,7 +20885,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="1611" spans="1:3" ht="388.8">
+    <row r="1611" spans="1:3" ht="409.5">
       <c r="A1611" s="5" t="s">
         <v>2280</v>
       </c>
@@ -20876,7 +20896,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="1612" spans="1:3" ht="230.4">
+    <row r="1612" spans="1:3" ht="240">
       <c r="A1612" s="44" t="s">
         <v>2281</v>
       </c>
@@ -20887,7 +20907,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="1613" spans="1:3">
+    <row r="1613" spans="1:3" ht="30">
       <c r="A1613" s="44" t="s">
         <v>2337</v>
       </c>
@@ -20920,7 +20940,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="1616" spans="1:3" ht="86.4">
+    <row r="1616" spans="1:3" ht="90">
       <c r="A1616" s="47" t="s">
         <v>2340</v>
       </c>
@@ -20931,7 +20951,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="1617" spans="1:3" ht="28.8">
+    <row r="1617" spans="1:3" ht="30">
       <c r="A1617" s="47" t="s">
         <v>2341</v>
       </c>
@@ -22363,7 +22383,7 @@
       </c>
       <c r="B1901" s="48"/>
     </row>
-    <row r="1902" spans="1:3" ht="43.2">
+    <row r="1902" spans="1:3" ht="45">
       <c r="A1902">
         <v>1901</v>
       </c>
@@ -22374,7 +22394,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="1903" spans="1:3" ht="86.4">
+    <row r="1903" spans="1:3" ht="90">
       <c r="A1903">
         <v>1902</v>
       </c>
@@ -22385,7 +22405,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="1904" spans="1:3" ht="216">
+    <row r="1904" spans="1:3" ht="225">
       <c r="A1904">
         <v>1903</v>
       </c>
@@ -22396,7 +22416,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="1905" spans="1:3" ht="144">
+    <row r="1905" spans="1:3" ht="150">
       <c r="A1905">
         <v>1904</v>
       </c>
@@ -22407,7 +22427,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="1906" spans="1:3" ht="144">
+    <row r="1906" spans="1:3" ht="150">
       <c r="A1906">
         <v>1905</v>
       </c>
@@ -22418,7 +22438,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="1907" spans="1:3" ht="115.2">
+    <row r="1907" spans="1:3" ht="120">
       <c r="A1907">
         <v>1906</v>
       </c>
@@ -22429,7 +22449,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="1908" spans="1:3" ht="144">
+    <row r="1908" spans="1:3" ht="150">
       <c r="A1908">
         <v>1907</v>
       </c>
@@ -22440,7 +22460,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="1909" spans="1:3" ht="144">
+    <row r="1909" spans="1:3" ht="150">
       <c r="A1909">
         <v>1908</v>
       </c>
@@ -22451,7 +22471,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="1910" spans="1:3" ht="100.8">
+    <row r="1910" spans="1:3" ht="105">
       <c r="A1910">
         <v>1909</v>
       </c>
@@ -22499,13 +22519,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -22685,10 +22705,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="68.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -23011,7 +23031,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15">
+    <row r="44" spans="1:2">
       <c r="A44" s="13" t="s">
         <v>263</v>
       </c>
@@ -23101,13 +23121,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="85.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>283</v>
       </c>
@@ -23115,7 +23135,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>285</v>
       </c>
@@ -23123,7 +23143,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>287</v>
       </c>
@@ -23131,7 +23151,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
       <c r="A4" s="25" t="s">
         <v>289</v>
       </c>
@@ -23139,7 +23159,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
       <c r="A5" s="25" t="s">
         <v>291</v>
       </c>
@@ -23147,7 +23167,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1">
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
       <c r="A6" s="25" t="s">
         <v>293</v>
       </c>
@@ -23155,7 +23175,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1">
       <c r="A7" s="25" t="s">
         <v>295</v>
       </c>
@@ -23163,7 +23183,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1">
       <c r="A8" s="25" t="s">
         <v>297</v>
       </c>
@@ -23171,7 +23191,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1">
       <c r="A9" s="25" t="s">
         <v>299</v>
       </c>
@@ -23179,7 +23199,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1">
       <c r="A10" s="25" t="s">
         <v>301</v>
       </c>
@@ -23187,7 +23207,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1">
       <c r="A11" s="25" t="s">
         <v>303</v>
       </c>
@@ -23195,7 +23215,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1">
       <c r="A12" s="25" t="s">
         <v>305</v>
       </c>
@@ -23203,7 +23223,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1">
       <c r="A13" s="25" t="s">
         <v>307</v>
       </c>
@@ -23211,7 +23231,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>309</v>
       </c>
@@ -23219,7 +23239,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1">
       <c r="A15" s="25" t="s">
         <v>311</v>
       </c>
@@ -23227,7 +23247,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1">
+    <row r="16" spans="1:2" ht="15.75" thickBot="1">
       <c r="A16" s="25" t="s">
         <v>313</v>
       </c>
@@ -23235,7 +23255,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1">
       <c r="A17" s="25" t="s">
         <v>315</v>
       </c>
@@ -23243,7 +23263,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1">
+    <row r="18" spans="1:2" ht="15.75" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>317</v>
       </c>
@@ -23251,7 +23271,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1">
       <c r="A19" s="25" t="s">
         <v>319</v>
       </c>
@@ -23259,7 +23279,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1">
+    <row r="20" spans="1:2" ht="15.75" thickBot="1">
       <c r="A20" s="25" t="s">
         <v>321</v>
       </c>
@@ -23267,7 +23287,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1">
       <c r="A21" s="25" t="s">
         <v>323</v>
       </c>
@@ -23275,7 +23295,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1">
+    <row r="22" spans="1:2" ht="15.75" thickBot="1">
       <c r="A22" s="25" t="s">
         <v>325</v>
       </c>
@@ -23283,7 +23303,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1">
+    <row r="23" spans="1:2" ht="15.75" thickBot="1">
       <c r="A23" s="25" t="s">
         <v>327</v>
       </c>
@@ -23291,7 +23311,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1">
+    <row r="24" spans="1:2" ht="15.75" thickBot="1">
       <c r="A24" s="25" t="s">
         <v>329</v>
       </c>
@@ -23299,7 +23319,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1">
       <c r="A25" s="25" t="s">
         <v>331</v>
       </c>
@@ -23307,7 +23327,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1">
+    <row r="26" spans="1:2" ht="15.75" thickBot="1">
       <c r="A26" s="25" t="s">
         <v>333</v>
       </c>
@@ -23315,7 +23335,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1">
+    <row r="27" spans="1:2" ht="15.75" thickBot="1">
       <c r="A27" s="25" t="s">
         <v>335</v>
       </c>
@@ -23323,7 +23343,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1">
+    <row r="28" spans="1:2" ht="15.75" thickBot="1">
       <c r="A28" s="25" t="s">
         <v>337</v>
       </c>
@@ -23331,7 +23351,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1">
+    <row r="29" spans="1:2" ht="15.75" thickBot="1">
       <c r="A29" s="25" t="s">
         <v>339</v>
       </c>
@@ -23339,7 +23359,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1">
+    <row r="30" spans="1:2" ht="15.75" thickBot="1">
       <c r="A30" s="25" t="s">
         <v>341</v>
       </c>
@@ -23347,7 +23367,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1">
+    <row r="31" spans="1:2" ht="15.75" thickBot="1">
       <c r="A31" s="25" t="s">
         <v>343</v>
       </c>
@@ -23355,7 +23375,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1">
+    <row r="32" spans="1:2" ht="15.75" thickBot="1">
       <c r="A32" s="25" t="s">
         <v>345</v>
       </c>
@@ -23363,7 +23383,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1">
+    <row r="33" spans="1:2" ht="15.75" thickBot="1">
       <c r="A33" s="25" t="s">
         <v>347</v>
       </c>
@@ -23371,7 +23391,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1">
+    <row r="34" spans="1:2" ht="15.75" thickBot="1">
       <c r="A34" s="25" t="s">
         <v>349</v>
       </c>
@@ -23379,7 +23399,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1">
+    <row r="35" spans="1:2" ht="15.75" thickBot="1">
       <c r="A35" s="25" t="s">
         <v>351</v>
       </c>

</xml_diff>

<commit_message>
Tnc, OPS-Invalid TIN, resource dropdown
Tnc, OPS-Invalid TIN, resource dropdown
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdassani\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vashok3\Documents\Git_AccessPayment\opp_3\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D68645-20B4-4E64-9622-F15128A1A353}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58176E2-1B13-4A22-8EF4-DAEBE679E43C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="2650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="2651">
   <si>
     <t>City</t>
   </si>
@@ -9866,6 +9866,9 @@
   </si>
   <si>
     <t>select PAY_PROC_ACPT_CD_VAL_DESC from OLE.PAY_PROC_VAL where PAY_PROC_CD = '{$pay_proc_cd}'</t>
+  </si>
+  <si>
+    <t>update OLE.PORTAL_USER set TC_ACCEPT_IND='N' where SSO_ID='{$id}'</t>
   </si>
 </sst>
 </file>
@@ -10618,20 +10621,20 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1"/>
+    <col min="12" max="12" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -11167,15 +11170,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1912"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1082" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1112" sqref="B1112"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B280" sqref="B280"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="136.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="136.54296875" customWidth="1"/>
+    <col min="3" max="3" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -11211,7 +11214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60">
+    <row r="4" spans="1:3" ht="58">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -11219,7 +11222,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="29">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -11254,7 +11257,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="29">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -11262,7 +11265,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="90">
+    <row r="10" spans="1:3" ht="87">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -11270,7 +11273,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="75">
+    <row r="11" spans="1:3" ht="72.5">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -11278,7 +11281,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="43.5">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -11286,7 +11289,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60">
+    <row r="13" spans="1:3" ht="58">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -11302,7 +11305,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60">
+    <row r="15" spans="1:3" ht="58">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -11310,7 +11313,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30">
+    <row r="16" spans="1:3" ht="29">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -11318,7 +11321,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -11326,7 +11329,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
@@ -11334,7 +11337,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90">
+    <row r="19" spans="1:3" ht="87">
       <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
@@ -11342,7 +11345,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75">
+    <row r="20" spans="1:3" ht="72.5">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -11350,7 +11353,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="29">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
@@ -11358,7 +11361,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -11366,7 +11369,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="29">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -11374,7 +11377,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="45">
+    <row r="24" spans="1:3" ht="43.5">
       <c r="A24" s="5" t="s">
         <v>88</v>
       </c>
@@ -11385,7 +11388,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="75">
+    <row r="25" spans="1:3" ht="72.5">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -11401,7 +11404,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="135">
+    <row r="27" spans="1:3" ht="130.5">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -11409,7 +11412,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="90">
+    <row r="28" spans="1:3" ht="87">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
@@ -11417,7 +11420,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="29">
       <c r="A29" s="5" t="s">
         <v>94</v>
       </c>
@@ -11425,7 +11428,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="150">
+    <row r="30" spans="1:3" ht="145">
       <c r="A30" s="5" t="s">
         <v>95</v>
       </c>
@@ -11436,7 +11439,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="165">
+    <row r="31" spans="1:3" ht="159.5">
       <c r="A31" s="5" t="s">
         <v>98</v>
       </c>
@@ -11447,7 +11450,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="165">
+    <row r="32" spans="1:3" ht="159.5">
       <c r="A32" s="5" t="s">
         <v>101</v>
       </c>
@@ -11458,7 +11461,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="195">
+    <row r="33" spans="1:4" ht="188.5">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -11469,7 +11472,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="120">
+    <row r="34" spans="1:4" ht="116">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -11477,7 +11480,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45">
+    <row r="35" spans="1:4" ht="43.5">
       <c r="A35" s="5" t="s">
         <v>108</v>
       </c>
@@ -11485,7 +11488,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="120">
+    <row r="36" spans="1:4" ht="116">
       <c r="A36" s="5" t="s">
         <v>113</v>
       </c>
@@ -11496,7 +11499,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="105">
+    <row r="37" spans="1:4" ht="101.5">
       <c r="A37" s="5" t="s">
         <v>112</v>
       </c>
@@ -11507,7 +11510,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="120">
+    <row r="38" spans="1:4" ht="116">
       <c r="A38" s="5" t="s">
         <v>114</v>
       </c>
@@ -11515,7 +11518,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="105">
+    <row r="39" spans="1:4" ht="101.5">
       <c r="A39" s="5" t="s">
         <v>117</v>
       </c>
@@ -11523,7 +11526,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="120">
+    <row r="40" spans="1:4" ht="116">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -11531,7 +11534,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="120">
+    <row r="41" spans="1:4" ht="116">
       <c r="A41" s="5" t="s">
         <v>121</v>
       </c>
@@ -11539,7 +11542,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="120">
+    <row r="42" spans="1:4" ht="116">
       <c r="A42" s="5" t="s">
         <v>122</v>
       </c>
@@ -11553,7 +11556,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="180">
+    <row r="43" spans="1:4" ht="174">
       <c r="A43" s="5" t="s">
         <v>124</v>
       </c>
@@ -11564,7 +11567,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="180">
+    <row r="44" spans="1:4" ht="174">
       <c r="A44" s="5" t="s">
         <v>125</v>
       </c>
@@ -11575,7 +11578,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="105">
+    <row r="45" spans="1:4" ht="101.5">
       <c r="A45" s="5" t="s">
         <v>126</v>
       </c>
@@ -11586,7 +11589,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="165">
+    <row r="46" spans="1:4" ht="159.5">
       <c r="A46" s="5" t="s">
         <v>127</v>
       </c>
@@ -11597,7 +11600,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="180">
+    <row r="47" spans="1:4" ht="174">
       <c r="A47" s="5" t="s">
         <v>128</v>
       </c>
@@ -11608,7 +11611,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="180">
+    <row r="48" spans="1:4" ht="174">
       <c r="A48" s="5" t="s">
         <v>129</v>
       </c>
@@ -11619,7 +11622,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="105">
+    <row r="49" spans="1:3" ht="101.5">
       <c r="A49" s="5" t="s">
         <v>130</v>
       </c>
@@ -11630,7 +11633,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="135">
+    <row r="50" spans="1:3" ht="130.5">
       <c r="A50" s="5" t="s">
         <v>131</v>
       </c>
@@ -11641,7 +11644,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="105">
+    <row r="51" spans="1:3" ht="101.5">
       <c r="A51" s="5" t="s">
         <v>132</v>
       </c>
@@ -11652,7 +11655,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="135">
+    <row r="52" spans="1:3" ht="130.5">
       <c r="A52" s="5" t="s">
         <v>133</v>
       </c>
@@ -11663,7 +11666,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="120">
+    <row r="53" spans="1:3" ht="116">
       <c r="A53" s="5" t="s">
         <v>134</v>
       </c>
@@ -11674,7 +11677,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="105">
+    <row r="54" spans="1:3" ht="101.5">
       <c r="A54" s="5" t="s">
         <v>135</v>
       </c>
@@ -11682,7 +11685,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="120">
+    <row r="55" spans="1:3" ht="116">
       <c r="A55" s="5" t="s">
         <v>137</v>
       </c>
@@ -11693,7 +11696,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="120">
+    <row r="56" spans="1:3" ht="116">
       <c r="A56" s="5" t="s">
         <v>138</v>
       </c>
@@ -11701,7 +11704,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="165">
+    <row r="57" spans="1:3" ht="159.5">
       <c r="A57" s="5" t="s">
         <v>144</v>
       </c>
@@ -11712,7 +11715,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="165">
+    <row r="58" spans="1:3" ht="159.5">
       <c r="A58" s="5" t="s">
         <v>145</v>
       </c>
@@ -11720,7 +11723,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="150">
+    <row r="59" spans="1:3" ht="145">
       <c r="A59" s="5" t="s">
         <v>149</v>
       </c>
@@ -11731,7 +11734,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="165">
+    <row r="60" spans="1:3" ht="159.5">
       <c r="A60" s="5" t="s">
         <v>151</v>
       </c>
@@ -11742,7 +11745,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="180">
+    <row r="61" spans="1:3" ht="174">
       <c r="A61" s="5" t="s">
         <v>152</v>
       </c>
@@ -11753,7 +11756,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="120">
+    <row r="62" spans="1:3" ht="116">
       <c r="A62" s="5" t="s">
         <v>153</v>
       </c>
@@ -11764,7 +11767,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="45">
+    <row r="63" spans="1:3" ht="43.5">
       <c r="A63" s="5" t="s">
         <v>154</v>
       </c>
@@ -11772,7 +11775,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="135">
+    <row r="64" spans="1:3" ht="130.5">
       <c r="A64" s="5" t="s">
         <v>173</v>
       </c>
@@ -11783,7 +11786,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="135">
+    <row r="65" spans="1:3" ht="130.5">
       <c r="A65" s="5" t="s">
         <v>174</v>
       </c>
@@ -11826,7 +11829,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="150">
+    <row r="70" spans="1:3" ht="145">
       <c r="A70" s="5" t="s">
         <v>190</v>
       </c>
@@ -11837,7 +11840,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="240">
+    <row r="71" spans="1:3" ht="232">
       <c r="A71" s="5" t="s">
         <v>193</v>
       </c>
@@ -11864,7 +11867,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="30">
+    <row r="74" spans="1:3" ht="29">
       <c r="A74" s="5" t="s">
         <v>276</v>
       </c>
@@ -11872,7 +11875,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="30">
+    <row r="75" spans="1:3" ht="29">
       <c r="A75" s="5" t="s">
         <v>279</v>
       </c>
@@ -11880,7 +11883,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="30">
+    <row r="76" spans="1:3" ht="29">
       <c r="A76" s="5" t="s">
         <v>281</v>
       </c>
@@ -11888,7 +11891,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="30">
+    <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
         <v>353</v>
       </c>
@@ -11920,7 +11923,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="30">
+    <row r="81" spans="1:2" ht="29">
       <c r="A81" s="5" t="s">
         <v>358</v>
       </c>
@@ -11944,7 +11947,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="30">
+    <row r="84" spans="1:2" ht="29">
       <c r="A84" s="5" t="s">
         <v>363</v>
       </c>
@@ -11952,7 +11955,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="30">
+    <row r="85" spans="1:2">
       <c r="A85" s="5" t="s">
         <v>364</v>
       </c>
@@ -11960,7 +11963,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30">
+    <row r="86" spans="1:2" ht="29">
       <c r="A86" s="5" t="s">
         <v>365</v>
       </c>
@@ -11976,7 +11979,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="30">
+    <row r="88" spans="1:2" ht="29">
       <c r="A88" s="5" t="s">
         <v>368</v>
       </c>
@@ -11992,7 +11995,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="30">
+    <row r="90" spans="1:2" ht="29">
       <c r="A90" s="5" t="s">
         <v>381</v>
       </c>
@@ -12040,7 +12043,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="45">
+    <row r="96" spans="1:2" ht="29">
       <c r="A96" s="5" t="s">
         <v>393</v>
       </c>
@@ -12056,7 +12059,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="30">
+    <row r="98" spans="1:3" ht="29">
       <c r="A98" s="5" t="s">
         <v>397</v>
       </c>
@@ -12096,7 +12099,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="195">
+    <row r="103" spans="1:3" ht="188.5">
       <c r="A103" s="5" t="s">
         <v>406</v>
       </c>
@@ -12107,7 +12110,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="285">
+    <row r="104" spans="1:3" ht="275.5">
       <c r="A104" s="5" t="s">
         <v>407</v>
       </c>
@@ -12118,7 +12121,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="240">
+    <row r="105" spans="1:3" ht="232">
       <c r="A105" s="5" t="s">
         <v>409</v>
       </c>
@@ -12129,7 +12132,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="30">
+    <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
         <v>412</v>
       </c>
@@ -12137,7 +12140,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="45">
+    <row r="107" spans="1:3" ht="43.5">
       <c r="A107" s="5" t="s">
         <v>414</v>
       </c>
@@ -12153,7 +12156,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="120">
+    <row r="109" spans="1:3" ht="116">
       <c r="A109" s="5" t="s">
         <v>421</v>
       </c>
@@ -12336,7 +12339,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="120">
+    <row r="127" spans="1:3" ht="116">
       <c r="A127" s="5" t="s">
         <v>462</v>
       </c>
@@ -12347,7 +12350,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="120">
+    <row r="128" spans="1:3" ht="116">
       <c r="A128" s="5" t="s">
         <v>463</v>
       </c>
@@ -12366,7 +12369,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="180">
+    <row r="130" spans="1:3" ht="174">
       <c r="A130" s="5" t="s">
         <v>466</v>
       </c>
@@ -12377,7 +12380,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="150">
+    <row r="131" spans="1:3" ht="145">
       <c r="A131" s="5" t="s">
         <v>470</v>
       </c>
@@ -12388,7 +12391,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="150">
+    <row r="132" spans="1:3" ht="145">
       <c r="A132" s="5" t="s">
         <v>471</v>
       </c>
@@ -12399,7 +12402,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="135">
+    <row r="133" spans="1:3" ht="130.5">
       <c r="A133" s="5" t="s">
         <v>474</v>
       </c>
@@ -12410,7 +12413,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="135">
+    <row r="134" spans="1:3" ht="130.5">
       <c r="A134" s="5" t="s">
         <v>476</v>
       </c>
@@ -12421,7 +12424,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="135">
+    <row r="135" spans="1:3" ht="130.5">
       <c r="A135" s="5" t="s">
         <v>477</v>
       </c>
@@ -12432,7 +12435,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="135">
+    <row r="136" spans="1:3" ht="130.5">
       <c r="A136" s="5" t="s">
         <v>480</v>
       </c>
@@ -12443,7 +12446,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="135">
+    <row r="137" spans="1:3" ht="130.5">
       <c r="A137" s="5" t="s">
         <v>482</v>
       </c>
@@ -12454,7 +12457,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="135">
+    <row r="138" spans="1:3" ht="130.5">
       <c r="A138" s="5" t="s">
         <v>484</v>
       </c>
@@ -12465,7 +12468,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="135">
+    <row r="139" spans="1:3" ht="130.5">
       <c r="A139" s="5" t="s">
         <v>485</v>
       </c>
@@ -12476,7 +12479,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="135">
+    <row r="140" spans="1:3" ht="130.5">
       <c r="A140" s="5" t="s">
         <v>488</v>
       </c>
@@ -12487,7 +12490,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="135">
+    <row r="141" spans="1:3" ht="130.5">
       <c r="A141" s="5" t="s">
         <v>490</v>
       </c>
@@ -12498,7 +12501,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="135">
+    <row r="142" spans="1:3" ht="130.5">
       <c r="A142" s="5" t="s">
         <v>491</v>
       </c>
@@ -12509,7 +12512,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="120">
+    <row r="143" spans="1:3" ht="116">
       <c r="A143" s="5" t="s">
         <v>497</v>
       </c>
@@ -12520,7 +12523,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="135">
+    <row r="144" spans="1:3" ht="130.5">
       <c r="A144" s="5" t="s">
         <v>500</v>
       </c>
@@ -12531,7 +12534,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="135">
+    <row r="145" spans="1:3" ht="130.5">
       <c r="A145" s="5" t="s">
         <v>501</v>
       </c>
@@ -12542,7 +12545,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="135">
+    <row r="146" spans="1:3" ht="130.5">
       <c r="A146" s="5" t="s">
         <v>503</v>
       </c>
@@ -12553,7 +12556,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="135">
+    <row r="147" spans="1:3" ht="130.5">
       <c r="A147" s="5" t="s">
         <v>506</v>
       </c>
@@ -12564,7 +12567,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="135">
+    <row r="148" spans="1:3" ht="130.5">
       <c r="A148" s="5" t="s">
         <v>507</v>
       </c>
@@ -12619,7 +12622,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="30">
+    <row r="153" spans="1:3" ht="29">
       <c r="A153" s="5" t="s">
         <v>531</v>
       </c>
@@ -12630,7 +12633,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="30">
+    <row r="154" spans="1:3">
       <c r="A154" s="5" t="s">
         <v>532</v>
       </c>
@@ -12641,7 +12644,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="90">
+    <row r="155" spans="1:3" ht="87">
       <c r="A155" s="5" t="s">
         <v>534</v>
       </c>
@@ -12652,7 +12655,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="45">
+    <row r="156" spans="1:3" ht="43.5">
       <c r="A156" s="5" t="s">
         <v>536</v>
       </c>
@@ -12663,7 +12666,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="180">
+    <row r="157" spans="1:3" ht="174">
       <c r="A157" s="5" t="s">
         <v>540</v>
       </c>
@@ -12674,7 +12677,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="165">
+    <row r="158" spans="1:3" ht="159.5">
       <c r="A158" s="5" t="s">
         <v>541</v>
       </c>
@@ -12693,7 +12696,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="75">
+    <row r="160" spans="1:3" ht="72.5">
       <c r="A160" s="5" t="s">
         <v>547</v>
       </c>
@@ -12704,7 +12707,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="60">
+    <row r="161" spans="1:3" ht="58">
       <c r="A161" s="5" t="s">
         <v>551</v>
       </c>
@@ -12712,7 +12715,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="45">
+    <row r="162" spans="1:3" ht="43.5">
       <c r="A162" s="5" t="s">
         <v>552</v>
       </c>
@@ -12731,7 +12734,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="105">
+    <row r="164" spans="1:3" ht="101.5">
       <c r="A164" s="5" t="s">
         <v>560</v>
       </c>
@@ -12739,7 +12742,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="105">
+    <row r="165" spans="1:3" ht="101.5">
       <c r="A165" s="5" t="s">
         <v>561</v>
       </c>
@@ -12818,7 +12821,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="30">
+    <row r="173" spans="1:3">
       <c r="A173" s="5" t="s">
         <v>571</v>
       </c>
@@ -12881,7 +12884,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="30">
+    <row r="179" spans="1:3">
       <c r="A179" s="5" t="s">
         <v>577</v>
       </c>
@@ -12892,7 +12895,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="30">
+    <row r="180" spans="1:3" ht="29">
       <c r="A180" s="5" t="s">
         <v>578</v>
       </c>
@@ -12914,7 +12917,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="30">
+    <row r="182" spans="1:3">
       <c r="A182" s="5" t="s">
         <v>580</v>
       </c>
@@ -12925,7 +12928,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="120">
+    <row r="183" spans="1:3" ht="116">
       <c r="A183" s="5" t="s">
         <v>581</v>
       </c>
@@ -12980,7 +12983,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="75">
+    <row r="188" spans="1:3" ht="72.5">
       <c r="A188" s="5" t="s">
         <v>586</v>
       </c>
@@ -12991,7 +12994,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="105">
+    <row r="189" spans="1:3" ht="101.5">
       <c r="A189" s="5" t="s">
         <v>587</v>
       </c>
@@ -13002,7 +13005,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="75">
+    <row r="190" spans="1:3" ht="72.5">
       <c r="A190" s="5" t="s">
         <v>667</v>
       </c>
@@ -13013,7 +13016,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="90">
+    <row r="191" spans="1:3" ht="87">
       <c r="A191" s="5" t="s">
         <v>668</v>
       </c>
@@ -13024,7 +13027,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="90">
+    <row r="192" spans="1:3" ht="87">
       <c r="A192" s="5" t="s">
         <v>669</v>
       </c>
@@ -13079,7 +13082,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="30">
+    <row r="197" spans="1:3" ht="29">
       <c r="A197" s="5" t="s">
         <v>674</v>
       </c>
@@ -13090,7 +13093,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="30">
+    <row r="198" spans="1:3" ht="29">
       <c r="A198" s="5" t="s">
         <v>675</v>
       </c>
@@ -13112,7 +13115,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="30">
+    <row r="200" spans="1:3" ht="29">
       <c r="A200" s="5" t="s">
         <v>677</v>
       </c>
@@ -13123,7 +13126,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="90">
+    <row r="201" spans="1:3" ht="87">
       <c r="A201" s="5" t="s">
         <v>678</v>
       </c>
@@ -13134,7 +13137,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="75">
+    <row r="202" spans="1:3" ht="72.5">
       <c r="A202" s="5" t="s">
         <v>679</v>
       </c>
@@ -13145,7 +13148,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="90">
+    <row r="203" spans="1:3" ht="87">
       <c r="A203" s="5" t="s">
         <v>680</v>
       </c>
@@ -13156,7 +13159,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="30">
+    <row r="204" spans="1:3" ht="29">
       <c r="A204" s="5" t="s">
         <v>681</v>
       </c>
@@ -13175,7 +13178,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="240">
+    <row r="206" spans="1:3" ht="217.5">
       <c r="A206" s="5" t="s">
         <v>683</v>
       </c>
@@ -13197,7 +13200,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="45">
+    <row r="208" spans="1:3" ht="43.5">
       <c r="A208" s="5" t="s">
         <v>685</v>
       </c>
@@ -13208,7 +13211,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="105">
+    <row r="209" spans="1:3" ht="101.5">
       <c r="A209" s="5" t="s">
         <v>686</v>
       </c>
@@ -13252,7 +13255,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="30">
+    <row r="213" spans="1:3" ht="29">
       <c r="A213" s="5" t="s">
         <v>690</v>
       </c>
@@ -13263,7 +13266,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="75">
+    <row r="214" spans="1:3" ht="72.5">
       <c r="A214" s="5" t="s">
         <v>691</v>
       </c>
@@ -13274,7 +13277,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="90">
+    <row r="215" spans="1:3" ht="87">
       <c r="A215" s="5" t="s">
         <v>692</v>
       </c>
@@ -13285,7 +13288,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="75">
+    <row r="216" spans="1:3" ht="72.5">
       <c r="A216" s="5" t="s">
         <v>693</v>
       </c>
@@ -13296,7 +13299,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="90">
+    <row r="217" spans="1:3" ht="87">
       <c r="A217" s="5" t="s">
         <v>694</v>
       </c>
@@ -13307,7 +13310,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="240">
+    <row r="218" spans="1:3" ht="217.5">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -13329,7 +13332,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="240">
+    <row r="220" spans="1:3" ht="203">
       <c r="A220" s="5" t="s">
         <v>696</v>
       </c>
@@ -13340,7 +13343,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="180">
+    <row r="221" spans="1:3" ht="159.5">
       <c r="A221" s="5" t="s">
         <v>697</v>
       </c>
@@ -13356,7 +13359,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="105">
+    <row r="223" spans="1:3" ht="101.5">
       <c r="A223" s="5" t="s">
         <v>699</v>
       </c>
@@ -13367,7 +13370,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="105">
+    <row r="224" spans="1:3" ht="101.5">
       <c r="A224" s="5" t="s">
         <v>700</v>
       </c>
@@ -13378,7 +13381,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="105">
+    <row r="225" spans="1:3" ht="101.5">
       <c r="A225" s="5" t="s">
         <v>701</v>
       </c>
@@ -13453,7 +13456,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="105">
+    <row r="234" spans="1:3" ht="87">
       <c r="A234" s="5" t="s">
         <v>710</v>
       </c>
@@ -13472,7 +13475,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="90">
+    <row r="236" spans="1:3" ht="87">
       <c r="A236" s="5" t="s">
         <v>712</v>
       </c>
@@ -13505,7 +13508,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="135">
+    <row r="239" spans="1:3" ht="130.5">
       <c r="A239" s="5" t="s">
         <v>715</v>
       </c>
@@ -13516,7 +13519,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="30">
+    <row r="240" spans="1:3" ht="29">
       <c r="A240" s="5" t="s">
         <v>716</v>
       </c>
@@ -13538,7 +13541,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="105">
+    <row r="242" spans="1:3" ht="101.5">
       <c r="A242" s="5" t="s">
         <v>785</v>
       </c>
@@ -13549,7 +13552,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="45">
+    <row r="243" spans="1:3" ht="43.5">
       <c r="A243" s="5" t="s">
         <v>786</v>
       </c>
@@ -13560,7 +13563,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="180">
+    <row r="244" spans="1:3" ht="174">
       <c r="A244" s="5" t="s">
         <v>787</v>
       </c>
@@ -13571,7 +13574,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="225">
+    <row r="245" spans="1:3" ht="217.5">
       <c r="A245" s="5" t="s">
         <v>789</v>
       </c>
@@ -13582,7 +13585,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="180">
+    <row r="246" spans="1:3" ht="174">
       <c r="A246" s="5" t="s">
         <v>794</v>
       </c>
@@ -13593,7 +13596,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="195">
+    <row r="247" spans="1:3" ht="188.5">
       <c r="A247" s="5" t="s">
         <v>799</v>
       </c>
@@ -13604,7 +13607,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="195">
+    <row r="248" spans="1:3" ht="188.5">
       <c r="A248" s="5" t="s">
         <v>802</v>
       </c>
@@ -13615,7 +13618,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="225">
+    <row r="249" spans="1:3" ht="217.5">
       <c r="A249" s="5" t="s">
         <v>805</v>
       </c>
@@ -13626,7 +13629,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="120">
+    <row r="250" spans="1:3" ht="116">
       <c r="A250" s="5" t="s">
         <v>825</v>
       </c>
@@ -13637,7 +13640,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="150">
+    <row r="251" spans="1:3" ht="145">
       <c r="A251" s="5" t="s">
         <v>828</v>
       </c>
@@ -13648,7 +13651,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="120">
+    <row r="252" spans="1:3" ht="116">
       <c r="A252" s="5" t="s">
         <v>831</v>
       </c>
@@ -13670,7 +13673,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="30">
+    <row r="254" spans="1:3" ht="29">
       <c r="A254" s="5" t="s">
         <v>839</v>
       </c>
@@ -13681,7 +13684,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="75">
+    <row r="255" spans="1:3" ht="72.5">
       <c r="A255" s="5" t="s">
         <v>840</v>
       </c>
@@ -13692,7 +13695,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="30">
+    <row r="256" spans="1:3" ht="29">
       <c r="A256" s="5" t="s">
         <v>841</v>
       </c>
@@ -13703,7 +13706,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="75">
+    <row r="257" spans="1:3" ht="72.5">
       <c r="A257" s="5" t="s">
         <v>842</v>
       </c>
@@ -13714,7 +13717,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="150">
+    <row r="258" spans="1:3" ht="145">
       <c r="A258" s="5" t="s">
         <v>848</v>
       </c>
@@ -13736,7 +13739,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="45">
+    <row r="260" spans="1:3" ht="43.5">
       <c r="A260" s="5" t="s">
         <v>852</v>
       </c>
@@ -13747,7 +13750,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="60">
+    <row r="261" spans="1:3" ht="58">
       <c r="A261" s="5" t="s">
         <v>855</v>
       </c>
@@ -13758,7 +13761,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="90">
+    <row r="262" spans="1:3" ht="87">
       <c r="A262" s="5" t="s">
         <v>858</v>
       </c>
@@ -13777,7 +13780,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="60">
+    <row r="264" spans="1:3" ht="58">
       <c r="A264" s="5" t="s">
         <v>863</v>
       </c>
@@ -13788,7 +13791,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="90">
+    <row r="265" spans="1:3" ht="87">
       <c r="A265" s="5" t="s">
         <v>866</v>
       </c>
@@ -13799,7 +13802,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="75">
+    <row r="266" spans="1:3" ht="72.5">
       <c r="A266" s="5" t="s">
         <v>869</v>
       </c>
@@ -13834,7 +13837,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="30">
+    <row r="270" spans="1:3" ht="29">
       <c r="A270" s="5" t="s">
         <v>883</v>
       </c>
@@ -13842,7 +13845,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="120">
+    <row r="271" spans="1:3" ht="101.5">
       <c r="A271" s="5" t="s">
         <v>884</v>
       </c>
@@ -13853,7 +13856,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="45">
+    <row r="272" spans="1:3" ht="43.5">
       <c r="A272" s="5" t="s">
         <v>885</v>
       </c>
@@ -13864,7 +13867,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="30">
+    <row r="273" spans="1:4" ht="29">
       <c r="A273" s="5" t="s">
         <v>886</v>
       </c>
@@ -13875,7 +13878,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="75">
+    <row r="274" spans="1:4" ht="72.5">
       <c r="A274" s="5" t="s">
         <v>890</v>
       </c>
@@ -13902,6 +13905,9 @@
       <c r="A276" s="5" t="s">
         <v>893</v>
       </c>
+      <c r="B276" s="48" t="s">
+        <v>2650</v>
+      </c>
     </row>
     <row r="277" spans="1:4">
       <c r="A277" s="5" t="s">
@@ -14523,7 +14529,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="401" spans="1:3" ht="30">
+    <row r="401" spans="1:3" ht="29">
       <c r="A401" s="2" t="s">
         <v>1018</v>
       </c>
@@ -14534,7 +14540,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="402" spans="1:3" ht="75">
+    <row r="402" spans="1:3" ht="72.5">
       <c r="A402" s="2" t="s">
         <v>1019</v>
       </c>
@@ -14545,7 +14551,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="60">
+    <row r="403" spans="1:3" ht="58">
       <c r="A403" s="2" t="s">
         <v>1020</v>
       </c>
@@ -14556,7 +14562,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="30">
+    <row r="404" spans="1:3" ht="29">
       <c r="A404" s="2" t="s">
         <v>1021</v>
       </c>
@@ -14567,7 +14573,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="30">
+    <row r="405" spans="1:3" ht="29">
       <c r="A405" s="2" t="s">
         <v>1022</v>
       </c>
@@ -14578,7 +14584,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="60">
+    <row r="406" spans="1:3" ht="43.5">
       <c r="A406" s="2" t="s">
         <v>1023</v>
       </c>
@@ -14589,7 +14595,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="407" spans="1:3" ht="30">
+    <row r="407" spans="1:3" ht="29">
       <c r="A407" s="2" t="s">
         <v>1024</v>
       </c>
@@ -14600,7 +14606,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="135">
+    <row r="408" spans="1:3" ht="130.5">
       <c r="A408" s="2" t="s">
         <v>1025</v>
       </c>
@@ -14611,7 +14617,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="409" spans="1:3" ht="45">
+    <row r="409" spans="1:3" ht="43.5">
       <c r="A409" s="2" t="s">
         <v>1026</v>
       </c>
@@ -14622,7 +14628,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="410" spans="1:3" ht="30">
+    <row r="410" spans="1:3" ht="29">
       <c r="A410" s="2" t="s">
         <v>1027</v>
       </c>
@@ -14633,7 +14639,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="30">
+    <row r="411" spans="1:3" ht="29">
       <c r="A411" s="2" t="s">
         <v>1028</v>
       </c>
@@ -14644,7 +14650,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="165">
+    <row r="412" spans="1:3" ht="159.5">
       <c r="A412" s="2" t="s">
         <v>1029</v>
       </c>
@@ -14655,7 +14661,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="180">
+    <row r="413" spans="1:3" ht="174">
       <c r="A413" s="2" t="s">
         <v>1030</v>
       </c>
@@ -14666,7 +14672,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="75">
+    <row r="414" spans="1:3" ht="72.5">
       <c r="A414" s="2" t="s">
         <v>1031</v>
       </c>
@@ -14688,7 +14694,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="75">
+    <row r="416" spans="1:3" ht="72.5">
       <c r="A416" s="2" t="s">
         <v>1033</v>
       </c>
@@ -14699,7 +14705,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="120">
+    <row r="417" spans="1:3" ht="116">
       <c r="A417" s="2" t="s">
         <v>1034</v>
       </c>
@@ -14710,7 +14716,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="135">
+    <row r="418" spans="1:3" ht="130.5">
       <c r="A418" s="2" t="s">
         <v>1035</v>
       </c>
@@ -14721,7 +14727,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="30">
+    <row r="419" spans="1:3" ht="29">
       <c r="A419" s="2" t="s">
         <v>1036</v>
       </c>
@@ -14831,7 +14837,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="75">
+    <row r="429" spans="1:3" ht="72.5">
       <c r="A429" s="2" t="s">
         <v>1046</v>
       </c>
@@ -19403,7 +19409,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="1341" spans="1:3" ht="135">
+    <row r="1341" spans="1:3" ht="130.5">
       <c r="A1341" s="51" t="s">
         <v>1958</v>
       </c>
@@ -19436,7 +19442,7 @@
         <v>2629</v>
       </c>
     </row>
-    <row r="1344" spans="1:3" ht="135">
+    <row r="1344" spans="1:3" ht="130.5">
       <c r="A1344" s="5" t="s">
         <v>1961</v>
       </c>
@@ -19447,7 +19453,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="1345" spans="1:3" ht="30">
+    <row r="1345" spans="1:3" ht="29">
       <c r="A1345" s="5" t="s">
         <v>1962</v>
       </c>
@@ -20238,7 +20244,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="1502" spans="1:3" ht="90">
+    <row r="1502" spans="1:3" ht="87">
       <c r="A1502" s="5" t="s">
         <v>2119</v>
       </c>
@@ -20249,7 +20255,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="1503" spans="1:3" ht="90">
+    <row r="1503" spans="1:3" ht="87">
       <c r="A1503" s="5" t="s">
         <v>2120</v>
       </c>
@@ -20260,7 +20266,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="1504" spans="1:3" ht="150">
+    <row r="1504" spans="1:3" ht="145">
       <c r="A1504" s="5" t="s">
         <v>2121</v>
       </c>
@@ -20271,7 +20277,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="1505" spans="1:3" ht="150">
+    <row r="1505" spans="1:3" ht="145">
       <c r="A1505" s="5" t="s">
         <v>2122</v>
       </c>
@@ -20282,7 +20288,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="1506" spans="1:3" ht="75">
+    <row r="1506" spans="1:3" ht="72.5">
       <c r="A1506" s="5" t="s">
         <v>2123</v>
       </c>
@@ -20290,7 +20296,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="1507" spans="1:3" ht="45">
+    <row r="1507" spans="1:3" ht="43.5">
       <c r="A1507" s="47" t="s">
         <v>2124</v>
       </c>
@@ -20301,7 +20307,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1508" spans="1:3" ht="45">
+    <row r="1508" spans="1:3" ht="43.5">
       <c r="A1508" s="44" t="s">
         <v>2125</v>
       </c>
@@ -20312,7 +20318,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1509" spans="1:3" ht="225">
+    <row r="1509" spans="1:3" ht="217.5">
       <c r="A1509" s="5" t="s">
         <v>2126</v>
       </c>
@@ -20795,7 +20801,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="1602" spans="1:3" ht="30">
+    <row r="1602" spans="1:3" ht="29">
       <c r="A1602" s="5" t="s">
         <v>2219</v>
       </c>
@@ -20817,7 +20823,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="1604" spans="1:3" ht="60">
+    <row r="1604" spans="1:3" ht="58">
       <c r="A1604" s="5" t="s">
         <v>2221</v>
       </c>
@@ -20828,7 +20834,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="1605" spans="1:3" ht="45">
+    <row r="1605" spans="1:3" ht="43.5">
       <c r="A1605" s="5" t="s">
         <v>2222</v>
       </c>
@@ -20836,7 +20842,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="1606" spans="1:3" ht="105">
+    <row r="1606" spans="1:3" ht="101.5">
       <c r="A1606" s="5" t="s">
         <v>2223</v>
       </c>
@@ -20866,7 +20872,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="1609" spans="1:3" ht="45">
+    <row r="1609" spans="1:3" ht="43.5">
       <c r="A1609" s="5" t="s">
         <v>2278</v>
       </c>
@@ -20877,7 +20883,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="1610" spans="1:3" ht="30">
+    <row r="1610" spans="1:3" ht="29">
       <c r="A1610" s="5" t="s">
         <v>2279</v>
       </c>
@@ -20885,7 +20891,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="1611" spans="1:3" ht="409.5">
+    <row r="1611" spans="1:3" ht="391.5">
       <c r="A1611" s="5" t="s">
         <v>2280</v>
       </c>
@@ -20896,7 +20902,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="1612" spans="1:3" ht="240">
+    <row r="1612" spans="1:3" ht="232">
       <c r="A1612" s="44" t="s">
         <v>2281</v>
       </c>
@@ -20907,7 +20913,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="1613" spans="1:3" ht="30">
+    <row r="1613" spans="1:3">
       <c r="A1613" s="44" t="s">
         <v>2337</v>
       </c>
@@ -20940,7 +20946,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="1616" spans="1:3" ht="90">
+    <row r="1616" spans="1:3" ht="87">
       <c r="A1616" s="47" t="s">
         <v>2340</v>
       </c>
@@ -20951,7 +20957,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="1617" spans="1:3" ht="30">
+    <row r="1617" spans="1:3" ht="29">
       <c r="A1617" s="47" t="s">
         <v>2341</v>
       </c>
@@ -22383,7 +22389,7 @@
       </c>
       <c r="B1901" s="48"/>
     </row>
-    <row r="1902" spans="1:3" ht="45">
+    <row r="1902" spans="1:3" ht="43.5">
       <c r="A1902">
         <v>1901</v>
       </c>
@@ -22394,7 +22400,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="1903" spans="1:3" ht="90">
+    <row r="1903" spans="1:3" ht="87">
       <c r="A1903">
         <v>1902</v>
       </c>
@@ -22405,7 +22411,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="1904" spans="1:3" ht="225">
+    <row r="1904" spans="1:3" ht="217.5">
       <c r="A1904">
         <v>1903</v>
       </c>
@@ -22416,7 +22422,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="1905" spans="1:3" ht="150">
+    <row r="1905" spans="1:3" ht="145">
       <c r="A1905">
         <v>1904</v>
       </c>
@@ -22427,7 +22433,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="1906" spans="1:3" ht="150">
+    <row r="1906" spans="1:3" ht="145">
       <c r="A1906">
         <v>1905</v>
       </c>
@@ -22438,7 +22444,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="1907" spans="1:3" ht="120">
+    <row r="1907" spans="1:3" ht="116">
       <c r="A1907">
         <v>1906</v>
       </c>
@@ -22449,7 +22455,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="1908" spans="1:3" ht="150">
+    <row r="1908" spans="1:3" ht="145">
       <c r="A1908">
         <v>1907</v>
       </c>
@@ -22460,7 +22466,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="1909" spans="1:3" ht="150">
+    <row r="1909" spans="1:3" ht="145">
       <c r="A1909">
         <v>1908</v>
       </c>
@@ -22471,7 +22477,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="1910" spans="1:3" ht="105">
+    <row r="1910" spans="1:3" ht="101.5">
       <c r="A1910">
         <v>1909</v>
       </c>
@@ -22519,13 +22525,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -22705,10 +22711,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -23031,7 +23037,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" ht="16">
       <c r="A44" s="13" t="s">
         <v>263</v>
       </c>
@@ -23121,13 +23127,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="85.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+    <row r="1" spans="1:2" ht="15" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>283</v>
       </c>
@@ -23135,7 +23141,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+    <row r="2" spans="1:2" ht="15" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>285</v>
       </c>
@@ -23143,7 +23149,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+    <row r="3" spans="1:2" ht="15" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>287</v>
       </c>
@@ -23151,7 +23157,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+    <row r="4" spans="1:2" ht="15" thickBot="1">
       <c r="A4" s="25" t="s">
         <v>289</v>
       </c>
@@ -23159,7 +23165,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+    <row r="5" spans="1:2" ht="15" thickBot="1">
       <c r="A5" s="25" t="s">
         <v>291</v>
       </c>
@@ -23167,7 +23173,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+    <row r="6" spans="1:2" ht="15" thickBot="1">
       <c r="A6" s="25" t="s">
         <v>293</v>
       </c>
@@ -23175,7 +23181,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1">
+    <row r="7" spans="1:2" ht="15" thickBot="1">
       <c r="A7" s="25" t="s">
         <v>295</v>
       </c>
@@ -23183,7 +23189,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+    <row r="8" spans="1:2" ht="15" thickBot="1">
       <c r="A8" s="25" t="s">
         <v>297</v>
       </c>
@@ -23191,7 +23197,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1">
+    <row r="9" spans="1:2" ht="15" thickBot="1">
       <c r="A9" s="25" t="s">
         <v>299</v>
       </c>
@@ -23199,7 +23205,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1">
+    <row r="10" spans="1:2" ht="15" thickBot="1">
       <c r="A10" s="25" t="s">
         <v>301</v>
       </c>
@@ -23207,7 +23213,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1">
+    <row r="11" spans="1:2" ht="15" thickBot="1">
       <c r="A11" s="25" t="s">
         <v>303</v>
       </c>
@@ -23215,7 +23221,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+    <row r="12" spans="1:2" ht="15" thickBot="1">
       <c r="A12" s="25" t="s">
         <v>305</v>
       </c>
@@ -23223,7 +23229,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1">
+    <row r="13" spans="1:2" ht="15" thickBot="1">
       <c r="A13" s="25" t="s">
         <v>307</v>
       </c>
@@ -23231,7 +23237,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1">
+    <row r="14" spans="1:2" ht="15" thickBot="1">
       <c r="A14" s="25" t="s">
         <v>309</v>
       </c>
@@ -23239,7 +23245,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1">
+    <row r="15" spans="1:2" ht="15" thickBot="1">
       <c r="A15" s="25" t="s">
         <v>311</v>
       </c>
@@ -23247,7 +23253,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1">
+    <row r="16" spans="1:2" ht="15" thickBot="1">
       <c r="A16" s="25" t="s">
         <v>313</v>
       </c>
@@ -23255,7 +23261,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1">
+    <row r="17" spans="1:2" ht="15" thickBot="1">
       <c r="A17" s="25" t="s">
         <v>315</v>
       </c>
@@ -23263,7 +23269,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1">
+    <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="25" t="s">
         <v>317</v>
       </c>
@@ -23271,7 +23277,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1">
+    <row r="19" spans="1:2" ht="15" thickBot="1">
       <c r="A19" s="25" t="s">
         <v>319</v>
       </c>
@@ -23279,7 +23285,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1">
+    <row r="20" spans="1:2" ht="15" thickBot="1">
       <c r="A20" s="25" t="s">
         <v>321</v>
       </c>
@@ -23287,7 +23293,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1">
+    <row r="21" spans="1:2" ht="15" thickBot="1">
       <c r="A21" s="25" t="s">
         <v>323</v>
       </c>
@@ -23295,7 +23301,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1">
+    <row r="22" spans="1:2" ht="15" thickBot="1">
       <c r="A22" s="25" t="s">
         <v>325</v>
       </c>
@@ -23303,7 +23309,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1">
+    <row r="23" spans="1:2" ht="15" thickBot="1">
       <c r="A23" s="25" t="s">
         <v>327</v>
       </c>
@@ -23311,7 +23317,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1">
+    <row r="24" spans="1:2" ht="15" thickBot="1">
       <c r="A24" s="25" t="s">
         <v>329</v>
       </c>
@@ -23319,7 +23325,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1">
+    <row r="25" spans="1:2" ht="15" thickBot="1">
       <c r="A25" s="25" t="s">
         <v>331</v>
       </c>
@@ -23327,7 +23333,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1">
+    <row r="26" spans="1:2" ht="15" thickBot="1">
       <c r="A26" s="25" t="s">
         <v>333</v>
       </c>
@@ -23335,7 +23341,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1">
+    <row r="27" spans="1:2" ht="15" thickBot="1">
       <c r="A27" s="25" t="s">
         <v>335</v>
       </c>
@@ -23343,7 +23349,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1">
+    <row r="28" spans="1:2" ht="15" thickBot="1">
       <c r="A28" s="25" t="s">
         <v>337</v>
       </c>
@@ -23351,7 +23357,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1">
+    <row r="29" spans="1:2" ht="15" thickBot="1">
       <c r="A29" s="25" t="s">
         <v>339</v>
       </c>
@@ -23359,7 +23365,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1">
+    <row r="30" spans="1:2" ht="15" thickBot="1">
       <c r="A30" s="25" t="s">
         <v>341</v>
       </c>
@@ -23367,7 +23373,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1">
+    <row r="31" spans="1:2" ht="15" thickBot="1">
       <c r="A31" s="25" t="s">
         <v>343</v>
       </c>
@@ -23375,7 +23381,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1">
+    <row r="32" spans="1:2" ht="15" thickBot="1">
       <c r="A32" s="25" t="s">
         <v>345</v>
       </c>
@@ -23383,7 +23389,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1">
+    <row r="33" spans="1:2" ht="15" thickBot="1">
       <c r="A33" s="25" t="s">
         <v>347</v>
       </c>
@@ -23391,7 +23397,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1">
+    <row r="34" spans="1:2" ht="15" thickBot="1">
       <c r="A34" s="25" t="s">
         <v>349</v>
       </c>
@@ -23399,7 +23405,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1">
+    <row r="35" spans="1:2" ht="15" thickBot="1">
       <c r="A35" s="25" t="s">
         <v>351</v>
       </c>

</xml_diff>

<commit_message>
Updating New User for STG1
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFiles/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFiles/DataFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdassani\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tathyush\Desktop\Team Members Autmation\Master Manage Users\CucumberFramework\Online-Portals\UPA\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D68645-20B4-4E64-9622-F15128A1A353}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A8F7A0-2764-4794-A549-86C656B3669C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="2650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2864" uniqueCount="2659">
   <si>
     <t>City</t>
   </si>
@@ -8376,18 +8376,6 @@
 on ps.PROV_TIN_NBR=ep.PROV_TIN_NBR join ole.PRODUCT_CONFIGURATION pc on pc.GROUP_NM=ps.PRTL_PRDCT_SELECTED_GRP_NM
 where ps.PRTL_PRDCT_SELECTED_GRP_NM='{$prdctSelected}' and ps.PRTL_PRDCT_SELECTED_STS_CD='A'
 and ep.PAY_METH_TYP_CD='{$tinType}' and pc.MINOR_CAT='USERS_MAX' and ep.ENRL_STS_CD='A'
-and  cast(pc.value as int) &gt; (SELECT count(pu.FST_NM)
-FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_TIN pt ON  pt.PORTAL_USER_ID = pu.PORTAL_USER_ID 
-WHERE pu.STS_CD in ('A','PR','P') and pt.PROV_TIN_NBR=ep.PROV_TIN_NBR )
-order by ps.LST_CHG_BY_DTTM desc
-fetch first row only</t>
-  </si>
-  <si>
-    <t>select ps.PROV_TIN_NBR as PROV_TAX_ID_NBR from
-ole.product_selection ps join ole.enrolled_provider ep
-on ps.PROV_TIN_NBR=ep.PROV_TIN_NBR join ole.PRODUCT_CONFIGURATION pc on pc.GROUP_NM=ps.PRTL_PRDCT_SELECTED_GRP_NM
-where ps.PRTL_PRDCT_SELECTED_GRP_NM='{$prdctSelected}' and ps.PRTL_PRDCT_SELECTED_STS_CD='A'
-and ep.PAY_METH_TYP_CD='{$tinType}' and pc.MINOR_CAT='USERS_MAX' and ep.ENRL_STS_CD='A'
 and  cast(pc.value as int) &lt; (SELECT count(pu.FST_NM)
 FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_TIN pt ON  pt.PORTAL_USER_ID = pu.PORTAL_USER_ID 
 WHERE pu.STS_CD in ('A','PR','P') and pt.PROV_TIN_NBR=ep.PROV_TIN_NBR )
@@ -9866,6 +9854,46 @@
   </si>
   <si>
     <t>select PAY_PROC_ACPT_CD_VAL_DESC from OLE.PAY_PROC_VAL where PAY_PROC_CD = '{$pay_proc_cd}'</t>
+  </si>
+  <si>
+    <t>select ps.PROV_TIN_NBR as PROV_TAX_ID_NBR from
+ole.product_selection ps join ole.enrolled_provider ep
+on ps.PROV_TIN_NBR=ep.PROV_TIN_NBR join ole.PRODUCT_CONFIGURATION pc on pc.GROUP_NM=ps.PRTL_PRDCT_SELECTED_GRP_NM
+where ps.PRTL_PRDCT_SELECTED_GRP_NM='{$prdctSelected}' and ps.PRTL_PRDCT_SELECTED_STS_CD='A'
+and ep.PAY_METH_TYP_CD='{$tinType}' and pc.MINOR_CAT='USERS_MAX' and ep.ENRL_STS_CD='A'
+--and  cast(pc.value as int) &gt; (SELECT count(pu.FST_NM)
+---FROM OLE.PORTAL_USER pu JOIN OLE.PORTAL_USER_TIN pt ON  pt.PORTAL_USER_ID = pu.PORTAL_USER_ID 
+---WHERE pu.STS_CD in ('A','PR','P') and pt.PROV_TIN_NBR=ep.PROV_TIN_NBR )
+order by ps.LST_CHG_BY_DTTM desc
+fetch first row only</t>
+  </si>
+  <si>
+    <t>1920</t>
+  </si>
+  <si>
+    <t>SELECT * FROM OLE.PORTAL_USER WHERE EMAIL_ADR_TXT = '{$email}'</t>
+  </si>
+  <si>
+    <t>get infor based on email address</t>
+  </si>
+  <si>
+    <t>1921</t>
+  </si>
+  <si>
+    <t>DELETE FROM OLE.PORTAL_USER_TIN WHERE PORTAL_USER_ID = '{$portal_user_id}'</t>
+  </si>
+  <si>
+    <t>1922</t>
+  </si>
+  <si>
+    <t>DELETE FROM OLE.PORTAL_USER WHERE PORTAL_USER_ID = '{$portal_user_id}'</t>
+  </si>
+  <si>
+    <t>1923</t>
+  </si>
+  <si>
+    <t>SELECT * FROM OLE.BILLING_SERVICE_PROVIDER WHERE BILLING_SERVICE_ID IN (SELECT BILLING_SERVICE_ID FROM OLE.BILLING_SERVICE WHERE BILLING_SERVICE_ID IN (SELECT BILLING_SERVICE_ID FROM OLE.PORTAL_USER_BS_TIN 
+  WHERE PORTAL_USER_ID IN (SELECT PORTAL_USER_ID FROM OLE.PORTAL_USER WHERE EMAIL_ADR_TXT = '{$emailadr}')))</t>
   </si>
 </sst>
 </file>
@@ -10663,16 +10691,16 @@
         <v>41</v>
       </c>
       <c r="J1" s="36" t="s">
+        <v>2238</v>
+      </c>
+      <c r="K1" s="36" t="s">
         <v>2239</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>2240</v>
       </c>
-      <c r="L1" s="36" t="s">
-        <v>2241</v>
-      </c>
       <c r="M1" s="38" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -10707,13 +10735,13 @@
         <v>8</v>
       </c>
       <c r="K2" s="39" t="s">
+        <v>2241</v>
+      </c>
+      <c r="L2" s="39" t="s">
         <v>2242</v>
       </c>
-      <c r="L2" s="39" t="s">
-        <v>2243</v>
-      </c>
       <c r="M2" t="s">
-        <v>2258</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -10740,13 +10768,13 @@
       </c>
       <c r="H3" s="9"/>
       <c r="J3" s="37" t="s">
+        <v>2243</v>
+      </c>
+      <c r="K3" s="39" t="s">
         <v>2244</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="L3" s="39" t="s">
         <v>2245</v>
-      </c>
-      <c r="L3" s="39" t="s">
-        <v>2246</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -10778,13 +10806,13 @@
         <v>14</v>
       </c>
       <c r="J4" s="37" t="s">
+        <v>2246</v>
+      </c>
+      <c r="K4" s="39" t="s">
         <v>2247</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="L4" s="39" t="s">
         <v>2248</v>
-      </c>
-      <c r="L4" s="39" t="s">
-        <v>2249</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -10816,7 +10844,7 @@
         <v>11</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
       <c r="K5" s="40"/>
       <c r="L5" s="40"/>
@@ -10847,13 +10875,13 @@
         <v>29</v>
       </c>
       <c r="J6" s="37" t="s">
+        <v>2250</v>
+      </c>
+      <c r="K6" s="39" t="s">
         <v>2251</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="L6" s="39" t="s">
         <v>2252</v>
-      </c>
-      <c r="L6" s="39" t="s">
-        <v>2253</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -10882,7 +10910,7 @@
         <v>29</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
@@ -10913,7 +10941,7 @@
         <v>29</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
@@ -10944,7 +10972,7 @@
         <v>29</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
@@ -11145,7 +11173,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
       <c r="F17" s="37" t="s">
         <v>616</v>
@@ -11165,10 +11193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1912"/>
+  <dimension ref="A1:D1930"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1082" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1112" sqref="B1112"/>
+    <sheetView tabSelected="1" topLeftCell="A1910" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1923" sqref="B1923"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11379,10 +11407,10 @@
         <v>88</v>
       </c>
       <c r="B24" s="27" t="s">
+        <v>2230</v>
+      </c>
+      <c r="C24" t="s">
         <v>2231</v>
-      </c>
-      <c r="C24" t="s">
-        <v>2232</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="75">
@@ -13869,10 +13897,10 @@
         <v>886</v>
       </c>
       <c r="B273" s="33" t="s">
+        <v>2232</v>
+      </c>
+      <c r="C273" s="34" t="s">
         <v>2233</v>
-      </c>
-      <c r="C273" s="34" t="s">
-        <v>2234</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="75">
@@ -13880,11 +13908,11 @@
         <v>890</v>
       </c>
       <c r="B274" s="33" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="C274" s="34"/>
       <c r="D274" s="34" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -13892,10 +13920,10 @@
         <v>892</v>
       </c>
       <c r="B275" s="35" t="s">
+        <v>2235</v>
+      </c>
+      <c r="C275" s="34" t="s">
         <v>2236</v>
-      </c>
-      <c r="C275" s="34" t="s">
-        <v>2237</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -14528,10 +14556,10 @@
         <v>1018</v>
       </c>
       <c r="B401" s="48" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="C401" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="402" spans="1:3" ht="75">
@@ -14539,10 +14567,10 @@
         <v>1019</v>
       </c>
       <c r="B402" s="48" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="C402" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="60">
@@ -14550,10 +14578,10 @@
         <v>1020</v>
       </c>
       <c r="B403" s="48" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="C403" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="30">
@@ -14561,10 +14589,10 @@
         <v>1021</v>
       </c>
       <c r="B404" s="48" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="C404" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="30">
@@ -14572,10 +14600,10 @@
         <v>1022</v>
       </c>
       <c r="B405" s="48" t="s">
-        <v>2289</v>
+        <v>2288</v>
       </c>
       <c r="C405" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="406" spans="1:3" ht="60">
@@ -14583,10 +14611,10 @@
         <v>1023</v>
       </c>
       <c r="B406" s="48" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="C406" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="30">
@@ -14594,10 +14622,10 @@
         <v>1024</v>
       </c>
       <c r="B407" s="48" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="C407" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="135">
@@ -14605,10 +14633,10 @@
         <v>1025</v>
       </c>
       <c r="B408" s="48" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
       <c r="C408" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="45">
@@ -14616,10 +14644,10 @@
         <v>1026</v>
       </c>
       <c r="B409" s="48" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="C409" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="410" spans="1:3" ht="30">
@@ -14627,10 +14655,10 @@
         <v>1027</v>
       </c>
       <c r="B410" s="27" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="C410" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="30">
@@ -14638,10 +14666,10 @@
         <v>1028</v>
       </c>
       <c r="B411" s="27" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="C411" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="165">
@@ -14649,10 +14677,10 @@
         <v>1029</v>
       </c>
       <c r="B412" s="27" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="C412" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="180">
@@ -14660,10 +14688,10 @@
         <v>1030</v>
       </c>
       <c r="B413" s="27" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="C413" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="75">
@@ -14671,10 +14699,10 @@
         <v>1031</v>
       </c>
       <c r="B414" s="27" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="C414" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="415" spans="1:3">
@@ -14682,10 +14710,10 @@
         <v>1032</v>
       </c>
       <c r="B415" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="C415" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="75">
@@ -14693,10 +14721,10 @@
         <v>1033</v>
       </c>
       <c r="B416" s="48" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="C416" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="120">
@@ -14704,10 +14732,10 @@
         <v>1034</v>
       </c>
       <c r="B417" s="48" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
       <c r="C417" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="418" spans="1:3" ht="135">
@@ -14715,10 +14743,10 @@
         <v>1035</v>
       </c>
       <c r="B418" s="48" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="C418" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="30">
@@ -14726,10 +14754,10 @@
         <v>1036</v>
       </c>
       <c r="B419" s="48" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="C419" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="420" spans="1:3">
@@ -14737,10 +14765,10 @@
         <v>1037</v>
       </c>
       <c r="B420" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="C420" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="421" spans="1:3">
@@ -14748,10 +14776,10 @@
         <v>1038</v>
       </c>
       <c r="B421" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="C421" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="422" spans="1:3">
@@ -14759,10 +14787,10 @@
         <v>1039</v>
       </c>
       <c r="B422" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="C422" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="423" spans="1:3">
@@ -14770,10 +14798,10 @@
         <v>1040</v>
       </c>
       <c r="B423" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="C423" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="424" spans="1:3">
@@ -14781,10 +14809,10 @@
         <v>1041</v>
       </c>
       <c r="B424" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="C424" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="425" spans="1:3">
@@ -14792,10 +14820,10 @@
         <v>1042</v>
       </c>
       <c r="B425" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="C425" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="426" spans="1:3">
@@ -14803,10 +14831,10 @@
         <v>1043</v>
       </c>
       <c r="B426" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="C426" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="427" spans="1:3">
@@ -14814,10 +14842,10 @@
         <v>1044</v>
       </c>
       <c r="B427" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="C427" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="428" spans="1:3">
@@ -14825,10 +14853,10 @@
         <v>1045</v>
       </c>
       <c r="B428" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="C428" s="49" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="75">
@@ -14836,10 +14864,10 @@
         <v>1046</v>
       </c>
       <c r="B429" s="48" t="s">
+        <v>2312</v>
+      </c>
+      <c r="C429" s="49" t="s">
         <v>2313</v>
-      </c>
-      <c r="C429" s="49" t="s">
-        <v>2314</v>
       </c>
     </row>
     <row r="430" spans="1:3">
@@ -18257,10 +18285,10 @@
         <v>1729</v>
       </c>
       <c r="B1112" s="55" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="C1112" s="55" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="1113" spans="1:3">
@@ -19408,10 +19436,10 @@
         <v>1958</v>
       </c>
       <c r="B1341" s="52" t="s">
+        <v>2627</v>
+      </c>
+      <c r="C1341" s="53" t="s">
         <v>2628</v>
-      </c>
-      <c r="C1341" s="53" t="s">
-        <v>2629</v>
       </c>
     </row>
     <row r="1342" spans="1:3">
@@ -19419,10 +19447,10 @@
         <v>1959</v>
       </c>
       <c r="B1342" s="53" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="C1342" s="53" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="1343" spans="1:3">
@@ -19430,10 +19458,10 @@
         <v>1960</v>
       </c>
       <c r="B1343" s="53" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="C1343" s="53" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="1344" spans="1:3" ht="135">
@@ -19441,10 +19469,10 @@
         <v>1961</v>
       </c>
       <c r="B1344" s="52" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="C1344" s="52" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="1345" spans="1:3" ht="30">
@@ -19452,10 +19480,10 @@
         <v>1962</v>
       </c>
       <c r="B1345" s="52" t="s">
+        <v>2644</v>
+      </c>
+      <c r="C1345" s="52" t="s">
         <v>2645</v>
-      </c>
-      <c r="C1345" s="52" t="s">
-        <v>2646</v>
       </c>
     </row>
     <row r="1346" spans="1:3">
@@ -20265,10 +20293,10 @@
         <v>2121</v>
       </c>
       <c r="B1504" s="7" t="s">
-        <v>2227</v>
+        <v>2649</v>
       </c>
       <c r="C1504" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="1505" spans="1:3" ht="150">
@@ -20276,10 +20304,10 @@
         <v>2122</v>
       </c>
       <c r="B1505" s="7" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="C1505" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="1506" spans="1:3" ht="75">
@@ -20295,10 +20323,10 @@
         <v>2124</v>
       </c>
       <c r="B1507" s="48" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
       <c r="C1507" s="46" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="1508" spans="1:3" ht="45">
@@ -20306,10 +20334,10 @@
         <v>2125</v>
       </c>
       <c r="B1508" s="45" t="s">
+        <v>2281</v>
+      </c>
+      <c r="C1508" s="46" t="s">
         <v>2282</v>
-      </c>
-      <c r="C1508" s="46" t="s">
-        <v>2283</v>
       </c>
     </row>
     <row r="1509" spans="1:3" ht="225">
@@ -20317,10 +20345,10 @@
         <v>2126</v>
       </c>
       <c r="B1509" s="48" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="C1509" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="1510" spans="1:3">
@@ -20328,10 +20356,10 @@
         <v>2127</v>
       </c>
       <c r="B1510" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="C1510" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="1511" spans="1:3">
@@ -20339,10 +20367,10 @@
         <v>2128</v>
       </c>
       <c r="B1511" t="s">
+        <v>2640</v>
+      </c>
+      <c r="C1511" t="s">
         <v>2641</v>
-      </c>
-      <c r="C1511" t="s">
-        <v>2642</v>
       </c>
     </row>
     <row r="1512" spans="1:3">
@@ -20800,10 +20828,10 @@
         <v>2219</v>
       </c>
       <c r="B1602" s="7" t="s">
+        <v>2258</v>
+      </c>
+      <c r="C1602" t="s">
         <v>2259</v>
-      </c>
-      <c r="C1602" t="s">
-        <v>2260</v>
       </c>
     </row>
     <row r="1603" spans="1:3">
@@ -20811,10 +20839,10 @@
         <v>2220</v>
       </c>
       <c r="B1603" s="7" t="s">
+        <v>2260</v>
+      </c>
+      <c r="C1603" t="s">
         <v>2261</v>
-      </c>
-      <c r="C1603" t="s">
-        <v>2262</v>
       </c>
     </row>
     <row r="1604" spans="1:3" ht="60">
@@ -20822,10 +20850,10 @@
         <v>2221</v>
       </c>
       <c r="B1604" s="7" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C1604" t="s">
         <v>2263</v>
-      </c>
-      <c r="C1604" t="s">
-        <v>2264</v>
       </c>
     </row>
     <row r="1605" spans="1:3" ht="45">
@@ -20833,7 +20861,7 @@
         <v>2222</v>
       </c>
       <c r="B1605" s="7" t="s">
-        <v>2265</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="1606" spans="1:3" ht="105">
@@ -20841,1545 +20869,1545 @@
         <v>2223</v>
       </c>
       <c r="B1606" s="7" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="C1606" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="1607" spans="1:3">
       <c r="A1607" s="43" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
       <c r="B1607" t="s">
+        <v>2266</v>
+      </c>
+      <c r="C1607" t="s">
         <v>2267</v>
-      </c>
-      <c r="C1607" t="s">
-        <v>2268</v>
       </c>
     </row>
     <row r="1608" spans="1:3">
       <c r="A1608" s="5" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
       <c r="B1608" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="1609" spans="1:3" ht="45">
       <c r="A1609" s="5" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
       <c r="B1609" s="7" t="s">
+        <v>2269</v>
+      </c>
+      <c r="C1609" t="s">
         <v>2270</v>
-      </c>
-      <c r="C1609" t="s">
-        <v>2271</v>
       </c>
     </row>
     <row r="1610" spans="1:3" ht="30">
       <c r="A1610" s="5" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
       <c r="B1610" s="7" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="1611" spans="1:3" ht="409.5">
       <c r="A1611" s="5" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="B1611" s="7" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
       <c r="C1611" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="1612" spans="1:3" ht="240">
       <c r="A1612" s="44" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="B1612" s="45" t="s">
+        <v>2284</v>
+      </c>
+      <c r="C1612" s="46" t="s">
         <v>2285</v>
-      </c>
-      <c r="C1612" s="46" t="s">
-        <v>2286</v>
       </c>
     </row>
     <row r="1613" spans="1:3" ht="30">
       <c r="A1613" s="44" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="B1613" s="48" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="C1613" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="1614" spans="1:3">
       <c r="A1614" s="47" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="B1614" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="C1614" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="1615" spans="1:3">
       <c r="A1615" s="47" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="B1615" s="48" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="C1615" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="1616" spans="1:3" ht="90">
       <c r="A1616" s="47" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="B1616" s="48" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="C1616" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="1617" spans="1:3" ht="30">
       <c r="A1617" s="47" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="B1617" s="48" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="C1617" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="1618" spans="1:3">
       <c r="A1618" s="50" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="1619" spans="1:3">
       <c r="A1619" s="50" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="1620" spans="1:3">
       <c r="A1620" s="50" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="1621" spans="1:3">
       <c r="A1621" s="50" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="1622" spans="1:3">
       <c r="A1622" s="50" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="1623" spans="1:3">
       <c r="A1623" s="50" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="1624" spans="1:3">
       <c r="A1624" s="50" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="1625" spans="1:3">
       <c r="A1625" s="50" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="1626" spans="1:3">
       <c r="A1626" s="50" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="1627" spans="1:3">
       <c r="A1627" s="50" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="1628" spans="1:3">
       <c r="A1628" s="50" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="1629" spans="1:3">
       <c r="A1629" s="50" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="1630" spans="1:3">
       <c r="A1630" s="50" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="1631" spans="1:3">
       <c r="A1631" s="50" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="1632" spans="1:3">
       <c r="A1632" s="50" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="1633" spans="1:1">
       <c r="A1633" s="50" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="1634" spans="1:1">
       <c r="A1634" s="50" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="1635" spans="1:1">
       <c r="A1635" s="50" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="1636" spans="1:1">
       <c r="A1636" s="50" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="1637" spans="1:1">
       <c r="A1637" s="50" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="1638" spans="1:1">
       <c r="A1638" s="50" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="1639" spans="1:1">
       <c r="A1639" s="50" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="1640" spans="1:1">
       <c r="A1640" s="50" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="1641" spans="1:1">
       <c r="A1641" s="50" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="1642" spans="1:1">
       <c r="A1642" s="50" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="1643" spans="1:1">
       <c r="A1643" s="50" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="1644" spans="1:1">
       <c r="A1644" s="50" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="1645" spans="1:1">
       <c r="A1645" s="50" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="1646" spans="1:1">
       <c r="A1646" s="50" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="1647" spans="1:1">
       <c r="A1647" s="50" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="1648" spans="1:1">
       <c r="A1648" s="50" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="1649" spans="1:1">
       <c r="A1649" s="50" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="1650" spans="1:1">
       <c r="A1650" s="50" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="1651" spans="1:1">
       <c r="A1651" s="50" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="1652" spans="1:1">
       <c r="A1652" s="50" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="1653" spans="1:1">
       <c r="A1653" s="50" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="1654" spans="1:1">
       <c r="A1654" s="50" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="1655" spans="1:1">
       <c r="A1655" s="50" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="1656" spans="1:1">
       <c r="A1656" s="50" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="1657" spans="1:1">
       <c r="A1657" s="50" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="1658" spans="1:1">
       <c r="A1658" s="50" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="1659" spans="1:1">
       <c r="A1659" s="50" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="1660" spans="1:1">
       <c r="A1660" s="50" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="1661" spans="1:1">
       <c r="A1661" s="50" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="1662" spans="1:1">
       <c r="A1662" s="50" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="1663" spans="1:1">
       <c r="A1663" s="50" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="1664" spans="1:1">
       <c r="A1664" s="50" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="1665" spans="1:1">
       <c r="A1665" s="50" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="1666" spans="1:1">
       <c r="A1666" s="50" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="1667" spans="1:1">
       <c r="A1667" s="50" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="1668" spans="1:1">
       <c r="A1668" s="50" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="1669" spans="1:1">
       <c r="A1669" s="50" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="1670" spans="1:1">
       <c r="A1670" s="50" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="1671" spans="1:1">
       <c r="A1671" s="50" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="1672" spans="1:1">
       <c r="A1672" s="50" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="1673" spans="1:1">
       <c r="A1673" s="50" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="1674" spans="1:1">
       <c r="A1674" s="50" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="1675" spans="1:1">
       <c r="A1675" s="50" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
     </row>
     <row r="1676" spans="1:1">
       <c r="A1676" s="50" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="1677" spans="1:1">
       <c r="A1677" s="50" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="1678" spans="1:1">
       <c r="A1678" s="50" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="1679" spans="1:1">
       <c r="A1679" s="50" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="1680" spans="1:1">
       <c r="A1680" s="50" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="1681" spans="1:1">
       <c r="A1681" s="50" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="1682" spans="1:1">
       <c r="A1682" s="50" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="1683" spans="1:1">
       <c r="A1683" s="50" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="1684" spans="1:1">
       <c r="A1684" s="50" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="1685" spans="1:1">
       <c r="A1685" s="50" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="1686" spans="1:1">
       <c r="A1686" s="50" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="1687" spans="1:1">
       <c r="A1687" s="50" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="1688" spans="1:1">
       <c r="A1688" s="50" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="1689" spans="1:1">
       <c r="A1689" s="50" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="1690" spans="1:1">
       <c r="A1690" s="50" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="1691" spans="1:1">
       <c r="A1691" s="50" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="1692" spans="1:1">
       <c r="A1692" s="50" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="1693" spans="1:1">
       <c r="A1693" s="50" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="1694" spans="1:1">
       <c r="A1694" s="50" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="1695" spans="1:1">
       <c r="A1695" s="50" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="1696" spans="1:1">
       <c r="A1696" s="50" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="1697" spans="1:1">
       <c r="A1697" s="50" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="1698" spans="1:1">
       <c r="A1698" s="50" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="1699" spans="1:1">
       <c r="A1699" s="50" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="1700" spans="1:1">
       <c r="A1700" s="50" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="1701" spans="1:1">
       <c r="A1701" s="50" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="1702" spans="1:1">
       <c r="A1702" s="50" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="1703" spans="1:1">
       <c r="A1703" s="50" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="1704" spans="1:1">
       <c r="A1704" s="50" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="1705" spans="1:1">
       <c r="A1705" s="50" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="1706" spans="1:1">
       <c r="A1706" s="50" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="1707" spans="1:1">
       <c r="A1707" s="50" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="1708" spans="1:1">
       <c r="A1708" s="50" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="1709" spans="1:1">
       <c r="A1709" s="50" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="1710" spans="1:1">
       <c r="A1710" s="50" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="1711" spans="1:1">
       <c r="A1711" s="50" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="1712" spans="1:1">
       <c r="A1712" s="50" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="1713" spans="1:1">
       <c r="A1713" s="50" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="1714" spans="1:1">
       <c r="A1714" s="50" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="1715" spans="1:1">
       <c r="A1715" s="50" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="1716" spans="1:1">
       <c r="A1716" s="50" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="1717" spans="1:1">
       <c r="A1717" s="50" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="1718" spans="1:1">
       <c r="A1718" s="50" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="1719" spans="1:1">
       <c r="A1719" s="50" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="1720" spans="1:1">
       <c r="A1720" s="50" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="1721" spans="1:1">
       <c r="A1721" s="50" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="1722" spans="1:1">
       <c r="A1722" s="50" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="1723" spans="1:1">
       <c r="A1723" s="50" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="1724" spans="1:1">
       <c r="A1724" s="50" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="1725" spans="1:1">
       <c r="A1725" s="50" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="1726" spans="1:1">
       <c r="A1726" s="50" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="1727" spans="1:1">
       <c r="A1727" s="50" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="1728" spans="1:1">
       <c r="A1728" s="50" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="1729" spans="1:1">
       <c r="A1729" s="50" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="1730" spans="1:1">
       <c r="A1730" s="50" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="1731" spans="1:1">
       <c r="A1731" s="50" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="1732" spans="1:1">
       <c r="A1732" s="50" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="1733" spans="1:1">
       <c r="A1733" s="50" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="1734" spans="1:1">
       <c r="A1734" s="50" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="1735" spans="1:1">
       <c r="A1735" s="50" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="1736" spans="1:1">
       <c r="A1736" s="50" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="1737" spans="1:1">
       <c r="A1737" s="50" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="1738" spans="1:1">
       <c r="A1738" s="50" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="1739" spans="1:1">
       <c r="A1739" s="50" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="1740" spans="1:1">
       <c r="A1740" s="50" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="1741" spans="1:1">
       <c r="A1741" s="50" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="1742" spans="1:1">
       <c r="A1742" s="50" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="1743" spans="1:1">
       <c r="A1743" s="50" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="1744" spans="1:1">
       <c r="A1744" s="50" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="1745" spans="1:1">
       <c r="A1745" s="50" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="1746" spans="1:1">
       <c r="A1746" s="50" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="1747" spans="1:1">
       <c r="A1747" s="50" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="1748" spans="1:1">
       <c r="A1748" s="50" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="1749" spans="1:1">
       <c r="A1749" s="50" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="1750" spans="1:1">
       <c r="A1750" s="50" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="1751" spans="1:1">
       <c r="A1751" s="50" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="1752" spans="1:1">
       <c r="A1752" s="50" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="1753" spans="1:1">
       <c r="A1753" s="50" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="1754" spans="1:1">
       <c r="A1754" s="50" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="1755" spans="1:1">
       <c r="A1755" s="50" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="1756" spans="1:1">
       <c r="A1756" s="50" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="1757" spans="1:1">
       <c r="A1757" s="50" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="1758" spans="1:1">
       <c r="A1758" s="50" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
     </row>
     <row r="1759" spans="1:1">
       <c r="A1759" s="50" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="1760" spans="1:1">
       <c r="A1760" s="50" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
     </row>
     <row r="1761" spans="1:1">
       <c r="A1761" s="50" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="1762" spans="1:1">
       <c r="A1762" s="50" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="1763" spans="1:1">
       <c r="A1763" s="50" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="1764" spans="1:1">
       <c r="A1764" s="50" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
     </row>
     <row r="1765" spans="1:1">
       <c r="A1765" s="50" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="1766" spans="1:1">
       <c r="A1766" s="50" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
     </row>
     <row r="1767" spans="1:1">
       <c r="A1767" s="50" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
     </row>
     <row r="1768" spans="1:1">
       <c r="A1768" s="50" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="1769" spans="1:1">
       <c r="A1769" s="50" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="1770" spans="1:1">
       <c r="A1770" s="50" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="1771" spans="1:1">
       <c r="A1771" s="50" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
     </row>
     <row r="1772" spans="1:1">
       <c r="A1772" s="50" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
     </row>
     <row r="1773" spans="1:1">
       <c r="A1773" s="50" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
     </row>
     <row r="1774" spans="1:1">
       <c r="A1774" s="50" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
     </row>
     <row r="1775" spans="1:1">
       <c r="A1775" s="50" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="1776" spans="1:1">
       <c r="A1776" s="50" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="1777" spans="1:1">
       <c r="A1777" s="50" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="1778" spans="1:1">
       <c r="A1778" s="50" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="1779" spans="1:1">
       <c r="A1779" s="50" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="1780" spans="1:1">
       <c r="A1780" s="50" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
     </row>
     <row r="1781" spans="1:1">
       <c r="A1781" s="50" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="1782" spans="1:1">
       <c r="A1782" s="50" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="1783" spans="1:1">
       <c r="A1783" s="50" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="1784" spans="1:1">
       <c r="A1784" s="50" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
     </row>
     <row r="1785" spans="1:1">
       <c r="A1785" s="50" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="1786" spans="1:1">
       <c r="A1786" s="50" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
     </row>
     <row r="1787" spans="1:1">
       <c r="A1787" s="50" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="1788" spans="1:1">
       <c r="A1788" s="50" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
     </row>
     <row r="1789" spans="1:1">
       <c r="A1789" s="50" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
     </row>
     <row r="1790" spans="1:1">
       <c r="A1790" s="50" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="1791" spans="1:1">
       <c r="A1791" s="50" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="1792" spans="1:1">
       <c r="A1792" s="50" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
     </row>
     <row r="1793" spans="1:1">
       <c r="A1793" s="50" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="1794" spans="1:1">
       <c r="A1794" s="50" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
     </row>
     <row r="1795" spans="1:1">
       <c r="A1795" s="50" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="1796" spans="1:1">
       <c r="A1796" s="50" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="1797" spans="1:1">
       <c r="A1797" s="50" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
     </row>
     <row r="1798" spans="1:1">
       <c r="A1798" s="50" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
     </row>
     <row r="1799" spans="1:1">
       <c r="A1799" s="50" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="1800" spans="1:1">
       <c r="A1800" s="50" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="1801" spans="1:1">
       <c r="A1801" s="50" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="1802" spans="1:1">
       <c r="A1802" s="50" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="1803" spans="1:1">
       <c r="A1803" s="50" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="1804" spans="1:1">
       <c r="A1804" s="50" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="1805" spans="1:1">
       <c r="A1805" s="50" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="1806" spans="1:1">
       <c r="A1806" s="50" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="1807" spans="1:1">
       <c r="A1807" s="50" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="1808" spans="1:1">
       <c r="A1808" s="50" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="1809" spans="1:1">
       <c r="A1809" s="50" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
     </row>
     <row r="1810" spans="1:1">
       <c r="A1810" s="50" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="1811" spans="1:1">
       <c r="A1811" s="50" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="1812" spans="1:1">
       <c r="A1812" s="50" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="1813" spans="1:1">
       <c r="A1813" s="50" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
     </row>
     <row r="1814" spans="1:1">
       <c r="A1814" s="50" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
    